<commit_message>
Save results from Baseline 2010-18 run.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E31F432-6B0E-444E-8B99-B0FA4A39B0C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE89A0A-CE7E-45AE-9FA0-376E635179C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25260" yWindow="2310" windowWidth="24030" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Year</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Baseline_2010_c38 9/6/20</t>
+  </si>
+  <si>
+    <t>Baseline_2010-18_c45 9/19/20</t>
+  </si>
+  <si>
+    <t>2010-18</t>
   </si>
 </sst>
 </file>
@@ -945,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,6 +1236,62 @@
         <v>2010</v>
       </c>
     </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1138.6194117777777</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G7" s="2">
+        <v>327.78053433333326</v>
+      </c>
+      <c r="H7" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I7" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="J7" s="2">
+        <v>769.26639155555551</v>
+      </c>
+      <c r="K7" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1374.8233372222221</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1142.9502087777778</v>
+      </c>
+      <c r="N7" s="3">
+        <v>4918.1879612222219</v>
+      </c>
+      <c r="O7" s="3">
+        <v>27227.338324777778</v>
+      </c>
+      <c r="P7" s="4">
+        <v>-4.72741111111111E-2</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>-3.8888888888888877E-5</v>
+      </c>
+      <c r="R7" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add files related to skill assessment.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE89A0A-CE7E-45AE-9FA0-376E635179C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576F0819-2423-42FF-ABA9-0254D15C1174}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33795" yWindow="-6390" windowWidth="23550" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2010" sheetId="1" r:id="rId1"/>
+    <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Year</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>2010-18</t>
+  </si>
+  <si>
+    <t>Baseline_C63_2010-18</t>
   </si>
 </sst>
 </file>
@@ -951,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,59 +1239,171 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>2010</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1044.2558590000001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.255063</v>
+      </c>
+      <c r="G6" s="2">
+        <v>327.58108499999997</v>
+      </c>
+      <c r="H6" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I6" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="J6" s="2">
+        <v>814.39868200000001</v>
+      </c>
+      <c r="K6" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1291.7937010000001</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1165.4429929999999</v>
+      </c>
+      <c r="N6" s="3">
+        <v>7166.0473629999997</v>
+      </c>
+      <c r="O6" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="P6" s="2">
+        <v>-0.464943</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>-1.3799999999999999E-4</v>
+      </c>
+      <c r="R6">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="2">
         <v>1138.6194117777777</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="2">
         <v>1901.5157334444443</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="2">
         <v>1.0119255555555557</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G8" s="2">
         <v>327.78053433333326</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H8" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I8" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J8" s="2">
         <v>769.26639155555551</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K8" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L8" s="2">
         <v>1374.8233372222221</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M8" s="2">
         <v>1142.9502087777778</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N8" s="3">
         <v>4918.1879612222219</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O8" s="3">
         <v>27227.338324777778</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P8" s="4">
         <v>-4.72741111111111E-2</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q8" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1138.6194117777777</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G9" s="2">
+        <v>327.78053433333326</v>
+      </c>
+      <c r="H9" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I9" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="J9" s="2">
+        <v>769.26639155555551</v>
+      </c>
+      <c r="K9" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1374.8233372222221</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1142.9502087777778</v>
+      </c>
+      <c r="N9" s="3">
+        <v>4918.1879612222219</v>
+      </c>
+      <c r="O9" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="P9" s="4">
+        <v>-4.72741111111111E-2</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>-3.8888888888888877E-5</v>
+      </c>
+      <c r="R9" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flow.cpp, .h, ReachRouting.cpp - Assimilate Reach segments into Reach subreaches.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1944AE36-9F6E-4F0D-A414-5A69F3FE106D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87673189-8EE8-423A-89C7-2BDEB871A35F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33390" yWindow="-3120" windowWidth="23085" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -968,7 +968,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:O8"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,7 +1419,18 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q9" s="4"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
flow2010.ic - This one was made by running Baseline for 2000-09. Flow.cpp, .h - Add CalcTotDailyEvapFromReaches() and m_totEvapFromReachesYr_m3 to FlowModel. WaterRights.cpp - Add the evap from reaches into the AET total in the AltWM Quick Check report.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A676777-E05E-4389-A4D7-771651257016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BDEE07-6913-4196-B1EE-BF94AA033C29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33390" yWindow="-3120" windowWidth="23085" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Year</t>
   </si>
@@ -117,15 +118,20 @@
   </si>
   <si>
     <t>Baseline 2010 C71</t>
+  </si>
+  <si>
+    <t>Baseline 2010 C81</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C81</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -604,7 +610,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -612,7 +618,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -968,18 +973,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="P12" sqref="P12:P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1032,7 +1037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1085,7 +1090,7 @@
         <v>-4.8000000000000001E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1141,7 +1146,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1197,7 +1202,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1253,7 +1258,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1309,7 +1314,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1355,7 +1360,7 @@
       <c r="O7" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="2">
         <v>-0.464943</v>
       </c>
       <c r="Q7" s="4">
@@ -1365,7 +1370,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1411,7 +1416,7 @@
       <c r="O8" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="2">
         <v>-0.473854</v>
       </c>
       <c r="Q8" s="4">
@@ -1421,7 +1426,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1461,13 +1466,13 @@
       <c r="M9" s="2">
         <v>1165.4420170000001</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="3">
         <v>7166.0351559999999</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="2">
         <v>-0.473854</v>
       </c>
       <c r="Q9" s="4">
@@ -1477,23 +1482,63 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="Q10" s="4"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>2010</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1034.060303</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.255063</v>
+      </c>
+      <c r="G10" s="2">
+        <v>327.58108499999997</v>
+      </c>
+      <c r="H10" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I10" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="J10" s="2">
+        <v>814.38360599999999</v>
+      </c>
+      <c r="K10" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1292.8286129999999</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1158.413818</v>
+      </c>
+      <c r="N10" s="3">
+        <v>7105.0297849999997</v>
+      </c>
+      <c r="O10" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="P10" s="2">
+        <v>3.7212749999999999</v>
+      </c>
+      <c r="Q10">
+        <v>1.106E-3</v>
+      </c>
+      <c r="R10">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1509,7 +1554,7 @@
       <c r="O11" s="2"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1555,7 +1600,7 @@
       <c r="O12" s="3">
         <v>27227.338324777778</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="2">
         <v>-4.72741111111111E-2</v>
       </c>
       <c r="Q12" s="4">
@@ -1565,7 +1610,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1611,7 +1656,7 @@
       <c r="O13" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="P13" s="4">
+      <c r="P13" s="2">
         <v>-4.72741111111111E-2</v>
       </c>
       <c r="Q13" s="4">
@@ -1621,7 +1666,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1667,11 +1712,67 @@
       <c r="O14" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="P14" s="4">
+      <c r="P14" s="2">
         <v>-4.72741111111111E-2</v>
       </c>
       <c r="Q14" s="4">
         <v>-3.8888888888888877E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1135.8478461111113</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G15" s="2">
+        <v>327.78053433333326</v>
+      </c>
+      <c r="H15" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I15" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="J15" s="2">
+        <v>769.26112866666654</v>
+      </c>
+      <c r="K15" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1378.3211942222222</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1141.5044894444445</v>
+      </c>
+      <c r="N15" s="3">
+        <v>4878.4023980000002</v>
+      </c>
+      <c r="O15" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="P15" s="2">
+        <v>4.7711666666666668</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="R15" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clackamas/flow2010.ic - Made from Baseline_2000-09_C82plus. Flow_Clackamas.xml - Remove initial_conditions field from <flow_model> block. Add "FLOW Monthly Clackamas flow skill assessment" and "FLOW Monthly Clackamas temperature skill assessment" reports. Reach_Clackamas.dbf - Add some new attributes.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BDEE07-6913-4196-B1EE-BF94AA033C29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBEEE69-E2C7-4841-BE13-F42760B3B49F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="40515" yWindow="-2895" windowWidth="9960" windowHeight="4635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Year</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C81</t>
+  </si>
+  <si>
+    <t>Baseline 2010 C82</t>
   </si>
 </sst>
 </file>
@@ -973,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12:P14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1539,83 +1542,70 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="Q11" s="4"/>
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11">
+        <v>2010</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.255063</v>
+      </c>
+      <c r="G11" s="2">
+        <v>327.58108499999997</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="J11" s="2">
+        <v>814.49517800000001</v>
+      </c>
+      <c r="K11" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1305.1243899999999</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1201.781982</v>
+      </c>
+      <c r="N11" s="3">
+        <v>7126.6015630000002</v>
+      </c>
+      <c r="O11" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="P11" s="2">
+        <v>3.3577499999999998</v>
+      </c>
+      <c r="Q11">
+        <v>9.8200000000000002E-4</v>
+      </c>
+      <c r="R11">
+        <v>2010</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G12" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H12" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I12" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="J12" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="K12" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="L12" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="M12" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="N12" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="O12" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="P12" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="Q12" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="R12" t="s">
-        <v>23</v>
-      </c>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
@@ -1654,7 +1644,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="O13" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="P13" s="2">
         <v>-4.72741111111111E-2</v>
@@ -1671,7 +1661,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
@@ -1717,6 +1707,9 @@
       </c>
       <c r="Q14" s="4">
         <v>-3.8888888888888877E-5</v>
+      </c>
+      <c r="R14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -1724,13 +1717,13 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E15" s="2">
         <v>1901.5157334444443</v>
@@ -1748,30 +1741,83 @@
         <v>8.145128999999999</v>
       </c>
       <c r="J15" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="K15" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="L15" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="M15" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="N15" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="O15" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="P15" s="2">
+        <v>-4.72741111111111E-2</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>-3.8888888888888877E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1135.8478461111113</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G16" s="2">
+        <v>327.78053433333326</v>
+      </c>
+      <c r="H16" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I16" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="J16" s="2">
+        <v>769.26112866666654</v>
+      </c>
+      <c r="K16" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1378.3211942222222</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1141.5044894444445</v>
+      </c>
+      <c r="N16" s="3">
+        <v>4878.4023980000002</v>
+      </c>
+      <c r="O16" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="P16" s="2">
         <v>4.7711666666666668</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="Q16" s="4">
         <v>1.4151111111111109E-3</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R16" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flow.cpp - Add logic to refrain from writing warning messages when the subreach volume values from an IC file are a tiny bit smaller than the minimum volumes for the subreaches.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBEEE69-E2C7-4841-BE13-F42760B3B49F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41FD485-B03C-426E-959B-03F3F5E94708}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="40515" yWindow="-2895" windowWidth="9960" windowHeight="4635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Year</t>
   </si>
@@ -127,6 +126,12 @@
   </si>
   <si>
     <t>Baseline 2010 C82</t>
+  </si>
+  <si>
+    <t>Baseline_2010_0.4.0</t>
+  </si>
+  <si>
+    <t>Baseline_2010-18_0.4.0</t>
   </si>
 </sst>
 </file>
@@ -976,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1598,70 +1603,83 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C12" s="3"/>
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>2010</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.255063</v>
+      </c>
+      <c r="G12" s="2">
+        <v>327.58108499999997</v>
+      </c>
+      <c r="H12" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I12" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="J12" s="2">
+        <v>814.49517800000001</v>
+      </c>
+      <c r="K12" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1305.1243899999999</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1201.781982</v>
+      </c>
+      <c r="N12" s="3">
+        <v>7126.6015630000002</v>
+      </c>
+      <c r="O12" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="P12" s="2">
+        <v>3.3577499999999998</v>
+      </c>
+      <c r="Q12">
+        <v>9.8200000000000002E-4</v>
+      </c>
+      <c r="R12">
+        <v>2010</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G13" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H13" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I13" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="J13" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="K13" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="L13" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="M13" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="N13" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="O13" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="P13" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="R13" t="s">
-        <v>23</v>
-      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
@@ -1700,7 +1718,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="O14" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="P14" s="2">
         <v>-4.72741111111111E-2</v>
@@ -1717,7 +1735,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
@@ -1763,6 +1781,9 @@
       </c>
       <c r="Q15" s="4">
         <v>-3.8888888888888877E-5</v>
+      </c>
+      <c r="R15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1770,13 +1791,13 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E16" s="2">
         <v>1901.5157334444443</v>
@@ -1794,31 +1815,137 @@
         <v>8.145128999999999</v>
       </c>
       <c r="J16" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="K16" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="L16" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="M16" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="N16" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="O16" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="P16" s="2">
+        <v>-4.72741111111111E-2</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>-3.8888888888888877E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1135.8478461111113</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G17" s="2">
+        <v>327.78053433333326</v>
+      </c>
+      <c r="H17" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I17" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="J17" s="2">
+        <v>769.26112866666654</v>
+      </c>
+      <c r="K17" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1378.3211942222222</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1141.5044894444445</v>
+      </c>
+      <c r="N17" s="3">
+        <v>4878.4023980000002</v>
+      </c>
+      <c r="O17" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="P17" s="2">
         <v>4.7711666666666668</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="Q17" s="4">
         <v>1.4151111111111109E-3</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R17" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1161.1572335555554</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G18" s="2">
+        <v>327.78053433333326</v>
+      </c>
+      <c r="H18" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I18" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="J18" s="2">
+        <v>769.37008311111106</v>
+      </c>
+      <c r="K18" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1383.6045464444442</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1161.284607111111</v>
+      </c>
+      <c r="N18" s="3">
+        <v>4883.9277073333324</v>
+      </c>
+      <c r="O18" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="P18" s="2">
+        <v>4.6342037777777776</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a column for water added by the FlowModel to the Quick Check report. This restores the mass balance discrepancy figure to what it was before the stream temperature code was added, at least for Baseline McKenzie 2010. Flow.cpp, .h - Add FlowModel methods MagicReachWaterReport_m3() and MagicHRUwaterReport_m3(). WaterRights.cpp - Add a column for water added by the FlowModel to the Quick Check report.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41FD485-B03C-426E-959B-03F3F5E94708}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D975DBC1-E54E-4CB3-879C-DEF13BC46C40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31725" yWindow="-7080" windowWidth="23565" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>Year</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Baseline_2010-18_0.4.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> added reach water (fraction)</t>
+  </si>
+  <si>
+    <t>Baseline_2010_C88+ 10/31/20</t>
   </si>
 </sst>
 </file>
@@ -981,18 +987,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="20" max="20" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1044,8 +1051,11 @@
       <c r="R1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1098,7 +1108,7 @@
         <v>-4.8000000000000001E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1154,7 +1164,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1210,7 +1220,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1266,7 +1276,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1322,7 +1332,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1378,7 +1388,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1434,7 +1444,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1490,7 +1500,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1546,7 +1556,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1602,7 +1612,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1658,84 +1668,91 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13">
+        <v>2010</v>
+      </c>
+      <c r="D13">
+        <v>1090.199341</v>
+      </c>
+      <c r="E13">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F13">
+        <v>1.255063</v>
+      </c>
+      <c r="G13">
+        <v>327.58108499999997</v>
+      </c>
+      <c r="H13">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I13">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="J13">
+        <v>814.49517800000001</v>
+      </c>
+      <c r="K13">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="L13">
+        <v>1305.1243899999999</v>
+      </c>
+      <c r="M13">
+        <v>1201.781982</v>
+      </c>
+      <c r="N13">
+        <v>7126.6015630000002</v>
+      </c>
+      <c r="O13">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="P13">
+        <v>3.3577499999999998</v>
+      </c>
+      <c r="Q13">
+        <v>9.8200000000000002E-4</v>
+      </c>
+      <c r="R13">
+        <v>2010</v>
+      </c>
+      <c r="S13">
+        <v>1.1180000000000001E-3</v>
+      </c>
+      <c r="T13" s="4">
+        <f>Q13-S13</f>
+        <v>-1.3600000000000005E-4</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G14" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H14" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I14" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="J14" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="K14" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="M14" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="N14" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="O14" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="P14" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="Q14" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="R14" t="s">
-        <v>23</v>
-      </c>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
@@ -1774,7 +1791,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="O15" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="P15" s="2">
         <v>-4.72741111111111E-2</v>
@@ -1786,12 +1803,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -1837,6 +1854,9 @@
       </c>
       <c r="Q16" s="4">
         <v>-3.8888888888888877E-5</v>
+      </c>
+      <c r="R16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
@@ -1844,13 +1864,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E17" s="2">
         <v>1901.5157334444443</v>
@@ -1868,31 +1888,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="J17" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="K17" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="L17" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="M17" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="N17" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="O17" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="P17" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="Q17" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="R17" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
@@ -1900,13 +1917,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E18" s="2">
         <v>1901.5157334444443</v>
@@ -1924,27 +1941,83 @@
         <v>8.145128999999999</v>
       </c>
       <c r="J18" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="K18" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="L18" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="M18" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="N18" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="O18" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="P18" s="2">
+        <v>4.7711666666666668</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="R18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1161.1572335555554</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G19" s="2">
+        <v>327.78053433333326</v>
+      </c>
+      <c r="H19" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I19" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="J19" s="2">
+        <v>769.37008311111106</v>
+      </c>
+      <c r="K19" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1383.6045464444442</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1161.284607111111</v>
+      </c>
+      <c r="N19" s="3">
+        <v>4883.9277073333324</v>
+      </c>
+      <c r="O19" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="P19" s="2">
         <v>4.6342037777777776</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="Q19" s="4">
         <v>1.3650000000000001E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flow_McKenzie.xml - Add flux for springs feeding Clear Lake at 724,180 m3/day to 23773373. Add 23773363 to flow skill assessment report. Add yearly versions of flow and temperature skill assessment reports. FluxExpr.cpp - Add temp_C field to <flux> block in Flow XML file. GlobalMethods.h - Add member m_temp_C to class FluxExpr.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D975DBC1-E54E-4CB3-879C-DEF13BC46C40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C12A657-5CD6-4549-B4FC-0A567E2FE239}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31725" yWindow="-7080" windowWidth="23565" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31725" yWindow="-7080" windowWidth="23565" windowHeight="13065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>Year</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>Baseline_2010_C88+ 10/31/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> water added by FlowModel (mm)</t>
+  </si>
+  <si>
+    <t>Baseline_2010-18_C89+</t>
+  </si>
+  <si>
+    <t>Baseline_2010_C89</t>
   </si>
 </sst>
 </file>
@@ -987,19 +996,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="20" max="20" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1022,40 +1032,43 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1080,35 +1093,36 @@
       <c r="H2" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>771.79455600000006</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>91.637016000000003</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>1252.926514</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>1928.181274</v>
       </c>
-      <c r="N2" s="3">
+      <c r="O2" s="3">
         <v>0</v>
       </c>
-      <c r="O2" s="3">
+      <c r="P2" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>-0.19644900000000001</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="4">
         <v>-4.8000000000000001E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1133,38 +1147,39 @@
       <c r="H3" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>814.39868200000001</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>93.229797000000005</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>1291.794678</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>1165.4429929999999</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>7166.1196289999998</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>-0.46396599999999999</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="R3" s="4">
         <v>-1.3799999999999999E-4</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>2010</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1189,38 +1204,39 @@
       <c r="H4" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>814.39868200000001</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>93.229797000000005</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>1291.794678</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>1165.4429929999999</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>7166.1196289999998</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P4" s="2">
+      <c r="Q4" s="2">
         <v>-0.46396599999999999</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="R4" s="4">
         <v>-1.3799999999999999E-4</v>
       </c>
-      <c r="R4" s="3">
+      <c r="S4" s="3">
         <v>2010</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1245,38 +1261,39 @@
       <c r="H5" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>814.39868200000001</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>93.229797000000005</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>1291.794678</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>1165.4429929999999</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="3">
         <v>7166.1196289999998</v>
       </c>
-      <c r="O5" s="3">
+      <c r="P5" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <v>-0.46396599999999999</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="R5" s="4">
         <v>-1.3799999999999999E-4</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1301,38 +1318,39 @@
       <c r="H6" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>814.39868200000001</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>93.229797000000005</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>1291.7937010000001</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>1165.4429929999999</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="3">
         <v>7166.0473629999997</v>
       </c>
-      <c r="O6" s="3">
+      <c r="P6" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <v>-0.464943</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="R6" s="4">
         <v>-1.3799999999999999E-4</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1357,38 +1375,39 @@
       <c r="H7" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>814.39868200000001</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>93.229797000000005</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>1291.7937010000001</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>1165.4429929999999</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="3">
         <v>7166.0473629999997</v>
       </c>
-      <c r="O7" s="3">
+      <c r="P7" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P7" s="2">
+      <c r="Q7" s="2">
         <v>-0.464943</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="R7" s="4">
         <v>-1.3799999999999999E-4</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>2010</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1413,38 +1432,39 @@
       <c r="H8" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>814.39868200000001</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>93.229797000000005</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>1291.7857670000001</v>
       </c>
-      <c r="M8" s="2">
+      <c r="N8" s="2">
         <v>1165.4420170000001</v>
       </c>
-      <c r="N8" s="3">
+      <c r="O8" s="3">
         <v>7166.0351559999999</v>
       </c>
-      <c r="O8" s="3">
+      <c r="P8" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P8" s="2">
+      <c r="Q8" s="2">
         <v>-0.473854</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="R8" s="4">
         <v>-1.3999999999999999E-4</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>2010</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1469,38 +1489,39 @@
       <c r="H9" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>814.39868200000001</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>93.229797000000005</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>1291.7857670000001</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>1165.4420170000001</v>
       </c>
-      <c r="N9" s="3">
+      <c r="O9" s="3">
         <v>7166.0351559999999</v>
       </c>
-      <c r="O9" s="3">
+      <c r="P9" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P9" s="2">
+      <c r="Q9" s="2">
         <v>-0.473854</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="R9" s="4">
         <v>-1.3999999999999999E-4</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1525,38 +1546,39 @@
       <c r="H10" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="2"/>
+      <c r="J10" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>814.38360599999999</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>93.229797000000005</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>1292.8286129999999</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>1158.413818</v>
       </c>
-      <c r="N10" s="3">
+      <c r="O10" s="3">
         <v>7105.0297849999997</v>
       </c>
-      <c r="O10" s="3">
+      <c r="P10" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P10" s="2">
+      <c r="Q10" s="2">
         <v>3.7212749999999999</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>1.106E-3</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>2010</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1581,38 +1603,39 @@
       <c r="H11" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>814.49517800000001</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>93.229797000000005</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>1305.1243899999999</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>1201.781982</v>
       </c>
-      <c r="N11" s="3">
+      <c r="O11" s="3">
         <v>7126.6015630000002</v>
       </c>
-      <c r="O11" s="3">
+      <c r="P11" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P11" s="2">
+      <c r="Q11" s="2">
         <v>3.3577499999999998</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>9.8200000000000002E-4</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>2010</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1637,38 +1660,39 @@
       <c r="H12" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <v>814.49517800000001</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>93.229797000000005</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <v>1305.1243899999999</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <v>1201.781982</v>
       </c>
-      <c r="N12" s="3">
+      <c r="O12" s="3">
         <v>7126.6015630000002</v>
       </c>
-      <c r="O12" s="3">
+      <c r="P12" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P12" s="2">
+      <c r="Q12" s="2">
         <v>3.3577499999999998</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>9.8200000000000002E-4</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>2010</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1678,137 +1702,143 @@
       <c r="C13">
         <v>2010</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>1090.199341</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>1990.4676509999999</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>1.255063</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>327.58108499999997</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="J13">
+      <c r="K13" s="2">
         <v>814.49517800000001</v>
       </c>
-      <c r="K13">
+      <c r="L13" s="2">
         <v>93.229797000000005</v>
       </c>
-      <c r="L13">
+      <c r="M13" s="2">
         <v>1305.1243899999999</v>
       </c>
-      <c r="M13">
+      <c r="N13" s="2">
         <v>1201.781982</v>
       </c>
-      <c r="N13">
+      <c r="O13" s="3">
         <v>7126.6015630000002</v>
       </c>
-      <c r="O13">
+      <c r="P13" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="P13">
+      <c r="Q13" s="2">
         <v>3.3577499999999998</v>
       </c>
-      <c r="Q13">
+      <c r="R13" s="4">
         <v>9.8200000000000002E-4</v>
       </c>
-      <c r="R13">
-        <v>2010</v>
-      </c>
       <c r="S13">
+        <v>2010</v>
+      </c>
+      <c r="T13">
         <v>1.1180000000000001E-3</v>
       </c>
-      <c r="T13" s="4">
-        <f>Q13-S13</f>
+      <c r="U13" s="4">
+        <f>R13-T13</f>
         <v>-1.3600000000000005E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14">
+        <v>2010</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.255063</v>
+      </c>
+      <c r="G14" s="2">
+        <v>327.58108499999997</v>
+      </c>
+      <c r="H14" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3.8222339999999999</v>
+      </c>
+      <c r="J14" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K14" s="2">
+        <v>814.49517800000001</v>
+      </c>
+      <c r="L14" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1305.1243899999999</v>
+      </c>
+      <c r="N14" s="2">
+        <v>1201.781982</v>
+      </c>
+      <c r="O14" s="3">
+        <v>7126.6015630000002</v>
+      </c>
+      <c r="P14" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>-0.46448400000000001</v>
+      </c>
+      <c r="R14" s="4">
+        <v>-1.36E-4</v>
+      </c>
+      <c r="S14">
+        <v>2010</v>
+      </c>
+      <c r="U14" s="4"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G15" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H15" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I15" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="J15" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="K15" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="L15" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="M15" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="N15" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="O15" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="P15" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="Q15" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="R15" t="s">
-        <v>23</v>
-      </c>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -1828,43 +1858,44 @@
       <c r="H16" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>769.26639155555551</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>1374.8233372222221</v>
       </c>
-      <c r="M16" s="2">
+      <c r="N16" s="2">
         <v>1142.9502087777778</v>
       </c>
-      <c r="N16" s="3">
+      <c r="O16" s="3">
         <v>4918.1879612222219</v>
       </c>
-      <c r="O16" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="P16" s="2">
+      <c r="P16" s="3">
+        <v>27227.338324777778</v>
+      </c>
+      <c r="Q16" s="2">
         <v>-4.72741111111111E-2</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="R16" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
@@ -1884,46 +1915,50 @@
       <c r="H17" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <v>769.26639155555551</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="L17" s="2">
+      <c r="M17" s="2">
         <v>1374.8233372222221</v>
       </c>
-      <c r="M17" s="2">
+      <c r="N17" s="2">
         <v>1142.9502087777778</v>
       </c>
-      <c r="N17" s="3">
+      <c r="O17" s="3">
         <v>4918.1879612222219</v>
       </c>
-      <c r="O17" s="3">
+      <c r="P17" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="P17" s="2">
+      <c r="Q17" s="2">
         <v>-4.72741111111111E-2</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="R17" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S17" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E18" s="2">
         <v>1901.5157334444443</v>
@@ -1937,49 +1972,47 @@
       <c r="H18" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="2"/>
+      <c r="J18" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="J18" s="2">
-        <v>769.26112866666654</v>
-      </c>
       <c r="K18" s="2">
+        <v>769.26639155555551</v>
+      </c>
+      <c r="L18" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="L18" s="2">
-        <v>1378.3211942222222</v>
-      </c>
       <c r="M18" s="2">
-        <v>1141.5044894444445</v>
-      </c>
-      <c r="N18" s="3">
-        <v>4878.4023980000002</v>
+        <v>1374.8233372222221</v>
+      </c>
+      <c r="N18" s="2">
+        <v>1142.9502087777778</v>
       </c>
       <c r="O18" s="3">
+        <v>4918.1879612222219</v>
+      </c>
+      <c r="P18" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="P18" s="2">
-        <v>4.7711666666666668</v>
-      </c>
-      <c r="Q18" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="R18" t="s">
-        <v>23</v>
+      <c r="Q18" s="2">
+        <v>-4.72741111111111E-2</v>
+      </c>
+      <c r="R18" s="4">
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E19" s="2">
         <v>1901.5157334444443</v>
@@ -1993,32 +2026,149 @@
       <c r="H19" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="J19" s="2">
+      <c r="K19" s="2">
+        <v>769.26112866666654</v>
+      </c>
+      <c r="L19" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1378.3211942222222</v>
+      </c>
+      <c r="N19" s="2">
+        <v>1141.5044894444445</v>
+      </c>
+      <c r="O19" s="3">
+        <v>4878.4023980000002</v>
+      </c>
+      <c r="P19" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>4.7711666666666668</v>
+      </c>
+      <c r="R19" s="4">
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1161.1572335555554</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G20" s="2">
+        <v>327.78053433333326</v>
+      </c>
+      <c r="H20" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K20" s="2">
         <v>769.37008311111106</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L20" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="L19" s="2">
+      <c r="M20" s="2">
         <v>1383.6045464444442</v>
       </c>
-      <c r="M19" s="2">
+      <c r="N20" s="2">
         <v>1161.284607111111</v>
       </c>
-      <c r="N19" s="3">
+      <c r="O20" s="3">
         <v>4883.9277073333324</v>
       </c>
-      <c r="O19" s="3">
+      <c r="P20" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="P19" s="2">
+      <c r="Q20" s="2">
         <v>4.6342037777777776</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="R20" s="4">
         <v>1.3650000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1161.1644491111113</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G21" s="2">
+        <v>354.15221155555554</v>
+      </c>
+      <c r="H21" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I21" s="2">
+        <v>4.6817598888888901</v>
+      </c>
+      <c r="J21" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K21" s="2">
+        <v>769.36972377777772</v>
+      </c>
+      <c r="L21" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1437.0445828888887</v>
+      </c>
+      <c r="N21" s="2">
+        <v>1161.2873196666667</v>
+      </c>
+      <c r="O21" s="3">
+        <v>4883.9277073333324</v>
+      </c>
+      <c r="P21" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>27.015940777777772</v>
+      </c>
+      <c r="R21" s="4">
+        <v>7.9151111111111106E-3</v>
+      </c>
+      <c r="S21" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HBV.csv - Adjust ET_MULT for HBVCALIB 8, 9, 25, and 34. Flow_McKenzie.xml - Replace all earlier High Cascades groundwater fluxes with 1) Clear Lake 23773411 2,683,868 m3/day, 2) Lookout Creek 23773411 31,218 m3/day, and 3) Blue R at and above Tidbits Cr 23773429 138,240 m3/day.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83792699-071A-477F-9271-9209AF439F90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD3D387-BE4A-4C1D-A541-D123C1154BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31725" yWindow="-7080" windowWidth="23565" windowHeight="13065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31725" yWindow="-7080" windowWidth="23565" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
   <si>
     <t>Year</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Baseline_2010-18_C90+</t>
+  </si>
+  <si>
+    <t>Baseline_2010-18_C91</t>
   </si>
 </sst>
 </file>
@@ -999,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="A15" sqref="A15:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1820,85 +1823,88 @@
       <c r="U14" s="4"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>2010</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.255063</v>
+      </c>
+      <c r="G15" s="2">
+        <v>347.02185100000003</v>
+      </c>
+      <c r="H15" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I15" s="2">
+        <v>3.8222320000000001</v>
+      </c>
+      <c r="J15" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K15" s="2">
+        <v>814.49505599999998</v>
+      </c>
+      <c r="L15" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1324.5814210000001</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1201.767212</v>
+      </c>
+      <c r="O15" s="3">
+        <v>7126.6015630000002</v>
+      </c>
+      <c r="P15" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>-0.46310800000000002</v>
+      </c>
+      <c r="R15" s="4">
+        <v>-1.34E-4</v>
+      </c>
+      <c r="S15">
+        <v>2010</v>
+      </c>
+      <c r="U15" s="4"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G16" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H16" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K16" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L16" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M16" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N16" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O16" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P16" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R16" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S16" t="s">
-        <v>23</v>
-      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
@@ -1938,7 +1944,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P17" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q17" s="2">
         <v>-4.72741111111111E-2</v>
@@ -1955,7 +1961,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
@@ -2002,6 +2008,9 @@
       </c>
       <c r="R18" s="4">
         <v>-3.8888888888888877E-5</v>
+      </c>
+      <c r="S18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -2009,13 +2018,13 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E19" s="2">
         <v>1901.5157334444443</v>
@@ -2034,31 +2043,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K19" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L19" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M19" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N19" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O19" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P19" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q19" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R19" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S19" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
@@ -2066,13 +2072,13 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E20" s="2">
         <v>1901.5157334444443</v>
@@ -2091,28 +2097,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K20" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L20" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M20" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N20" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O20" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P20" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q20" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R20" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S20" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
@@ -2120,13 +2129,13 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
       </c>
       <c r="D21" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E21" s="2">
         <v>1901.5157334444443</v>
@@ -2135,28 +2144,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G21" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H21" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I21" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I21" s="2"/>
       <c r="J21" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K21" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L21" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M21" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N21" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O21" s="3">
         <v>4883.9277073333324</v>
@@ -2165,13 +2172,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q21" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R21" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S21" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
@@ -2179,13 +2183,13 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E22" s="2">
         <v>1901.5157334444443</v>
@@ -2194,28 +2198,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G22" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H22" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I22" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J22" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K22" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L22" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M22" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N22" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O22" s="3">
         <v>4883.9277073333324</v>
@@ -2224,12 +2228,130 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q22" s="2">
+        <v>27.015940777777772</v>
+      </c>
+      <c r="R22" s="4">
+        <v>7.9151111111111106E-3</v>
+      </c>
+      <c r="S22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1161.1599054444443</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G23" s="2">
+        <v>337.20870333333335</v>
+      </c>
+      <c r="H23" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I23" s="2">
+        <v>4.6813607777777788</v>
+      </c>
+      <c r="J23" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K23" s="2">
+        <v>769.36992711111111</v>
+      </c>
+      <c r="L23" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N23" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O23" s="3">
+        <v>4883.9277073333324</v>
+      </c>
+      <c r="P23" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q23" s="2">
         <v>9.9787694444444455</v>
       </c>
-      <c r="R22" s="4">
+      <c r="R23" s="4">
         <v>2.9230000000000003E-3</v>
       </c>
-      <c r="S22" t="s">
+      <c r="S23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1161.1599054444443</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G24" s="2">
+        <v>347.23312744444445</v>
+      </c>
+      <c r="H24" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I24" s="2">
+        <v>4.6813607777777788</v>
+      </c>
+      <c r="J24" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K24" s="2">
+        <v>769.36992711111111</v>
+      </c>
+      <c r="L24" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M24" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N24" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O24" s="3">
+        <v>4883.9277073333324</v>
+      </c>
+      <c r="P24" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R24" s="4">
+        <v>-3.7111111111111107E-5</v>
+      </c>
+      <c r="S24" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flow_McKenzie.xml - Add FLOW McKenzie Ditch analysis" report. Reach_McKenzie.dbf - Add attributes Q_MIN and IN_RUNOFF. Flow.cpp, .h - Add Reach attributes Q_MIN and IN_RUNOFF. Adjust the NominalLowFlow_cms() algorithm to lower the nominal low flows everywhere except in the headwater reaches.  This reduces the amount of magic water that the model adds to keep the little streams from going dry. Add logic to populate Reach layer attributes WIDTH_MIN, DEPTH_MIN, and Q_MIN.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3B144C-F588-4246-BFC5-2B4AEFD818ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886033CD-52CE-4020-952C-D8AFFDEDFAFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
   <si>
     <t>Year</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C98</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C106</t>
   </si>
 </sst>
 </file>
@@ -1020,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27:R27"/>
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2551,6 +2554,65 @@
         <v>23</v>
       </c>
     </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1186.9521077777779</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G28" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H28" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I28" s="5">
+        <v>12.968491888888888</v>
+      </c>
+      <c r="J28" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K28" s="2">
+        <v>645.94098588888892</v>
+      </c>
+      <c r="L28" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M28" s="2">
+        <v>1465.1962754444444</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1191.1222331111112</v>
+      </c>
+      <c r="O28" s="3">
+        <v>4695.8937716666669</v>
+      </c>
+      <c r="P28" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>1.3484236666666667</v>
+      </c>
+      <c r="R28" s="4">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S28" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
These notes cover changes in this version and in the previous version. Flow.cpp, Flow.h - Make Spring a friend class to FlowModel. Zero out the SPRING_CMS column in the Reach layer in FlowModel::InitRun() and StartStep(). Add FlowModel method GetReachFromCOMID(). FluxExpr.cpp, GlobalMethods.h - Simplify the Spring class.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1359BAD8-DE22-4B0A-A52B-9865550BD702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5429A2BB-06E0-497C-9228-BE0C79EE7E49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,8 +171,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -657,7 +658,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -668,6 +669,11 @@
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1023,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:R29"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2022,22 +2028,57 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="2"/>
+      <c r="C18">
+        <v>2010</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1.2021059999999999</v>
+      </c>
+      <c r="G18" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H18" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I18" s="2">
+        <v>4.714696</v>
+      </c>
+      <c r="J18" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K18" s="2">
+        <v>677.33367899999996</v>
+      </c>
+      <c r="L18" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1393.5979</v>
+      </c>
+      <c r="N18" s="2">
+        <v>1207.1701660000001</v>
+      </c>
+      <c r="O18" s="3">
+        <v>6798.6591799999997</v>
+      </c>
+      <c r="P18" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>2.8124359999999999</v>
+      </c>
+      <c r="R18" s="8">
+        <v>8.3299999999999997E-4</v>
+      </c>
+      <c r="S18">
+        <v>2010</v>
+      </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -2657,6 +2698,53 @@
         <v>1.3527740000000001</v>
       </c>
       <c r="R29" s="4">
+        <v>3.9611111111111119E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="10">
+        <v>1186.9540608888888</v>
+      </c>
+      <c r="E30" s="10">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G30" s="10">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H30" s="10">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I30" s="10">
+        <v>5.3768950000000002</v>
+      </c>
+      <c r="J30" s="10">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K30" s="10">
+        <v>645.94088411111113</v>
+      </c>
+      <c r="L30" s="10">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M30" s="10">
+        <v>1457.6001788888889</v>
+      </c>
+      <c r="N30" s="10">
+        <v>1191.1331380000001</v>
+      </c>
+      <c r="O30" s="11">
+        <v>4695.8937716666669</v>
+      </c>
+      <c r="P30" s="11">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q30" s="10">
+        <v>1.3527740000000001</v>
+      </c>
+      <c r="R30" s="12">
         <v>3.9611111111111119E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Log entry for versions 116, 117, and 118. Update the reservoir data for BLU. Add logic to allow reading INT16 NetCDF climate data. Reservoirs/DataSources/Blue_River_rule_priorities - added. Rules_BR/MaxD_Daily_BiOP_MaxD.csv, Blue_River_rule_priorities.csv, MaxD_FloodDcrsRate_Blue.csv, MaxI_FloodIncrsRate_Blue.csv, MaxI_MaxFloodIncrsRate_Blue.csv, Max_EvaculationRelease.csv, Max_con_flow_blue_river.csv, Min_Flow_at_Blue_River.csv - Update reservoir data. Flow.cpp, .h - Add logic for reading INT16 NetCDF climate data.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319777BF-D452-411D-8D92-C8B35AA2B7BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1852E5BD-8AB6-4224-BB68-6A0EFFB03E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
   <si>
     <t>Year</t>
   </si>
@@ -177,15 +177,17 @@
   </si>
   <si>
     <t>Baseline 2010-18 C116</t>
+  </si>
+  <si>
+    <t>Baseline 2010 C117+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -323,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,6 +508,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,8 +689,8 @@
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1038,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2152,85 +2160,87 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="8"/>
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20">
+        <v>2010</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1.2021059999999999</v>
+      </c>
+      <c r="G20" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H20" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I20" s="2">
+        <v>4.7315529999999999</v>
+      </c>
+      <c r="J20" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K20" s="2">
+        <v>677.32995600000004</v>
+      </c>
+      <c r="L20" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1390.210327</v>
+      </c>
+      <c r="N20" s="2">
+        <v>1207.1636960000001</v>
+      </c>
+      <c r="O20" s="9">
+        <v>6722.8808589999999</v>
+      </c>
+      <c r="P20" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>-0.60218700000000003</v>
+      </c>
+      <c r="R20" s="4">
+        <v>-1.7799999999999999E-4</v>
+      </c>
+      <c r="S20">
+        <v>2010</v>
+      </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G21" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H21" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K21" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L21" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M21" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N21" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O21" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P21" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R21" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S21" t="s">
-        <v>23</v>
-      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="4"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
@@ -2270,7 +2280,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P22" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q22" s="2">
         <v>-4.72741111111111E-2</v>
@@ -2287,7 +2297,7 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
@@ -2335,19 +2345,22 @@
       <c r="R23" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S23" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E24" s="2">
         <v>1901.5157334444443</v>
@@ -2366,31 +2379,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K24" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L24" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M24" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N24" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O24" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P24" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q24" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R24" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S24" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
@@ -2398,13 +2408,13 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E25" s="2">
         <v>1901.5157334444443</v>
@@ -2423,28 +2433,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K25" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L25" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M25" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N25" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O25" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P25" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q25" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R25" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
@@ -2452,13 +2465,13 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E26" s="2">
         <v>1901.5157334444443</v>
@@ -2467,28 +2480,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G26" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H26" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I26" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I26" s="2"/>
       <c r="J26" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K26" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L26" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M26" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N26" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O26" s="3">
         <v>4883.9277073333324</v>
@@ -2497,13 +2508,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q26" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R26" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S26" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -2511,13 +2519,13 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E27" s="2">
         <v>1901.5157334444443</v>
@@ -2526,28 +2534,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G27" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H27" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I27" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J27" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K27" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L27" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M27" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N27" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O27" s="3">
         <v>4883.9277073333324</v>
@@ -2556,10 +2564,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q27" s="2">
-        <v>9.9787694444444455</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R27" s="4">
-        <v>2.9230000000000003E-3</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S27" t="s">
         <v>23</v>
@@ -2570,7 +2578,7 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -2585,7 +2593,7 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G28" s="2">
-        <v>347.23312744444445</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H28" s="2">
         <v>9.775355222222224</v>
@@ -2615,10 +2623,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q28" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R28" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S28" t="s">
         <v>23</v>
@@ -2629,55 +2637,55 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E29" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F29" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G29" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G29" s="2">
+        <v>347.23312744444445</v>
       </c>
       <c r="H29" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I29" s="5">
-        <v>13.853347222222222</v>
+      <c r="I29" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J29" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K29" s="5">
-        <v>691.23065866666673</v>
+      <c r="K29" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L29" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M29" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N29" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O29" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M29" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O29" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P29" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q29" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R29" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q29" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R29" s="4">
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S29" t="s">
         <v>23</v>
@@ -2688,13 +2696,13 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="2">
-        <v>1186.9521077777779</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E30" s="2">
         <v>1901.5157334444443</v>
@@ -2702,58 +2710,58 @@
       <c r="F30" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G30" s="2">
-        <v>280.33542888888883</v>
+      <c r="G30" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H30" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I30" s="5">
-        <v>12.968491888888888</v>
+        <v>13.853347222222222</v>
       </c>
       <c r="J30" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K30" s="2">
-        <v>645.94098588888892</v>
+      <c r="K30" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L30" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M30" s="2">
-        <v>1465.1962754444444</v>
-      </c>
-      <c r="N30" s="2">
-        <v>1191.1222331111112</v>
-      </c>
-      <c r="O30" s="3">
+      <c r="M30" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N30" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O30" s="6">
         <v>4695.8937716666669</v>
       </c>
       <c r="P30" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q30" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R30" s="4">
-        <v>3.9399999999999998E-4</v>
+      <c r="Q30" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R30" s="7">
+        <v>5.926666666666668E-4</v>
       </c>
       <c r="S30" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
+      <c r="A31" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="9" t="s">
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E31" s="2">
         <v>1901.5157334444443</v>
@@ -2767,48 +2775,48 @@
       <c r="H31" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I31" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I31" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J31" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K31" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L31" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M31" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N31" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O31" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P31" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q31" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R31" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S31" s="9" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S31" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="9" t="s">
+      <c r="B32" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="2">
@@ -2856,7 +2864,66 @@
       <c r="R32" s="4">
         <v>-2.8933333333333328E-4</v>
       </c>
-      <c r="S32" s="9" t="s">
+      <c r="S32" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1186.9497747777777</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G33" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H33" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I33" s="2">
+        <v>5.3913398888888899</v>
+      </c>
+      <c r="J33" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K33" s="2">
+        <v>645.93823922222225</v>
+      </c>
+      <c r="L33" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M33" s="2">
+        <v>1455.3145886666666</v>
+      </c>
+      <c r="N33" s="2">
+        <v>1191.1280516666666</v>
+      </c>
+      <c r="O33" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P33" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>-0.95070599999999983</v>
+      </c>
+      <c r="R33" s="4">
+        <v>-2.8933333333333328E-4</v>
+      </c>
+      <c r="S33" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Begin updating the CGR reservoir data. Flow.cpp - Remove a blank line.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1852E5BD-8AB6-4224-BB68-6A0EFFB03E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19976AC-2F07-4E6F-A593-3ACD9238B652}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
   <si>
     <t>Year</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>Baseline 2010 C117+</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C118</t>
+  </si>
+  <si>
+    <t>using new precip file</t>
   </si>
 </sst>
 </file>
@@ -678,7 +684,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -691,6 +697,7 @@
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1046,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2219,85 +2226,84 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="4"/>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21">
+        <v>2010</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E21" s="10">
+        <v>189.328384</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1.5146299999999999</v>
+      </c>
+      <c r="G21" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H21" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I21" s="2">
+        <v>14.906940000000001</v>
+      </c>
+      <c r="J21" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K21" s="2">
+        <v>352.67175300000002</v>
+      </c>
+      <c r="L21" s="2">
+        <v>8.8870590000000007</v>
+      </c>
+      <c r="M21" s="2">
+        <v>578.58209199999999</v>
+      </c>
+      <c r="N21" s="2">
+        <v>638.01348900000005</v>
+      </c>
+      <c r="O21" s="3">
+        <v>9898.6386719999991</v>
+      </c>
+      <c r="P21" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>0.269785</v>
+      </c>
+      <c r="R21" s="4">
+        <v>1.7000000000000001E-4</v>
+      </c>
+      <c r="S21">
+        <v>2010</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G22" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H22" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K22" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L22" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M22" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N22" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O22" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P22" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R22" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S22" t="s">
-        <v>23</v>
-      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="4"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
@@ -2337,7 +2343,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P23" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q23" s="2">
         <v>-4.72741111111111E-2</v>
@@ -2354,7 +2360,7 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -2402,19 +2408,22 @@
       <c r="R24" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S24" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E25" s="2">
         <v>1901.5157334444443</v>
@@ -2433,31 +2442,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K25" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L25" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M25" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N25" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O25" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P25" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q25" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R25" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S25" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
@@ -2465,13 +2471,13 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E26" s="2">
         <v>1901.5157334444443</v>
@@ -2490,28 +2496,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K26" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L26" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M26" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N26" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O26" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P26" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q26" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R26" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S26" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -2519,13 +2528,13 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E27" s="2">
         <v>1901.5157334444443</v>
@@ -2534,28 +2543,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G27" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H27" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I27" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I27" s="2"/>
       <c r="J27" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K27" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L27" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M27" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N27" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O27" s="3">
         <v>4883.9277073333324</v>
@@ -2564,13 +2571,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q27" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R27" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S27" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
@@ -2578,13 +2582,13 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E28" s="2">
         <v>1901.5157334444443</v>
@@ -2593,28 +2597,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G28" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H28" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I28" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J28" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K28" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L28" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M28" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N28" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O28" s="3">
         <v>4883.9277073333324</v>
@@ -2623,10 +2627,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q28" s="2">
-        <v>9.9787694444444455</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R28" s="4">
-        <v>2.9230000000000003E-3</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S28" t="s">
         <v>23</v>
@@ -2637,7 +2641,7 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -2652,7 +2656,7 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G29" s="2">
-        <v>347.23312744444445</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H29" s="2">
         <v>9.775355222222224</v>
@@ -2682,10 +2686,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q29" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R29" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S29" t="s">
         <v>23</v>
@@ -2696,55 +2700,55 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E30" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F30" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G30" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G30" s="2">
+        <v>347.23312744444445</v>
       </c>
       <c r="H30" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I30" s="5">
-        <v>13.853347222222222</v>
+      <c r="I30" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J30" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K30" s="5">
-        <v>691.23065866666673</v>
+      <c r="K30" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L30" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M30" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N30" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O30" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M30" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N30" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O30" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P30" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q30" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R30" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q30" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R30" s="4">
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S30" t="s">
         <v>23</v>
@@ -2755,13 +2759,13 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="2">
-        <v>1186.9521077777779</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E31" s="2">
         <v>1901.5157334444443</v>
@@ -2769,58 +2773,58 @@
       <c r="F31" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G31" s="2">
-        <v>280.33542888888883</v>
+      <c r="G31" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H31" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I31" s="5">
-        <v>12.968491888888888</v>
+        <v>13.853347222222222</v>
       </c>
       <c r="J31" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K31" s="2">
-        <v>645.94098588888892</v>
+      <c r="K31" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L31" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M31" s="2">
-        <v>1465.1962754444444</v>
-      </c>
-      <c r="N31" s="2">
-        <v>1191.1222331111112</v>
-      </c>
-      <c r="O31" s="3">
+      <c r="M31" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N31" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O31" s="6">
         <v>4695.8937716666669</v>
       </c>
       <c r="P31" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q31" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R31" s="4">
-        <v>3.9399999999999998E-4</v>
+      <c r="Q31" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R31" s="7">
+        <v>5.926666666666668E-4</v>
       </c>
       <c r="S31" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
+      <c r="A32" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="8" t="s">
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E32" s="2">
         <v>1901.5157334444443</v>
@@ -2834,37 +2838,37 @@
       <c r="H32" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I32" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I32" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J32" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K32" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L32" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M32" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N32" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O32" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P32" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q32" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R32" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S32" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S32" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2873,7 +2877,7 @@
         <v>16</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>23</v>
@@ -2927,7 +2931,126 @@
         <v>23</v>
       </c>
     </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1186.9497747777777</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G34" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H34" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I34" s="2">
+        <v>5.3913398888888899</v>
+      </c>
+      <c r="J34" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K34" s="2">
+        <v>645.93823922222225</v>
+      </c>
+      <c r="L34" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M34" s="2">
+        <v>1455.3145886666666</v>
+      </c>
+      <c r="N34" s="2">
+        <v>1191.1280516666666</v>
+      </c>
+      <c r="O34" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P34" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>-0.95070599999999983</v>
+      </c>
+      <c r="R34" s="4">
+        <v>-2.8933333333333328E-4</v>
+      </c>
+      <c r="S34" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G35" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H35" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I35" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J35" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K35" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L35" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M35" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N35" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O35" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P35" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R35" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S35" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CW3M_Installer_McKenzie_0.4.1.exe 11/23/20 from CW3M ver. 124 on GitHub.  Stream temperatures are being simulated, although not yet with the effects of vegetation or streambank shading.  A coarse calibration has been done.  Reservoir data has been updated for Blue River and Cougar.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19976AC-2F07-4E6F-A593-3ACD9238B652}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD40BFC8-CB32-41A3-AAFA-9EEE04CF8358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="55">
   <si>
     <t>Year</t>
   </si>
@@ -185,7 +185,16 @@
     <t>Baseline 2010-18 C118</t>
   </si>
   <si>
-    <t>using new precip file</t>
+    <t>Baseline 2010 C123</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C123</t>
+  </si>
+  <si>
+    <t>CW3M 0.4.1</t>
+  </si>
+  <si>
+    <t>Demo 2010</t>
   </si>
 </sst>
 </file>
@@ -684,7 +693,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -697,7 +706,6 @@
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1053,14 +1061,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U35"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -2226,6 +2235,9 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
       <c r="B21" t="s">
         <v>51</v>
       </c>
@@ -2235,11 +2247,11 @@
       <c r="D21" s="2">
         <v>1090.199341</v>
       </c>
-      <c r="E21" s="10">
-        <v>189.328384</v>
+      <c r="E21" s="2">
+        <v>1990.4676509999999</v>
       </c>
       <c r="F21" s="2">
-        <v>1.5146299999999999</v>
+        <v>1.2021059999999999</v>
       </c>
       <c r="G21" s="2">
         <v>280.16485599999999</v>
@@ -2248,119 +2260,121 @@
         <v>10.610913999999999</v>
       </c>
       <c r="I21" s="2">
-        <v>14.906940000000001</v>
+        <v>4.7315529999999999</v>
       </c>
       <c r="J21" s="2">
         <v>8.8404570000000007</v>
       </c>
       <c r="K21" s="2">
-        <v>352.67175300000002</v>
+        <v>677.32977300000005</v>
       </c>
       <c r="L21" s="2">
-        <v>8.8870590000000007</v>
+        <v>93.229797000000005</v>
       </c>
       <c r="M21" s="2">
-        <v>578.58209199999999</v>
+        <v>1390.239624</v>
       </c>
       <c r="N21" s="2">
-        <v>638.01348900000005</v>
+        <v>1207.1339109999999</v>
       </c>
       <c r="O21" s="3">
-        <v>9898.6386719999991</v>
+        <v>6722.8808589999999</v>
       </c>
       <c r="P21" s="3">
         <v>29450.638672000001</v>
       </c>
       <c r="Q21" s="2">
-        <v>0.269785</v>
+        <v>-0.60285900000000003</v>
       </c>
       <c r="R21" s="4">
-        <v>1.7000000000000001E-4</v>
+        <v>-1.7799999999999999E-4</v>
       </c>
       <c r="S21">
         <v>2010</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="4"/>
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22">
+        <v>2010</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E22" s="5">
+        <v>2031.3264160000001</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1.1987909999999999</v>
+      </c>
+      <c r="G22" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H22" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I22" s="2">
+        <v>4.6530839999999998</v>
+      </c>
+      <c r="J22" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K22" s="2">
+        <v>674.30981399999996</v>
+      </c>
+      <c r="L22" s="2">
+        <v>96.277434999999997</v>
+      </c>
+      <c r="M22" s="2">
+        <v>1418.5771480000001</v>
+      </c>
+      <c r="N22" s="2">
+        <v>1218.7666019999999</v>
+      </c>
+      <c r="O22" s="3">
+        <v>6704.8530270000001</v>
+      </c>
+      <c r="P22" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>-1.381945</v>
+      </c>
+      <c r="R22" s="4">
+        <v>-4.0400000000000001E-4</v>
+      </c>
+      <c r="S22">
+        <v>2010</v>
+      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G23" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H23" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K23" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L23" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M23" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N23" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O23" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P23" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R23" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S23" t="s">
-        <v>23</v>
-      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="4"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -2400,7 +2414,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P24" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q24" s="2">
         <v>-4.72741111111111E-2</v>
@@ -2417,7 +2431,7 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -2465,19 +2479,22 @@
       <c r="R25" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S25" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E26" s="2">
         <v>1901.5157334444443</v>
@@ -2496,31 +2513,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K26" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L26" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M26" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N26" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O26" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P26" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q26" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R26" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S26" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -2528,13 +2542,13 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E27" s="2">
         <v>1901.5157334444443</v>
@@ -2553,28 +2567,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K27" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L27" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M27" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N27" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O27" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P27" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q27" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R27" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S27" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
@@ -2582,13 +2599,13 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E28" s="2">
         <v>1901.5157334444443</v>
@@ -2597,28 +2614,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G28" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H28" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I28" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I28" s="2"/>
       <c r="J28" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K28" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L28" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M28" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N28" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O28" s="3">
         <v>4883.9277073333324</v>
@@ -2627,13 +2642,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q28" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R28" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S28" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
@@ -2641,13 +2653,13 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E29" s="2">
         <v>1901.5157334444443</v>
@@ -2656,28 +2668,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G29" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H29" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I29" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J29" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K29" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L29" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M29" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N29" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O29" s="3">
         <v>4883.9277073333324</v>
@@ -2686,10 +2698,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q29" s="2">
-        <v>9.9787694444444455</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R29" s="4">
-        <v>2.9230000000000003E-3</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S29" t="s">
         <v>23</v>
@@ -2700,7 +2712,7 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -2715,7 +2727,7 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G30" s="2">
-        <v>347.23312744444445</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H30" s="2">
         <v>9.775355222222224</v>
@@ -2745,10 +2757,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q30" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R30" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S30" t="s">
         <v>23</v>
@@ -2759,55 +2771,55 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E31" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F31" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G31" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G31" s="2">
+        <v>347.23312744444445</v>
       </c>
       <c r="H31" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I31" s="5">
-        <v>13.853347222222222</v>
+      <c r="I31" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J31" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K31" s="5">
-        <v>691.23065866666673</v>
+      <c r="K31" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L31" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M31" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N31" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O31" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M31" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N31" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O31" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P31" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q31" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R31" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q31" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R31" s="4">
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S31" t="s">
         <v>23</v>
@@ -2818,13 +2830,13 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="2">
-        <v>1186.9521077777779</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E32" s="2">
         <v>1901.5157334444443</v>
@@ -2832,58 +2844,58 @@
       <c r="F32" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G32" s="2">
-        <v>280.33542888888883</v>
+      <c r="G32" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H32" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I32" s="5">
-        <v>12.968491888888888</v>
+        <v>13.853347222222222</v>
       </c>
       <c r="J32" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K32" s="2">
-        <v>645.94098588888892</v>
+      <c r="K32" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L32" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M32" s="2">
-        <v>1465.1962754444444</v>
-      </c>
-      <c r="N32" s="2">
-        <v>1191.1222331111112</v>
-      </c>
-      <c r="O32" s="3">
+      <c r="M32" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N32" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O32" s="6">
         <v>4695.8937716666669</v>
       </c>
       <c r="P32" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q32" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R32" s="4">
-        <v>3.9399999999999998E-4</v>
+      <c r="Q32" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R32" s="7">
+        <v>5.926666666666668E-4</v>
       </c>
       <c r="S32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
+      <c r="A33" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="8" t="s">
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E33" s="2">
         <v>1901.5157334444443</v>
@@ -2897,37 +2909,37 @@
       <c r="H33" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I33" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I33" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J33" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K33" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L33" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M33" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N33" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O33" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P33" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q33" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R33" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S33" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S33" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2936,7 +2948,7 @@
         <v>16</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>23</v>
@@ -2995,13 +3007,13 @@
         <v>16</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E35" s="2">
         <v>1901.5157334444443</v>
@@ -3016,22 +3028,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I35" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J35" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K35" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L35" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M35" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N35" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O35" s="3">
         <v>4661.9885795555556</v>
@@ -3040,12 +3052,145 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q35" s="2">
+        <v>-0.95070599999999983</v>
+      </c>
+      <c r="R35" s="4">
+        <v>-2.8933333333333328E-4</v>
+      </c>
+      <c r="S35" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G36" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H36" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I36" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J36" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K36" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L36" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M36" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N36" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O36" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P36" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q36" s="2">
         <v>-1.0069492222222223</v>
       </c>
-      <c r="R35" s="4">
+      <c r="R36" s="4">
         <v>-3.0444444444444448E-4</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="S36" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="2">
+        <f>AVERAGE(D28:D36)</f>
+        <v>1176.9484893703707</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" ref="E37:R37" si="0">AVERAGE(E28:E36)</f>
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99402413580246907</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" si="0"/>
+        <v>308.82293032098761</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I37" s="5">
+        <f t="shared" si="0"/>
+        <v>7.1295036805555574</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K37" s="5">
+        <f t="shared" si="0"/>
+        <v>705.82954383950619</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="0"/>
+        <v>83.470620444444435</v>
+      </c>
+      <c r="M37" s="5">
+        <f t="shared" si="0"/>
+        <v>1432.1165123580245</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="0"/>
+        <v>1179.5111099259257</v>
+      </c>
+      <c r="O37" s="6">
+        <f t="shared" si="0"/>
+        <v>4768.1626790370356</v>
+      </c>
+      <c r="P37" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324888893</v>
+      </c>
+      <c r="Q37" s="2">
+        <f t="shared" si="0"/>
+        <v>4.6790465308641975</v>
+      </c>
+      <c r="R37" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3632839506172842E-3</v>
+      </c>
+      <c r="S37" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement a better guess at the cloudiness fraction. Add CW3MdigitalHandbook/McKenzie/Cloudiness.xlsx. Flow_McKenzie.xml - Use the new actual weather precip file that includes 2019 and uses int16 instead of float. Add SkillAssessment/SeasonalAnalysis.xlsx - a tool for finding the average of values for a single calendar day over multiple years. ReachRouting.cpp - Add logic to estimate cloudiness based on the difference between actual incoming shortwave radiation and a nominal maximum clear sky SW for the McKenzie basin.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD40BFC8-CB32-41A3-AAFA-9EEE04CF8358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B69CEDA-6142-4A0A-B8DC-D7783402367C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="57">
   <si>
     <t>Year</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>Demo 2010</t>
+  </si>
+  <si>
+    <t>with new precip file</t>
+  </si>
+  <si>
+    <t>and new cloudiness</t>
   </si>
 </sst>
 </file>
@@ -1061,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2353,142 +2359,140 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="4"/>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23">
+        <v>2010</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1980.798828</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.2017960000000001</v>
+      </c>
+      <c r="G23" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H23" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I23" s="2">
+        <v>4.7564500000000001</v>
+      </c>
+      <c r="J23" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K23" s="2">
+        <v>676.66839600000003</v>
+      </c>
+      <c r="L23" s="2">
+        <v>92.796302999999995</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1384.2856449999999</v>
+      </c>
+      <c r="N23" s="2">
+        <v>1204.5405270000001</v>
+      </c>
+      <c r="O23" s="3">
+        <v>6726.0224609999996</v>
+      </c>
+      <c r="P23" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>-0.60085699999999997</v>
+      </c>
+      <c r="R23" s="4">
+        <v>-1.7799999999999999E-4</v>
+      </c>
+      <c r="S23">
+        <v>2010</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
       <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" t="s">
-        <v>23</v>
+        <v>56</v>
+      </c>
+      <c r="C24">
+        <v>2010</v>
       </c>
       <c r="D24" s="2">
-        <v>1138.6194117777777</v>
+        <v>1090.199341</v>
       </c>
       <c r="E24" s="2">
-        <v>1901.5157334444443</v>
+        <v>1980.798828</v>
       </c>
       <c r="F24" s="2">
-        <v>1.0119255555555557</v>
+        <v>1.2017960000000001</v>
       </c>
       <c r="G24" s="2">
-        <v>327.78053433333326</v>
+        <v>280.16485599999999</v>
       </c>
       <c r="H24" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I24" s="2"/>
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I24" s="2">
+        <v>4.7564849999999996</v>
+      </c>
       <c r="J24" s="2">
-        <v>8.145128999999999</v>
+        <v>8.8404570000000007</v>
       </c>
       <c r="K24" s="2">
-        <v>769.26639155555551</v>
+        <v>676.69219999999996</v>
       </c>
       <c r="L24" s="2">
-        <v>83.47062044444445</v>
+        <v>92.796302999999995</v>
       </c>
       <c r="M24" s="2">
-        <v>1374.8233372222221</v>
+        <v>1384.267456</v>
       </c>
       <c r="N24" s="2">
-        <v>1142.9502087777778</v>
+        <v>1204.5352780000001</v>
       </c>
       <c r="O24" s="3">
-        <v>4918.1879612222219</v>
+        <v>6726.0209960000002</v>
       </c>
       <c r="P24" s="3">
-        <v>27227.338324777778</v>
+        <v>29450.638672000001</v>
       </c>
       <c r="Q24" s="2">
-        <v>-4.72741111111111E-2</v>
+        <v>-0.60052700000000003</v>
       </c>
       <c r="R24" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S24" t="s">
-        <v>23</v>
+        <v>-1.7799999999999999E-4</v>
+      </c>
+      <c r="S24">
+        <v>2010</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E25" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G25" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H25" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K25" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L25" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M25" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N25" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O25" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P25" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q25" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R25" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S25" t="s">
-        <v>23</v>
-      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="4"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
@@ -2528,13 +2532,16 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P26" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q26" s="2">
         <v>-4.72741111111111E-2</v>
       </c>
       <c r="R26" s="4">
         <v>-3.8888888888888877E-5</v>
+      </c>
+      <c r="S26" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -2542,13 +2549,13 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E27" s="2">
         <v>1901.5157334444443</v>
@@ -2567,28 +2574,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K27" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L27" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M27" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N27" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O27" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P27" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q27" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R27" s="4">
-        <v>1.4151111111111109E-3</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
       <c r="S27" t="s">
         <v>23</v>
@@ -2599,13 +2606,13 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="2">
-        <v>1161.1572335555554</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E28" s="2">
         <v>1901.5157334444443</v>
@@ -2624,28 +2631,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K28" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L28" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M28" s="2">
-        <v>1383.6045464444442</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N28" s="2">
-        <v>1161.284607111111</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O28" s="3">
-        <v>4883.9277073333324</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P28" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q28" s="2">
-        <v>4.6342037777777776</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R28" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
@@ -2653,13 +2660,13 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="2">
-        <v>1161.1644491111113</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E29" s="2">
         <v>1901.5157334444443</v>
@@ -2668,40 +2675,38 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G29" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H29" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I29" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I29" s="2"/>
       <c r="J29" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K29" s="2">
-        <v>769.36972377777772</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L29" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M29" s="2">
-        <v>1437.0445828888887</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N29" s="2">
-        <v>1161.2873196666667</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O29" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P29" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q29" s="2">
-        <v>27.015940777777772</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R29" s="4">
-        <v>7.9151111111111106E-3</v>
+        <v>1.4151111111111109E-3</v>
       </c>
       <c r="S29" t="s">
         <v>23</v>
@@ -2712,13 +2717,13 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E30" s="2">
         <v>1901.5157334444443</v>
@@ -2727,28 +2732,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G30" s="2">
-        <v>337.20870333333335</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H30" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I30" s="2">
-        <v>4.6813607777777788</v>
-      </c>
+      <c r="I30" s="2"/>
       <c r="J30" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K30" s="2">
-        <v>769.36992711111111</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L30" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M30" s="2">
-        <v>1403.060424888889</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N30" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O30" s="3">
         <v>4883.9277073333324</v>
@@ -2757,13 +2760,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q30" s="2">
-        <v>9.9787694444444455</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R30" s="4">
-        <v>2.9230000000000003E-3</v>
-      </c>
-      <c r="S30" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -2771,13 +2771,13 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E31" s="2">
         <v>1901.5157334444443</v>
@@ -2786,28 +2786,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G31" s="2">
-        <v>347.23312744444445</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H31" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I31" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J31" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K31" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L31" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M31" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N31" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O31" s="3">
         <v>4883.9277073333324</v>
@@ -2816,10 +2816,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q31" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R31" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S31" t="s">
         <v>23</v>
@@ -2830,55 +2830,55 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E32" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F32" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G32" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G32" s="2">
+        <v>337.20870333333335</v>
       </c>
       <c r="H32" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I32" s="5">
-        <v>13.853347222222222</v>
+      <c r="I32" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J32" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K32" s="5">
-        <v>691.23065866666673</v>
+      <c r="K32" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L32" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M32" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N32" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O32" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M32" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N32" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O32" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P32" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q32" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R32" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q32" s="2">
+        <v>9.9787694444444455</v>
+      </c>
+      <c r="R32" s="4">
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S32" t="s">
         <v>23</v>
@@ -2889,72 +2889,72 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="2">
-        <v>1186.9521077777779</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E33" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F33" s="2">
-        <v>0.97970299999999988</v>
+        <v>1.0119255555555557</v>
       </c>
       <c r="G33" s="2">
-        <v>280.33542888888883</v>
+        <v>347.23312744444445</v>
       </c>
       <c r="H33" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I33" s="5">
-        <v>12.968491888888888</v>
+      <c r="I33" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J33" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K33" s="2">
-        <v>645.94098588888892</v>
+        <v>769.36992711111111</v>
       </c>
       <c r="L33" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M33" s="2">
-        <v>1465.1962754444444</v>
+        <v>1403.060424888889</v>
       </c>
       <c r="N33" s="2">
-        <v>1191.1222331111112</v>
+        <v>1161.2856514444443</v>
       </c>
       <c r="O33" s="3">
-        <v>4695.8937716666669</v>
+        <v>4883.9277073333324</v>
       </c>
       <c r="P33" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q33" s="2">
-        <v>1.3484236666666667</v>
+        <v>-4.5654777777777787E-2</v>
       </c>
       <c r="R33" s="4">
-        <v>3.9399999999999998E-4</v>
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+      <c r="A34" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="8" t="s">
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="2">
-        <v>1186.9497747777777</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E34" s="2">
         <v>1901.5157334444443</v>
@@ -2962,58 +2962,58 @@
       <c r="F34" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G34" s="2">
-        <v>280.33542888888883</v>
+      <c r="G34" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H34" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I34" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I34" s="5">
+        <v>13.853347222222222</v>
       </c>
       <c r="J34" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K34" s="2">
-        <v>645.93823922222225</v>
+      <c r="K34" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L34" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M34" s="2">
-        <v>1455.3145886666666</v>
-      </c>
-      <c r="N34" s="2">
-        <v>1191.1280516666666</v>
-      </c>
-      <c r="O34" s="3">
-        <v>4661.9885795555556</v>
+      <c r="M34" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N34" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O34" s="6">
+        <v>4695.8937716666669</v>
       </c>
       <c r="P34" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q34" s="2">
-        <v>-0.95070599999999983</v>
-      </c>
-      <c r="R34" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S34" s="8" t="s">
+      <c r="Q34" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R34" s="7">
+        <v>5.926666666666668E-4</v>
+      </c>
+      <c r="S34" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
+      <c r="A35" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="8" t="s">
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E35" s="2">
         <v>1901.5157334444443</v>
@@ -3027,37 +3027,37 @@
       <c r="H35" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I35" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I35" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J35" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K35" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L35" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M35" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N35" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O35" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P35" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q35" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R35" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S35" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S35" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3066,13 +3066,13 @@
         <v>16</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E36" s="2">
         <v>1901.5157334444443</v>
@@ -3087,22 +3087,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I36" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J36" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K36" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L36" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M36" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N36" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O36" s="3">
         <v>4661.9885795555556</v>
@@ -3111,10 +3111,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q36" s="2">
-        <v>-1.0069492222222223</v>
+        <v>-0.95070599999999983</v>
       </c>
       <c r="R36" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S36" s="8" t="s">
         <v>23</v>
@@ -3125,72 +3125,190 @@
         <v>16</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D37" s="2">
-        <f>AVERAGE(D28:D36)</f>
+        <v>1186.9497747777777</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G37" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H37" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I37" s="2">
+        <v>5.3913398888888899</v>
+      </c>
+      <c r="J37" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K37" s="2">
+        <v>645.93823922222225</v>
+      </c>
+      <c r="L37" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M37" s="2">
+        <v>1455.3145886666666</v>
+      </c>
+      <c r="N37" s="2">
+        <v>1191.1280516666666</v>
+      </c>
+      <c r="O37" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P37" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>-0.95070599999999983</v>
+      </c>
+      <c r="R37" s="4">
+        <v>-2.8933333333333328E-4</v>
+      </c>
+      <c r="S37" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G38" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H38" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I38" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J38" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K38" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L38" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M38" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N38" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O38" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P38" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R38" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S38" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="2">
+        <f>AVERAGE(D30:D38)</f>
         <v>1176.9484893703707</v>
       </c>
-      <c r="E37" s="2">
-        <f t="shared" ref="E37:R37" si="0">AVERAGE(E28:E36)</f>
+      <c r="E39" s="2">
+        <f t="shared" ref="E39:R39" si="0">AVERAGE(E30:E38)</f>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F39" s="2">
         <f t="shared" si="0"/>
         <v>0.99402413580246907</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G39" s="5">
         <f t="shared" si="0"/>
         <v>308.82293032098761</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H39" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I39" s="5">
         <f t="shared" si="0"/>
         <v>7.1295036805555574</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J39" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K37" s="5">
+      <c r="K39" s="5">
         <f t="shared" si="0"/>
         <v>705.82954383950619</v>
       </c>
-      <c r="L37" s="2">
+      <c r="L39" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M37" s="5">
+      <c r="M39" s="5">
         <f t="shared" si="0"/>
         <v>1432.1165123580245</v>
       </c>
-      <c r="N37" s="2">
+      <c r="N39" s="2">
         <f t="shared" si="0"/>
         <v>1179.5111099259257</v>
       </c>
-      <c r="O37" s="6">
+      <c r="O39" s="6">
         <f t="shared" si="0"/>
         <v>4768.1626790370356</v>
       </c>
-      <c r="P37" s="3">
+      <c r="P39" s="3">
         <f t="shared" si="0"/>
         <v>27227.338324888893</v>
       </c>
-      <c r="Q37" s="2">
+      <c r="Q39" s="2">
         <f t="shared" si="0"/>
         <v>4.6790465308641975</v>
       </c>
-      <c r="R37" s="7">
+      <c r="R39" s="7">
         <f t="shared" si="0"/>
         <v>1.3632839506172842E-3</v>
       </c>
-      <c r="S37" s="8" t="s">
+      <c r="S39" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flow_McKenzie.xml - Roll back a change made prematurely in a previous revision. ReachRouting.cpp - Correct a bug in the new cloudiness calculation.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B69CEDA-6142-4A0A-B8DC-D7783402367C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D1874D-4E8E-42EF-B78D-6C8C66DDF690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
   <si>
     <t>Year</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>and new cloudiness</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C125</t>
   </si>
 </sst>
 </file>
@@ -1067,10 +1070,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3253,7 +3257,7 @@
         <v>1176.9484893703707</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" ref="E39:R39" si="0">AVERAGE(E30:E38)</f>
+        <f t="shared" ref="E39:R40" si="0">AVERAGE(E30:E38)</f>
         <v>1901.5157334444443</v>
       </c>
       <c r="F39" s="2">
@@ -3309,6 +3313,80 @@
         <v>1.3632839506172842E-3</v>
       </c>
       <c r="S39" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="2">
+        <f>AVERAGE(D31:D39)</f>
+        <v>1178.7030733497943</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="0"/>
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99203508916323713</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="0"/>
+        <v>306.71652987517137</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1295036805555565</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="0"/>
+        <v>698.76948392043903</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="0"/>
+        <v>83.470620444444435</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="0"/>
+        <v>1437.5067307928668</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="0"/>
+        <v>1181.53627690535</v>
+      </c>
+      <c r="O40" s="3">
+        <f t="shared" si="0"/>
+        <v>4755.299898115225</v>
+      </c>
+      <c r="P40" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324888893</v>
+      </c>
+      <c r="Q40" s="2">
+        <f t="shared" si="0"/>
+        <v>4.684029058984911</v>
+      </c>
+      <c r="R40" s="4">
+        <f t="shared" si="0"/>
+        <v>1.363093278463649E-3</v>
+      </c>
+      <c r="S40" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Save updates to documentation.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D1874D-4E8E-42EF-B78D-6C8C66DDF690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846D7B0F-91E6-4708-A585-194C73DFBADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
   <si>
     <t>Year</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C125</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C128</t>
   </si>
 </sst>
 </file>
@@ -1070,11 +1073,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U40"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S40" sqref="S40"/>
+      <selection pane="bottomLeft" activeCell="U49" sqref="U49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3390,6 +3393,65 @@
         <v>23</v>
       </c>
     </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1186.9773491111109</v>
+      </c>
+      <c r="E41" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G41" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H41" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I41" s="2">
+        <v>5.3870271111111121</v>
+      </c>
+      <c r="J41" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K41" s="2">
+        <v>645.93808322222219</v>
+      </c>
+      <c r="L41" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M41" s="2">
+        <v>1455.5792641111111</v>
+      </c>
+      <c r="N41" s="2">
+        <v>1191.1918266666667</v>
+      </c>
+      <c r="O41" s="3">
+        <v>4661.9885253333332</v>
+      </c>
+      <c r="P41" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>-0.64567288888888896</v>
+      </c>
+      <c r="R41" s="4">
+        <v>-2.0755555555555555E-4</v>
+      </c>
+      <c r="S41" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Hook up the temperature in the reservoirs to the temperature of the inflows to the reservoirs. Flow.cpp, .h - Change GetResOutflow() to GetResOutflowWP(). That is where inflow to the reservoir gets mixed into the reservoir water, and where the reservoir discharge gets taken out of the reservoir water. ReachRouting.cpp - Get rid of a compiler warning.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846D7B0F-91E6-4708-A585-194C73DFBADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FE0517-6789-4519-918B-5D90BE6A15CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1164" yWindow="744" windowWidth="20796" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
   <si>
     <t>Year</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C128</t>
+  </si>
+  <si>
+    <t>Baseline 2010 C132+</t>
   </si>
 </sst>
 </file>
@@ -1073,11 +1076,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U41"/>
+  <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U49" sqref="U49"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2478,85 +2481,87 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="4"/>
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25">
+        <v>2010</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1.2021059999999999</v>
+      </c>
+      <c r="G25" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H25" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I25" s="2">
+        <v>4.7315519999999998</v>
+      </c>
+      <c r="J25" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K25" s="2">
+        <v>677.33013900000003</v>
+      </c>
+      <c r="L25" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M25" s="2">
+        <v>1390.240601</v>
+      </c>
+      <c r="N25" s="2">
+        <v>1207.132568</v>
+      </c>
+      <c r="O25" s="3">
+        <v>6722.8808589999999</v>
+      </c>
+      <c r="P25" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>-0.60285699999999998</v>
+      </c>
+      <c r="R25" s="4">
+        <v>-1.7799999999999999E-4</v>
+      </c>
+      <c r="S25">
+        <v>2010</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F26" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G26" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H26" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K26" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L26" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M26" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N26" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O26" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P26" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q26" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R26" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S26" t="s">
-        <v>23</v>
-      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="4"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
@@ -2596,7 +2601,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P27" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q27" s="2">
         <v>-4.72741111111111E-2</v>
@@ -2613,7 +2618,7 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -2661,19 +2666,22 @@
       <c r="R28" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S28" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E29" s="2">
         <v>1901.5157334444443</v>
@@ -2692,31 +2700,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K29" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L29" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M29" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N29" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O29" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P29" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q29" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R29" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S29" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -2724,13 +2729,13 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E30" s="2">
         <v>1901.5157334444443</v>
@@ -2749,28 +2754,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K30" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L30" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M30" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N30" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O30" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P30" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q30" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R30" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S30" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -2778,13 +2786,13 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E31" s="2">
         <v>1901.5157334444443</v>
@@ -2793,28 +2801,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G31" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H31" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I31" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I31" s="2"/>
       <c r="J31" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K31" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L31" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M31" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N31" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O31" s="3">
         <v>4883.9277073333324</v>
@@ -2823,13 +2829,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q31" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R31" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S31" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
@@ -2837,13 +2840,13 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E32" s="2">
         <v>1901.5157334444443</v>
@@ -2852,28 +2855,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G32" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H32" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I32" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J32" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K32" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L32" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M32" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N32" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O32" s="3">
         <v>4883.9277073333324</v>
@@ -2882,10 +2885,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q32" s="2">
-        <v>9.9787694444444455</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R32" s="4">
-        <v>2.9230000000000003E-3</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S32" t="s">
         <v>23</v>
@@ -2896,7 +2899,7 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
@@ -2911,7 +2914,7 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G33" s="2">
-        <v>347.23312744444445</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H33" s="2">
         <v>9.775355222222224</v>
@@ -2941,10 +2944,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q33" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R33" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S33" t="s">
         <v>23</v>
@@ -2955,55 +2958,55 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E34" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F34" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G34" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G34" s="2">
+        <v>347.23312744444445</v>
       </c>
       <c r="H34" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I34" s="5">
-        <v>13.853347222222222</v>
+      <c r="I34" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J34" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K34" s="5">
-        <v>691.23065866666673</v>
+      <c r="K34" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L34" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M34" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N34" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O34" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M34" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N34" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O34" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P34" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q34" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R34" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q34" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R34" s="4">
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S34" t="s">
         <v>23</v>
@@ -3014,13 +3017,13 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="2">
-        <v>1186.9521077777779</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E35" s="2">
         <v>1901.5157334444443</v>
@@ -3028,58 +3031,58 @@
       <c r="F35" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G35" s="2">
-        <v>280.33542888888883</v>
+      <c r="G35" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H35" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I35" s="5">
-        <v>12.968491888888888</v>
+        <v>13.853347222222222</v>
       </c>
       <c r="J35" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K35" s="2">
-        <v>645.94098588888892</v>
+      <c r="K35" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L35" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M35" s="2">
-        <v>1465.1962754444444</v>
-      </c>
-      <c r="N35" s="2">
-        <v>1191.1222331111112</v>
-      </c>
-      <c r="O35" s="3">
+      <c r="M35" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N35" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O35" s="6">
         <v>4695.8937716666669</v>
       </c>
       <c r="P35" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q35" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R35" s="4">
-        <v>3.9399999999999998E-4</v>
+      <c r="Q35" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R35" s="7">
+        <v>5.926666666666668E-4</v>
       </c>
       <c r="S35" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
+      <c r="A36" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="8" t="s">
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E36" s="2">
         <v>1901.5157334444443</v>
@@ -3093,37 +3096,37 @@
       <c r="H36" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I36" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I36" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J36" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K36" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L36" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M36" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N36" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O36" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P36" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q36" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R36" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S36" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S36" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3132,7 +3135,7 @@
         <v>16</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>23</v>
@@ -3191,13 +3194,13 @@
         <v>16</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E38" s="2">
         <v>1901.5157334444443</v>
@@ -3212,22 +3215,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I38" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J38" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K38" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L38" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M38" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N38" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O38" s="3">
         <v>4661.9885795555556</v>
@@ -3236,10 +3239,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q38" s="2">
-        <v>-1.0069492222222223</v>
+        <v>-0.95070599999999983</v>
       </c>
       <c r="R38" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S38" s="8" t="s">
         <v>23</v>
@@ -3250,70 +3253,55 @@
         <v>16</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="2">
-        <f>AVERAGE(D30:D38)</f>
-        <v>1176.9484893703707</v>
+        <v>1186.8557127777776</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" ref="E39:R40" si="0">AVERAGE(E30:E38)</f>
         <v>1901.5157334444443</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99402413580246907</v>
-      </c>
-      <c r="G39" s="5">
-        <f t="shared" si="0"/>
-        <v>308.82293032098761</v>
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G39" s="2">
+        <v>280.33542888888883</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I39" s="5">
-        <f t="shared" si="0"/>
-        <v>7.1295036805555574</v>
+      <c r="I39" s="2">
+        <v>5.3870291111111106</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K39" s="5">
-        <f t="shared" si="0"/>
-        <v>705.82954383950619</v>
+      <c r="K39" s="2">
+        <v>645.93811044444442</v>
       </c>
       <c r="L39" s="2">
-        <f t="shared" si="0"/>
-        <v>83.470620444444435</v>
-      </c>
-      <c r="M39" s="5">
-        <f t="shared" si="0"/>
-        <v>1432.1165123580245</v>
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M39" s="2">
+        <v>1455.2552082222223</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="0"/>
-        <v>1179.5111099259257</v>
-      </c>
-      <c r="O39" s="6">
-        <f t="shared" si="0"/>
-        <v>4768.1626790370356</v>
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O39" s="3">
+        <v>4661.9885795555556</v>
       </c>
       <c r="P39" s="3">
-        <f t="shared" si="0"/>
-        <v>27227.338324888893</v>
+        <v>27227.338324888889</v>
       </c>
       <c r="Q39" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6790465308641975</v>
-      </c>
-      <c r="R39" s="7">
-        <f t="shared" si="0"/>
-        <v>1.3632839506172842E-3</v>
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R39" s="4">
+        <v>-3.0444444444444448E-4</v>
       </c>
       <c r="S39" s="8" t="s">
         <v>23</v>
@@ -3324,58 +3312,58 @@
         <v>16</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="2">
         <f>AVERAGE(D31:D39)</f>
-        <v>1178.7030733497943</v>
+        <v>1176.9484893703707</v>
       </c>
       <c r="E40" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E40:R41" si="0">AVERAGE(E31:E39)</f>
         <v>1901.5157334444443</v>
       </c>
       <c r="F40" s="2">
         <f t="shared" si="0"/>
-        <v>0.99203508916323713</v>
-      </c>
-      <c r="G40" s="2">
+        <v>0.99402413580246907</v>
+      </c>
+      <c r="G40" s="5">
         <f t="shared" si="0"/>
-        <v>306.71652987517137</v>
+        <v>308.82293032098761</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="5">
         <f t="shared" si="0"/>
-        <v>7.1295036805555565</v>
+        <v>7.1295036805555574</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="5">
         <f t="shared" si="0"/>
-        <v>698.76948392043903</v>
+        <v>705.82954383950619</v>
       </c>
       <c r="L40" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M40" s="2">
+      <c r="M40" s="5">
         <f t="shared" si="0"/>
-        <v>1437.5067307928668</v>
+        <v>1432.1165123580245</v>
       </c>
       <c r="N40" s="2">
         <f t="shared" si="0"/>
-        <v>1181.53627690535</v>
-      </c>
-      <c r="O40" s="3">
+        <v>1179.5111099259257</v>
+      </c>
+      <c r="O40" s="6">
         <f t="shared" si="0"/>
-        <v>4755.299898115225</v>
+        <v>4768.1626790370356</v>
       </c>
       <c r="P40" s="3">
         <f t="shared" si="0"/>
@@ -3383,11 +3371,11 @@
       </c>
       <c r="Q40" s="2">
         <f t="shared" si="0"/>
-        <v>4.684029058984911</v>
-      </c>
-      <c r="R40" s="4">
+        <v>4.6790465308641975</v>
+      </c>
+      <c r="R40" s="7">
         <f t="shared" si="0"/>
-        <v>1.363093278463649E-3</v>
+        <v>1.3632839506172842E-3</v>
       </c>
       <c r="S40" s="8" t="s">
         <v>23</v>
@@ -3398,57 +3386,131 @@
         <v>16</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="2">
+        <f>AVERAGE(D32:D40)</f>
+        <v>1178.7030733497943</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="0"/>
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F41" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99203508916323713</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="0"/>
+        <v>306.71652987517137</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1295036805555565</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" si="0"/>
+        <v>698.76948392043903</v>
+      </c>
+      <c r="L41" s="2">
+        <f t="shared" si="0"/>
+        <v>83.470620444444435</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="0"/>
+        <v>1437.5067307928668</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="0"/>
+        <v>1181.53627690535</v>
+      </c>
+      <c r="O41" s="3">
+        <f t="shared" si="0"/>
+        <v>4755.299898115225</v>
+      </c>
+      <c r="P41" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324888893</v>
+      </c>
+      <c r="Q41" s="2">
+        <f t="shared" si="0"/>
+        <v>4.684029058984911</v>
+      </c>
+      <c r="R41" s="4">
+        <f t="shared" si="0"/>
+        <v>1.363093278463649E-3</v>
+      </c>
+      <c r="S41" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="2">
         <v>1186.9773491111109</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E42" s="2">
         <v>1901.5157334444443</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F42" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G42" s="2">
         <v>280.33542888888883</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H42" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I42" s="2">
         <v>5.3870271111111121</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J42" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K42" s="2">
         <v>645.93808322222219</v>
       </c>
-      <c r="L41" s="2">
+      <c r="L42" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M41" s="2">
+      <c r="M42" s="2">
         <v>1455.5792641111111</v>
       </c>
-      <c r="N41" s="2">
+      <c r="N42" s="2">
         <v>1191.1918266666667</v>
       </c>
-      <c r="O41" s="3">
+      <c r="O42" s="3">
         <v>4661.9885253333332</v>
       </c>
-      <c r="P41" s="3">
+      <c r="P42" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q41" s="2">
+      <c r="Q42" s="2">
         <v>-0.64567288888888896</v>
       </c>
-      <c r="R41" s="4">
+      <c r="R42" s="4">
         <v>-2.0755555555555555E-4</v>
       </c>
-      <c r="S41" s="8" t="s">
+      <c r="S42" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ReachRouting.cpp - Correct a logic error in the estimate of cloudiness.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FE0517-6789-4519-918B-5D90BE6A15CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0606D94-4E0C-4305-9DF2-861C2CB1939D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1164" yWindow="744" windowWidth="20796" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
   <si>
     <t>Year</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>Baseline 2010 C132+</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C133</t>
+  </si>
+  <si>
+    <t>Baseline 2010 C133+</t>
   </si>
 </sst>
 </file>
@@ -1076,11 +1082,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U42"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2540,85 +2546,87 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="4"/>
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26">
+        <v>2010</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1.2021059999999999</v>
+      </c>
+      <c r="G26" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H26" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I26" s="2">
+        <v>4.7316050000000001</v>
+      </c>
+      <c r="J26" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K26" s="2">
+        <v>677.36926300000005</v>
+      </c>
+      <c r="L26" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1390.2100829999999</v>
+      </c>
+      <c r="N26" s="2">
+        <v>1207.1236570000001</v>
+      </c>
+      <c r="O26" s="3">
+        <v>6722.8803710000002</v>
+      </c>
+      <c r="P26" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>-0.60321499999999995</v>
+      </c>
+      <c r="R26" s="4">
+        <v>-1.7899999999999999E-4</v>
+      </c>
+      <c r="S26">
+        <v>2010</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E27" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F27" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G27" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H27" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K27" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L27" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M27" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N27" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O27" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P27" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q27" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R27" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S27" t="s">
-        <v>23</v>
-      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="4"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -2658,7 +2666,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P28" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q28" s="2">
         <v>-4.72741111111111E-2</v>
@@ -2675,7 +2683,7 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -2723,19 +2731,22 @@
       <c r="R29" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S29" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E30" s="2">
         <v>1901.5157334444443</v>
@@ -2754,31 +2765,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K30" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L30" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M30" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N30" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O30" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P30" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q30" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R30" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S30" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -2786,13 +2794,13 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E31" s="2">
         <v>1901.5157334444443</v>
@@ -2811,28 +2819,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K31" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L31" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M31" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N31" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O31" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P31" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q31" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R31" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S31" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
@@ -2840,13 +2851,13 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E32" s="2">
         <v>1901.5157334444443</v>
@@ -2855,28 +2866,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G32" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H32" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I32" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I32" s="2"/>
       <c r="J32" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K32" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L32" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M32" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N32" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O32" s="3">
         <v>4883.9277073333324</v>
@@ -2885,13 +2894,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q32" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R32" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S32" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
@@ -2899,13 +2905,13 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E33" s="2">
         <v>1901.5157334444443</v>
@@ -2914,28 +2920,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G33" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H33" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I33" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J33" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K33" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L33" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M33" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N33" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O33" s="3">
         <v>4883.9277073333324</v>
@@ -2944,10 +2950,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q33" s="2">
-        <v>9.9787694444444455</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R33" s="4">
-        <v>2.9230000000000003E-3</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S33" t="s">
         <v>23</v>
@@ -2958,7 +2964,7 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
@@ -2973,7 +2979,7 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G34" s="2">
-        <v>347.23312744444445</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H34" s="2">
         <v>9.775355222222224</v>
@@ -3003,10 +3009,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q34" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R34" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S34" t="s">
         <v>23</v>
@@ -3017,55 +3023,55 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E35" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F35" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G35" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G35" s="2">
+        <v>347.23312744444445</v>
       </c>
       <c r="H35" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I35" s="5">
-        <v>13.853347222222222</v>
+      <c r="I35" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J35" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K35" s="5">
-        <v>691.23065866666673</v>
+      <c r="K35" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L35" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M35" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N35" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O35" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M35" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N35" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O35" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P35" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q35" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R35" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q35" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R35" s="4">
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S35" t="s">
         <v>23</v>
@@ -3076,13 +3082,13 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="2">
-        <v>1186.9521077777779</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E36" s="2">
         <v>1901.5157334444443</v>
@@ -3090,58 +3096,58 @@
       <c r="F36" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G36" s="2">
-        <v>280.33542888888883</v>
+      <c r="G36" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H36" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I36" s="5">
-        <v>12.968491888888888</v>
+        <v>13.853347222222222</v>
       </c>
       <c r="J36" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K36" s="2">
-        <v>645.94098588888892</v>
+      <c r="K36" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L36" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M36" s="2">
-        <v>1465.1962754444444</v>
-      </c>
-      <c r="N36" s="2">
-        <v>1191.1222331111112</v>
-      </c>
-      <c r="O36" s="3">
+      <c r="M36" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N36" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O36" s="6">
         <v>4695.8937716666669</v>
       </c>
       <c r="P36" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q36" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R36" s="4">
-        <v>3.9399999999999998E-4</v>
+      <c r="Q36" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R36" s="7">
+        <v>5.926666666666668E-4</v>
       </c>
       <c r="S36" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="8" t="s">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" t="s">
         <v>23</v>
       </c>
       <c r="D37" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E37" s="2">
         <v>1901.5157334444443</v>
@@ -3155,37 +3161,37 @@
       <c r="H37" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I37" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I37" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J37" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K37" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L37" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M37" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N37" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O37" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P37" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q37" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R37" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S37" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S37" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3194,7 +3200,7 @@
         <v>16</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>23</v>
@@ -3253,13 +3259,13 @@
         <v>16</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E39" s="2">
         <v>1901.5157334444443</v>
@@ -3274,22 +3280,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I39" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J39" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K39" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L39" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M39" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N39" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O39" s="3">
         <v>4661.9885795555556</v>
@@ -3298,10 +3304,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q39" s="2">
-        <v>-1.0069492222222223</v>
+        <v>-0.95070599999999983</v>
       </c>
       <c r="R39" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S39" s="8" t="s">
         <v>23</v>
@@ -3312,132 +3318,117 @@
         <v>16</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="2">
-        <f>AVERAGE(D31:D39)</f>
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G40" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H40" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I40" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J40" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K40" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L40" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M40" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N40" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O40" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P40" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R40" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S40" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="2">
+        <f>AVERAGE(D32:D40)</f>
         <v>1176.9484893703707</v>
       </c>
-      <c r="E40" s="2">
-        <f t="shared" ref="E40:R41" si="0">AVERAGE(E31:E39)</f>
+      <c r="E41" s="2">
+        <f t="shared" ref="E41:R42" si="0">AVERAGE(E32:E40)</f>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F41" s="2">
         <f t="shared" si="0"/>
         <v>0.99402413580246907</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G41" s="5">
         <f t="shared" si="0"/>
         <v>308.82293032098761</v>
-      </c>
-      <c r="H40" s="2">
-        <f t="shared" si="0"/>
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I40" s="5">
-        <f t="shared" si="0"/>
-        <v>7.1295036805555574</v>
-      </c>
-      <c r="J40" s="2">
-        <f t="shared" si="0"/>
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K40" s="5">
-        <f t="shared" si="0"/>
-        <v>705.82954383950619</v>
-      </c>
-      <c r="L40" s="2">
-        <f t="shared" si="0"/>
-        <v>83.470620444444435</v>
-      </c>
-      <c r="M40" s="5">
-        <f t="shared" si="0"/>
-        <v>1432.1165123580245</v>
-      </c>
-      <c r="N40" s="2">
-        <f t="shared" si="0"/>
-        <v>1179.5111099259257</v>
-      </c>
-      <c r="O40" s="6">
-        <f t="shared" si="0"/>
-        <v>4768.1626790370356</v>
-      </c>
-      <c r="P40" s="3">
-        <f t="shared" si="0"/>
-        <v>27227.338324888893</v>
-      </c>
-      <c r="Q40" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6790465308641975</v>
-      </c>
-      <c r="R40" s="7">
-        <f t="shared" si="0"/>
-        <v>1.3632839506172842E-3</v>
-      </c>
-      <c r="S40" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="2">
-        <f>AVERAGE(D32:D40)</f>
-        <v>1178.7030733497943</v>
-      </c>
-      <c r="E41" s="2">
-        <f t="shared" si="0"/>
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F41" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99203508916323713</v>
-      </c>
-      <c r="G41" s="2">
-        <f t="shared" si="0"/>
-        <v>306.71652987517137</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="5">
         <f t="shared" si="0"/>
-        <v>7.1295036805555565</v>
+        <v>7.1295036805555574</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="5">
         <f t="shared" si="0"/>
-        <v>698.76948392043903</v>
+        <v>705.82954383950619</v>
       </c>
       <c r="L41" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M41" s="2">
+      <c r="M41" s="5">
         <f t="shared" si="0"/>
-        <v>1437.5067307928668</v>
+        <v>1432.1165123580245</v>
       </c>
       <c r="N41" s="2">
         <f t="shared" si="0"/>
-        <v>1181.53627690535</v>
-      </c>
-      <c r="O41" s="3">
+        <v>1179.5111099259257</v>
+      </c>
+      <c r="O41" s="6">
         <f t="shared" si="0"/>
-        <v>4755.299898115225</v>
+        <v>4768.1626790370356</v>
       </c>
       <c r="P41" s="3">
         <f t="shared" si="0"/>
@@ -3445,72 +3436,205 @@
       </c>
       <c r="Q41" s="2">
         <f t="shared" si="0"/>
+        <v>4.6790465308641975</v>
+      </c>
+      <c r="R41" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3632839506172842E-3</v>
+      </c>
+      <c r="S41" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="2">
+        <f>AVERAGE(D33:D41)</f>
+        <v>1178.7030733497943</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="0"/>
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F42" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99203508916323713</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="0"/>
+        <v>306.71652987517137</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1295036805555565</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K42" s="2">
+        <f t="shared" si="0"/>
+        <v>698.76948392043903</v>
+      </c>
+      <c r="L42" s="2">
+        <f t="shared" si="0"/>
+        <v>83.470620444444435</v>
+      </c>
+      <c r="M42" s="2">
+        <f t="shared" si="0"/>
+        <v>1437.5067307928668</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" si="0"/>
+        <v>1181.53627690535</v>
+      </c>
+      <c r="O42" s="3">
+        <f t="shared" si="0"/>
+        <v>4755.299898115225</v>
+      </c>
+      <c r="P42" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324888893</v>
+      </c>
+      <c r="Q42" s="2">
+        <f t="shared" si="0"/>
         <v>4.684029058984911</v>
       </c>
-      <c r="R41" s="4">
+      <c r="R42" s="4">
         <f t="shared" si="0"/>
         <v>1.363093278463649E-3</v>
       </c>
-      <c r="S41" s="8" t="s">
+      <c r="S42" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="8" t="s">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C43" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D43" s="2">
         <v>1186.9773491111109</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E43" s="2">
         <v>1901.5157334444443</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F43" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G43" s="2">
         <v>280.33542888888883</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H43" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I43" s="2">
         <v>5.3870271111111121</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J43" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K43" s="2">
         <v>645.93808322222219</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L43" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M42" s="2">
+      <c r="M43" s="2">
         <v>1455.5792641111111</v>
       </c>
-      <c r="N42" s="2">
+      <c r="N43" s="2">
         <v>1191.1918266666667</v>
       </c>
-      <c r="O42" s="3">
+      <c r="O43" s="3">
         <v>4661.9885253333332</v>
       </c>
-      <c r="P42" s="3">
+      <c r="P43" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q42" s="2">
+      <c r="Q43" s="2">
         <v>-0.64567288888888896</v>
       </c>
-      <c r="R42" s="4">
+      <c r="R43" s="4">
         <v>-2.0755555555555555E-4</v>
       </c>
-      <c r="S42" s="8" t="s">
+      <c r="S43" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1186.9773355555556</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G44" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H44" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I44" s="2">
+        <v>5.3870271111111121</v>
+      </c>
+      <c r="J44" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K44" s="2">
+        <v>645.93833411111109</v>
+      </c>
+      <c r="L44" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M44" s="2">
+        <v>1455.5790065555557</v>
+      </c>
+      <c r="N44" s="2">
+        <v>1191.1918131111113</v>
+      </c>
+      <c r="O44" s="3">
+        <v>4661.9885253333332</v>
+      </c>
+      <c r="P44" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>-0.64567966666666665</v>
+      </c>
+      <c r="R44" s="4">
+        <v>-2.0744444444444445E-4</v>
+      </c>
+      <c r="S44" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
This log entry is for versions 135 and 136. Flow.cpp, .h - Add static Evap_m_s() to class Reach. ReachRouting.cpp, GlobalMethods.h - Add, and comment out, ReachRouting::ApplyEnergyFluxes().
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395EDB03-3575-4B38-803B-E8AE83BC4EB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EE1B5D-A859-42A4-BA53-BA17F510398C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1164" yWindow="744" windowWidth="20796" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1164" yWindow="744" windowWidth="21468" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="63">
   <si>
     <t>Year</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Baseline 2010 C134</t>
+  </si>
+  <si>
+    <t>Baseline 2010 C135+</t>
   </si>
 </sst>
 </file>
@@ -1082,11 +1085,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U44"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2605,143 +2608,146 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="4"/>
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27">
+        <v>2010</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1.2021059999999999</v>
+      </c>
+      <c r="G27" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H27" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I27" s="2">
+        <v>4.7315519999999998</v>
+      </c>
+      <c r="J27" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K27" s="2">
+        <v>677.33013900000003</v>
+      </c>
+      <c r="L27" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M27" s="2">
+        <v>1390.240601</v>
+      </c>
+      <c r="N27" s="2">
+        <v>1207.132568</v>
+      </c>
+      <c r="O27" s="3">
+        <v>6722.8808589999999</v>
+      </c>
+      <c r="P27" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>-0.60285699999999998</v>
+      </c>
+      <c r="R27" s="4">
+        <v>-1.7799999999999999E-4</v>
+      </c>
+      <c r="S27">
+        <v>2010</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" t="s">
-        <v>23</v>
+        <v>62</v>
+      </c>
+      <c r="C28">
+        <v>2010</v>
       </c>
       <c r="D28" s="2">
-        <v>1138.6194117777777</v>
+        <v>1090.199341</v>
       </c>
       <c r="E28" s="2">
-        <v>1901.5157334444443</v>
+        <v>1990.4676509999999</v>
       </c>
       <c r="F28" s="2">
-        <v>1.0119255555555557</v>
+        <v>1.2021059999999999</v>
       </c>
       <c r="G28" s="2">
-        <v>327.78053433333326</v>
+        <v>280.16485599999999</v>
       </c>
       <c r="H28" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I28" s="2"/>
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I28" s="2">
+        <v>4.7313720000000004</v>
+      </c>
       <c r="J28" s="2">
-        <v>8.145128999999999</v>
+        <v>8.8404570000000007</v>
       </c>
       <c r="K28" s="2">
-        <v>769.26639155555551</v>
+        <v>677.32769800000005</v>
       </c>
       <c r="L28" s="2">
-        <v>83.47062044444445</v>
+        <v>93.229797000000005</v>
       </c>
       <c r="M28" s="2">
-        <v>1374.8233372222221</v>
+        <v>1390.3298339999999</v>
       </c>
       <c r="N28" s="2">
-        <v>1142.9502087777778</v>
+        <v>1207.145874</v>
       </c>
       <c r="O28" s="3">
-        <v>4918.1879612222219</v>
+        <v>6722.8872069999998</v>
       </c>
       <c r="P28" s="3">
-        <v>27227.338324777778</v>
+        <v>29450.638672000001</v>
       </c>
       <c r="Q28" s="2">
-        <v>-4.72741111111111E-2</v>
+        <v>-0.50258000000000003</v>
       </c>
       <c r="R28" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S28" t="s">
-        <v>23</v>
+        <v>-1.4899999999999999E-4</v>
+      </c>
+      <c r="S28">
+        <v>2010</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F29" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G29" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H29" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K29" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L29" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M29" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N29" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O29" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P29" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q29" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R29" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S29" t="s">
-        <v>23</v>
-      </c>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="4"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -2781,7 +2787,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P30" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q30" s="2">
         <v>-4.72741111111111E-2</v>
@@ -2789,19 +2795,22 @@
       <c r="R30" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S30" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E31" s="2">
         <v>1901.5157334444443</v>
@@ -2820,28 +2829,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K31" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L31" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M31" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N31" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O31" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P31" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q31" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R31" s="4">
-        <v>1.4151111111111109E-3</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
       <c r="S31" t="s">
         <v>23</v>
@@ -2852,13 +2861,13 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="2">
-        <v>1161.1572335555554</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E32" s="2">
         <v>1901.5157334444443</v>
@@ -2877,28 +2886,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K32" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L32" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M32" s="2">
-        <v>1383.6045464444442</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N32" s="2">
-        <v>1161.284607111111</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O32" s="3">
-        <v>4883.9277073333324</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P32" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q32" s="2">
-        <v>4.6342037777777776</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R32" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
@@ -2906,13 +2915,13 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="2">
-        <v>1161.1644491111113</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E33" s="2">
         <v>1901.5157334444443</v>
@@ -2921,40 +2930,38 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G33" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H33" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I33" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I33" s="2"/>
       <c r="J33" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K33" s="2">
-        <v>769.36972377777772</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L33" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M33" s="2">
-        <v>1437.0445828888887</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N33" s="2">
-        <v>1161.2873196666667</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O33" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P33" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q33" s="2">
-        <v>27.015940777777772</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R33" s="4">
-        <v>7.9151111111111106E-3</v>
+        <v>1.4151111111111109E-3</v>
       </c>
       <c r="S33" t="s">
         <v>23</v>
@@ -2965,13 +2972,13 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E34" s="2">
         <v>1901.5157334444443</v>
@@ -2980,28 +2987,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G34" s="2">
-        <v>337.20870333333335</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H34" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I34" s="2">
-        <v>4.6813607777777788</v>
-      </c>
+      <c r="I34" s="2"/>
       <c r="J34" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K34" s="2">
-        <v>769.36992711111111</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L34" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M34" s="2">
-        <v>1403.060424888889</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N34" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O34" s="3">
         <v>4883.9277073333324</v>
@@ -3010,13 +3015,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q34" s="2">
-        <v>9.9787694444444455</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R34" s="4">
-        <v>2.9230000000000003E-3</v>
-      </c>
-      <c r="S34" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
@@ -3024,13 +3026,13 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E35" s="2">
         <v>1901.5157334444443</v>
@@ -3039,28 +3041,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G35" s="2">
-        <v>347.23312744444445</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H35" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I35" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J35" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K35" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L35" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M35" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N35" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O35" s="3">
         <v>4883.9277073333324</v>
@@ -3069,10 +3071,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q35" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R35" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S35" t="s">
         <v>23</v>
@@ -3083,55 +3085,55 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E36" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F36" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G36" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G36" s="2">
+        <v>337.20870333333335</v>
       </c>
       <c r="H36" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I36" s="5">
-        <v>13.853347222222222</v>
+      <c r="I36" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J36" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K36" s="5">
-        <v>691.23065866666673</v>
+      <c r="K36" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L36" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M36" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N36" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O36" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M36" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N36" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O36" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P36" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q36" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R36" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q36" s="2">
+        <v>9.9787694444444455</v>
+      </c>
+      <c r="R36" s="4">
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S36" t="s">
         <v>23</v>
@@ -3142,72 +3144,72 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
         <v>23</v>
       </c>
       <c r="D37" s="2">
-        <v>1186.9521077777779</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E37" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F37" s="2">
-        <v>0.97970299999999988</v>
+        <v>1.0119255555555557</v>
       </c>
       <c r="G37" s="2">
-        <v>280.33542888888883</v>
+        <v>347.23312744444445</v>
       </c>
       <c r="H37" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I37" s="5">
-        <v>12.968491888888888</v>
+      <c r="I37" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J37" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K37" s="2">
-        <v>645.94098588888892</v>
+        <v>769.36992711111111</v>
       </c>
       <c r="L37" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M37" s="2">
-        <v>1465.1962754444444</v>
+        <v>1403.060424888889</v>
       </c>
       <c r="N37" s="2">
-        <v>1191.1222331111112</v>
+        <v>1161.2856514444443</v>
       </c>
       <c r="O37" s="3">
-        <v>4695.8937716666669</v>
+        <v>4883.9277073333324</v>
       </c>
       <c r="P37" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q37" s="2">
-        <v>1.3484236666666667</v>
+        <v>-4.5654777777777787E-2</v>
       </c>
       <c r="R37" s="4">
-        <v>3.9399999999999998E-4</v>
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S37" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="8" t="s">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="2">
-        <v>1186.9497747777777</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E38" s="2">
         <v>1901.5157334444443</v>
@@ -3215,58 +3217,58 @@
       <c r="F38" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G38" s="2">
-        <v>280.33542888888883</v>
+      <c r="G38" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H38" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I38" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I38" s="5">
+        <v>13.853347222222222</v>
       </c>
       <c r="J38" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K38" s="2">
-        <v>645.93823922222225</v>
+      <c r="K38" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L38" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M38" s="2">
-        <v>1455.3145886666666</v>
-      </c>
-      <c r="N38" s="2">
-        <v>1191.1280516666666</v>
-      </c>
-      <c r="O38" s="3">
-        <v>4661.9885795555556</v>
+      <c r="M38" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N38" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O38" s="6">
+        <v>4695.8937716666669</v>
       </c>
       <c r="P38" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q38" s="2">
-        <v>-0.95070599999999983</v>
-      </c>
-      <c r="R38" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S38" s="8" t="s">
+      <c r="Q38" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R38" s="7">
+        <v>5.926666666666668E-4</v>
+      </c>
+      <c r="S38" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="8" t="s">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E39" s="2">
         <v>1901.5157334444443</v>
@@ -3280,37 +3282,37 @@
       <c r="H39" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I39" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I39" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J39" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K39" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L39" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M39" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N39" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O39" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P39" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q39" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R39" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S39" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S39" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3319,13 +3321,13 @@
         <v>16</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E40" s="2">
         <v>1901.5157334444443</v>
@@ -3340,22 +3342,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I40" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J40" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K40" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L40" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M40" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N40" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O40" s="3">
         <v>4661.9885795555556</v>
@@ -3364,10 +3366,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q40" s="2">
-        <v>-1.0069492222222223</v>
+        <v>-0.95070599999999983</v>
       </c>
       <c r="R40" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S40" s="8" t="s">
         <v>23</v>
@@ -3378,264 +3380,382 @@
         <v>16</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="2">
-        <f>AVERAGE(D32:D40)</f>
+        <v>1186.9497747777777</v>
+      </c>
+      <c r="E41" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G41" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H41" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I41" s="2">
+        <v>5.3913398888888899</v>
+      </c>
+      <c r="J41" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K41" s="2">
+        <v>645.93823922222225</v>
+      </c>
+      <c r="L41" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M41" s="2">
+        <v>1455.3145886666666</v>
+      </c>
+      <c r="N41" s="2">
+        <v>1191.1280516666666</v>
+      </c>
+      <c r="O41" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P41" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>-0.95070599999999983</v>
+      </c>
+      <c r="R41" s="4">
+        <v>-2.8933333333333328E-4</v>
+      </c>
+      <c r="S41" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E42" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G42" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H42" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I42" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J42" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K42" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L42" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M42" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N42" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O42" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P42" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R42" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S42" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="2">
+        <f>AVERAGE(D34:D42)</f>
         <v>1176.9484893703707</v>
       </c>
-      <c r="E41" s="2">
-        <f t="shared" ref="E41:R42" si="0">AVERAGE(E32:E40)</f>
+      <c r="E43" s="2">
+        <f t="shared" ref="E43:R44" si="0">AVERAGE(E34:E42)</f>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F43" s="2">
         <f t="shared" si="0"/>
         <v>0.99402413580246907</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G43" s="5">
         <f t="shared" si="0"/>
         <v>308.82293032098761</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H43" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I41" s="5">
+      <c r="I43" s="5">
         <f t="shared" si="0"/>
         <v>7.1295036805555574</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J43" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K41" s="5">
+      <c r="K43" s="5">
         <f t="shared" si="0"/>
         <v>705.82954383950619</v>
       </c>
-      <c r="L41" s="2">
+      <c r="L43" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M41" s="5">
+      <c r="M43" s="5">
         <f t="shared" si="0"/>
         <v>1432.1165123580245</v>
       </c>
-      <c r="N41" s="2">
+      <c r="N43" s="2">
         <f t="shared" si="0"/>
         <v>1179.5111099259257</v>
       </c>
-      <c r="O41" s="6">
+      <c r="O43" s="6">
         <f t="shared" si="0"/>
         <v>4768.1626790370356</v>
       </c>
-      <c r="P41" s="3">
+      <c r="P43" s="3">
         <f t="shared" si="0"/>
         <v>27227.338324888893</v>
       </c>
-      <c r="Q41" s="2">
+      <c r="Q43" s="2">
         <f t="shared" si="0"/>
         <v>4.6790465308641975</v>
       </c>
-      <c r="R41" s="7">
+      <c r="R43" s="7">
         <f t="shared" si="0"/>
         <v>1.3632839506172842E-3</v>
       </c>
-      <c r="S41" s="8" t="s">
+      <c r="S43" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="8" t="s">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C44" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="2">
-        <f>AVERAGE(D33:D41)</f>
+      <c r="D44" s="2">
+        <f>AVERAGE(D35:D43)</f>
         <v>1178.7030733497943</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E44" s="2">
         <f t="shared" si="0"/>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F44" s="2">
         <f t="shared" si="0"/>
         <v>0.99203508916323713</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G44" s="2">
         <f t="shared" si="0"/>
         <v>306.71652987517137</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H44" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I44" s="2">
         <f t="shared" si="0"/>
         <v>7.1295036805555565</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J44" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K44" s="2">
         <f t="shared" si="0"/>
         <v>698.76948392043903</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L44" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M42" s="2">
+      <c r="M44" s="2">
         <f t="shared" si="0"/>
         <v>1437.5067307928668</v>
       </c>
-      <c r="N42" s="2">
+      <c r="N44" s="2">
         <f t="shared" si="0"/>
         <v>1181.53627690535</v>
       </c>
-      <c r="O42" s="3">
+      <c r="O44" s="3">
         <f t="shared" si="0"/>
         <v>4755.299898115225</v>
       </c>
-      <c r="P42" s="3">
+      <c r="P44" s="3">
         <f t="shared" si="0"/>
         <v>27227.338324888893</v>
       </c>
-      <c r="Q42" s="2">
+      <c r="Q44" s="2">
         <f t="shared" si="0"/>
         <v>4.684029058984911</v>
       </c>
-      <c r="R42" s="4">
+      <c r="R44" s="4">
         <f t="shared" si="0"/>
         <v>1.363093278463649E-3</v>
       </c>
-      <c r="S42" s="8" t="s">
+      <c r="S44" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="8" t="s">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C45" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D45" s="2">
         <v>1186.9773491111109</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E45" s="2">
         <v>1901.5157334444443</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F45" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G45" s="2">
         <v>280.33542888888883</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H45" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I45" s="2">
         <v>5.3870271111111121</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J45" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K45" s="2">
         <v>645.93808322222219</v>
       </c>
-      <c r="L43" s="2">
+      <c r="L45" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M43" s="2">
+      <c r="M45" s="2">
         <v>1455.5792641111111</v>
       </c>
-      <c r="N43" s="2">
+      <c r="N45" s="2">
         <v>1191.1918266666667</v>
       </c>
-      <c r="O43" s="3">
+      <c r="O45" s="3">
         <v>4661.9885253333332</v>
       </c>
-      <c r="P43" s="3">
+      <c r="P45" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q43" s="2">
+      <c r="Q45" s="2">
         <v>-0.64567288888888896</v>
       </c>
-      <c r="R43" s="4">
+      <c r="R45" s="4">
         <v>-2.0755555555555555E-4</v>
       </c>
-      <c r="S43" s="8" t="s">
+      <c r="S45" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="8" t="s">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C46" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D46" s="2">
         <v>1186.9773355555556</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E46" s="2">
         <v>1901.5157334444443</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F46" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G46" s="2">
         <v>280.33542888888883</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H46" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I46" s="2">
         <v>5.3870271111111121</v>
       </c>
-      <c r="J44" s="2">
+      <c r="J46" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K46" s="2">
         <v>645.93833411111109</v>
       </c>
-      <c r="L44" s="2">
+      <c r="L46" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M44" s="2">
+      <c r="M46" s="2">
         <v>1455.5790065555557</v>
       </c>
-      <c r="N44" s="2">
+      <c r="N46" s="2">
         <v>1191.1918131111113</v>
       </c>
-      <c r="O44" s="3">
+      <c r="O46" s="3">
         <v>4661.9885253333332</v>
       </c>
-      <c r="P44" s="3">
+      <c r="P46" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q44" s="2">
+      <c r="Q46" s="2">
         <v>-0.64567966666666665</v>
       </c>
-      <c r="R44" s="4">
+      <c r="R46" s="4">
         <v>-2.0744444444444445E-4</v>
       </c>
-      <c r="S44" s="8" t="s">
+      <c r="S46" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GlobalMethods.h - Remove obsolete comments. ReachRouting.cpp - Remove the old version of SolveReachKinematicWave(). The new version calls ApplyEnergyFluxes().
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EE1B5D-A859-42A4-BA53-BA17F510398C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C019AB-2B38-4424-BE18-65B2FC99546D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1164" yWindow="744" windowWidth="21468" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="64">
   <si>
     <t>Year</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Baseline 2010 C135+</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C136</t>
   </si>
 </sst>
 </file>
@@ -1085,11 +1088,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U46"/>
+  <dimension ref="A1:U48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27:XFD27"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2726,85 +2729,87 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="4"/>
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29">
+        <v>2010</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1.2021059999999999</v>
+      </c>
+      <c r="G29" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H29" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I29" s="2">
+        <v>4.7315519999999998</v>
+      </c>
+      <c r="J29" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K29" s="2">
+        <v>677.33013900000003</v>
+      </c>
+      <c r="L29" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M29" s="2">
+        <v>1390.240601</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1207.132568</v>
+      </c>
+      <c r="O29" s="3">
+        <v>6722.8808589999999</v>
+      </c>
+      <c r="P29" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>-0.60285699999999998</v>
+      </c>
+      <c r="R29" s="4">
+        <v>-1.7799999999999999E-4</v>
+      </c>
+      <c r="S29">
+        <v>2010</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E30" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F30" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G30" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H30" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K30" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L30" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M30" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N30" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O30" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P30" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q30" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R30" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S30" t="s">
-        <v>23</v>
-      </c>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="4"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
@@ -2844,7 +2849,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P31" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q31" s="2">
         <v>-4.72741111111111E-2</v>
@@ -2861,7 +2866,7 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
@@ -2909,19 +2914,22 @@
       <c r="R32" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S32" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E33" s="2">
         <v>1901.5157334444443</v>
@@ -2940,31 +2948,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K33" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L33" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M33" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N33" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O33" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P33" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q33" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R33" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S33" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
@@ -2972,13 +2977,13 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E34" s="2">
         <v>1901.5157334444443</v>
@@ -2997,28 +3002,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K34" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L34" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M34" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N34" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O34" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P34" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q34" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R34" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S34" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
@@ -3026,13 +3034,13 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E35" s="2">
         <v>1901.5157334444443</v>
@@ -3041,28 +3049,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G35" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H35" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I35" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I35" s="2"/>
       <c r="J35" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K35" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L35" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M35" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N35" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O35" s="3">
         <v>4883.9277073333324</v>
@@ -3071,13 +3077,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q35" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R35" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S35" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
@@ -3085,13 +3088,13 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E36" s="2">
         <v>1901.5157334444443</v>
@@ -3100,28 +3103,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G36" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H36" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I36" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J36" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K36" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L36" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M36" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N36" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O36" s="3">
         <v>4883.9277073333324</v>
@@ -3130,10 +3133,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q36" s="2">
-        <v>9.9787694444444455</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R36" s="4">
-        <v>2.9230000000000003E-3</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S36" t="s">
         <v>23</v>
@@ -3144,7 +3147,7 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
         <v>23</v>
@@ -3159,7 +3162,7 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G37" s="2">
-        <v>347.23312744444445</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H37" s="2">
         <v>9.775355222222224</v>
@@ -3189,10 +3192,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q37" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R37" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S37" t="s">
         <v>23</v>
@@ -3203,55 +3206,55 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E38" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F38" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G38" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G38" s="2">
+        <v>347.23312744444445</v>
       </c>
       <c r="H38" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I38" s="5">
-        <v>13.853347222222222</v>
+      <c r="I38" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J38" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K38" s="5">
-        <v>691.23065866666673</v>
+      <c r="K38" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L38" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M38" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N38" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O38" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M38" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N38" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O38" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P38" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q38" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R38" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q38" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R38" s="4">
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S38" t="s">
         <v>23</v>
@@ -3262,13 +3265,13 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="2">
-        <v>1186.9521077777779</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E39" s="2">
         <v>1901.5157334444443</v>
@@ -3276,58 +3279,58 @@
       <c r="F39" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G39" s="2">
-        <v>280.33542888888883</v>
+      <c r="G39" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H39" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I39" s="5">
-        <v>12.968491888888888</v>
+        <v>13.853347222222222</v>
       </c>
       <c r="J39" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K39" s="2">
-        <v>645.94098588888892</v>
+      <c r="K39" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L39" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M39" s="2">
-        <v>1465.1962754444444</v>
-      </c>
-      <c r="N39" s="2">
-        <v>1191.1222331111112</v>
-      </c>
-      <c r="O39" s="3">
+      <c r="M39" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N39" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O39" s="6">
         <v>4695.8937716666669</v>
       </c>
       <c r="P39" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q39" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R39" s="4">
-        <v>3.9399999999999998E-4</v>
+      <c r="Q39" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R39" s="7">
+        <v>5.926666666666668E-4</v>
       </c>
       <c r="S39" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" s="8" t="s">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E40" s="2">
         <v>1901.5157334444443</v>
@@ -3341,37 +3344,37 @@
       <c r="H40" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I40" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I40" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J40" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K40" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L40" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M40" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N40" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O40" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P40" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q40" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R40" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S40" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S40" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3380,7 +3383,7 @@
         <v>16</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>23</v>
@@ -3439,13 +3442,13 @@
         <v>16</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E42" s="2">
         <v>1901.5157334444443</v>
@@ -3460,22 +3463,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I42" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J42" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K42" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L42" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M42" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N42" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O42" s="3">
         <v>4661.9885795555556</v>
@@ -3484,10 +3487,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q42" s="2">
-        <v>-1.0069492222222223</v>
+        <v>-0.95070599999999983</v>
       </c>
       <c r="R42" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S42" s="8" t="s">
         <v>23</v>
@@ -3498,132 +3501,117 @@
         <v>16</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D43" s="2">
-        <f>AVERAGE(D34:D42)</f>
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G43" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H43" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I43" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J43" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K43" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L43" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M43" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N43" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O43" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P43" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R43" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S43" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="2">
+        <f>AVERAGE(D35:D43)</f>
         <v>1176.9484893703707</v>
       </c>
-      <c r="E43" s="2">
-        <f t="shared" ref="E43:R44" si="0">AVERAGE(E34:E42)</f>
+      <c r="E44" s="2">
+        <f t="shared" ref="E44:R45" si="0">AVERAGE(E35:E43)</f>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F44" s="2">
         <f t="shared" si="0"/>
         <v>0.99402413580246907</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G44" s="5">
         <f t="shared" si="0"/>
         <v>308.82293032098761</v>
-      </c>
-      <c r="H43" s="2">
-        <f t="shared" si="0"/>
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I43" s="5">
-        <f t="shared" si="0"/>
-        <v>7.1295036805555574</v>
-      </c>
-      <c r="J43" s="2">
-        <f t="shared" si="0"/>
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K43" s="5">
-        <f t="shared" si="0"/>
-        <v>705.82954383950619</v>
-      </c>
-      <c r="L43" s="2">
-        <f t="shared" si="0"/>
-        <v>83.470620444444435</v>
-      </c>
-      <c r="M43" s="5">
-        <f t="shared" si="0"/>
-        <v>1432.1165123580245</v>
-      </c>
-      <c r="N43" s="2">
-        <f t="shared" si="0"/>
-        <v>1179.5111099259257</v>
-      </c>
-      <c r="O43" s="6">
-        <f t="shared" si="0"/>
-        <v>4768.1626790370356</v>
-      </c>
-      <c r="P43" s="3">
-        <f t="shared" si="0"/>
-        <v>27227.338324888893</v>
-      </c>
-      <c r="Q43" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6790465308641975</v>
-      </c>
-      <c r="R43" s="7">
-        <f t="shared" si="0"/>
-        <v>1.3632839506172842E-3</v>
-      </c>
-      <c r="S43" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="2">
-        <f>AVERAGE(D35:D43)</f>
-        <v>1178.7030733497943</v>
-      </c>
-      <c r="E44" s="2">
-        <f t="shared" si="0"/>
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F44" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99203508916323713</v>
-      </c>
-      <c r="G44" s="2">
-        <f t="shared" si="0"/>
-        <v>306.71652987517137</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I44" s="5">
         <f t="shared" si="0"/>
-        <v>7.1295036805555565</v>
+        <v>7.1295036805555574</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="5">
         <f t="shared" si="0"/>
-        <v>698.76948392043903</v>
+        <v>705.82954383950619</v>
       </c>
       <c r="L44" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M44" s="2">
+      <c r="M44" s="5">
         <f t="shared" si="0"/>
-        <v>1437.5067307928668</v>
+        <v>1432.1165123580245</v>
       </c>
       <c r="N44" s="2">
         <f t="shared" si="0"/>
-        <v>1181.53627690535</v>
-      </c>
-      <c r="O44" s="3">
+        <v>1179.5111099259257</v>
+      </c>
+      <c r="O44" s="6">
         <f t="shared" si="0"/>
-        <v>4755.299898115225</v>
+        <v>4768.1626790370356</v>
       </c>
       <c r="P44" s="3">
         <f t="shared" si="0"/>
@@ -3631,71 +3619,86 @@
       </c>
       <c r="Q44" s="2">
         <f t="shared" si="0"/>
+        <v>4.6790465308641975</v>
+      </c>
+      <c r="R44" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3632839506172842E-3</v>
+      </c>
+      <c r="S44" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="2">
+        <f>AVERAGE(D36:D44)</f>
+        <v>1178.7030733497943</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="0"/>
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F45" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99203508916323713</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="0"/>
+        <v>306.71652987517137</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1295036805555565</v>
+      </c>
+      <c r="J45" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K45" s="2">
+        <f t="shared" si="0"/>
+        <v>698.76948392043903</v>
+      </c>
+      <c r="L45" s="2">
+        <f t="shared" si="0"/>
+        <v>83.470620444444435</v>
+      </c>
+      <c r="M45" s="2">
+        <f t="shared" si="0"/>
+        <v>1437.5067307928668</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="0"/>
+        <v>1181.53627690535</v>
+      </c>
+      <c r="O45" s="3">
+        <f t="shared" si="0"/>
+        <v>4755.299898115225</v>
+      </c>
+      <c r="P45" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324888893</v>
+      </c>
+      <c r="Q45" s="2">
+        <f t="shared" si="0"/>
         <v>4.684029058984911</v>
       </c>
-      <c r="R44" s="4">
+      <c r="R45" s="4">
         <f t="shared" si="0"/>
         <v>1.363093278463649E-3</v>
       </c>
-      <c r="S44" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="2">
-        <v>1186.9773491111109</v>
-      </c>
-      <c r="E45" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F45" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G45" s="2">
-        <v>280.33542888888883</v>
-      </c>
-      <c r="H45" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I45" s="2">
-        <v>5.3870271111111121</v>
-      </c>
-      <c r="J45" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K45" s="2">
-        <v>645.93808322222219</v>
-      </c>
-      <c r="L45" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M45" s="2">
-        <v>1455.5792641111111</v>
-      </c>
-      <c r="N45" s="2">
-        <v>1191.1918266666667</v>
-      </c>
-      <c r="O45" s="3">
-        <v>4661.9885253333332</v>
-      </c>
-      <c r="P45" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q45" s="2">
-        <v>-0.64567288888888896</v>
-      </c>
-      <c r="R45" s="4">
-        <v>-2.0755555555555555E-4</v>
-      </c>
       <c r="S45" s="8" t="s">
         <v>23</v>
       </c>
@@ -3705,13 +3708,13 @@
         <v>16</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="2">
-        <v>1186.9773355555556</v>
+        <v>1186.9773491111109</v>
       </c>
       <c r="E46" s="2">
         <v>1901.5157334444443</v>
@@ -3732,16 +3735,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K46" s="2">
-        <v>645.93833411111109</v>
+        <v>645.93808322222219</v>
       </c>
       <c r="L46" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M46" s="2">
-        <v>1455.5790065555557</v>
+        <v>1455.5792641111111</v>
       </c>
       <c r="N46" s="2">
-        <v>1191.1918131111113</v>
+        <v>1191.1918266666667</v>
       </c>
       <c r="O46" s="3">
         <v>4661.9885253333332</v>
@@ -3750,12 +3753,130 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q46" s="2">
+        <v>-0.64567288888888896</v>
+      </c>
+      <c r="R46" s="4">
+        <v>-2.0755555555555555E-4</v>
+      </c>
+      <c r="S46" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1186.9773355555556</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G47" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H47" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I47" s="2">
+        <v>5.3870271111111121</v>
+      </c>
+      <c r="J47" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K47" s="2">
+        <v>645.93833411111109</v>
+      </c>
+      <c r="L47" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M47" s="2">
+        <v>1455.5790065555557</v>
+      </c>
+      <c r="N47" s="2">
+        <v>1191.1918131111113</v>
+      </c>
+      <c r="O47" s="3">
+        <v>4661.9885253333332</v>
+      </c>
+      <c r="P47" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q47" s="2">
         <v>-0.64567966666666665</v>
       </c>
-      <c r="R46" s="4">
+      <c r="R47" s="4">
         <v>-2.0744444444444445E-4</v>
       </c>
-      <c r="S46" s="8" t="s">
+      <c r="S47" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1186.9773355555556</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G48" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H48" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I48" s="2">
+        <v>5.3870271111111121</v>
+      </c>
+      <c r="J48" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K48" s="2">
+        <v>645.9383002222221</v>
+      </c>
+      <c r="L48" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M48" s="2">
+        <v>1455.5790607777778</v>
+      </c>
+      <c r="N48" s="2">
+        <v>1191.1918131111113</v>
+      </c>
+      <c r="O48" s="3">
+        <v>4661.9885253333332</v>
+      </c>
+      <c r="P48" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>-0.64565933333333325</v>
+      </c>
+      <c r="R48" s="4">
+        <v>-2.0744444444444445E-4</v>
+      </c>
+      <c r="S48" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add solar_radiation_multiplier field to the <reservoir> block in the Flow XML file. Flow.cpp, .h - Add Reach::GetSubreachShade-a-lator_W_m2(), but just with placeholder code. Add Reservoir::m_resSWmult. GlobalMethods.h, ReachRouting.cpp - Pass shortwave amount to ApplyEnergyFluxes() after doing the Shade-a-lator adjustment, instead of doing the Shade-a-lator adjustment in ApplyEnergyFluxes() itself.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C019AB-2B38-4424-BE18-65B2FC99546D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DF7FDA-EB4C-40A4-8544-5FB05E1EEC9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1164" yWindow="744" windowWidth="21468" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="65">
   <si>
     <t>Year</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C136</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C138</t>
   </si>
 </sst>
 </file>
@@ -1088,11 +1091,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U48"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O55" sqref="O55"/>
+      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3880,6 +3883,65 @@
         <v>23</v>
       </c>
     </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1187.0067003333331</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G49" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H49" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I49" s="2">
+        <v>5.3870271111111121</v>
+      </c>
+      <c r="J49" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K49" s="2">
+        <v>645.93713388888887</v>
+      </c>
+      <c r="L49" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M49" s="2">
+        <v>1455.6553682222225</v>
+      </c>
+      <c r="N49" s="2">
+        <v>1191.1764458888888</v>
+      </c>
+      <c r="O49" s="3">
+        <v>4661.9885253333332</v>
+      </c>
+      <c r="P49" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>-0.61525011111111105</v>
+      </c>
+      <c r="R49" s="4">
+        <v>-1.7433333333333333E-4</v>
+      </c>
+      <c r="S49" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Include water temperatures in the IC Flow initial conditions file. Flow.cpp, .h - Add m_ICincludesWP to class FlowModel. Add code to ReadState() and SaveState(), preserving the ability to read old IC files which don't include water temperatures.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DF7FDA-EB4C-40A4-8544-5FB05E1EEC9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D74B0C-F9BD-4166-9495-6AB730F0F979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1164" yWindow="744" windowWidth="21468" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
   <si>
     <t>Year</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C138</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18_C151</t>
   </si>
 </sst>
 </file>
@@ -1091,11 +1094,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U49"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V54" sqref="V54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2791,85 +2794,87 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="4"/>
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30">
+        <v>2010</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1090.199341</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1.2021059999999999</v>
+      </c>
+      <c r="G30" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H30" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I30" s="2">
+        <v>4.7315560000000003</v>
+      </c>
+      <c r="J30" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K30" s="2">
+        <v>677.33081100000004</v>
+      </c>
+      <c r="L30" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M30" s="2">
+        <v>1392.387207</v>
+      </c>
+      <c r="N30" s="2">
+        <v>1206.9267580000001</v>
+      </c>
+      <c r="O30" s="3">
+        <v>6722.8813479999999</v>
+      </c>
+      <c r="P30" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>1.338606</v>
+      </c>
+      <c r="R30" s="4">
+        <v>3.9599999999999998E-4</v>
+      </c>
+      <c r="S30">
+        <v>2010</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E31" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F31" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G31" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H31" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K31" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L31" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M31" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N31" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O31" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P31" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q31" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R31" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S31" t="s">
-        <v>23</v>
-      </c>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="4"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
@@ -2909,7 +2914,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P32" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q32" s="2">
         <v>-4.72741111111111E-2</v>
@@ -2926,7 +2931,7 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
@@ -2974,19 +2979,22 @@
       <c r="R33" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S33" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E34" s="2">
         <v>1901.5157334444443</v>
@@ -3005,31 +3013,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K34" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L34" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M34" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N34" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O34" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P34" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q34" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R34" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S34" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
@@ -3037,13 +3042,13 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E35" s="2">
         <v>1901.5157334444443</v>
@@ -3062,28 +3067,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K35" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L35" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M35" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N35" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O35" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P35" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q35" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R35" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S35" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
@@ -3091,13 +3099,13 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E36" s="2">
         <v>1901.5157334444443</v>
@@ -3106,28 +3114,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G36" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H36" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I36" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I36" s="2"/>
       <c r="J36" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K36" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L36" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M36" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N36" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O36" s="3">
         <v>4883.9277073333324</v>
@@ -3136,13 +3142,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q36" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R36" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S36" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
@@ -3150,13 +3153,13 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
         <v>23</v>
       </c>
       <c r="D37" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E37" s="2">
         <v>1901.5157334444443</v>
@@ -3165,28 +3168,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G37" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H37" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I37" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J37" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K37" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L37" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M37" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N37" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O37" s="3">
         <v>4883.9277073333324</v>
@@ -3195,10 +3198,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q37" s="2">
-        <v>9.9787694444444455</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R37" s="4">
-        <v>2.9230000000000003E-3</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S37" t="s">
         <v>23</v>
@@ -3209,7 +3212,7 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
@@ -3224,7 +3227,7 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G38" s="2">
-        <v>347.23312744444445</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H38" s="2">
         <v>9.775355222222224</v>
@@ -3254,10 +3257,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q38" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R38" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S38" t="s">
         <v>23</v>
@@ -3268,55 +3271,55 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E39" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F39" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G39" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G39" s="2">
+        <v>347.23312744444445</v>
       </c>
       <c r="H39" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I39" s="5">
-        <v>13.853347222222222</v>
+      <c r="I39" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J39" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K39" s="5">
-        <v>691.23065866666673</v>
+      <c r="K39" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L39" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M39" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N39" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O39" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M39" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N39" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O39" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P39" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q39" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R39" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q39" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R39" s="4">
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S39" t="s">
         <v>23</v>
@@ -3327,13 +3330,13 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="2">
-        <v>1186.9521077777779</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E40" s="2">
         <v>1901.5157334444443</v>
@@ -3341,58 +3344,58 @@
       <c r="F40" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G40" s="2">
-        <v>280.33542888888883</v>
+      <c r="G40" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H40" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I40" s="5">
-        <v>12.968491888888888</v>
+        <v>13.853347222222222</v>
       </c>
       <c r="J40" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K40" s="2">
-        <v>645.94098588888892</v>
+      <c r="K40" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L40" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M40" s="2">
-        <v>1465.1962754444444</v>
-      </c>
-      <c r="N40" s="2">
-        <v>1191.1222331111112</v>
-      </c>
-      <c r="O40" s="3">
+      <c r="M40" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N40" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O40" s="6">
         <v>4695.8937716666669</v>
       </c>
       <c r="P40" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q40" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R40" s="4">
-        <v>3.9399999999999998E-4</v>
+      <c r="Q40" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R40" s="7">
+        <v>5.926666666666668E-4</v>
       </c>
       <c r="S40" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="8" t="s">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E41" s="2">
         <v>1901.5157334444443</v>
@@ -3406,37 +3409,37 @@
       <c r="H41" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I41" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I41" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J41" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K41" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L41" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M41" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N41" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O41" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P41" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q41" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R41" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S41" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S41" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3445,7 +3448,7 @@
         <v>16</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>23</v>
@@ -3504,13 +3507,13 @@
         <v>16</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D43" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E43" s="2">
         <v>1901.5157334444443</v>
@@ -3525,22 +3528,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I43" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J43" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K43" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L43" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M43" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N43" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O43" s="3">
         <v>4661.9885795555556</v>
@@ -3549,10 +3552,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q43" s="2">
-        <v>-1.0069492222222223</v>
+        <v>-0.95070599999999983</v>
       </c>
       <c r="R43" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S43" s="8" t="s">
         <v>23</v>
@@ -3563,132 +3566,117 @@
         <v>16</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="2">
-        <f>AVERAGE(D35:D43)</f>
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G44" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H44" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I44" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J44" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K44" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L44" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M44" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N44" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O44" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P44" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R44" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S44" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="2">
+        <f>AVERAGE(D36:D44)</f>
         <v>1176.9484893703707</v>
       </c>
-      <c r="E44" s="2">
-        <f t="shared" ref="E44:R45" si="0">AVERAGE(E35:E43)</f>
+      <c r="E45" s="2">
+        <f t="shared" ref="E45:R46" si="0">AVERAGE(E36:E44)</f>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F45" s="2">
         <f t="shared" si="0"/>
         <v>0.99402413580246907</v>
       </c>
-      <c r="G44" s="5">
+      <c r="G45" s="5">
         <f t="shared" si="0"/>
         <v>308.82293032098761</v>
-      </c>
-      <c r="H44" s="2">
-        <f t="shared" si="0"/>
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I44" s="5">
-        <f t="shared" si="0"/>
-        <v>7.1295036805555574</v>
-      </c>
-      <c r="J44" s="2">
-        <f t="shared" si="0"/>
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K44" s="5">
-        <f t="shared" si="0"/>
-        <v>705.82954383950619</v>
-      </c>
-      <c r="L44" s="2">
-        <f t="shared" si="0"/>
-        <v>83.470620444444435</v>
-      </c>
-      <c r="M44" s="5">
-        <f t="shared" si="0"/>
-        <v>1432.1165123580245</v>
-      </c>
-      <c r="N44" s="2">
-        <f t="shared" si="0"/>
-        <v>1179.5111099259257</v>
-      </c>
-      <c r="O44" s="6">
-        <f t="shared" si="0"/>
-        <v>4768.1626790370356</v>
-      </c>
-      <c r="P44" s="3">
-        <f t="shared" si="0"/>
-        <v>27227.338324888893</v>
-      </c>
-      <c r="Q44" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6790465308641975</v>
-      </c>
-      <c r="R44" s="7">
-        <f t="shared" si="0"/>
-        <v>1.3632839506172842E-3</v>
-      </c>
-      <c r="S44" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="2">
-        <f>AVERAGE(D36:D44)</f>
-        <v>1178.7030733497943</v>
-      </c>
-      <c r="E45" s="2">
-        <f t="shared" si="0"/>
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F45" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99203508916323713</v>
-      </c>
-      <c r="G45" s="2">
-        <f t="shared" si="0"/>
-        <v>306.71652987517137</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I45" s="5">
         <f t="shared" si="0"/>
-        <v>7.1295036805555565</v>
+        <v>7.1295036805555574</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="5">
         <f t="shared" si="0"/>
-        <v>698.76948392043903</v>
+        <v>705.82954383950619</v>
       </c>
       <c r="L45" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M45" s="5">
         <f t="shared" si="0"/>
-        <v>1437.5067307928668</v>
+        <v>1432.1165123580245</v>
       </c>
       <c r="N45" s="2">
         <f t="shared" si="0"/>
-        <v>1181.53627690535</v>
-      </c>
-      <c r="O45" s="3">
+        <v>1179.5111099259257</v>
+      </c>
+      <c r="O45" s="6">
         <f t="shared" si="0"/>
-        <v>4755.299898115225</v>
+        <v>4768.1626790370356</v>
       </c>
       <c r="P45" s="3">
         <f t="shared" si="0"/>
@@ -3696,71 +3684,86 @@
       </c>
       <c r="Q45" s="2">
         <f t="shared" si="0"/>
+        <v>4.6790465308641975</v>
+      </c>
+      <c r="R45" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3632839506172842E-3</v>
+      </c>
+      <c r="S45" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="2">
+        <f>AVERAGE(D37:D45)</f>
+        <v>1178.7030733497943</v>
+      </c>
+      <c r="E46" s="2">
+        <f t="shared" si="0"/>
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F46" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99203508916323713</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="0"/>
+        <v>306.71652987517137</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1295036805555565</v>
+      </c>
+      <c r="J46" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K46" s="2">
+        <f t="shared" si="0"/>
+        <v>698.76948392043903</v>
+      </c>
+      <c r="L46" s="2">
+        <f t="shared" si="0"/>
+        <v>83.470620444444435</v>
+      </c>
+      <c r="M46" s="2">
+        <f t="shared" si="0"/>
+        <v>1437.5067307928668</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="0"/>
+        <v>1181.53627690535</v>
+      </c>
+      <c r="O46" s="3">
+        <f t="shared" si="0"/>
+        <v>4755.299898115225</v>
+      </c>
+      <c r="P46" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324888893</v>
+      </c>
+      <c r="Q46" s="2">
+        <f t="shared" si="0"/>
         <v>4.684029058984911</v>
       </c>
-      <c r="R45" s="4">
+      <c r="R46" s="4">
         <f t="shared" si="0"/>
         <v>1.363093278463649E-3</v>
       </c>
-      <c r="S45" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="2">
-        <v>1186.9773491111109</v>
-      </c>
-      <c r="E46" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F46" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G46" s="2">
-        <v>280.33542888888883</v>
-      </c>
-      <c r="H46" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I46" s="2">
-        <v>5.3870271111111121</v>
-      </c>
-      <c r="J46" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K46" s="2">
-        <v>645.93808322222219</v>
-      </c>
-      <c r="L46" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M46" s="2">
-        <v>1455.5792641111111</v>
-      </c>
-      <c r="N46" s="2">
-        <v>1191.1918266666667</v>
-      </c>
-      <c r="O46" s="3">
-        <v>4661.9885253333332</v>
-      </c>
-      <c r="P46" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q46" s="2">
-        <v>-0.64567288888888896</v>
-      </c>
-      <c r="R46" s="4">
-        <v>-2.0755555555555555E-4</v>
-      </c>
       <c r="S46" s="8" t="s">
         <v>23</v>
       </c>
@@ -3770,13 +3773,13 @@
         <v>16</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="2">
-        <v>1186.9773355555556</v>
+        <v>1186.9773491111109</v>
       </c>
       <c r="E47" s="2">
         <v>1901.5157334444443</v>
@@ -3797,16 +3800,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K47" s="2">
-        <v>645.93833411111109</v>
+        <v>645.93808322222219</v>
       </c>
       <c r="L47" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M47" s="2">
-        <v>1455.5790065555557</v>
+        <v>1455.5792641111111</v>
       </c>
       <c r="N47" s="2">
-        <v>1191.1918131111113</v>
+        <v>1191.1918266666667</v>
       </c>
       <c r="O47" s="3">
         <v>4661.9885253333332</v>
@@ -3815,10 +3818,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q47" s="2">
-        <v>-0.64567966666666665</v>
+        <v>-0.64567288888888896</v>
       </c>
       <c r="R47" s="4">
-        <v>-2.0744444444444445E-4</v>
+        <v>-2.0755555555555555E-4</v>
       </c>
       <c r="S47" s="8" t="s">
         <v>23</v>
@@ -3829,7 +3832,7 @@
         <v>16</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>23</v>
@@ -3856,13 +3859,13 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K48" s="2">
-        <v>645.9383002222221</v>
+        <v>645.93833411111109</v>
       </c>
       <c r="L48" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M48" s="2">
-        <v>1455.5790607777778</v>
+        <v>1455.5790065555557</v>
       </c>
       <c r="N48" s="2">
         <v>1191.1918131111113</v>
@@ -3874,7 +3877,7 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q48" s="2">
-        <v>-0.64565933333333325</v>
+        <v>-0.64567966666666665</v>
       </c>
       <c r="R48" s="4">
         <v>-2.0744444444444445E-4</v>
@@ -3888,13 +3891,13 @@
         <v>16</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D49" s="2">
-        <v>1187.0067003333331</v>
+        <v>1186.9773355555556</v>
       </c>
       <c r="E49" s="2">
         <v>1901.5157334444443</v>
@@ -3915,16 +3918,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K49" s="2">
-        <v>645.93713388888887</v>
+        <v>645.9383002222221</v>
       </c>
       <c r="L49" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M49" s="2">
-        <v>1455.6553682222225</v>
+        <v>1455.5790607777778</v>
       </c>
       <c r="N49" s="2">
-        <v>1191.1764458888888</v>
+        <v>1191.1918131111113</v>
       </c>
       <c r="O49" s="3">
         <v>4661.9885253333332</v>
@@ -3933,12 +3936,130 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q49" s="2">
+        <v>-0.64565933333333325</v>
+      </c>
+      <c r="R49" s="4">
+        <v>-2.0744444444444445E-4</v>
+      </c>
+      <c r="S49" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1187.0067003333331</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G50" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H50" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I50" s="2">
+        <v>5.3870271111111121</v>
+      </c>
+      <c r="J50" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K50" s="2">
+        <v>645.93713388888887</v>
+      </c>
+      <c r="L50" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M50" s="2">
+        <v>1455.6553682222225</v>
+      </c>
+      <c r="N50" s="2">
+        <v>1191.1764458888888</v>
+      </c>
+      <c r="O50" s="3">
+        <v>4661.9885253333332</v>
+      </c>
+      <c r="P50" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q50" s="2">
         <v>-0.61525011111111105</v>
       </c>
-      <c r="R49" s="4">
+      <c r="R50" s="4">
         <v>-1.7433333333333333E-4</v>
       </c>
-      <c r="S49" s="8" t="s">
+      <c r="S50" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1187.0063613333334</v>
+      </c>
+      <c r="E51" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G51" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H51" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I51" s="2">
+        <v>5.3870315555555557</v>
+      </c>
+      <c r="J51" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K51" s="2">
+        <v>645.93916833333344</v>
+      </c>
+      <c r="L51" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M51" s="2">
+        <v>1455.7051053333334</v>
+      </c>
+      <c r="N51" s="2">
+        <v>1191.1759305555559</v>
+      </c>
+      <c r="O51" s="3">
+        <v>4661.988498222222</v>
+      </c>
+      <c r="P51" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>-0.56365988888888896</v>
+      </c>
+      <c r="R51" s="4">
+        <v>-1.5888888888888889E-4</v>
+      </c>
+      <c r="S51" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
McKenzie/flow2010.ic - New IC file which includes water temperatures, from the Baseline_2000-09_C155 run.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D74B0C-F9BD-4166-9495-6AB730F0F979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C414CD1-B808-4FB0-8D2D-2E5452F97AEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="67">
   <si>
     <t>Year</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Baseline 2010-18_C151</t>
+  </si>
+  <si>
+    <t>Baseline 2010_C155+</t>
   </si>
 </sst>
 </file>
@@ -1094,11 +1097,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V54" sqref="V54"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2853,85 +2856,87 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="4"/>
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31">
+        <v>2010</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1136.616577</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1.2021059999999999</v>
+      </c>
+      <c r="G31" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H31" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I31" s="2">
+        <v>4.5522390000000001</v>
+      </c>
+      <c r="J31" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K31" s="2">
+        <v>677.62432899999999</v>
+      </c>
+      <c r="L31" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M31" s="5">
+        <v>1397.4351810000001</v>
+      </c>
+      <c r="N31" s="5">
+        <v>1247.803345</v>
+      </c>
+      <c r="O31" s="3">
+        <v>6725.3081050000001</v>
+      </c>
+      <c r="P31" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>1.318765</v>
+      </c>
+      <c r="R31" s="4">
+        <v>3.8499999999999998E-4</v>
+      </c>
+      <c r="S31">
+        <v>2010</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E32" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F32" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G32" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H32" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K32" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L32" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M32" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N32" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O32" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P32" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q32" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R32" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S32" t="s">
-        <v>23</v>
-      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="4"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
@@ -2971,7 +2976,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P33" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q33" s="2">
         <v>-4.72741111111111E-2</v>
@@ -2988,7 +2993,7 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
@@ -3036,19 +3041,22 @@
       <c r="R34" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S34" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E35" s="2">
         <v>1901.5157334444443</v>
@@ -3067,31 +3075,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K35" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L35" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M35" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N35" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O35" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P35" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q35" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R35" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S35" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
@@ -3099,13 +3104,13 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E36" s="2">
         <v>1901.5157334444443</v>
@@ -3124,28 +3129,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K36" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L36" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M36" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N36" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O36" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P36" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q36" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R36" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S36" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
@@ -3153,13 +3161,13 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C37" t="s">
         <v>23</v>
       </c>
       <c r="D37" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E37" s="2">
         <v>1901.5157334444443</v>
@@ -3168,28 +3176,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G37" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H37" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I37" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I37" s="2"/>
       <c r="J37" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K37" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L37" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M37" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N37" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O37" s="3">
         <v>4883.9277073333324</v>
@@ -3198,13 +3204,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q37" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R37" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S37" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
@@ -3212,13 +3215,13 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E38" s="2">
         <v>1901.5157334444443</v>
@@ -3227,28 +3230,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G38" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H38" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I38" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J38" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K38" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L38" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M38" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N38" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O38" s="3">
         <v>4883.9277073333324</v>
@@ -3257,10 +3260,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q38" s="2">
-        <v>9.9787694444444455</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R38" s="4">
-        <v>2.9230000000000003E-3</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S38" t="s">
         <v>23</v>
@@ -3271,7 +3274,7 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
         <v>23</v>
@@ -3286,7 +3289,7 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G39" s="2">
-        <v>347.23312744444445</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H39" s="2">
         <v>9.775355222222224</v>
@@ -3316,10 +3319,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q39" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R39" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S39" t="s">
         <v>23</v>
@@ -3330,55 +3333,55 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E40" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F40" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G40" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G40" s="2">
+        <v>347.23312744444445</v>
       </c>
       <c r="H40" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I40" s="5">
-        <v>13.853347222222222</v>
+      <c r="I40" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J40" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K40" s="5">
-        <v>691.23065866666673</v>
+      <c r="K40" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L40" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M40" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N40" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O40" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M40" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N40" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O40" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P40" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q40" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R40" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q40" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R40" s="4">
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S40" t="s">
         <v>23</v>
@@ -3389,13 +3392,13 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="2">
-        <v>1186.9521077777779</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E41" s="2">
         <v>1901.5157334444443</v>
@@ -3403,58 +3406,58 @@
       <c r="F41" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G41" s="2">
-        <v>280.33542888888883</v>
+      <c r="G41" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H41" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I41" s="5">
-        <v>12.968491888888888</v>
+        <v>13.853347222222222</v>
       </c>
       <c r="J41" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K41" s="2">
-        <v>645.94098588888892</v>
+      <c r="K41" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L41" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M41" s="2">
-        <v>1465.1962754444444</v>
-      </c>
-      <c r="N41" s="2">
-        <v>1191.1222331111112</v>
-      </c>
-      <c r="O41" s="3">
+      <c r="M41" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N41" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O41" s="6">
         <v>4695.8937716666669</v>
       </c>
       <c r="P41" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q41" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R41" s="4">
-        <v>3.9399999999999998E-4</v>
+      <c r="Q41" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R41" s="7">
+        <v>5.926666666666668E-4</v>
       </c>
       <c r="S41" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="8" t="s">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E42" s="2">
         <v>1901.5157334444443</v>
@@ -3468,37 +3471,37 @@
       <c r="H42" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I42" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I42" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J42" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K42" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L42" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M42" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N42" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O42" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P42" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q42" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R42" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S42" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S42" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3507,7 +3510,7 @@
         <v>16</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>23</v>
@@ -3566,13 +3569,13 @@
         <v>16</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E44" s="2">
         <v>1901.5157334444443</v>
@@ -3587,22 +3590,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I44" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J44" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K44" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L44" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M44" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N44" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O44" s="3">
         <v>4661.9885795555556</v>
@@ -3611,10 +3614,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q44" s="2">
-        <v>-1.0069492222222223</v>
+        <v>-0.95070599999999983</v>
       </c>
       <c r="R44" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S44" s="8" t="s">
         <v>23</v>
@@ -3625,132 +3628,117 @@
         <v>16</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="2">
-        <f>AVERAGE(D36:D44)</f>
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G45" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H45" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I45" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J45" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K45" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L45" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M45" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N45" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O45" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P45" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R45" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S45" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="2">
+        <f>AVERAGE(D37:D45)</f>
         <v>1176.9484893703707</v>
       </c>
-      <c r="E45" s="2">
-        <f t="shared" ref="E45:R46" si="0">AVERAGE(E36:E44)</f>
+      <c r="E46" s="2">
+        <f t="shared" ref="E46:R47" si="0">AVERAGE(E37:E45)</f>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F46" s="2">
         <f t="shared" si="0"/>
         <v>0.99402413580246907</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G46" s="5">
         <f t="shared" si="0"/>
         <v>308.82293032098761</v>
-      </c>
-      <c r="H45" s="2">
-        <f t="shared" si="0"/>
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I45" s="5">
-        <f t="shared" si="0"/>
-        <v>7.1295036805555574</v>
-      </c>
-      <c r="J45" s="2">
-        <f t="shared" si="0"/>
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K45" s="5">
-        <f t="shared" si="0"/>
-        <v>705.82954383950619</v>
-      </c>
-      <c r="L45" s="2">
-        <f t="shared" si="0"/>
-        <v>83.470620444444435</v>
-      </c>
-      <c r="M45" s="5">
-        <f t="shared" si="0"/>
-        <v>1432.1165123580245</v>
-      </c>
-      <c r="N45" s="2">
-        <f t="shared" si="0"/>
-        <v>1179.5111099259257</v>
-      </c>
-      <c r="O45" s="6">
-        <f t="shared" si="0"/>
-        <v>4768.1626790370356</v>
-      </c>
-      <c r="P45" s="3">
-        <f t="shared" si="0"/>
-        <v>27227.338324888893</v>
-      </c>
-      <c r="Q45" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6790465308641975</v>
-      </c>
-      <c r="R45" s="7">
-        <f t="shared" si="0"/>
-        <v>1.3632839506172842E-3</v>
-      </c>
-      <c r="S45" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="2">
-        <f>AVERAGE(D37:D45)</f>
-        <v>1178.7030733497943</v>
-      </c>
-      <c r="E46" s="2">
-        <f t="shared" si="0"/>
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F46" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99203508916323713</v>
-      </c>
-      <c r="G46" s="2">
-        <f t="shared" si="0"/>
-        <v>306.71652987517137</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I46" s="5">
         <f t="shared" si="0"/>
-        <v>7.1295036805555565</v>
+        <v>7.1295036805555574</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K46" s="5">
         <f t="shared" si="0"/>
-        <v>698.76948392043903</v>
+        <v>705.82954383950619</v>
       </c>
       <c r="L46" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M46" s="5">
         <f t="shared" si="0"/>
-        <v>1437.5067307928668</v>
+        <v>1432.1165123580245</v>
       </c>
       <c r="N46" s="2">
         <f t="shared" si="0"/>
-        <v>1181.53627690535</v>
-      </c>
-      <c r="O46" s="3">
+        <v>1179.5111099259257</v>
+      </c>
+      <c r="O46" s="6">
         <f t="shared" si="0"/>
-        <v>4755.299898115225</v>
+        <v>4768.1626790370356</v>
       </c>
       <c r="P46" s="3">
         <f t="shared" si="0"/>
@@ -3758,71 +3746,86 @@
       </c>
       <c r="Q46" s="2">
         <f t="shared" si="0"/>
+        <v>4.6790465308641975</v>
+      </c>
+      <c r="R46" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3632839506172842E-3</v>
+      </c>
+      <c r="S46" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="2">
+        <f>AVERAGE(D38:D46)</f>
+        <v>1178.7030733497943</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" si="0"/>
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F47" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99203508916323713</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="0"/>
+        <v>306.71652987517137</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1295036805555565</v>
+      </c>
+      <c r="J47" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K47" s="2">
+        <f t="shared" si="0"/>
+        <v>698.76948392043903</v>
+      </c>
+      <c r="L47" s="2">
+        <f t="shared" si="0"/>
+        <v>83.470620444444435</v>
+      </c>
+      <c r="M47" s="2">
+        <f t="shared" si="0"/>
+        <v>1437.5067307928668</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" si="0"/>
+        <v>1181.53627690535</v>
+      </c>
+      <c r="O47" s="3">
+        <f t="shared" si="0"/>
+        <v>4755.299898115225</v>
+      </c>
+      <c r="P47" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324888893</v>
+      </c>
+      <c r="Q47" s="2">
+        <f t="shared" si="0"/>
         <v>4.684029058984911</v>
       </c>
-      <c r="R46" s="4">
+      <c r="R47" s="4">
         <f t="shared" si="0"/>
         <v>1.363093278463649E-3</v>
       </c>
-      <c r="S46" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1186.9773491111109</v>
-      </c>
-      <c r="E47" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F47" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G47" s="2">
-        <v>280.33542888888883</v>
-      </c>
-      <c r="H47" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I47" s="2">
-        <v>5.3870271111111121</v>
-      </c>
-      <c r="J47" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K47" s="2">
-        <v>645.93808322222219</v>
-      </c>
-      <c r="L47" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M47" s="2">
-        <v>1455.5792641111111</v>
-      </c>
-      <c r="N47" s="2">
-        <v>1191.1918266666667</v>
-      </c>
-      <c r="O47" s="3">
-        <v>4661.9885253333332</v>
-      </c>
-      <c r="P47" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q47" s="2">
-        <v>-0.64567288888888896</v>
-      </c>
-      <c r="R47" s="4">
-        <v>-2.0755555555555555E-4</v>
-      </c>
       <c r="S47" s="8" t="s">
         <v>23</v>
       </c>
@@ -3832,13 +3835,13 @@
         <v>16</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D48" s="2">
-        <v>1186.9773355555556</v>
+        <v>1186.9773491111109</v>
       </c>
       <c r="E48" s="2">
         <v>1901.5157334444443</v>
@@ -3859,16 +3862,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K48" s="2">
-        <v>645.93833411111109</v>
+        <v>645.93808322222219</v>
       </c>
       <c r="L48" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M48" s="2">
-        <v>1455.5790065555557</v>
+        <v>1455.5792641111111</v>
       </c>
       <c r="N48" s="2">
-        <v>1191.1918131111113</v>
+        <v>1191.1918266666667</v>
       </c>
       <c r="O48" s="3">
         <v>4661.9885253333332</v>
@@ -3877,10 +3880,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q48" s="2">
-        <v>-0.64567966666666665</v>
+        <v>-0.64567288888888896</v>
       </c>
       <c r="R48" s="4">
-        <v>-2.0744444444444445E-4</v>
+        <v>-2.0755555555555555E-4</v>
       </c>
       <c r="S48" s="8" t="s">
         <v>23</v>
@@ -3891,7 +3894,7 @@
         <v>16</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>23</v>
@@ -3918,13 +3921,13 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K49" s="2">
-        <v>645.9383002222221</v>
+        <v>645.93833411111109</v>
       </c>
       <c r="L49" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M49" s="2">
-        <v>1455.5790607777778</v>
+        <v>1455.5790065555557</v>
       </c>
       <c r="N49" s="2">
         <v>1191.1918131111113</v>
@@ -3936,7 +3939,7 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q49" s="2">
-        <v>-0.64565933333333325</v>
+        <v>-0.64567966666666665</v>
       </c>
       <c r="R49" s="4">
         <v>-2.0744444444444445E-4</v>
@@ -3950,13 +3953,13 @@
         <v>16</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D50" s="2">
-        <v>1187.0067003333331</v>
+        <v>1186.9773355555556</v>
       </c>
       <c r="E50" s="2">
         <v>1901.5157334444443</v>
@@ -3977,16 +3980,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K50" s="2">
-        <v>645.93713388888887</v>
+        <v>645.9383002222221</v>
       </c>
       <c r="L50" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M50" s="2">
-        <v>1455.6553682222225</v>
+        <v>1455.5790607777778</v>
       </c>
       <c r="N50" s="2">
-        <v>1191.1764458888888</v>
+        <v>1191.1918131111113</v>
       </c>
       <c r="O50" s="3">
         <v>4661.9885253333332</v>
@@ -3995,27 +3998,27 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q50" s="2">
-        <v>-0.61525011111111105</v>
+        <v>-0.64565933333333325</v>
       </c>
       <c r="R50" s="4">
-        <v>-1.7433333333333333E-4</v>
+        <v>-2.0744444444444445E-4</v>
       </c>
       <c r="S50" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>16</v>
-      </c>
-      <c r="B51" t="s">
-        <v>65</v>
+      <c r="A51" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D51" s="2">
-        <v>1187.0063613333334</v>
+        <v>1187.0067003333331</v>
       </c>
       <c r="E51" s="2">
         <v>1901.5157334444443</v>
@@ -4030,36 +4033,95 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I51" s="2">
-        <v>5.3870315555555557</v>
+        <v>5.3870271111111121</v>
       </c>
       <c r="J51" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K51" s="2">
-        <v>645.93916833333344</v>
+        <v>645.93713388888887</v>
       </c>
       <c r="L51" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M51" s="2">
-        <v>1455.7051053333334</v>
+        <v>1455.6553682222225</v>
       </c>
       <c r="N51" s="2">
-        <v>1191.1759305555559</v>
+        <v>1191.1764458888888</v>
       </c>
       <c r="O51" s="3">
-        <v>4661.988498222222</v>
+        <v>4661.9885253333332</v>
       </c>
       <c r="P51" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q51" s="2">
+        <v>-0.61525011111111105</v>
+      </c>
+      <c r="R51" s="4">
+        <v>-1.7433333333333333E-4</v>
+      </c>
+      <c r="S51" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1187.0063613333334</v>
+      </c>
+      <c r="E52" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G52" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H52" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I52" s="2">
+        <v>5.3870315555555557</v>
+      </c>
+      <c r="J52" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K52" s="2">
+        <v>645.93916833333344</v>
+      </c>
+      <c r="L52" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M52" s="2">
+        <v>1455.7051053333334</v>
+      </c>
+      <c r="N52" s="2">
+        <v>1191.1759305555559</v>
+      </c>
+      <c r="O52" s="3">
+        <v>4661.988498222222</v>
+      </c>
+      <c r="P52" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q52" s="2">
         <v>-0.56365988888888896</v>
       </c>
-      <c r="R51" s="4">
+      <c r="R52" s="4">
         <v>-1.5888888888888889E-4</v>
       </c>
-      <c r="S51" s="8" t="s">
+      <c r="S52" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CW3MdigitalHandbook.docx - Add notes about release 0.4.2.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C414CD1-B808-4FB0-8D2D-2E5452F97AEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4EB2AC-3E4E-42BD-811E-EB2EDC55FCD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="68">
   <si>
     <t>Year</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Baseline 2010_C155+</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18_C156</t>
   </si>
 </sst>
 </file>
@@ -1097,11 +1100,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U52"/>
+  <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="S54" sqref="S54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4125,6 +4128,65 @@
         <v>23</v>
       </c>
     </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="5">
+        <v>1208.5438095555555</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G53" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H53" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I53" s="2">
+        <v>5.3172314444444444</v>
+      </c>
+      <c r="J53" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K53" s="2">
+        <v>645.97183577777787</v>
+      </c>
+      <c r="L53" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M53" s="5">
+        <v>1460.2614338888889</v>
+      </c>
+      <c r="N53" s="5">
+        <v>1208.0519340000001</v>
+      </c>
+      <c r="O53" s="3">
+        <v>4662.6060926666669</v>
+      </c>
+      <c r="P53" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q53" s="2">
+        <v>-0.5663084444444445</v>
+      </c>
+      <c r="R53" s="4">
+        <v>-1.5933333333333332E-4</v>
+      </c>
+      <c r="S53" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
CW3MdigitalHandbook.docx - Add details on calculation of flow rates and water temperatures. Flow.cpp - Add logic to default temperature of water running off from the land into the reach to DEFAULT_SOIL_H2O_TEMP_DEGC when W2A_SLP and W2A_INT are both zero or are not present in the HBV CSV file. ReachRouting.cpp - Add some comments.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4EB2AC-3E4E-42BD-811E-EB2EDC55FCD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB4034A-B3D0-406B-B1A9-2E5029959EF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34410" yWindow="-4155" windowWidth="22395" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="70">
   <si>
     <t>Year</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>Baseline 2010-18_C156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline 2010 </t>
+  </si>
+  <si>
+    <t>CW3M 0.4.2</t>
   </si>
 </sst>
 </file>
@@ -1100,11 +1106,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U53"/>
+  <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S54" sqref="S54"/>
+      <selection pane="bottomLeft" activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2918,85 +2924,87 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="4"/>
+      <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32">
+        <v>2010</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1136.616577</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1.2021059999999999</v>
+      </c>
+      <c r="G32" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H32" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I32" s="2">
+        <v>4.5522390000000001</v>
+      </c>
+      <c r="J32" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K32" s="2">
+        <v>677.62432899999999</v>
+      </c>
+      <c r="L32" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M32" s="2">
+        <v>1397.4351810000001</v>
+      </c>
+      <c r="N32" s="2">
+        <v>1247.803345</v>
+      </c>
+      <c r="O32" s="3">
+        <v>6725.3081050000001</v>
+      </c>
+      <c r="P32" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>1.318765</v>
+      </c>
+      <c r="R32" s="4">
+        <v>3.8499999999999998E-4</v>
+      </c>
+      <c r="S32">
+        <v>2010</v>
+      </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E33" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G33" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H33" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K33" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L33" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M33" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N33" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O33" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P33" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q33" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R33" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S33" t="s">
-        <v>23</v>
-      </c>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="4"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
@@ -3036,7 +3044,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P34" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q34" s="2">
         <v>-4.72741111111111E-2</v>
@@ -3053,7 +3061,7 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
@@ -3101,19 +3109,22 @@
       <c r="R35" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S35" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E36" s="2">
         <v>1901.5157334444443</v>
@@ -3132,31 +3143,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K36" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L36" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M36" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N36" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O36" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P36" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q36" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R36" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S36" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
@@ -3164,13 +3172,13 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
         <v>23</v>
       </c>
       <c r="D37" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E37" s="2">
         <v>1901.5157334444443</v>
@@ -3189,28 +3197,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K37" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L37" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M37" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N37" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O37" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P37" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q37" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R37" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S37" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
@@ -3218,13 +3229,13 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E38" s="2">
         <v>1901.5157334444443</v>
@@ -3233,28 +3244,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G38" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H38" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I38" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I38" s="2"/>
       <c r="J38" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K38" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L38" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M38" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N38" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O38" s="3">
         <v>4883.9277073333324</v>
@@ -3263,13 +3272,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q38" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R38" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S38" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
@@ -3277,13 +3283,13 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C39" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E39" s="2">
         <v>1901.5157334444443</v>
@@ -3292,28 +3298,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G39" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H39" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I39" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J39" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K39" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L39" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M39" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N39" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O39" s="3">
         <v>4883.9277073333324</v>
@@ -3322,10 +3328,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q39" s="2">
-        <v>9.9787694444444455</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R39" s="4">
-        <v>2.9230000000000003E-3</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S39" t="s">
         <v>23</v>
@@ -3336,7 +3342,7 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
         <v>23</v>
@@ -3351,7 +3357,7 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G40" s="2">
-        <v>347.23312744444445</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H40" s="2">
         <v>9.775355222222224</v>
@@ -3381,10 +3387,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q40" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R40" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S40" t="s">
         <v>23</v>
@@ -3395,55 +3401,55 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E41" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F41" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G41" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G41" s="2">
+        <v>347.23312744444445</v>
       </c>
       <c r="H41" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I41" s="5">
-        <v>13.853347222222222</v>
+      <c r="I41" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J41" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K41" s="5">
-        <v>691.23065866666673</v>
+      <c r="K41" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L41" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M41" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N41" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O41" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M41" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N41" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O41" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P41" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q41" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R41" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q41" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R41" s="4">
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S41" t="s">
         <v>23</v>
@@ -3454,13 +3460,13 @@
         <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="2">
-        <v>1186.9521077777779</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E42" s="2">
         <v>1901.5157334444443</v>
@@ -3468,58 +3474,58 @@
       <c r="F42" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G42" s="2">
-        <v>280.33542888888883</v>
+      <c r="G42" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H42" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I42" s="5">
-        <v>12.968491888888888</v>
+        <v>13.853347222222222</v>
       </c>
       <c r="J42" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K42" s="2">
-        <v>645.94098588888892</v>
+      <c r="K42" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L42" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M42" s="2">
-        <v>1465.1962754444444</v>
-      </c>
-      <c r="N42" s="2">
-        <v>1191.1222331111112</v>
-      </c>
-      <c r="O42" s="3">
+      <c r="M42" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N42" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O42" s="6">
         <v>4695.8937716666669</v>
       </c>
       <c r="P42" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q42" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R42" s="4">
-        <v>3.9399999999999998E-4</v>
+      <c r="Q42" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R42" s="7">
+        <v>5.926666666666668E-4</v>
       </c>
       <c r="S42" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="8" t="s">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
         <v>23</v>
       </c>
       <c r="D43" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E43" s="2">
         <v>1901.5157334444443</v>
@@ -3533,37 +3539,37 @@
       <c r="H43" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I43" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I43" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J43" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K43" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L43" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M43" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N43" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O43" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P43" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q43" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R43" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S43" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S43" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3572,7 +3578,7 @@
         <v>16</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>23</v>
@@ -3631,13 +3637,13 @@
         <v>16</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E45" s="2">
         <v>1901.5157334444443</v>
@@ -3652,22 +3658,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I45" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J45" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K45" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L45" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M45" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N45" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O45" s="3">
         <v>4661.9885795555556</v>
@@ -3676,10 +3682,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q45" s="2">
-        <v>-1.0069492222222223</v>
+        <v>-0.95070599999999983</v>
       </c>
       <c r="R45" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S45" s="8" t="s">
         <v>23</v>
@@ -3690,132 +3696,117 @@
         <v>16</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="2">
-        <f>AVERAGE(D37:D45)</f>
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G46" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H46" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I46" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J46" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K46" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L46" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M46" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N46" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O46" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P46" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q46" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R46" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S46" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="2">
+        <f>AVERAGE(D38:D46)</f>
         <v>1176.9484893703707</v>
       </c>
-      <c r="E46" s="2">
-        <f t="shared" ref="E46:R47" si="0">AVERAGE(E37:E45)</f>
+      <c r="E47" s="2">
+        <f t="shared" ref="E47:R48" si="0">AVERAGE(E38:E46)</f>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F47" s="2">
         <f t="shared" si="0"/>
         <v>0.99402413580246907</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G47" s="5">
         <f t="shared" si="0"/>
         <v>308.82293032098761</v>
-      </c>
-      <c r="H46" s="2">
-        <f t="shared" si="0"/>
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I46" s="5">
-        <f t="shared" si="0"/>
-        <v>7.1295036805555574</v>
-      </c>
-      <c r="J46" s="2">
-        <f t="shared" si="0"/>
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K46" s="5">
-        <f t="shared" si="0"/>
-        <v>705.82954383950619</v>
-      </c>
-      <c r="L46" s="2">
-        <f t="shared" si="0"/>
-        <v>83.470620444444435</v>
-      </c>
-      <c r="M46" s="5">
-        <f t="shared" si="0"/>
-        <v>1432.1165123580245</v>
-      </c>
-      <c r="N46" s="2">
-        <f t="shared" si="0"/>
-        <v>1179.5111099259257</v>
-      </c>
-      <c r="O46" s="6">
-        <f t="shared" si="0"/>
-        <v>4768.1626790370356</v>
-      </c>
-      <c r="P46" s="3">
-        <f t="shared" si="0"/>
-        <v>27227.338324888893</v>
-      </c>
-      <c r="Q46" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6790465308641975</v>
-      </c>
-      <c r="R46" s="7">
-        <f t="shared" si="0"/>
-        <v>1.3632839506172842E-3</v>
-      </c>
-      <c r="S46" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="2">
-        <f>AVERAGE(D38:D46)</f>
-        <v>1178.7030733497943</v>
-      </c>
-      <c r="E47" s="2">
-        <f t="shared" si="0"/>
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F47" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99203508916323713</v>
-      </c>
-      <c r="G47" s="2">
-        <f t="shared" si="0"/>
-        <v>306.71652987517137</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I47" s="2">
+      <c r="I47" s="5">
         <f t="shared" si="0"/>
-        <v>7.1295036805555565</v>
+        <v>7.1295036805555574</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K47" s="5">
         <f t="shared" si="0"/>
-        <v>698.76948392043903</v>
+        <v>705.82954383950619</v>
       </c>
       <c r="L47" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M47" s="2">
+      <c r="M47" s="5">
         <f t="shared" si="0"/>
-        <v>1437.5067307928668</v>
+        <v>1432.1165123580245</v>
       </c>
       <c r="N47" s="2">
         <f t="shared" si="0"/>
-        <v>1181.53627690535</v>
-      </c>
-      <c r="O47" s="3">
+        <v>1179.5111099259257</v>
+      </c>
+      <c r="O47" s="6">
         <f t="shared" si="0"/>
-        <v>4755.299898115225</v>
+        <v>4768.1626790370356</v>
       </c>
       <c r="P47" s="3">
         <f t="shared" si="0"/>
@@ -3823,71 +3814,86 @@
       </c>
       <c r="Q47" s="2">
         <f t="shared" si="0"/>
+        <v>4.6790465308641975</v>
+      </c>
+      <c r="R47" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3632839506172842E-3</v>
+      </c>
+      <c r="S47" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="2">
+        <f>AVERAGE(D39:D47)</f>
+        <v>1178.7030733497943</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="0"/>
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F48" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99203508916323713</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="0"/>
+        <v>306.71652987517137</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1295036805555565</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K48" s="2">
+        <f t="shared" si="0"/>
+        <v>698.76948392043903</v>
+      </c>
+      <c r="L48" s="2">
+        <f t="shared" si="0"/>
+        <v>83.470620444444435</v>
+      </c>
+      <c r="M48" s="2">
+        <f t="shared" si="0"/>
+        <v>1437.5067307928668</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="0"/>
+        <v>1181.53627690535</v>
+      </c>
+      <c r="O48" s="3">
+        <f t="shared" si="0"/>
+        <v>4755.299898115225</v>
+      </c>
+      <c r="P48" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324888893</v>
+      </c>
+      <c r="Q48" s="2">
+        <f t="shared" si="0"/>
         <v>4.684029058984911</v>
       </c>
-      <c r="R47" s="4">
+      <c r="R48" s="4">
         <f t="shared" si="0"/>
         <v>1.363093278463649E-3</v>
       </c>
-      <c r="S47" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1186.9773491111109</v>
-      </c>
-      <c r="E48" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F48" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G48" s="2">
-        <v>280.33542888888883</v>
-      </c>
-      <c r="H48" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I48" s="2">
-        <v>5.3870271111111121</v>
-      </c>
-      <c r="J48" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K48" s="2">
-        <v>645.93808322222219</v>
-      </c>
-      <c r="L48" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M48" s="2">
-        <v>1455.5792641111111</v>
-      </c>
-      <c r="N48" s="2">
-        <v>1191.1918266666667</v>
-      </c>
-      <c r="O48" s="3">
-        <v>4661.9885253333332</v>
-      </c>
-      <c r="P48" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q48" s="2">
-        <v>-0.64567288888888896</v>
-      </c>
-      <c r="R48" s="4">
-        <v>-2.0755555555555555E-4</v>
-      </c>
       <c r="S48" s="8" t="s">
         <v>23</v>
       </c>
@@ -3897,13 +3903,13 @@
         <v>16</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D49" s="2">
-        <v>1186.9773355555556</v>
+        <v>1186.9773491111109</v>
       </c>
       <c r="E49" s="2">
         <v>1901.5157334444443</v>
@@ -3924,16 +3930,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K49" s="2">
-        <v>645.93833411111109</v>
+        <v>645.93808322222219</v>
       </c>
       <c r="L49" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M49" s="2">
-        <v>1455.5790065555557</v>
+        <v>1455.5792641111111</v>
       </c>
       <c r="N49" s="2">
-        <v>1191.1918131111113</v>
+        <v>1191.1918266666667</v>
       </c>
       <c r="O49" s="3">
         <v>4661.9885253333332</v>
@@ -3942,10 +3948,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q49" s="2">
-        <v>-0.64567966666666665</v>
+        <v>-0.64567288888888896</v>
       </c>
       <c r="R49" s="4">
-        <v>-2.0744444444444445E-4</v>
+        <v>-2.0755555555555555E-4</v>
       </c>
       <c r="S49" s="8" t="s">
         <v>23</v>
@@ -3956,7 +3962,7 @@
         <v>16</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>23</v>
@@ -3983,13 +3989,13 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K50" s="2">
-        <v>645.9383002222221</v>
+        <v>645.93833411111109</v>
       </c>
       <c r="L50" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M50" s="2">
-        <v>1455.5790607777778</v>
+        <v>1455.5790065555557</v>
       </c>
       <c r="N50" s="2">
         <v>1191.1918131111113</v>
@@ -4001,7 +4007,7 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q50" s="2">
-        <v>-0.64565933333333325</v>
+        <v>-0.64567966666666665</v>
       </c>
       <c r="R50" s="4">
         <v>-2.0744444444444445E-4</v>
@@ -4015,13 +4021,13 @@
         <v>16</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D51" s="2">
-        <v>1187.0067003333331</v>
+        <v>1186.9773355555556</v>
       </c>
       <c r="E51" s="2">
         <v>1901.5157334444443</v>
@@ -4042,16 +4048,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K51" s="2">
-        <v>645.93713388888887</v>
+        <v>645.9383002222221</v>
       </c>
       <c r="L51" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M51" s="2">
-        <v>1455.6553682222225</v>
+        <v>1455.5790607777778</v>
       </c>
       <c r="N51" s="2">
-        <v>1191.1764458888888</v>
+        <v>1191.1918131111113</v>
       </c>
       <c r="O51" s="3">
         <v>4661.9885253333332</v>
@@ -4060,27 +4066,27 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q51" s="2">
-        <v>-0.61525011111111105</v>
+        <v>-0.64565933333333325</v>
       </c>
       <c r="R51" s="4">
-        <v>-1.7433333333333333E-4</v>
+        <v>-2.0744444444444445E-4</v>
       </c>
       <c r="S51" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52" t="s">
-        <v>65</v>
+      <c r="A52" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D52" s="2">
-        <v>1187.0063613333334</v>
+        <v>1187.0067003333331</v>
       </c>
       <c r="E52" s="2">
         <v>1901.5157334444443</v>
@@ -4095,34 +4101,34 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I52" s="2">
-        <v>5.3870315555555557</v>
+        <v>5.3870271111111121</v>
       </c>
       <c r="J52" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K52" s="2">
-        <v>645.93916833333344</v>
+        <v>645.93713388888887</v>
       </c>
       <c r="L52" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M52" s="2">
-        <v>1455.7051053333334</v>
+        <v>1455.6553682222225</v>
       </c>
       <c r="N52" s="2">
-        <v>1191.1759305555559</v>
+        <v>1191.1764458888888</v>
       </c>
       <c r="O52" s="3">
-        <v>4661.988498222222</v>
+        <v>4661.9885253333332</v>
       </c>
       <c r="P52" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q52" s="2">
-        <v>-0.56365988888888896</v>
+        <v>-0.61525011111111105</v>
       </c>
       <c r="R52" s="4">
-        <v>-1.5888888888888889E-4</v>
+        <v>-1.7433333333333333E-4</v>
       </c>
       <c r="S52" s="8" t="s">
         <v>23</v>
@@ -4133,13 +4139,13 @@
         <v>16</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D53" s="5">
-        <v>1208.5438095555555</v>
+      <c r="D53" s="2">
+        <v>1187.0063613333334</v>
       </c>
       <c r="E53" s="2">
         <v>1901.5157334444443</v>
@@ -4154,36 +4160,95 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I53" s="2">
-        <v>5.3172314444444444</v>
+        <v>5.3870315555555557</v>
       </c>
       <c r="J53" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K53" s="2">
-        <v>645.97183577777787</v>
+        <v>645.93916833333344</v>
       </c>
       <c r="L53" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M53" s="5">
-        <v>1460.2614338888889</v>
-      </c>
-      <c r="N53" s="5">
-        <v>1208.0519340000001</v>
+      <c r="M53" s="2">
+        <v>1455.7051053333334</v>
+      </c>
+      <c r="N53" s="2">
+        <v>1191.1759305555559</v>
       </c>
       <c r="O53" s="3">
-        <v>4662.6060926666669</v>
+        <v>4661.988498222222</v>
       </c>
       <c r="P53" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q53" s="2">
+        <v>-0.56365988888888896</v>
+      </c>
+      <c r="R53" s="4">
+        <v>-1.5888888888888889E-4</v>
+      </c>
+      <c r="S53" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="5">
+        <v>1208.5438095555555</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G54" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H54" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I54" s="2">
+        <v>5.3172314444444444</v>
+      </c>
+      <c r="J54" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K54" s="2">
+        <v>645.97183577777787</v>
+      </c>
+      <c r="L54" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M54" s="5">
+        <v>1460.2614338888889</v>
+      </c>
+      <c r="N54" s="5">
+        <v>1208.0519340000001</v>
+      </c>
+      <c r="O54" s="3">
+        <v>4662.6060926666669</v>
+      </c>
+      <c r="P54" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q54" s="2">
         <v>-0.5663084444444445</v>
       </c>
-      <c r="R53" s="4">
+      <c r="R54" s="4">
         <v>-1.5933333333333332E-4</v>
       </c>
-      <c r="S53" s="8" t="s">
+      <c r="S54" s="8" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Start to bring up the NSantiam simulation again. CW3M_NSantiam.envx - Instead of using the generic Reporter.xml, use NSantiam/Reporter_NSantiam.xml. McKenzie/flow2010.ic - Replace the old 2010 IC file with one made by Baseline_2000-09_C165_newWeather. The new 2000-09 weather is 0.6 deg C warmer and about 10% drier. Flow_McKenzie.xml - Add TMAX and TMIN to the McKenzie basin weather reports. Flow_NSantiam.xml - Remove the IC file specification. Reach_NSantiam.dbf - Add new attributes related to the stream temperature submodel. Reporter_NSantiam.xml - Add this new file to the repository. CW3M.sln - Set the MCfire submodel as not included in the CW3M build.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB4034A-B3D0-406B-B1A9-2E5029959EF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9155B3-C773-4C7B-AFBB-F0DCC6ACA890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34410" yWindow="-4155" windowWidth="22395" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
+    <sheet name="2000-09" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="74">
   <si>
     <t>Year</t>
   </si>
@@ -240,6 +241,18 @@
   </si>
   <si>
     <t>CW3M 0.4.2</t>
+  </si>
+  <si>
+    <t>2000-09</t>
+  </si>
+  <si>
+    <t>Baseline_2000-09_C81</t>
+  </si>
+  <si>
+    <t>Baseline_2000-09_newWeather</t>
+  </si>
+  <si>
+    <t>CW3M C165</t>
   </si>
 </sst>
 </file>
@@ -738,7 +751,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -751,6 +764,15 @@
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1108,9 +1130,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S33" sqref="S33"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4256,4 +4278,248 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD88AF4-3325-45AB-9D19-94573DCD22C4}">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1092.1001221000001</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1790.8143431000001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.0697084000000001</v>
+      </c>
+      <c r="G2" s="2">
+        <v>327.85034159999998</v>
+      </c>
+      <c r="H2" s="2">
+        <v>9.3183378000000001</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2">
+        <v>7.7646284999999988</v>
+      </c>
+      <c r="K2" s="2">
+        <v>741.50434550000011</v>
+      </c>
+      <c r="L2" s="2">
+        <v>85.286103100000005</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1294.5123962</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1097.7140259</v>
+      </c>
+      <c r="O2" s="3">
+        <v>5839.5391357999997</v>
+      </c>
+      <c r="P2" s="3">
+        <v>25979.647461100001</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>5.6286456000000005</v>
+      </c>
+      <c r="R2" s="4">
+        <v>1.7227000000000002E-3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="2">
+        <v>641.53857870000013</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1609.2949586000002</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.0377343999999999</v>
+      </c>
+      <c r="G3" s="2">
+        <v>280.39512939999997</v>
+      </c>
+      <c r="H3" s="2">
+        <v>9.3183378000000001</v>
+      </c>
+      <c r="I3" s="2">
+        <v>11.447250100000002</v>
+      </c>
+      <c r="J3" s="2">
+        <v>7.7646284999999988</v>
+      </c>
+      <c r="K3" s="2">
+        <v>634.34777839999992</v>
+      </c>
+      <c r="L3" s="2">
+        <v>61.771183299999997</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1148.1819335</v>
+      </c>
+      <c r="N3" s="2">
+        <v>700.97914120000007</v>
+      </c>
+      <c r="O3" s="3">
+        <v>6439.1138917000007</v>
+      </c>
+      <c r="P3" s="3">
+        <v>25979.647461100001</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>1.2676099999999945E-2</v>
+      </c>
+      <c r="R3" s="4">
+        <v>-3.8799999999999994E-5</v>
+      </c>
+      <c r="S3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Flow.cpp, .h - Reduce Manning N default from 0.3 s/m^(1/3) (= 0.446 s/ft^(1/3))) to 0.04 s/m^(1/3) (= 0.059 s/ft^(1/3)).
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9155B3-C773-4C7B-AFBB-F0DCC6ACA890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD86BD4F-2D6F-4062-A117-300E715C89CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="76">
   <si>
     <t>Year</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>CW3M C165</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18_C167 with m_n = 0.15</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18_C167 with m_n = 0.04</t>
   </si>
 </sst>
 </file>
@@ -1128,11 +1134,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U54"/>
+  <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4274,6 +4280,118 @@
         <v>23</v>
       </c>
     </row>
+    <row r="55" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1207.0222438888889</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G55" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H55" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I55" s="2">
+        <v>5.3316344444444441</v>
+      </c>
+      <c r="J55" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K55" s="2">
+        <v>645.95907266666666</v>
+      </c>
+      <c r="L55" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M55" s="2">
+        <v>1460.4185112222222</v>
+      </c>
+      <c r="N55" s="2">
+        <v>1206.2352837777776</v>
+      </c>
+      <c r="O55" s="3">
+        <v>4662.5755209999998</v>
+      </c>
+      <c r="P55" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q55" s="2">
+        <v>-0.73148200000000008</v>
+      </c>
+      <c r="R55" s="4">
+        <v>-2.0655555555555556E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1206.5233695555557</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G56" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H56" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I56" s="2">
+        <v>5.3531247777777775</v>
+      </c>
+      <c r="J56" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K56" s="2">
+        <v>645.94818811111122</v>
+      </c>
+      <c r="L56" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M56" s="2">
+        <v>1460.5092637777777</v>
+      </c>
+      <c r="N56" s="2">
+        <v>1205.5020886666666</v>
+      </c>
+      <c r="O56" s="3">
+        <v>4662.5708008888896</v>
+      </c>
+      <c r="P56" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q56" s="2">
+        <v>-0.90742522222222222</v>
+      </c>
+      <c r="R56" s="4">
+        <v>-2.5755555555555558E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -4284,7 +4402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD88AF4-3325-45AB-9D19-94573DCD22C4}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CW3MdataDictionary.xlsx and Reach_McKenzie.dbf - Add Reach attribute DIRECTION, and redefine BANK_L_IDU and BANK_R_IDU as IDU indices instead of IDU IDs. Flow.cpp, .h - In AssignIDUsToStreamBanks(), populate the new Reach attribute DIRECTION. In GetSubreachShade_a_lator_W_m2(), use DIRECTION.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD86BD4F-2D6F-4062-A117-300E715C89CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E318AAEB-E441-4F04-A19F-080F6C6703A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="77">
   <si>
     <t>Year</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>Baseline 2010-18_C167 with m_n = 0.04</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C173</t>
   </si>
 </sst>
 </file>
@@ -1134,11 +1137,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U56"/>
+  <dimension ref="A1:U58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3011,85 +3014,75 @@
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="4"/>
+      <c r="D33" s="5">
+        <v>831.51080300000001</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1990.4676509999999</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1.2021059999999999</v>
+      </c>
+      <c r="G33" s="2">
+        <v>280.16485599999999</v>
+      </c>
+      <c r="H33" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I33" s="2">
+        <v>5.7589379999999997</v>
+      </c>
+      <c r="J33" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K33" s="2">
+        <v>677.34448199999997</v>
+      </c>
+      <c r="L33" s="2">
+        <v>93.229797000000005</v>
+      </c>
+      <c r="M33" s="5">
+        <v>1310.7667240000001</v>
+      </c>
+      <c r="N33" s="5">
+        <v>1029.4914550000001</v>
+      </c>
+      <c r="O33" s="3">
+        <v>6633.4262699999999</v>
+      </c>
+      <c r="P33" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>-4.2353000000000002E-2</v>
+      </c>
+      <c r="R33" s="4">
+        <v>-1.4E-5</v>
+      </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E34" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G34" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H34" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K34" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L34" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M34" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N34" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O34" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P34" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q34" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R34" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S34" t="s">
-        <v>23</v>
-      </c>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="4"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
@@ -3129,7 +3122,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P35" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q35" s="2">
         <v>-4.72741111111111E-2</v>
@@ -3146,7 +3139,7 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
@@ -3194,19 +3187,22 @@
       <c r="R36" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S36" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
         <v>23</v>
       </c>
       <c r="D37" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E37" s="2">
         <v>1901.5157334444443</v>
@@ -3225,31 +3221,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K37" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L37" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M37" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N37" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O37" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P37" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q37" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R37" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S37" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
@@ -3257,13 +3250,13 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E38" s="2">
         <v>1901.5157334444443</v>
@@ -3282,28 +3275,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K38" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L38" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M38" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N38" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O38" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P38" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q38" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R38" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S38" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
@@ -3311,13 +3307,13 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E39" s="2">
         <v>1901.5157334444443</v>
@@ -3326,28 +3322,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G39" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H39" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I39" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I39" s="2"/>
       <c r="J39" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K39" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L39" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M39" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N39" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O39" s="3">
         <v>4883.9277073333324</v>
@@ -3356,13 +3350,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q39" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R39" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S39" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
@@ -3370,13 +3361,13 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E40" s="2">
         <v>1901.5157334444443</v>
@@ -3385,28 +3376,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G40" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H40" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I40" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J40" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K40" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L40" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M40" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N40" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O40" s="3">
         <v>4883.9277073333324</v>
@@ -3415,10 +3406,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q40" s="2">
-        <v>9.9787694444444455</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R40" s="4">
-        <v>2.9230000000000003E-3</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S40" t="s">
         <v>23</v>
@@ -3429,7 +3420,7 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
@@ -3444,7 +3435,7 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G41" s="2">
-        <v>347.23312744444445</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H41" s="2">
         <v>9.775355222222224</v>
@@ -3474,10 +3465,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q41" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R41" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S41" t="s">
         <v>23</v>
@@ -3488,55 +3479,55 @@
         <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E42" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F42" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G42" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G42" s="2">
+        <v>347.23312744444445</v>
       </c>
       <c r="H42" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I42" s="5">
-        <v>13.853347222222222</v>
+      <c r="I42" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J42" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K42" s="5">
-        <v>691.23065866666673</v>
+      <c r="K42" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L42" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M42" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N42" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O42" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M42" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N42" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O42" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P42" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q42" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R42" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q42" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R42" s="4">
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S42" t="s">
         <v>23</v>
@@ -3547,13 +3538,13 @@
         <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
       </c>
       <c r="D43" s="2">
-        <v>1186.9521077777779</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E43" s="2">
         <v>1901.5157334444443</v>
@@ -3561,58 +3552,58 @@
       <c r="F43" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G43" s="2">
-        <v>280.33542888888883</v>
+      <c r="G43" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H43" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I43" s="5">
-        <v>12.968491888888888</v>
+        <v>13.853347222222222</v>
       </c>
       <c r="J43" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K43" s="2">
-        <v>645.94098588888892</v>
+      <c r="K43" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L43" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M43" s="2">
-        <v>1465.1962754444444</v>
-      </c>
-      <c r="N43" s="2">
-        <v>1191.1222331111112</v>
-      </c>
-      <c r="O43" s="3">
+      <c r="M43" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N43" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O43" s="6">
         <v>4695.8937716666669</v>
       </c>
       <c r="P43" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q43" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R43" s="4">
-        <v>3.9399999999999998E-4</v>
+      <c r="Q43" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R43" s="7">
+        <v>5.926666666666668E-4</v>
       </c>
       <c r="S43" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="8" t="s">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E44" s="2">
         <v>1901.5157334444443</v>
@@ -3626,37 +3617,37 @@
       <c r="H44" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I44" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I44" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J44" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K44" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L44" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M44" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N44" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O44" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P44" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q44" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R44" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S44" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S44" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3665,7 +3656,7 @@
         <v>16</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>23</v>
@@ -3724,13 +3715,13 @@
         <v>16</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E46" s="2">
         <v>1901.5157334444443</v>
@@ -3745,22 +3736,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I46" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J46" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K46" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L46" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M46" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N46" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O46" s="3">
         <v>4661.9885795555556</v>
@@ -3769,10 +3760,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q46" s="2">
-        <v>-1.0069492222222223</v>
+        <v>-0.95070599999999983</v>
       </c>
       <c r="R46" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S46" s="8" t="s">
         <v>23</v>
@@ -3783,132 +3774,117 @@
         <v>16</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="2">
-        <f>AVERAGE(D38:D46)</f>
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G47" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H47" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I47" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J47" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K47" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L47" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M47" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N47" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O47" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P47" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R47" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S47" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="2">
+        <f>AVERAGE(D39:D47)</f>
         <v>1176.9484893703707</v>
       </c>
-      <c r="E47" s="2">
-        <f t="shared" ref="E47:R48" si="0">AVERAGE(E38:E46)</f>
+      <c r="E48" s="2">
+        <f t="shared" ref="E48:R49" si="0">AVERAGE(E39:E47)</f>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F48" s="2">
         <f t="shared" si="0"/>
         <v>0.99402413580246907</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G48" s="5">
         <f t="shared" si="0"/>
         <v>308.82293032098761</v>
-      </c>
-      <c r="H47" s="2">
-        <f t="shared" si="0"/>
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I47" s="5">
-        <f t="shared" si="0"/>
-        <v>7.1295036805555574</v>
-      </c>
-      <c r="J47" s="2">
-        <f t="shared" si="0"/>
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K47" s="5">
-        <f t="shared" si="0"/>
-        <v>705.82954383950619</v>
-      </c>
-      <c r="L47" s="2">
-        <f t="shared" si="0"/>
-        <v>83.470620444444435</v>
-      </c>
-      <c r="M47" s="5">
-        <f t="shared" si="0"/>
-        <v>1432.1165123580245</v>
-      </c>
-      <c r="N47" s="2">
-        <f t="shared" si="0"/>
-        <v>1179.5111099259257</v>
-      </c>
-      <c r="O47" s="6">
-        <f t="shared" si="0"/>
-        <v>4768.1626790370356</v>
-      </c>
-      <c r="P47" s="3">
-        <f t="shared" si="0"/>
-        <v>27227.338324888893</v>
-      </c>
-      <c r="Q47" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6790465308641975</v>
-      </c>
-      <c r="R47" s="7">
-        <f t="shared" si="0"/>
-        <v>1.3632839506172842E-3</v>
-      </c>
-      <c r="S47" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="2">
-        <f>AVERAGE(D39:D47)</f>
-        <v>1178.7030733497943</v>
-      </c>
-      <c r="E48" s="2">
-        <f t="shared" si="0"/>
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F48" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99203508916323713</v>
-      </c>
-      <c r="G48" s="2">
-        <f t="shared" si="0"/>
-        <v>306.71652987517137</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I48" s="5">
         <f t="shared" si="0"/>
-        <v>7.1295036805555565</v>
+        <v>7.1295036805555574</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K48" s="2">
+      <c r="K48" s="5">
         <f t="shared" si="0"/>
-        <v>698.76948392043903</v>
+        <v>705.82954383950619</v>
       </c>
       <c r="L48" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M48" s="2">
+      <c r="M48" s="5">
         <f t="shared" si="0"/>
-        <v>1437.5067307928668</v>
+        <v>1432.1165123580245</v>
       </c>
       <c r="N48" s="2">
         <f t="shared" si="0"/>
-        <v>1181.53627690535</v>
-      </c>
-      <c r="O48" s="3">
+        <v>1179.5111099259257</v>
+      </c>
+      <c r="O48" s="6">
         <f t="shared" si="0"/>
-        <v>4755.299898115225</v>
+        <v>4768.1626790370356</v>
       </c>
       <c r="P48" s="3">
         <f t="shared" si="0"/>
@@ -3916,71 +3892,86 @@
       </c>
       <c r="Q48" s="2">
         <f t="shared" si="0"/>
+        <v>4.6790465308641975</v>
+      </c>
+      <c r="R48" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3632839506172842E-3</v>
+      </c>
+      <c r="S48" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="2">
+        <f>AVERAGE(D40:D48)</f>
+        <v>1178.7030733497943</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="0"/>
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F49" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99203508916323713</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="0"/>
+        <v>306.71652987517137</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1295036805555565</v>
+      </c>
+      <c r="J49" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K49" s="2">
+        <f t="shared" si="0"/>
+        <v>698.76948392043903</v>
+      </c>
+      <c r="L49" s="2">
+        <f t="shared" si="0"/>
+        <v>83.470620444444435</v>
+      </c>
+      <c r="M49" s="2">
+        <f t="shared" si="0"/>
+        <v>1437.5067307928668</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="0"/>
+        <v>1181.53627690535</v>
+      </c>
+      <c r="O49" s="3">
+        <f t="shared" si="0"/>
+        <v>4755.299898115225</v>
+      </c>
+      <c r="P49" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324888893</v>
+      </c>
+      <c r="Q49" s="2">
+        <f t="shared" si="0"/>
         <v>4.684029058984911</v>
       </c>
-      <c r="R48" s="4">
+      <c r="R49" s="4">
         <f t="shared" si="0"/>
         <v>1.363093278463649E-3</v>
       </c>
-      <c r="S48" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1186.9773491111109</v>
-      </c>
-      <c r="E49" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F49" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G49" s="2">
-        <v>280.33542888888883</v>
-      </c>
-      <c r="H49" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I49" s="2">
-        <v>5.3870271111111121</v>
-      </c>
-      <c r="J49" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K49" s="2">
-        <v>645.93808322222219</v>
-      </c>
-      <c r="L49" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M49" s="2">
-        <v>1455.5792641111111</v>
-      </c>
-      <c r="N49" s="2">
-        <v>1191.1918266666667</v>
-      </c>
-      <c r="O49" s="3">
-        <v>4661.9885253333332</v>
-      </c>
-      <c r="P49" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q49" s="2">
-        <v>-0.64567288888888896</v>
-      </c>
-      <c r="R49" s="4">
-        <v>-2.0755555555555555E-4</v>
-      </c>
       <c r="S49" s="8" t="s">
         <v>23</v>
       </c>
@@ -3990,13 +3981,13 @@
         <v>16</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D50" s="2">
-        <v>1186.9773355555556</v>
+        <v>1186.9773491111109</v>
       </c>
       <c r="E50" s="2">
         <v>1901.5157334444443</v>
@@ -4017,16 +4008,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K50" s="2">
-        <v>645.93833411111109</v>
+        <v>645.93808322222219</v>
       </c>
       <c r="L50" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M50" s="2">
-        <v>1455.5790065555557</v>
+        <v>1455.5792641111111</v>
       </c>
       <c r="N50" s="2">
-        <v>1191.1918131111113</v>
+        <v>1191.1918266666667</v>
       </c>
       <c r="O50" s="3">
         <v>4661.9885253333332</v>
@@ -4035,10 +4026,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q50" s="2">
-        <v>-0.64567966666666665</v>
+        <v>-0.64567288888888896</v>
       </c>
       <c r="R50" s="4">
-        <v>-2.0744444444444445E-4</v>
+        <v>-2.0755555555555555E-4</v>
       </c>
       <c r="S50" s="8" t="s">
         <v>23</v>
@@ -4049,7 +4040,7 @@
         <v>16</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>23</v>
@@ -4076,13 +4067,13 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K51" s="2">
-        <v>645.9383002222221</v>
+        <v>645.93833411111109</v>
       </c>
       <c r="L51" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M51" s="2">
-        <v>1455.5790607777778</v>
+        <v>1455.5790065555557</v>
       </c>
       <c r="N51" s="2">
         <v>1191.1918131111113</v>
@@ -4094,7 +4085,7 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q51" s="2">
-        <v>-0.64565933333333325</v>
+        <v>-0.64567966666666665</v>
       </c>
       <c r="R51" s="4">
         <v>-2.0744444444444445E-4</v>
@@ -4108,13 +4099,13 @@
         <v>16</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D52" s="2">
-        <v>1187.0067003333331</v>
+        <v>1186.9773355555556</v>
       </c>
       <c r="E52" s="2">
         <v>1901.5157334444443</v>
@@ -4135,16 +4126,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K52" s="2">
-        <v>645.93713388888887</v>
+        <v>645.9383002222221</v>
       </c>
       <c r="L52" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M52" s="2">
-        <v>1455.6553682222225</v>
+        <v>1455.5790607777778</v>
       </c>
       <c r="N52" s="2">
-        <v>1191.1764458888888</v>
+        <v>1191.1918131111113</v>
       </c>
       <c r="O52" s="3">
         <v>4661.9885253333332</v>
@@ -4153,27 +4144,27 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q52" s="2">
-        <v>-0.61525011111111105</v>
+        <v>-0.64565933333333325</v>
       </c>
       <c r="R52" s="4">
-        <v>-1.7433333333333333E-4</v>
+        <v>-2.0744444444444445E-4</v>
       </c>
       <c r="S52" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>16</v>
-      </c>
-      <c r="B53" t="s">
-        <v>65</v>
+      <c r="A53" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D53" s="2">
-        <v>1187.0063613333334</v>
+        <v>1187.0067003333331</v>
       </c>
       <c r="E53" s="2">
         <v>1901.5157334444443</v>
@@ -4188,34 +4179,34 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I53" s="2">
-        <v>5.3870315555555557</v>
+        <v>5.3870271111111121</v>
       </c>
       <c r="J53" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K53" s="2">
-        <v>645.93916833333344</v>
+        <v>645.93713388888887</v>
       </c>
       <c r="L53" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M53" s="2">
-        <v>1455.7051053333334</v>
+        <v>1455.6553682222225</v>
       </c>
       <c r="N53" s="2">
-        <v>1191.1759305555559</v>
+        <v>1191.1764458888888</v>
       </c>
       <c r="O53" s="3">
-        <v>4661.988498222222</v>
+        <v>4661.9885253333332</v>
       </c>
       <c r="P53" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q53" s="2">
-        <v>-0.56365988888888896</v>
+        <v>-0.61525011111111105</v>
       </c>
       <c r="R53" s="4">
-        <v>-1.5888888888888889E-4</v>
+        <v>-1.7433333333333333E-4</v>
       </c>
       <c r="S53" s="8" t="s">
         <v>23</v>
@@ -4226,13 +4217,13 @@
         <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D54" s="5">
-        <v>1208.5438095555555</v>
+      <c r="D54" s="2">
+        <v>1187.0063613333334</v>
       </c>
       <c r="E54" s="2">
         <v>1901.5157334444443</v>
@@ -4247,51 +4238,51 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I54" s="2">
-        <v>5.3172314444444444</v>
+        <v>5.3870315555555557</v>
       </c>
       <c r="J54" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K54" s="2">
-        <v>645.97183577777787</v>
+        <v>645.93916833333344</v>
       </c>
       <c r="L54" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M54" s="5">
-        <v>1460.2614338888889</v>
-      </c>
-      <c r="N54" s="5">
-        <v>1208.0519340000001</v>
+      <c r="M54" s="2">
+        <v>1455.7051053333334</v>
+      </c>
+      <c r="N54" s="2">
+        <v>1191.1759305555559</v>
       </c>
       <c r="O54" s="3">
-        <v>4662.6060926666669</v>
+        <v>4661.988498222222</v>
       </c>
       <c r="P54" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q54" s="2">
-        <v>-0.5663084444444445</v>
+        <v>-0.56365988888888896</v>
       </c>
       <c r="R54" s="4">
-        <v>-1.5933333333333332E-4</v>
+        <v>-1.5888888888888889E-4</v>
       </c>
       <c r="S54" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>16</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>74</v>
+      <c r="B55" t="s">
+        <v>67</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D55" s="2">
-        <v>1207.0222438888889</v>
+      <c r="D55" s="5">
+        <v>1208.5438095555555</v>
       </c>
       <c r="E55" s="2">
         <v>1901.5157334444443</v>
@@ -4306,34 +4297,37 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I55" s="2">
-        <v>5.3316344444444441</v>
+        <v>5.3172314444444444</v>
       </c>
       <c r="J55" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K55" s="2">
-        <v>645.95907266666666</v>
+        <v>645.97183577777787</v>
       </c>
       <c r="L55" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M55" s="2">
-        <v>1460.4185112222222</v>
-      </c>
-      <c r="N55" s="2">
-        <v>1206.2352837777776</v>
+      <c r="M55" s="5">
+        <v>1460.2614338888889</v>
+      </c>
+      <c r="N55" s="5">
+        <v>1208.0519340000001</v>
       </c>
       <c r="O55" s="3">
-        <v>4662.5755209999998</v>
+        <v>4662.6060926666669</v>
       </c>
       <c r="P55" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q55" s="2">
-        <v>-0.73148200000000008</v>
+        <v>-0.5663084444444445</v>
       </c>
       <c r="R55" s="4">
-        <v>-2.0655555555555556E-4</v>
+        <v>-1.5933333333333332E-4</v>
+      </c>
+      <c r="S55" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
@@ -4341,13 +4335,13 @@
         <v>16</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D56" s="2">
-        <v>1206.5233695555557</v>
+        <v>1207.0222438888889</v>
       </c>
       <c r="E56" s="2">
         <v>1901.5157334444443</v>
@@ -4362,34 +4356,149 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I56" s="2">
-        <v>5.3531247777777775</v>
+        <v>5.3316344444444441</v>
       </c>
       <c r="J56" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K56" s="2">
-        <v>645.94818811111122</v>
+        <v>645.95907266666666</v>
       </c>
       <c r="L56" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M56" s="2">
-        <v>1460.5092637777777</v>
+        <v>1460.4185112222222</v>
       </c>
       <c r="N56" s="2">
-        <v>1205.5020886666666</v>
+        <v>1206.2352837777776</v>
       </c>
       <c r="O56" s="3">
-        <v>4662.5708008888896</v>
+        <v>4662.5755209999998</v>
       </c>
       <c r="P56" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q56" s="2">
+        <v>-0.73148200000000008</v>
+      </c>
+      <c r="R56" s="4">
+        <v>-2.0655555555555556E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1206.5233695555557</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G57" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H57" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I57" s="2">
+        <v>5.3531247777777775</v>
+      </c>
+      <c r="J57" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K57" s="2">
+        <v>645.94818811111122</v>
+      </c>
+      <c r="L57" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M57" s="2">
+        <v>1460.5092637777777</v>
+      </c>
+      <c r="N57" s="2">
+        <v>1205.5020886666666</v>
+      </c>
+      <c r="O57" s="3">
+        <v>4662.5708008888896</v>
+      </c>
+      <c r="P57" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q57" s="2">
         <v>-0.90742522222222222</v>
       </c>
-      <c r="R56" s="4">
+      <c r="R57" s="4">
         <v>-2.5755555555555558E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1080.801350777778</v>
+      </c>
+      <c r="E58" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G58" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H58" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I58" s="2">
+        <v>5.7424886666666666</v>
+      </c>
+      <c r="J58" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K58" s="2">
+        <v>645.86557344444441</v>
+      </c>
+      <c r="L58" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M58" s="5">
+        <v>1430.3511555555554</v>
+      </c>
+      <c r="N58" s="2">
+        <v>1110.4303452222223</v>
+      </c>
+      <c r="O58" s="3">
+        <v>4638.5936415555561</v>
+      </c>
+      <c r="P58" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q58" s="2">
+        <v>-0.8872363333333334</v>
+      </c>
+      <c r="R58" s="4">
+        <v>-2.5788888888888888E-4</v>
+      </c>
+      <c r="S58" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reach_McKenzie.dbf - Store new version of DIRECTION, with values constrained to 0 <= DIRECTION < 360. Flow.cpp - Add ::Direction_deg(). In AssignIDUsToStreamBanks(), use the direction from the nominal midpoint of the reach to the IDU centroid to decide whether the IDU is on the left bank or on the right bank.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E318AAEB-E441-4F04-A19F-080F6C6703A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CDD1BA-93D5-457D-8FEE-9478C7767992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="78">
   <si>
     <t>Year</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>Baseline 2010-18 C173</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C174</t>
   </si>
 </sst>
 </file>
@@ -1137,11 +1140,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U58"/>
+  <dimension ref="A1:U59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58:XFD58"/>
+      <selection pane="bottomLeft" activeCell="S59" sqref="S59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4498,6 +4501,65 @@
         <v>-2.5788888888888888E-4</v>
       </c>
       <c r="S58" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1080.801350777778</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G59" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H59" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I59" s="2">
+        <v>5.7424886666666666</v>
+      </c>
+      <c r="J59" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K59" s="2">
+        <v>645.86557344444441</v>
+      </c>
+      <c r="L59" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M59" s="2">
+        <v>1430.3511555555554</v>
+      </c>
+      <c r="N59" s="2">
+        <v>1110.4303452222223</v>
+      </c>
+      <c r="O59" s="3">
+        <v>4638.5936415555561</v>
+      </c>
+      <c r="P59" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q59" s="2">
+        <v>-0.8872363333333334</v>
+      </c>
+      <c r="R59" s="4">
+        <v>-2.5788888888888888E-4</v>
+      </c>
+      <c r="S59" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ClimateScenarios.xml - Correct the paths in scenario #8. Scenario.cpp - Correct a logic error that happens if the CLIMATE_DRIVE environment variable is undefined and the specified path begins with a backslash.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50473614-0EC1-4AE6-A12C-5B8823FFB61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB26FA8-F50D-4A9B-A1EF-2FCF5B8E33BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="82">
   <si>
     <t>Year</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>Baseline_2010-18 12/16</t>
+  </si>
+  <si>
+    <t>Baseline 2010 C189</t>
+  </si>
+  <si>
+    <t>Demo_Baseline 2010-18 C192</t>
   </si>
 </sst>
 </file>
@@ -1147,11 +1153,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U60"/>
+  <dimension ref="A1:U62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O60" sqref="O60"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S63" sqref="S63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3080,85 +3086,86 @@
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="4"/>
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34">
+        <v>2010</v>
+      </c>
+      <c r="D34" s="2">
+        <v>831.51080300000001</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1908.5467530000001</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1.2276739999999999</v>
+      </c>
+      <c r="G34" s="5">
+        <v>302.74935900000003</v>
+      </c>
+      <c r="H34" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I34" s="2">
+        <v>6.4022730000000001</v>
+      </c>
+      <c r="J34" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K34" s="5">
+        <v>755.04443400000002</v>
+      </c>
+      <c r="L34" s="2">
+        <v>59.834083999999997</v>
+      </c>
+      <c r="M34" s="5">
+        <v>1296.8793949999999</v>
+      </c>
+      <c r="N34" s="5">
+        <v>941.98541299999999</v>
+      </c>
+      <c r="O34" s="6">
+        <v>5853.7861329999996</v>
+      </c>
+      <c r="P34" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>1.5360050000000001</v>
+      </c>
+      <c r="R34">
+        <v>5.0199999999999995E-4</v>
+      </c>
+      <c r="S34">
+        <v>2010</v>
+      </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E35" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F35" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G35" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H35" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K35" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L35" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M35" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N35" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O35" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P35" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q35" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R35" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S35" t="s">
-        <v>23</v>
-      </c>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="2"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
@@ -3198,7 +3205,7 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P36" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q36" s="2">
         <v>-4.72741111111111E-2</v>
@@ -3215,7 +3222,7 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
         <v>23</v>
@@ -3263,19 +3270,22 @@
       <c r="R37" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S37" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E38" s="2">
         <v>1901.5157334444443</v>
@@ -3294,31 +3304,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K38" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L38" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M38" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N38" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O38" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P38" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q38" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R38" s="4">
-        <v>1.4151111111111109E-3</v>
-      </c>
-      <c r="S38" t="s">
-        <v>23</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
@@ -3326,13 +3333,13 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="2">
-        <v>1161.1572335555554</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E39" s="2">
         <v>1901.5157334444443</v>
@@ -3351,28 +3358,31 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K39" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L39" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M39" s="2">
-        <v>1383.6045464444442</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N39" s="2">
-        <v>1161.284607111111</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O39" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P39" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q39" s="2">
-        <v>4.6342037777777776</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R39" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>1.4151111111111109E-3</v>
+      </c>
+      <c r="S39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
@@ -3380,13 +3390,13 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="2">
-        <v>1161.1644491111113</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E40" s="2">
         <v>1901.5157334444443</v>
@@ -3395,28 +3405,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G40" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H40" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I40" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I40" s="2"/>
       <c r="J40" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K40" s="2">
-        <v>769.36972377777772</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L40" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M40" s="2">
-        <v>1437.0445828888887</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N40" s="2">
-        <v>1161.2873196666667</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O40" s="3">
         <v>4883.9277073333324</v>
@@ -3425,13 +3433,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q40" s="2">
-        <v>27.015940777777772</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R40" s="4">
-        <v>7.9151111111111106E-3</v>
-      </c>
-      <c r="S40" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
@@ -3439,13 +3444,13 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E41" s="2">
         <v>1901.5157334444443</v>
@@ -3454,28 +3459,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G41" s="2">
-        <v>337.20870333333335</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H41" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I41" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J41" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K41" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L41" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M41" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N41" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O41" s="3">
         <v>4883.9277073333324</v>
@@ -3484,10 +3489,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q41" s="2">
-        <v>9.9787694444444455</v>
+        <v>27.015940777777772</v>
       </c>
       <c r="R41" s="4">
-        <v>2.9230000000000003E-3</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S41" t="s">
         <v>23</v>
@@ -3498,7 +3503,7 @@
         <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
@@ -3513,7 +3518,7 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G42" s="2">
-        <v>347.23312744444445</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H42" s="2">
         <v>9.775355222222224</v>
@@ -3543,10 +3548,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q42" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R42" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S42" t="s">
         <v>23</v>
@@ -3557,55 +3562,55 @@
         <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
       </c>
       <c r="D43" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E43" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F43" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G43" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G43" s="2">
+        <v>347.23312744444445</v>
       </c>
       <c r="H43" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I43" s="5">
-        <v>13.853347222222222</v>
+      <c r="I43" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J43" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K43" s="5">
-        <v>691.23065866666673</v>
+      <c r="K43" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L43" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M43" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N43" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O43" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M43" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N43" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O43" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P43" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q43" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R43" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q43" s="2">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R43" s="4">
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S43" t="s">
         <v>23</v>
@@ -3616,13 +3621,13 @@
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="2">
-        <v>1186.9521077777779</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E44" s="2">
         <v>1901.5157334444443</v>
@@ -3630,58 +3635,58 @@
       <c r="F44" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G44" s="2">
-        <v>280.33542888888883</v>
+      <c r="G44" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H44" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I44" s="5">
-        <v>12.968491888888888</v>
+        <v>13.853347222222222</v>
       </c>
       <c r="J44" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K44" s="2">
-        <v>645.94098588888892</v>
+      <c r="K44" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L44" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M44" s="2">
-        <v>1465.1962754444444</v>
-      </c>
-      <c r="N44" s="2">
-        <v>1191.1222331111112</v>
-      </c>
-      <c r="O44" s="3">
+      <c r="M44" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N44" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O44" s="6">
         <v>4695.8937716666669</v>
       </c>
       <c r="P44" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q44" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R44" s="4">
-        <v>3.9399999999999998E-4</v>
+      <c r="Q44" s="5">
+        <v>2.0880971111111108</v>
+      </c>
+      <c r="R44" s="7">
+        <v>5.926666666666668E-4</v>
       </c>
       <c r="S44" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="8" t="s">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E45" s="2">
         <v>1901.5157334444443</v>
@@ -3695,37 +3700,37 @@
       <c r="H45" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I45" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I45" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J45" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K45" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L45" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M45" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N45" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O45" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P45" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q45" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R45" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S45" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S45" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3734,7 +3739,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>23</v>
@@ -3793,13 +3798,13 @@
         <v>16</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E47" s="2">
         <v>1901.5157334444443</v>
@@ -3814,22 +3819,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I47" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J47" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K47" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L47" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M47" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N47" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O47" s="3">
         <v>4661.9885795555556</v>
@@ -3838,10 +3843,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q47" s="2">
-        <v>-1.0069492222222223</v>
+        <v>-0.95070599999999983</v>
       </c>
       <c r="R47" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S47" s="8" t="s">
         <v>23</v>
@@ -3852,132 +3857,117 @@
         <v>16</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D48" s="2">
-        <f>AVERAGE(D39:D47)</f>
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G48" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H48" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I48" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J48" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K48" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L48" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M48" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N48" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O48" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P48" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R48" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S48" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="2">
+        <f>AVERAGE(D40:D48)</f>
         <v>1176.9484893703707</v>
       </c>
-      <c r="E48" s="2">
-        <f t="shared" ref="E48:R49" si="0">AVERAGE(E39:E47)</f>
+      <c r="E49" s="2">
+        <f t="shared" ref="E49:R50" si="0">AVERAGE(E40:E48)</f>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F49" s="2">
         <f t="shared" si="0"/>
         <v>0.99402413580246907</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G49" s="5">
         <f t="shared" si="0"/>
         <v>308.82293032098761</v>
-      </c>
-      <c r="H48" s="2">
-        <f t="shared" si="0"/>
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I48" s="5">
-        <f t="shared" si="0"/>
-        <v>7.1295036805555574</v>
-      </c>
-      <c r="J48" s="2">
-        <f t="shared" si="0"/>
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K48" s="5">
-        <f t="shared" si="0"/>
-        <v>705.82954383950619</v>
-      </c>
-      <c r="L48" s="2">
-        <f t="shared" si="0"/>
-        <v>83.470620444444435</v>
-      </c>
-      <c r="M48" s="5">
-        <f t="shared" si="0"/>
-        <v>1432.1165123580245</v>
-      </c>
-      <c r="N48" s="2">
-        <f t="shared" si="0"/>
-        <v>1179.5111099259257</v>
-      </c>
-      <c r="O48" s="6">
-        <f t="shared" si="0"/>
-        <v>4768.1626790370356</v>
-      </c>
-      <c r="P48" s="3">
-        <f t="shared" si="0"/>
-        <v>27227.338324888893</v>
-      </c>
-      <c r="Q48" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6790465308641975</v>
-      </c>
-      <c r="R48" s="7">
-        <f t="shared" si="0"/>
-        <v>1.3632839506172842E-3</v>
-      </c>
-      <c r="S48" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="2">
-        <f>AVERAGE(D40:D48)</f>
-        <v>1178.7030733497943</v>
-      </c>
-      <c r="E49" s="2">
-        <f t="shared" si="0"/>
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F49" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99203508916323713</v>
-      </c>
-      <c r="G49" s="2">
-        <f t="shared" si="0"/>
-        <v>306.71652987517137</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I49" s="5">
         <f t="shared" si="0"/>
-        <v>7.1295036805555565</v>
+        <v>7.1295036805555574</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K49" s="2">
+      <c r="K49" s="5">
         <f t="shared" si="0"/>
-        <v>698.76948392043903</v>
+        <v>705.82954383950619</v>
       </c>
       <c r="L49" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M49" s="2">
+      <c r="M49" s="5">
         <f t="shared" si="0"/>
-        <v>1437.5067307928668</v>
+        <v>1432.1165123580245</v>
       </c>
       <c r="N49" s="2">
         <f t="shared" si="0"/>
-        <v>1181.53627690535</v>
-      </c>
-      <c r="O49" s="3">
+        <v>1179.5111099259257</v>
+      </c>
+      <c r="O49" s="6">
         <f t="shared" si="0"/>
-        <v>4755.299898115225</v>
+        <v>4768.1626790370356</v>
       </c>
       <c r="P49" s="3">
         <f t="shared" si="0"/>
@@ -3985,71 +3975,86 @@
       </c>
       <c r="Q49" s="2">
         <f t="shared" si="0"/>
+        <v>4.6790465308641975</v>
+      </c>
+      <c r="R49" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3632839506172842E-3</v>
+      </c>
+      <c r="S49" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="2">
+        <f>AVERAGE(D41:D49)</f>
+        <v>1178.7030733497943</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="0"/>
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F50" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99203508916323713</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="0"/>
+        <v>306.71652987517137</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1295036805555565</v>
+      </c>
+      <c r="J50" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K50" s="2">
+        <f t="shared" si="0"/>
+        <v>698.76948392043903</v>
+      </c>
+      <c r="L50" s="2">
+        <f t="shared" si="0"/>
+        <v>83.470620444444435</v>
+      </c>
+      <c r="M50" s="2">
+        <f t="shared" si="0"/>
+        <v>1437.5067307928668</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="0"/>
+        <v>1181.53627690535</v>
+      </c>
+      <c r="O50" s="3">
+        <f t="shared" si="0"/>
+        <v>4755.299898115225</v>
+      </c>
+      <c r="P50" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324888893</v>
+      </c>
+      <c r="Q50" s="2">
+        <f t="shared" si="0"/>
         <v>4.684029058984911</v>
       </c>
-      <c r="R49" s="4">
+      <c r="R50" s="4">
         <f t="shared" si="0"/>
         <v>1.363093278463649E-3</v>
       </c>
-      <c r="S49" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1186.9773491111109</v>
-      </c>
-      <c r="E50" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F50" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G50" s="2">
-        <v>280.33542888888883</v>
-      </c>
-      <c r="H50" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I50" s="2">
-        <v>5.3870271111111121</v>
-      </c>
-      <c r="J50" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K50" s="2">
-        <v>645.93808322222219</v>
-      </c>
-      <c r="L50" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M50" s="2">
-        <v>1455.5792641111111</v>
-      </c>
-      <c r="N50" s="2">
-        <v>1191.1918266666667</v>
-      </c>
-      <c r="O50" s="3">
-        <v>4661.9885253333332</v>
-      </c>
-      <c r="P50" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q50" s="2">
-        <v>-0.64567288888888896</v>
-      </c>
-      <c r="R50" s="4">
-        <v>-2.0755555555555555E-4</v>
-      </c>
       <c r="S50" s="8" t="s">
         <v>23</v>
       </c>
@@ -4059,13 +4064,13 @@
         <v>16</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D51" s="2">
-        <v>1186.9773355555556</v>
+        <v>1186.9773491111109</v>
       </c>
       <c r="E51" s="2">
         <v>1901.5157334444443</v>
@@ -4086,16 +4091,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K51" s="2">
-        <v>645.93833411111109</v>
+        <v>645.93808322222219</v>
       </c>
       <c r="L51" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M51" s="2">
-        <v>1455.5790065555557</v>
+        <v>1455.5792641111111</v>
       </c>
       <c r="N51" s="2">
-        <v>1191.1918131111113</v>
+        <v>1191.1918266666667</v>
       </c>
       <c r="O51" s="3">
         <v>4661.9885253333332</v>
@@ -4104,10 +4109,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q51" s="2">
-        <v>-0.64567966666666665</v>
+        <v>-0.64567288888888896</v>
       </c>
       <c r="R51" s="4">
-        <v>-2.0744444444444445E-4</v>
+        <v>-2.0755555555555555E-4</v>
       </c>
       <c r="S51" s="8" t="s">
         <v>23</v>
@@ -4118,7 +4123,7 @@
         <v>16</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>23</v>
@@ -4145,13 +4150,13 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K52" s="2">
-        <v>645.9383002222221</v>
+        <v>645.93833411111109</v>
       </c>
       <c r="L52" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M52" s="2">
-        <v>1455.5790607777778</v>
+        <v>1455.5790065555557</v>
       </c>
       <c r="N52" s="2">
         <v>1191.1918131111113</v>
@@ -4163,7 +4168,7 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q52" s="2">
-        <v>-0.64565933333333325</v>
+        <v>-0.64567966666666665</v>
       </c>
       <c r="R52" s="4">
         <v>-2.0744444444444445E-4</v>
@@ -4177,13 +4182,13 @@
         <v>16</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D53" s="2">
-        <v>1187.0067003333331</v>
+        <v>1186.9773355555556</v>
       </c>
       <c r="E53" s="2">
         <v>1901.5157334444443</v>
@@ -4204,16 +4209,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K53" s="2">
-        <v>645.93713388888887</v>
+        <v>645.9383002222221</v>
       </c>
       <c r="L53" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M53" s="2">
-        <v>1455.6553682222225</v>
+        <v>1455.5790607777778</v>
       </c>
       <c r="N53" s="2">
-        <v>1191.1764458888888</v>
+        <v>1191.1918131111113</v>
       </c>
       <c r="O53" s="3">
         <v>4661.9885253333332</v>
@@ -4222,27 +4227,27 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q53" s="2">
-        <v>-0.61525011111111105</v>
+        <v>-0.64565933333333325</v>
       </c>
       <c r="R53" s="4">
-        <v>-1.7433333333333333E-4</v>
+        <v>-2.0744444444444445E-4</v>
       </c>
       <c r="S53" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>16</v>
-      </c>
-      <c r="B54" t="s">
-        <v>65</v>
+      <c r="A54" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D54" s="2">
-        <v>1187.0063613333334</v>
+        <v>1187.0067003333331</v>
       </c>
       <c r="E54" s="2">
         <v>1901.5157334444443</v>
@@ -4257,34 +4262,34 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I54" s="2">
-        <v>5.3870315555555557</v>
+        <v>5.3870271111111121</v>
       </c>
       <c r="J54" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K54" s="2">
-        <v>645.93916833333344</v>
+        <v>645.93713388888887</v>
       </c>
       <c r="L54" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M54" s="2">
-        <v>1455.7051053333334</v>
+        <v>1455.6553682222225</v>
       </c>
       <c r="N54" s="2">
-        <v>1191.1759305555559</v>
+        <v>1191.1764458888888</v>
       </c>
       <c r="O54" s="3">
-        <v>4661.988498222222</v>
+        <v>4661.9885253333332</v>
       </c>
       <c r="P54" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q54" s="2">
-        <v>-0.56365988888888896</v>
+        <v>-0.61525011111111105</v>
       </c>
       <c r="R54" s="4">
-        <v>-1.5888888888888889E-4</v>
+        <v>-1.7433333333333333E-4</v>
       </c>
       <c r="S54" s="8" t="s">
         <v>23</v>
@@ -4295,13 +4300,13 @@
         <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D55" s="5">
-        <v>1208.5438095555555</v>
+      <c r="D55" s="2">
+        <v>1187.0063613333334</v>
       </c>
       <c r="E55" s="2">
         <v>1901.5157334444443</v>
@@ -4316,51 +4321,51 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I55" s="2">
-        <v>5.3172314444444444</v>
+        <v>5.3870315555555557</v>
       </c>
       <c r="J55" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K55" s="2">
-        <v>645.97183577777787</v>
+        <v>645.93916833333344</v>
       </c>
       <c r="L55" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M55" s="5">
-        <v>1460.2614338888889</v>
-      </c>
-      <c r="N55" s="5">
-        <v>1208.0519340000001</v>
+      <c r="M55" s="2">
+        <v>1455.7051053333334</v>
+      </c>
+      <c r="N55" s="2">
+        <v>1191.1759305555559</v>
       </c>
       <c r="O55" s="3">
-        <v>4662.6060926666669</v>
+        <v>4661.988498222222</v>
       </c>
       <c r="P55" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q55" s="2">
-        <v>-0.5663084444444445</v>
+        <v>-0.56365988888888896</v>
       </c>
       <c r="R55" s="4">
-        <v>-1.5933333333333332E-4</v>
+        <v>-1.5888888888888889E-4</v>
       </c>
       <c r="S55" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>74</v>
+      <c r="B56" t="s">
+        <v>67</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D56" s="2">
-        <v>1207.0222438888889</v>
+      <c r="D56" s="5">
+        <v>1208.5438095555555</v>
       </c>
       <c r="E56" s="2">
         <v>1901.5157334444443</v>
@@ -4375,34 +4380,37 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I56" s="2">
-        <v>5.3316344444444441</v>
+        <v>5.3172314444444444</v>
       </c>
       <c r="J56" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K56" s="2">
-        <v>645.95907266666666</v>
+        <v>645.97183577777787</v>
       </c>
       <c r="L56" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M56" s="2">
-        <v>1460.4185112222222</v>
-      </c>
-      <c r="N56" s="2">
-        <v>1206.2352837777776</v>
+      <c r="M56" s="5">
+        <v>1460.2614338888889</v>
+      </c>
+      <c r="N56" s="5">
+        <v>1208.0519340000001</v>
       </c>
       <c r="O56" s="3">
-        <v>4662.5755209999998</v>
+        <v>4662.6060926666669</v>
       </c>
       <c r="P56" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q56" s="2">
-        <v>-0.73148200000000008</v>
+        <v>-0.5663084444444445</v>
       </c>
       <c r="R56" s="4">
-        <v>-2.0655555555555556E-4</v>
+        <v>-1.5933333333333332E-4</v>
+      </c>
+      <c r="S56" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
@@ -4410,13 +4418,13 @@
         <v>16</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D57" s="2">
-        <v>1206.5233695555557</v>
+        <v>1207.0222438888889</v>
       </c>
       <c r="E57" s="2">
         <v>1901.5157334444443</v>
@@ -4431,48 +4439,48 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I57" s="2">
-        <v>5.3531247777777775</v>
+        <v>5.3316344444444441</v>
       </c>
       <c r="J57" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K57" s="2">
-        <v>645.94818811111122</v>
+        <v>645.95907266666666</v>
       </c>
       <c r="L57" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M57" s="2">
-        <v>1460.5092637777777</v>
+        <v>1460.4185112222222</v>
       </c>
       <c r="N57" s="2">
-        <v>1205.5020886666666</v>
+        <v>1206.2352837777776</v>
       </c>
       <c r="O57" s="3">
-        <v>4662.5708008888896</v>
+        <v>4662.5755209999998</v>
       </c>
       <c r="P57" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q57" s="2">
-        <v>-0.90742522222222222</v>
+        <v>-0.73148200000000008</v>
       </c>
       <c r="R57" s="4">
-        <v>-2.5755555555555558E-4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+        <v>-2.0655555555555556E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>16</v>
       </c>
-      <c r="B58" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="B58" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D58" s="2">
-        <v>1080.801350777778</v>
+        <v>1206.5233695555557</v>
       </c>
       <c r="E58" s="2">
         <v>1901.5157334444443</v>
@@ -4487,37 +4495,34 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I58" s="2">
-        <v>5.7424886666666666</v>
+        <v>5.3531247777777775</v>
       </c>
       <c r="J58" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K58" s="2">
-        <v>645.86557344444441</v>
+        <v>645.94818811111122</v>
       </c>
       <c r="L58" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M58" s="5">
-        <v>1430.3511555555554</v>
+      <c r="M58" s="2">
+        <v>1460.5092637777777</v>
       </c>
       <c r="N58" s="2">
-        <v>1110.4303452222223</v>
+        <v>1205.5020886666666</v>
       </c>
       <c r="O58" s="3">
-        <v>4638.5936415555561</v>
+        <v>4662.5708008888896</v>
       </c>
       <c r="P58" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q58" s="2">
-        <v>-0.8872363333333334</v>
+        <v>-0.90742522222222222</v>
       </c>
       <c r="R58" s="4">
-        <v>-2.5788888888888888E-4</v>
-      </c>
-      <c r="S58" t="s">
-        <v>23</v>
+        <v>-2.5755555555555558E-4</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.3">
@@ -4525,7 +4530,7 @@
         <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" t="s">
         <v>23</v>
@@ -4557,7 +4562,7 @@
       <c r="L59" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M59" s="2">
+      <c r="M59" s="5">
         <v>1430.3511555555554</v>
       </c>
       <c r="N59" s="2">
@@ -4584,19 +4589,19 @@
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C60" t="s">
         <v>23</v>
       </c>
-      <c r="D60" s="5">
-        <v>897.84913466666671</v>
-      </c>
-      <c r="E60" s="5">
-        <v>1763.5263265555557</v>
+      <c r="D60" s="2">
+        <v>1080.801350777778</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1901.5157334444443</v>
       </c>
       <c r="F60" s="2">
-        <v>1.0174076666666665</v>
+        <v>0.97970299999999988</v>
       </c>
       <c r="G60" s="2">
         <v>280.33542888888883</v>
@@ -4604,37 +4609,155 @@
       <c r="H60" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I60" s="5">
-        <v>7.299440555555555</v>
+      <c r="I60" s="2">
+        <v>5.7424886666666666</v>
       </c>
       <c r="J60" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K60" s="2">
-        <v>646.63056122222224</v>
-      </c>
-      <c r="L60" s="5">
-        <v>60.018756111111117</v>
-      </c>
-      <c r="M60" s="5">
-        <v>1342.5421007777777</v>
-      </c>
-      <c r="N60" s="5">
-        <v>902.73358833333339</v>
-      </c>
-      <c r="O60" s="6">
-        <v>5459.5160589999996</v>
+        <v>645.86557344444441</v>
+      </c>
+      <c r="L60" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M60" s="2">
+        <v>1430.3511555555554</v>
+      </c>
+      <c r="N60" s="2">
+        <v>1110.4303452222223</v>
+      </c>
+      <c r="O60" s="3">
+        <v>4638.5936415555561</v>
       </c>
       <c r="P60" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q60" s="2">
+        <v>-0.8872363333333334</v>
+      </c>
+      <c r="R60" s="4">
+        <v>-2.5788888888888888E-4</v>
+      </c>
+      <c r="S60" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="5">
+        <v>897.84913466666671</v>
+      </c>
+      <c r="E61" s="5">
+        <v>1763.5263265555557</v>
+      </c>
+      <c r="F61" s="2">
+        <v>1.0174076666666665</v>
+      </c>
+      <c r="G61" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H61" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I61" s="5">
+        <v>7.299440555555555</v>
+      </c>
+      <c r="J61" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K61" s="2">
+        <v>646.63056122222224</v>
+      </c>
+      <c r="L61" s="5">
+        <v>60.018756111111117</v>
+      </c>
+      <c r="M61" s="5">
+        <v>1342.5421007777777</v>
+      </c>
+      <c r="N61" s="5">
+        <v>902.73358833333339</v>
+      </c>
+      <c r="O61" s="6">
+        <v>5459.5160589999996</v>
+      </c>
+      <c r="P61" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q61" s="2">
         <v>0.26704155555555559</v>
       </c>
-      <c r="R60" s="4">
+      <c r="R61" s="4">
         <v>4.2666666666666656E-5</v>
       </c>
-      <c r="S60" t="s">
+      <c r="S61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="5">
+        <v>1000.3124864444443</v>
+      </c>
+      <c r="E62" s="2">
+        <v>1763.5263265555557</v>
+      </c>
+      <c r="F62" s="2">
+        <v>0.999942</v>
+      </c>
+      <c r="G62" s="5">
+        <v>305.6782124444444</v>
+      </c>
+      <c r="H62" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I62" s="2">
+        <v>6.8948233333333331</v>
+      </c>
+      <c r="J62" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K62" s="5">
+        <v>673.17452677777771</v>
+      </c>
+      <c r="L62" s="2">
+        <v>60.018756111111117</v>
+      </c>
+      <c r="M62" s="5">
+        <v>1321.9402533333332</v>
+      </c>
+      <c r="N62" s="5">
+        <v>1024.1975572222223</v>
+      </c>
+      <c r="O62" s="6">
+        <v>4583.9874403333333</v>
+      </c>
+      <c r="P62" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q62" s="2">
+        <v>0.28907633333333327</v>
+      </c>
+      <c r="R62" s="4">
+        <v>6.222222222222222E-5</v>
+      </c>
+      <c r="S62" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ClimateScenarios.xml - Correct the paths for climate scenario #13. Add ScenarioData/Baseline_2000-09 and ../Baseline_2010-current, cloned from ../Baseline.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB26FA8-F50D-4A9B-A1EF-2FCF5B8E33BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0D34E3-112E-4745-ADD5-8DDC9A15BA1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="83">
   <si>
     <t>Year</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>Demo_Baseline 2010-18 C192</t>
+  </si>
+  <si>
+    <t>Baseline_2010-current_2010-19_C193</t>
   </si>
 </sst>
 </file>
@@ -776,7 +779,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -798,6 +801,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1153,17 +1159,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U62"/>
+  <dimension ref="A1:U63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S63" sqref="S63"/>
+      <selection pane="bottomLeft" activeCell="D63" sqref="D63:R63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" customWidth="1"/>
     <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -4758,6 +4764,65 @@
         <v>6.222222222222222E-5</v>
       </c>
       <c r="S62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" s="13">
+        <v>1000.3124864444443</v>
+      </c>
+      <c r="E63" s="13">
+        <v>1763.5263265555557</v>
+      </c>
+      <c r="F63" s="13">
+        <v>0.999942</v>
+      </c>
+      <c r="G63" s="13">
+        <v>305.6782124444444</v>
+      </c>
+      <c r="H63" s="13">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I63" s="13">
+        <v>6.8948233333333331</v>
+      </c>
+      <c r="J63" s="13">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K63" s="13">
+        <v>673.17452677777771</v>
+      </c>
+      <c r="L63" s="13">
+        <v>60.018756111111117</v>
+      </c>
+      <c r="M63" s="13">
+        <v>1321.9402533333332</v>
+      </c>
+      <c r="N63" s="13">
+        <v>1024.1975572222223</v>
+      </c>
+      <c r="O63" s="14">
+        <v>4583.9874403333333</v>
+      </c>
+      <c r="P63" s="14">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q63" s="13">
+        <v>0.28907633333333327</v>
+      </c>
+      <c r="R63" s="15">
+        <v>6.222222222222222E-5</v>
+      </c>
+      <c r="S63" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Save new Flow IC file. flow2010.ic - From Baseline_2000-09_C194.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0D34E3-112E-4745-ADD5-8DDC9A15BA1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60971AF4-CB57-43F4-A207-75461448E72F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
-    <sheet name="2000-09" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="2000-09" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="85">
   <si>
     <t>Year</t>
   </si>
@@ -281,6 +282,12 @@
   </si>
   <si>
     <t>Baseline_2010-current_2010-19_C193</t>
+  </si>
+  <si>
+    <t>Baseline_2000-09_C194</t>
+  </si>
+  <si>
+    <t>Baseline_2010-current_2010-19_C195</t>
   </si>
 </sst>
 </file>
@@ -1159,11 +1166,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U63"/>
+  <dimension ref="A1:U64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63:R63"/>
+      <selection pane="bottomLeft" activeCell="S65" sqref="S65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4826,6 +4833,65 @@
         <v>23</v>
       </c>
     </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="5">
+        <v>1070.3662515555557</v>
+      </c>
+      <c r="E64" s="2">
+        <v>1763.5263265555557</v>
+      </c>
+      <c r="F64" s="2">
+        <v>0.999942</v>
+      </c>
+      <c r="G64" s="2">
+        <v>305.6782124444444</v>
+      </c>
+      <c r="H64" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I64" s="2">
+        <v>6.8224234444444436</v>
+      </c>
+      <c r="J64" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K64" s="2">
+        <v>672.51038266666671</v>
+      </c>
+      <c r="L64" s="2">
+        <v>60.018756111111117</v>
+      </c>
+      <c r="M64" s="5">
+        <v>1335.0520562222218</v>
+      </c>
+      <c r="N64" s="5">
+        <v>1081.7151217777778</v>
+      </c>
+      <c r="O64" s="3">
+        <v>4576.182644333333</v>
+      </c>
+      <c r="P64" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q64" s="2">
+        <v>0.27293466666666671</v>
+      </c>
+      <c r="R64" s="4">
+        <v>5.7555555555555559E-5</v>
+      </c>
+      <c r="S64" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -4833,17 +4899,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD84CEC-7113-4714-90A2-84947C9E014D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD88AF4-3325-45AB-9D19-94573DCD22C4}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" customWidth="1"/>
     <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
@@ -5018,56 +5097,132 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="5">
+        <v>931.63393560000009</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1609.2949586000002</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.0215697000000001</v>
+      </c>
+      <c r="G4" s="5">
+        <v>305.74331049999995</v>
+      </c>
+      <c r="H4" s="2">
+        <v>9.3183378000000001</v>
+      </c>
+      <c r="I4" s="2">
+        <v>8.1064159</v>
+      </c>
+      <c r="J4" s="2">
+        <v>7.7646284999999988</v>
+      </c>
+      <c r="K4" s="5">
+        <v>654.30700679999995</v>
+      </c>
+      <c r="L4" s="2">
+        <v>61.771183299999997</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1196.3218261999998</v>
+      </c>
+      <c r="N4" s="5">
+        <v>945.03428959999997</v>
+      </c>
+      <c r="O4" s="6">
+        <v>5406.1934815999994</v>
+      </c>
+      <c r="P4" s="3">
+        <v>25979.647461100001</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>8.0406299999999972E-2</v>
+      </c>
+      <c r="R4" s="4">
+        <v>-1.6500000000000015E-5</v>
+      </c>
+      <c r="S4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="15"/>
+    </row>
+    <row r="6" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="P6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add logic to permit specification of whether row 0 in a climate dataset is at the north edge or the south edge of the grid. ClimateScenarios.xml - Add the row_0_location_N_or_S attribute to all the gridded climate scenarios. flow2010.ic - This was made by running the equivalent of this version, so interpreting the Baseline_2019versionOfGridMET_2000-09 dataset as having row 0 in the north, which is correct. Scenario.cpp - Add the row_0_location_N_or_S attribute to the <climate_scenario> block. Flow.cpp, .h - Add m_row0inSouth to both ClimateDataInfo and FlowScenario. Replace the old kludge logic which determines the location of row 0 based on whether the dataset has single year or multiyear files with new logic which uses the m_row0inSouth member of the ClimateDataInfo class.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60971AF4-CB57-43F4-A207-75461448E72F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F6285C-D05E-4120-A456-834C0DD21578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="87">
   <si>
     <t>Year</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>Baseline_2010-current_2010-19_C195</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_Dec22</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_Dec22_1800</t>
   </si>
 </sst>
 </file>
@@ -1166,11 +1172,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U64"/>
+  <dimension ref="A1:U66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S65" sqref="S65"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M66" sqref="M66:O66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4890,6 +4896,121 @@
       </c>
       <c r="S64" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" s="5">
+        <v>1246.3303018888889</v>
+      </c>
+      <c r="E65" s="5">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F65" s="2">
+        <v>0.94846033333333346</v>
+      </c>
+      <c r="G65" s="2">
+        <v>305.6782124444444</v>
+      </c>
+      <c r="H65" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I65" s="5">
+        <v>6.3587768888888885</v>
+      </c>
+      <c r="J65" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K65" s="5">
+        <v>628.90788111111101</v>
+      </c>
+      <c r="L65" s="5">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M65" s="5">
+        <v>1456.3722873333334</v>
+      </c>
+      <c r="N65" s="5">
+        <v>1283.7495253333334</v>
+      </c>
+      <c r="O65" s="6">
+        <v>3986.0738390000001</v>
+      </c>
+      <c r="P65" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q65" s="2">
+        <v>0.12974411111111114</v>
+      </c>
+      <c r="R65" s="4">
+        <v>2.3444444444444448E-5</v>
+      </c>
+      <c r="S65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="5">
+        <v>1380.5085448888888</v>
+      </c>
+      <c r="E66" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F66" s="2">
+        <v>0.94846033333333346</v>
+      </c>
+      <c r="G66" s="2">
+        <v>305.6782124444444</v>
+      </c>
+      <c r="H66" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I66" s="2">
+        <v>6.1288343333333337</v>
+      </c>
+      <c r="J66" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K66" s="2">
+        <v>628.9703199999999</v>
+      </c>
+      <c r="L66" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M66" s="5">
+        <v>1487.9843207777781</v>
+      </c>
+      <c r="N66" s="5">
+        <v>1386.0215385555557</v>
+      </c>
+      <c r="O66" s="6">
+        <v>4013.3543294444444</v>
+      </c>
+      <c r="P66" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q66" s="2">
+        <v>0.12792911111111113</v>
+      </c>
+      <c r="R66" s="4">
+        <v>2.1888888888888887E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct bugs in the calculation of Reach attributes RAD_SW_IN and RAD_LW_OUT. ClimateScenarios.xml - Add and then comment out a climate scenario which uses David Rupp's new actual weather data files. Flow_McKenzie.xml - Refine the "FLOW McKenzie Thermal Energy Budget for streams" reports. Flow_NSantiam.xml - Begin to add air temperature outputs. ReachRouting.cpp - Correct bugs in the calculation of Reach attributes RAD_SW_IN and RAD_LW_OUT.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AED83A-AE44-412F-A8CA-B7D676C8D9AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE647476-A8F2-4F90-BC39-EFE1D75E1F30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="2000-09" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="90">
   <si>
     <t>Year</t>
   </si>
@@ -297,6 +296,12 @@
   </si>
   <si>
     <t>Demo_Baseline_2010-18 C204</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_C208+ 2010 using D Rupp's climate data</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_C203</t>
   </si>
 </sst>
 </file>
@@ -1175,11 +1180,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U67"/>
+  <dimension ref="A1:U70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3167,201 +3172,174 @@
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="2"/>
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35">
+        <v>2010</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1.2075180000000001</v>
+      </c>
+      <c r="G35" s="2">
+        <v>298.60159299999998</v>
+      </c>
+      <c r="H35" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I35" s="2">
+        <v>4.7158709999999999</v>
+      </c>
+      <c r="J35" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K35" s="2">
+        <v>716.32672100000002</v>
+      </c>
+      <c r="L35" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="M35" s="2">
+        <v>1410.700439</v>
+      </c>
+      <c r="N35" s="2">
+        <v>1361.7288820000001</v>
+      </c>
+      <c r="O35" s="3">
+        <v>6933.6865230000003</v>
+      </c>
+      <c r="P35" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>1.205797</v>
+      </c>
+      <c r="R35" s="4">
+        <v>3.3599999999999998E-4</v>
+      </c>
+      <c r="S35">
+        <v>2010</v>
+      </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" t="s">
-        <v>23</v>
-      </c>
-      <c r="D36" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E36" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F36" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G36" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H36" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K36" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L36" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M36" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N36" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O36" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P36" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q36" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R36" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="4"/>
+    </row>
+    <row r="37" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>16</v>
       </c>
-      <c r="B37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" t="s">
-        <v>23</v>
+      <c r="B37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37">
+        <v>2010</v>
       </c>
       <c r="D37" s="2">
-        <v>1138.6194117777777</v>
+        <v>1284.0238039999999</v>
       </c>
       <c r="E37" s="2">
-        <v>1901.5157334444443</v>
+        <v>1990.4650879999999</v>
       </c>
       <c r="F37" s="2">
-        <v>1.0119255555555557</v>
+        <v>1.443354</v>
       </c>
       <c r="G37" s="2">
-        <v>327.78053433333326</v>
+        <v>298.60159299999998</v>
       </c>
       <c r="H37" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I37" s="2"/>
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I37" s="2">
+        <v>4.8117099999999997</v>
+      </c>
       <c r="J37" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K37" s="2">
-        <v>769.26639155555551</v>
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K37" s="5">
+        <v>737.62927200000001</v>
       </c>
       <c r="L37" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M37" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N37" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O37" s="3">
-        <v>4918.1879612222219</v>
+        <v>93.234084999999993</v>
+      </c>
+      <c r="M37" s="5">
+        <v>1400.039673</v>
+      </c>
+      <c r="N37" s="5">
+        <v>1351.4182129999999</v>
+      </c>
+      <c r="O37" s="6">
+        <v>8159.9951170000004</v>
       </c>
       <c r="P37" s="3">
-        <v>27227.338324888889</v>
+        <v>29450.638672000001</v>
       </c>
       <c r="Q37" s="2">
-        <v>-4.72741111111111E-2</v>
+        <v>1.205238</v>
       </c>
       <c r="R37" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S37" t="s">
-        <v>23</v>
+        <v>3.3599999999999998E-4</v>
+      </c>
+      <c r="S37">
+        <v>2010</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" t="s">
-        <v>23</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F38" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G38" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H38" s="2">
-        <v>9.775355222222224</v>
-      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
       <c r="I38" s="2"/>
-      <c r="J38" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K38" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L38" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M38" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N38" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O38" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P38" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q38" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="2"/>
       <c r="R38" s="4">
         <v>-3.8888888888888877E-5</v>
       </c>
+      <c r="S38" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C39" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E39" s="2">
         <v>1901.5157334444443</v>
@@ -3380,28 +3358,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K39" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L39" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M39" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N39" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O39" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P39" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q39" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R39" s="4">
-        <v>1.4151111111111109E-3</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
       <c r="S39" t="s">
         <v>23</v>
@@ -3412,13 +3390,13 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="2">
-        <v>1161.1572335555554</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E40" s="2">
         <v>1901.5157334444443</v>
@@ -3437,28 +3415,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K40" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L40" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M40" s="2">
-        <v>1383.6045464444442</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N40" s="2">
-        <v>1161.284607111111</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O40" s="3">
-        <v>4883.9277073333324</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P40" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q40" s="2">
-        <v>4.6342037777777776</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R40" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
@@ -3466,13 +3444,13 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="2">
-        <v>1161.1644491111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E41" s="2">
         <v>1901.5157334444443</v>
@@ -3481,40 +3459,38 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G41" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H41" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I41" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I41" s="2"/>
       <c r="J41" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K41" s="2">
-        <v>769.36972377777772</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L41" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M41" s="2">
-        <v>1437.0445828888887</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N41" s="2">
-        <v>1161.2873196666667</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O41" s="3">
-        <v>4883.9277073333324</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P41" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q41" s="2">
-        <v>27.015940777777772</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R41" s="4">
-        <v>7.9151111111111106E-3</v>
+        <v>1.4151111111111109E-3</v>
       </c>
       <c r="S41" t="s">
         <v>23</v>
@@ -3525,13 +3501,13 @@
         <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="2">
-        <v>1161.1599054444443</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E42" s="2">
         <v>1901.5157334444443</v>
@@ -3540,43 +3516,38 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G42" s="2">
-        <v>337.20870333333335</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H42" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I42" s="2">
-        <v>4.6813607777777788</v>
-      </c>
+      <c r="I42" s="2"/>
       <c r="J42" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K42" s="2">
-        <v>769.36992711111111</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L42" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M42" s="2">
-        <v>1403.060424888889</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N42" s="2">
-        <v>1161.2856514444443</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O42" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P42" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q42" s="2">
-        <v>9.9787694444444455</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R42" s="4">
-        <v>2.9230000000000003E-3</v>
-      </c>
-      <c r="S42" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
@@ -3584,13 +3555,13 @@
         <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
       </c>
       <c r="D43" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E43" s="2">
         <v>1901.5157334444443</v>
@@ -3599,28 +3570,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G43" s="2">
-        <v>347.23312744444445</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H43" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I43" s="2">
-        <v>4.6813607777777788</v>
-      </c>
+      <c r="I43" s="2"/>
       <c r="J43" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K43" s="2">
-        <v>769.36992711111111</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L43" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M43" s="2">
-        <v>1403.060424888889</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N43" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O43" s="3">
         <v>4883.9277073333324</v>
@@ -3629,10 +3598,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q43" s="2">
-        <v>-4.5654777777777787E-2</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R43" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S43" t="s">
         <v>23</v>
@@ -3643,55 +3612,55 @@
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E44" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F44" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G44" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G44" s="2">
+        <v>354.15221155555554</v>
       </c>
       <c r="H44" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I44" s="5">
-        <v>13.853347222222222</v>
+      <c r="I44" s="2">
+        <v>4.6817598888888901</v>
       </c>
       <c r="J44" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K44" s="5">
-        <v>691.23065866666673</v>
+      <c r="K44" s="2">
+        <v>769.36972377777772</v>
       </c>
       <c r="L44" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M44" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N44" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O44" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M44" s="2">
+        <v>1437.0445828888887</v>
+      </c>
+      <c r="N44" s="2">
+        <v>1161.2873196666667</v>
+      </c>
+      <c r="O44" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P44" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q44" s="5">
-        <v>2.0880971111111108</v>
-      </c>
-      <c r="R44" s="7">
-        <v>5.926666666666668E-4</v>
+      <c r="Q44" s="2">
+        <v>27.015940777777772</v>
+      </c>
+      <c r="R44" s="4">
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S44" t="s">
         <v>23</v>
@@ -3702,131 +3671,131 @@
         <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="2">
-        <v>1186.9521077777779</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E45" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F45" s="2">
-        <v>0.97970299999999988</v>
+        <v>1.0119255555555557</v>
       </c>
       <c r="G45" s="2">
-        <v>280.33542888888883</v>
+        <v>337.20870333333335</v>
       </c>
       <c r="H45" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I45" s="5">
-        <v>12.968491888888888</v>
+      <c r="I45" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J45" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K45" s="2">
-        <v>645.94098588888892</v>
+        <v>769.36992711111111</v>
       </c>
       <c r="L45" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M45" s="2">
-        <v>1465.1962754444444</v>
+        <v>1403.060424888889</v>
       </c>
       <c r="N45" s="2">
-        <v>1191.1222331111112</v>
+        <v>1161.2856514444443</v>
       </c>
       <c r="O45" s="3">
-        <v>4695.8937716666669</v>
+        <v>4883.9277073333324</v>
       </c>
       <c r="P45" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q45" s="2">
-        <v>1.3484236666666667</v>
+        <v>9.9787694444444455</v>
       </c>
       <c r="R45" s="4">
-        <v>3.9399999999999998E-4</v>
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S45" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C46" s="8" t="s">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="2">
-        <v>1186.9497747777777</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E46" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F46" s="2">
-        <v>0.97970299999999988</v>
+        <v>1.0119255555555557</v>
       </c>
       <c r="G46" s="2">
-        <v>280.33542888888883</v>
+        <v>347.23312744444445</v>
       </c>
       <c r="H46" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I46" s="2">
-        <v>5.3913398888888899</v>
+        <v>4.6813607777777788</v>
       </c>
       <c r="J46" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K46" s="2">
-        <v>645.93823922222225</v>
+        <v>769.36992711111111</v>
       </c>
       <c r="L46" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M46" s="2">
-        <v>1455.3145886666666</v>
+        <v>1403.060424888889</v>
       </c>
       <c r="N46" s="2">
-        <v>1191.1280516666666</v>
+        <v>1161.2856514444443</v>
       </c>
       <c r="O46" s="3">
-        <v>4661.9885795555556</v>
+        <v>4883.9277073333324</v>
       </c>
       <c r="P46" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q46" s="2">
-        <v>-0.95070599999999983</v>
-      </c>
-      <c r="R46" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S46" s="8" t="s">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R46" s="7">
+        <v>5.926666666666668E-4</v>
+      </c>
+      <c r="S46" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="8" t="s">
+      <c r="A47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="2">
-        <v>1186.9497747777777</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E47" s="2">
         <v>1901.5157334444443</v>
@@ -3834,58 +3803,58 @@
       <c r="F47" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G47" s="2">
-        <v>280.33542888888883</v>
+      <c r="G47" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H47" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I47" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I47" s="5">
+        <v>13.853347222222222</v>
       </c>
       <c r="J47" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K47" s="2">
-        <v>645.93823922222225</v>
+      <c r="K47" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L47" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M47" s="2">
-        <v>1455.3145886666666</v>
-      </c>
-      <c r="N47" s="2">
-        <v>1191.1280516666666</v>
-      </c>
-      <c r="O47" s="3">
-        <v>4661.9885795555556</v>
+      <c r="M47" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N47" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O47" s="6">
+        <v>4695.8937716666669</v>
       </c>
       <c r="P47" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q47" s="2">
-        <v>-0.95070599999999983</v>
+      <c r="Q47" s="5">
+        <v>2.0880971111111108</v>
       </c>
       <c r="R47" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S47" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S47" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C48" s="8" t="s">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" t="s">
         <v>23</v>
       </c>
       <c r="D48" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E48" s="2">
         <v>1901.5157334444443</v>
@@ -3899,35 +3868,35 @@
       <c r="H48" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I48" s="2">
-        <v>5.3870291111111106</v>
+      <c r="I48" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J48" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K48" s="2">
-        <v>645.93811044444442</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L48" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M48" s="2">
-        <v>1455.2552082222223</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N48" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O48" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P48" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q48" s="2">
-        <v>-1.0069492222222223</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R48" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S48" s="8" t="s">
         <v>23</v>
@@ -3938,321 +3907,321 @@
         <v>16</v>
       </c>
       <c r="B49" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1186.9497747777777</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G49" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H49" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I49" s="2">
+        <v>5.3913398888888899</v>
+      </c>
+      <c r="J49" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K49" s="2">
+        <v>645.93823922222225</v>
+      </c>
+      <c r="L49" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M49" s="2">
+        <v>1455.3145886666666</v>
+      </c>
+      <c r="N49" s="2">
+        <v>1191.1280516666666</v>
+      </c>
+      <c r="O49" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P49" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>-0.95070599999999983</v>
+      </c>
+      <c r="R49" s="4">
+        <v>-2.8933333333333328E-4</v>
+      </c>
+      <c r="S49" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1186.9497747777777</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G50" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H50" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I50" s="2">
+        <v>5.3913398888888899</v>
+      </c>
+      <c r="J50" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K50" s="2">
+        <v>645.93823922222225</v>
+      </c>
+      <c r="L50" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M50" s="2">
+        <v>1455.3145886666666</v>
+      </c>
+      <c r="N50" s="2">
+        <v>1191.1280516666666</v>
+      </c>
+      <c r="O50" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P50" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q50" s="2">
+        <v>-0.95070599999999983</v>
+      </c>
+      <c r="R50" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S50" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E51" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G51" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H51" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I51" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J51" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K51" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L51" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M51" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N51" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O51" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P51" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R51" s="7">
+        <f t="shared" ref="E51:R53" si="0">AVERAGE(R42:R50)</f>
+        <v>1.3632839506172842E-3</v>
+      </c>
+      <c r="S51" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="2">
-        <f>AVERAGE(D40:D48)</f>
+      <c r="C52" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" s="2">
+        <f>AVERAGE(D43:D51)</f>
         <v>1176.9484893703707</v>
       </c>
-      <c r="E49" s="2">
-        <f t="shared" ref="E49:R50" si="0">AVERAGE(E40:E48)</f>
+      <c r="E52" s="2">
+        <f t="shared" si="0"/>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F52" s="2">
         <f t="shared" si="0"/>
         <v>0.99402413580246907</v>
       </c>
-      <c r="G49" s="5">
+      <c r="G52" s="5">
         <f t="shared" si="0"/>
         <v>308.82293032098761</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H52" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I49" s="5">
+      <c r="I52" s="5">
         <f t="shared" si="0"/>
         <v>7.1295036805555574</v>
       </c>
-      <c r="J49" s="2">
+      <c r="J52" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K49" s="5">
+      <c r="K52" s="5">
         <f t="shared" si="0"/>
         <v>705.82954383950619</v>
       </c>
-      <c r="L49" s="2">
+      <c r="L52" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M49" s="5">
+      <c r="M52" s="5">
         <f t="shared" si="0"/>
         <v>1432.1165123580245</v>
       </c>
-      <c r="N49" s="2">
+      <c r="N52" s="2">
         <f t="shared" si="0"/>
         <v>1179.5111099259257</v>
       </c>
-      <c r="O49" s="6">
+      <c r="O52" s="6">
         <f t="shared" si="0"/>
         <v>4768.1626790370356</v>
       </c>
-      <c r="P49" s="3">
+      <c r="P52" s="3">
         <f t="shared" si="0"/>
         <v>27227.338324888893</v>
       </c>
-      <c r="Q49" s="2">
+      <c r="Q52" s="2">
         <f t="shared" si="0"/>
         <v>4.6790465308641975</v>
       </c>
-      <c r="R49" s="7">
+      <c r="R52" s="4">
         <f t="shared" si="0"/>
-        <v>1.3632839506172842E-3</v>
-      </c>
-      <c r="S49" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" s="8" t="s">
+        <v>1.363093278463649E-3</v>
+      </c>
+      <c r="S52" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D50" s="2">
-        <f>AVERAGE(D41:D49)</f>
+      <c r="C53" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="2">
+        <f>AVERAGE(D44:D52)</f>
         <v>1178.7030733497943</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E53" s="2">
         <f t="shared" si="0"/>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F53" s="2">
         <f t="shared" si="0"/>
         <v>0.99203508916323713</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G53" s="2">
         <f t="shared" si="0"/>
         <v>306.71652987517137</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H53" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I50" s="2">
+      <c r="I53" s="2">
         <f t="shared" si="0"/>
         <v>7.1295036805555565</v>
       </c>
-      <c r="J50" s="2">
+      <c r="J53" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K50" s="2">
+      <c r="K53" s="2">
         <f t="shared" si="0"/>
         <v>698.76948392043903</v>
       </c>
-      <c r="L50" s="2">
+      <c r="L53" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M50" s="2">
+      <c r="M53" s="2">
         <f t="shared" si="0"/>
         <v>1437.5067307928668</v>
       </c>
-      <c r="N50" s="2">
+      <c r="N53" s="2">
         <f t="shared" si="0"/>
         <v>1181.53627690535</v>
       </c>
-      <c r="O50" s="3">
+      <c r="O53" s="3">
         <f t="shared" si="0"/>
         <v>4755.299898115225</v>
       </c>
-      <c r="P50" s="3">
+      <c r="P53" s="3">
         <f t="shared" si="0"/>
         <v>27227.338324888893</v>
       </c>
-      <c r="Q50" s="2">
+      <c r="Q53" s="2">
         <f t="shared" si="0"/>
         <v>4.684029058984911</v>
       </c>
-      <c r="R50" s="4">
-        <f t="shared" si="0"/>
-        <v>1.363093278463649E-3</v>
-      </c>
-      <c r="S50" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A51" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D51" s="2">
-        <v>1186.9773491111109</v>
-      </c>
-      <c r="E51" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F51" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G51" s="2">
-        <v>280.33542888888883</v>
-      </c>
-      <c r="H51" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I51" s="2">
-        <v>5.3870271111111121</v>
-      </c>
-      <c r="J51" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K51" s="2">
-        <v>645.93808322222219</v>
-      </c>
-      <c r="L51" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M51" s="2">
-        <v>1455.5792641111111</v>
-      </c>
-      <c r="N51" s="2">
-        <v>1191.1918266666667</v>
-      </c>
-      <c r="O51" s="3">
-        <v>4661.9885253333332</v>
-      </c>
-      <c r="P51" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q51" s="2">
-        <v>-0.64567288888888896</v>
-      </c>
-      <c r="R51" s="4">
+      <c r="R53" s="4">
         <v>-2.0755555555555555E-4</v>
-      </c>
-      <c r="S51" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A52" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1186.9773355555556</v>
-      </c>
-      <c r="E52" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F52" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G52" s="2">
-        <v>280.33542888888883</v>
-      </c>
-      <c r="H52" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I52" s="2">
-        <v>5.3870271111111121</v>
-      </c>
-      <c r="J52" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K52" s="2">
-        <v>645.93833411111109</v>
-      </c>
-      <c r="L52" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M52" s="2">
-        <v>1455.5790065555557</v>
-      </c>
-      <c r="N52" s="2">
-        <v>1191.1918131111113</v>
-      </c>
-      <c r="O52" s="3">
-        <v>4661.9885253333332</v>
-      </c>
-      <c r="P52" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q52" s="2">
-        <v>-0.64567966666666665</v>
-      </c>
-      <c r="R52" s="4">
-        <v>-2.0744444444444445E-4</v>
-      </c>
-      <c r="S52" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D53" s="2">
-        <v>1186.9773355555556</v>
-      </c>
-      <c r="E53" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F53" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G53" s="2">
-        <v>280.33542888888883</v>
-      </c>
-      <c r="H53" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I53" s="2">
-        <v>5.3870271111111121</v>
-      </c>
-      <c r="J53" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K53" s="2">
-        <v>645.9383002222221</v>
-      </c>
-      <c r="L53" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M53" s="2">
-        <v>1455.5790607777778</v>
-      </c>
-      <c r="N53" s="2">
-        <v>1191.1918131111113</v>
-      </c>
-      <c r="O53" s="3">
-        <v>4661.9885253333332</v>
-      </c>
-      <c r="P53" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q53" s="2">
-        <v>-0.64565933333333325</v>
-      </c>
-      <c r="R53" s="4">
-        <v>-2.0744444444444445E-4</v>
       </c>
       <c r="S53" s="8" t="s">
         <v>23</v>
@@ -4263,13 +4232,13 @@
         <v>16</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D54" s="2">
-        <v>1187.0067003333331</v>
+        <v>1186.9773491111109</v>
       </c>
       <c r="E54" s="2">
         <v>1901.5157334444443</v>
@@ -4290,16 +4259,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K54" s="2">
-        <v>645.93713388888887</v>
+        <v>645.93808322222219</v>
       </c>
       <c r="L54" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M54" s="2">
-        <v>1455.6553682222225</v>
+        <v>1455.5792641111111</v>
       </c>
       <c r="N54" s="2">
-        <v>1191.1764458888888</v>
+        <v>1191.1918266666667</v>
       </c>
       <c r="O54" s="3">
         <v>4661.9885253333332</v>
@@ -4308,27 +4277,27 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q54" s="2">
-        <v>-0.61525011111111105</v>
+        <v>-0.64567288888888896</v>
       </c>
       <c r="R54" s="4">
-        <v>-1.7433333333333333E-4</v>
+        <v>-2.0744444444444445E-4</v>
       </c>
       <c r="S54" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>16</v>
-      </c>
-      <c r="B55" t="s">
-        <v>65</v>
+      <c r="A55" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D55" s="2">
-        <v>1187.0063613333334</v>
+        <v>1186.9773355555556</v>
       </c>
       <c r="E55" s="2">
         <v>1901.5157334444443</v>
@@ -4343,51 +4312,51 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I55" s="2">
-        <v>5.3870315555555557</v>
+        <v>5.3870271111111121</v>
       </c>
       <c r="J55" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K55" s="2">
-        <v>645.93916833333344</v>
+        <v>645.93833411111109</v>
       </c>
       <c r="L55" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M55" s="2">
-        <v>1455.7051053333334</v>
+        <v>1455.5790065555557</v>
       </c>
       <c r="N55" s="2">
-        <v>1191.1759305555559</v>
+        <v>1191.1918131111113</v>
       </c>
       <c r="O55" s="3">
-        <v>4661.988498222222</v>
+        <v>4661.9885253333332</v>
       </c>
       <c r="P55" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q55" s="2">
-        <v>-0.56365988888888896</v>
+        <v>-0.64567966666666665</v>
       </c>
       <c r="R55" s="4">
-        <v>-1.5888888888888889E-4</v>
+        <v>-2.0744444444444445E-4</v>
       </c>
       <c r="S55" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>16</v>
-      </c>
-      <c r="B56" t="s">
-        <v>67</v>
+      <c r="A56" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D56" s="5">
-        <v>1208.5438095555555</v>
+      <c r="D56" s="2">
+        <v>1186.9773355555556</v>
       </c>
       <c r="E56" s="2">
         <v>1901.5157334444443</v>
@@ -4402,51 +4371,51 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I56" s="2">
-        <v>5.3172314444444444</v>
+        <v>5.3870271111111121</v>
       </c>
       <c r="J56" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K56" s="2">
-        <v>645.97183577777787</v>
+        <v>645.9383002222221</v>
       </c>
       <c r="L56" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M56" s="5">
-        <v>1460.2614338888889</v>
-      </c>
-      <c r="N56" s="5">
-        <v>1208.0519340000001</v>
+      <c r="M56" s="2">
+        <v>1455.5790607777778</v>
+      </c>
+      <c r="N56" s="2">
+        <v>1191.1918131111113</v>
       </c>
       <c r="O56" s="3">
-        <v>4662.6060926666669</v>
+        <v>4661.9885253333332</v>
       </c>
       <c r="P56" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q56" s="2">
-        <v>-0.5663084444444445</v>
+        <v>-0.64565933333333325</v>
       </c>
       <c r="R56" s="4">
-        <v>-1.5933333333333332E-4</v>
+        <v>-1.7433333333333333E-4</v>
       </c>
       <c r="S56" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>74</v>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A57" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D57" s="2">
-        <v>1207.0222438888889</v>
+        <v>1187.0067003333331</v>
       </c>
       <c r="E57" s="2">
         <v>1901.5157334444443</v>
@@ -4461,48 +4430,51 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I57" s="2">
-        <v>5.3316344444444441</v>
+        <v>5.3870271111111121</v>
       </c>
       <c r="J57" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K57" s="2">
-        <v>645.95907266666666</v>
+        <v>645.93713388888887</v>
       </c>
       <c r="L57" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M57" s="2">
-        <v>1460.4185112222222</v>
+        <v>1455.6553682222225</v>
       </c>
       <c r="N57" s="2">
-        <v>1206.2352837777776</v>
+        <v>1191.1764458888888</v>
       </c>
       <c r="O57" s="3">
-        <v>4662.5755209999998</v>
+        <v>4661.9885253333332</v>
       </c>
       <c r="P57" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q57" s="2">
-        <v>-0.73148200000000008</v>
+        <v>-0.61525011111111105</v>
       </c>
       <c r="R57" s="4">
-        <v>-2.0655555555555556E-4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+        <v>-1.5888888888888889E-4</v>
+      </c>
+      <c r="S57" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>75</v>
+      <c r="B58" t="s">
+        <v>65</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D58" s="2">
-        <v>1206.5233695555557</v>
+        <v>1187.0063613333334</v>
       </c>
       <c r="E58" s="2">
         <v>1901.5157334444443</v>
@@ -4517,34 +4489,37 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I58" s="2">
-        <v>5.3531247777777775</v>
+        <v>5.3870315555555557</v>
       </c>
       <c r="J58" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K58" s="2">
-        <v>645.94818811111122</v>
+        <v>645.93916833333344</v>
       </c>
       <c r="L58" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M58" s="2">
-        <v>1460.5092637777777</v>
+        <v>1455.7051053333334</v>
       </c>
       <c r="N58" s="2">
-        <v>1205.5020886666666</v>
+        <v>1191.1759305555559</v>
       </c>
       <c r="O58" s="3">
-        <v>4662.5708008888896</v>
+        <v>4661.988498222222</v>
       </c>
       <c r="P58" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q58" s="2">
-        <v>-0.90742522222222222</v>
+        <v>-0.56365988888888896</v>
       </c>
       <c r="R58" s="4">
-        <v>-2.5755555555555558E-4</v>
+        <v>-1.5933333333333332E-4</v>
+      </c>
+      <c r="S58" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.3">
@@ -4552,13 +4527,13 @@
         <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" t="s">
-        <v>23</v>
-      </c>
-      <c r="D59" s="2">
-        <v>1080.801350777778</v>
+        <v>67</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="5">
+        <v>1208.5438095555555</v>
       </c>
       <c r="E59" s="2">
         <v>1901.5157334444443</v>
@@ -4573,51 +4548,48 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I59" s="2">
-        <v>5.7424886666666666</v>
+        <v>5.3172314444444444</v>
       </c>
       <c r="J59" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K59" s="2">
-        <v>645.86557344444441</v>
+        <v>645.97183577777787</v>
       </c>
       <c r="L59" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M59" s="5">
-        <v>1430.3511555555554</v>
-      </c>
-      <c r="N59" s="2">
-        <v>1110.4303452222223</v>
+        <v>1460.2614338888889</v>
+      </c>
+      <c r="N59" s="5">
+        <v>1208.0519340000001</v>
       </c>
       <c r="O59" s="3">
-        <v>4638.5936415555561</v>
+        <v>4662.6060926666669</v>
       </c>
       <c r="P59" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q59" s="2">
-        <v>-0.8872363333333334</v>
+        <v>-0.5663084444444445</v>
       </c>
       <c r="R59" s="4">
-        <v>-2.5788888888888888E-4</v>
-      </c>
-      <c r="S59" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+        <v>-2.0655555555555556E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>16</v>
       </c>
-      <c r="B60" t="s">
-        <v>77</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B60" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D60" s="2">
-        <v>1080.801350777778</v>
+        <v>1207.0222438888889</v>
       </c>
       <c r="E60" s="2">
         <v>1901.5157334444443</v>
@@ -4632,57 +4604,54 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I60" s="2">
-        <v>5.7424886666666666</v>
+        <v>5.3316344444444441</v>
       </c>
       <c r="J60" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K60" s="2">
-        <v>645.86557344444441</v>
+        <v>645.95907266666666</v>
       </c>
       <c r="L60" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M60" s="2">
-        <v>1430.3511555555554</v>
+        <v>1460.4185112222222</v>
       </c>
       <c r="N60" s="2">
-        <v>1110.4303452222223</v>
+        <v>1206.2352837777776</v>
       </c>
       <c r="O60" s="3">
-        <v>4638.5936415555561</v>
+        <v>4662.5755209999998</v>
       </c>
       <c r="P60" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q60" s="2">
-        <v>-0.8872363333333334</v>
+        <v>-0.73148200000000008</v>
       </c>
       <c r="R60" s="4">
-        <v>-2.5788888888888888E-4</v>
-      </c>
-      <c r="S60" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+        <v>-2.5755555555555558E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>16</v>
       </c>
-      <c r="B61" t="s">
-        <v>79</v>
-      </c>
-      <c r="C61" t="s">
-        <v>23</v>
-      </c>
-      <c r="D61" s="5">
-        <v>897.84913466666671</v>
-      </c>
-      <c r="E61" s="5">
-        <v>1763.5263265555557</v>
+      <c r="B61" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1206.5233695555557</v>
+      </c>
+      <c r="E61" s="2">
+        <v>1901.5157334444443</v>
       </c>
       <c r="F61" s="2">
-        <v>1.0174076666666665</v>
+        <v>0.97970299999999988</v>
       </c>
       <c r="G61" s="2">
         <v>280.33542888888883</v>
@@ -4690,35 +4659,35 @@
       <c r="H61" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I61" s="5">
-        <v>7.299440555555555</v>
+      <c r="I61" s="2">
+        <v>5.3531247777777775</v>
       </c>
       <c r="J61" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K61" s="2">
-        <v>646.63056122222224</v>
-      </c>
-      <c r="L61" s="5">
-        <v>60.018756111111117</v>
-      </c>
-      <c r="M61" s="5">
-        <v>1342.5421007777777</v>
-      </c>
-      <c r="N61" s="5">
-        <v>902.73358833333339</v>
-      </c>
-      <c r="O61" s="6">
-        <v>5459.5160589999996</v>
+        <v>645.94818811111122</v>
+      </c>
+      <c r="L61" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M61" s="2">
+        <v>1460.5092637777777</v>
+      </c>
+      <c r="N61" s="2">
+        <v>1205.5020886666666</v>
+      </c>
+      <c r="O61" s="3">
+        <v>4662.5708008888896</v>
       </c>
       <c r="P61" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q61" s="2">
-        <v>0.26704155555555559</v>
+        <v>-0.90742522222222222</v>
       </c>
       <c r="R61" s="4">
-        <v>4.2666666666666656E-5</v>
+        <v>-2.5788888888888888E-4</v>
       </c>
       <c r="S61" t="s">
         <v>23</v>
@@ -4729,55 +4698,55 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C62" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="5">
-        <v>1000.3124864444443</v>
+      <c r="D62" s="2">
+        <v>1080.801350777778</v>
       </c>
       <c r="E62" s="2">
-        <v>1763.5263265555557</v>
+        <v>1901.5157334444443</v>
       </c>
       <c r="F62" s="2">
-        <v>0.999942</v>
-      </c>
-      <c r="G62" s="5">
-        <v>305.6782124444444</v>
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G62" s="2">
+        <v>280.33542888888883</v>
       </c>
       <c r="H62" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I62" s="2">
-        <v>6.8948233333333331</v>
+        <v>5.7424886666666666</v>
       </c>
       <c r="J62" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K62" s="5">
-        <v>673.17452677777771</v>
+      <c r="K62" s="2">
+        <v>645.86557344444441</v>
       </c>
       <c r="L62" s="2">
-        <v>60.018756111111117</v>
+        <v>83.47062044444445</v>
       </c>
       <c r="M62" s="5">
-        <v>1321.9402533333332</v>
-      </c>
-      <c r="N62" s="5">
-        <v>1024.1975572222223</v>
-      </c>
-      <c r="O62" s="6">
-        <v>4583.9874403333333</v>
+        <v>1430.3511555555554</v>
+      </c>
+      <c r="N62" s="2">
+        <v>1110.4303452222223</v>
+      </c>
+      <c r="O62" s="3">
+        <v>4638.5936415555561</v>
       </c>
       <c r="P62" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q62" s="2">
-        <v>0.28907633333333327</v>
+        <v>-0.8872363333333334</v>
       </c>
       <c r="R62" s="4">
-        <v>6.222222222222222E-5</v>
+        <v>-2.5788888888888888E-4</v>
       </c>
       <c r="S62" t="s">
         <v>23</v>
@@ -4788,55 +4757,55 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C63" t="s">
         <v>23</v>
       </c>
-      <c r="D63" s="13">
-        <v>1000.3124864444443</v>
-      </c>
-      <c r="E63" s="13">
-        <v>1763.5263265555557</v>
-      </c>
-      <c r="F63" s="13">
-        <v>0.999942</v>
-      </c>
-      <c r="G63" s="13">
-        <v>305.6782124444444</v>
-      </c>
-      <c r="H63" s="13">
+      <c r="D63" s="2">
+        <v>1080.801350777778</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F63" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G63" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H63" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I63" s="13">
-        <v>6.8948233333333331</v>
-      </c>
-      <c r="J63" s="13">
+      <c r="I63" s="2">
+        <v>5.7424886666666666</v>
+      </c>
+      <c r="J63" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K63" s="13">
-        <v>673.17452677777771</v>
-      </c>
-      <c r="L63" s="13">
-        <v>60.018756111111117</v>
-      </c>
-      <c r="M63" s="13">
-        <v>1321.9402533333332</v>
-      </c>
-      <c r="N63" s="13">
-        <v>1024.1975572222223</v>
-      </c>
-      <c r="O63" s="14">
-        <v>4583.9874403333333</v>
-      </c>
-      <c r="P63" s="14">
+      <c r="K63" s="2">
+        <v>645.86557344444441</v>
+      </c>
+      <c r="L63" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M63" s="2">
+        <v>1430.3511555555554</v>
+      </c>
+      <c r="N63" s="2">
+        <v>1110.4303452222223</v>
+      </c>
+      <c r="O63" s="3">
+        <v>4638.5936415555561</v>
+      </c>
+      <c r="P63" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q63" s="13">
-        <v>0.28907633333333327</v>
-      </c>
-      <c r="R63" s="15">
-        <v>6.222222222222222E-5</v>
+      <c r="Q63" s="2">
+        <v>-0.8872363333333334</v>
+      </c>
+      <c r="R63" s="4">
+        <v>4.2666666666666656E-5</v>
       </c>
       <c r="S63" t="s">
         <v>23</v>
@@ -4847,55 +4816,55 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C64" t="s">
         <v>23</v>
       </c>
       <c r="D64" s="5">
-        <v>1070.3662515555557</v>
-      </c>
-      <c r="E64" s="2">
+        <v>897.84913466666671</v>
+      </c>
+      <c r="E64" s="5">
         <v>1763.5263265555557</v>
       </c>
       <c r="F64" s="2">
-        <v>0.999942</v>
+        <v>1.0174076666666665</v>
       </c>
       <c r="G64" s="2">
-        <v>305.6782124444444</v>
+        <v>280.33542888888883</v>
       </c>
       <c r="H64" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I64" s="2">
-        <v>6.8224234444444436</v>
+      <c r="I64" s="5">
+        <v>7.299440555555555</v>
       </c>
       <c r="J64" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K64" s="2">
-        <v>672.51038266666671</v>
-      </c>
-      <c r="L64" s="2">
+        <v>646.63056122222224</v>
+      </c>
+      <c r="L64" s="5">
         <v>60.018756111111117</v>
       </c>
       <c r="M64" s="5">
-        <v>1335.0520562222218</v>
+        <v>1342.5421007777777</v>
       </c>
       <c r="N64" s="5">
-        <v>1081.7151217777778</v>
-      </c>
-      <c r="O64" s="3">
-        <v>4576.182644333333</v>
+        <v>902.73358833333339</v>
+      </c>
+      <c r="O64" s="6">
+        <v>5459.5160589999996</v>
       </c>
       <c r="P64" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q64" s="2">
-        <v>0.27293466666666671</v>
+        <v>0.26704155555555559</v>
       </c>
       <c r="R64" s="4">
-        <v>5.7555555555555559E-5</v>
+        <v>6.222222222222222E-5</v>
       </c>
       <c r="S64" t="s">
         <v>23</v>
@@ -4906,55 +4875,55 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C65" t="s">
         <v>23</v>
       </c>
       <c r="D65" s="5">
-        <v>1246.3303018888889</v>
-      </c>
-      <c r="E65" s="5">
-        <v>1890.2624783333331</v>
+        <v>1000.3124864444443</v>
+      </c>
+      <c r="E65" s="2">
+        <v>1763.5263265555557</v>
       </c>
       <c r="F65" s="2">
-        <v>0.94846033333333346</v>
-      </c>
-      <c r="G65" s="2">
+        <v>0.999942</v>
+      </c>
+      <c r="G65" s="5">
         <v>305.6782124444444</v>
       </c>
       <c r="H65" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I65" s="5">
-        <v>6.3587768888888885</v>
+      <c r="I65" s="2">
+        <v>6.8948233333333331</v>
       </c>
       <c r="J65" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K65" s="5">
-        <v>628.90788111111101</v>
-      </c>
-      <c r="L65" s="5">
-        <v>82.308506444444433</v>
+        <v>673.17452677777771</v>
+      </c>
+      <c r="L65" s="2">
+        <v>60.018756111111117</v>
       </c>
       <c r="M65" s="5">
-        <v>1456.3722873333334</v>
+        <v>1321.9402533333332</v>
       </c>
       <c r="N65" s="5">
-        <v>1283.7495253333334</v>
+        <v>1024.1975572222223</v>
       </c>
       <c r="O65" s="6">
-        <v>3986.0738390000001</v>
+        <v>4583.9874403333333</v>
       </c>
       <c r="P65" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q65" s="2">
-        <v>0.12974411111111114</v>
-      </c>
-      <c r="R65" s="4">
-        <v>2.3444444444444448E-5</v>
+        <v>0.28907633333333327</v>
+      </c>
+      <c r="R65" s="15">
+        <v>6.222222222222222E-5</v>
       </c>
       <c r="S65" t="s">
         <v>23</v>
@@ -4965,55 +4934,55 @@
         <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="5">
-        <v>1380.5085448888888</v>
-      </c>
-      <c r="E66" s="2">
-        <v>1890.2624783333331</v>
-      </c>
-      <c r="F66" s="2">
-        <v>0.94846033333333346</v>
-      </c>
-      <c r="G66" s="2">
+      <c r="D66" s="13">
+        <v>1000.3124864444443</v>
+      </c>
+      <c r="E66" s="13">
+        <v>1763.5263265555557</v>
+      </c>
+      <c r="F66" s="13">
+        <v>0.999942</v>
+      </c>
+      <c r="G66" s="13">
         <v>305.6782124444444</v>
       </c>
-      <c r="H66" s="2">
+      <c r="H66" s="13">
         <v>9.775355222222224</v>
       </c>
-      <c r="I66" s="2">
-        <v>6.1288343333333337</v>
-      </c>
-      <c r="J66" s="2">
+      <c r="I66" s="13">
+        <v>6.8948233333333331</v>
+      </c>
+      <c r="J66" s="13">
         <v>8.145128999999999</v>
       </c>
-      <c r="K66" s="2">
-        <v>628.9703199999999</v>
-      </c>
-      <c r="L66" s="2">
-        <v>82.308506444444433</v>
-      </c>
-      <c r="M66" s="5">
-        <v>1487.9843207777781</v>
-      </c>
-      <c r="N66" s="5">
-        <v>1386.0215385555557</v>
-      </c>
-      <c r="O66" s="6">
-        <v>4013.3543294444444</v>
-      </c>
-      <c r="P66" s="3">
+      <c r="K66" s="13">
+        <v>673.17452677777771</v>
+      </c>
+      <c r="L66" s="13">
+        <v>60.018756111111117</v>
+      </c>
+      <c r="M66" s="13">
+        <v>1321.9402533333332</v>
+      </c>
+      <c r="N66" s="13">
+        <v>1024.1975572222223</v>
+      </c>
+      <c r="O66" s="14">
+        <v>4583.9874403333333</v>
+      </c>
+      <c r="P66" s="14">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q66" s="2">
-        <v>0.12792911111111113</v>
+      <c r="Q66" s="13">
+        <v>0.28907633333333327</v>
       </c>
       <c r="R66" s="4">
-        <v>2.1888888888888887E-5</v>
+        <v>5.7555555555555559E-5</v>
       </c>
       <c r="S66" t="s">
         <v>23</v>
@@ -5024,58 +4993,229 @@
         <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C67" t="s">
         <v>23</v>
       </c>
-      <c r="D67" s="2">
-        <v>1242.9115804444446</v>
+      <c r="D67" s="5">
+        <v>1070.3662515555557</v>
       </c>
       <c r="E67" s="2">
-        <v>1890.2624783333331</v>
+        <v>1763.5263265555557</v>
       </c>
       <c r="F67" s="2">
-        <v>1.059004111111111</v>
+        <v>0.999942</v>
       </c>
       <c r="G67" s="2">
-        <v>299.96642388888887</v>
+        <v>305.6782124444444</v>
       </c>
       <c r="H67" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I67" s="2">
-        <v>5.6808013333333331</v>
+        <v>6.8224234444444436</v>
       </c>
       <c r="J67" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K67" s="5">
-        <v>676.49806711111114</v>
+      <c r="K67" s="2">
+        <v>672.51038266666671</v>
       </c>
       <c r="L67" s="2">
-        <v>82.308506444444433</v>
-      </c>
-      <c r="M67" s="2">
-        <v>1459.1644423333332</v>
-      </c>
-      <c r="N67" s="2">
-        <v>1223.6673176666666</v>
-      </c>
-      <c r="O67" s="6">
-        <v>5486.7290039999998</v>
+        <v>60.018756111111117</v>
+      </c>
+      <c r="M67" s="5">
+        <v>1335.0520562222218</v>
+      </c>
+      <c r="N67" s="5">
+        <v>1081.7151217777778</v>
+      </c>
+      <c r="O67" s="3">
+        <v>4576.182644333333</v>
       </c>
       <c r="P67" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q67" s="2">
+        <v>0.27293466666666671</v>
+      </c>
+      <c r="R67" s="4">
+        <v>2.3444444444444448E-5</v>
+      </c>
+      <c r="S67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" t="s">
+        <v>23</v>
+      </c>
+      <c r="D68" s="5">
+        <v>1246.3303018888889</v>
+      </c>
+      <c r="E68" s="5">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F68" s="2">
+        <v>0.94846033333333346</v>
+      </c>
+      <c r="G68" s="2">
+        <v>305.6782124444444</v>
+      </c>
+      <c r="H68" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I68" s="5">
+        <v>6.3587768888888885</v>
+      </c>
+      <c r="J68" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K68" s="5">
+        <v>628.90788111111101</v>
+      </c>
+      <c r="L68" s="5">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M68" s="5">
+        <v>1456.3722873333334</v>
+      </c>
+      <c r="N68" s="5">
+        <v>1283.7495253333334</v>
+      </c>
+      <c r="O68" s="6">
+        <v>3986.0738390000001</v>
+      </c>
+      <c r="P68" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q68" s="2">
+        <v>0.12974411111111114</v>
+      </c>
+      <c r="R68" s="4">
+        <v>2.1888888888888887E-5</v>
+      </c>
+      <c r="S68" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="5">
+        <v>1380.5085448888888</v>
+      </c>
+      <c r="E69" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F69" s="2">
+        <v>0.94846033333333346</v>
+      </c>
+      <c r="G69" s="2">
+        <v>305.6782124444444</v>
+      </c>
+      <c r="H69" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I69" s="2">
+        <v>6.1288343333333337</v>
+      </c>
+      <c r="J69" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K69" s="2">
+        <v>628.9703199999999</v>
+      </c>
+      <c r="L69" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M69" s="5">
+        <v>1487.9843207777781</v>
+      </c>
+      <c r="N69" s="5">
+        <v>1386.0215385555557</v>
+      </c>
+      <c r="O69" s="6">
+        <v>4013.3543294444444</v>
+      </c>
+      <c r="P69" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q69" s="2">
+        <v>0.12792911111111113</v>
+      </c>
+      <c r="R69" s="4">
+        <v>1.4777777777777775E-5</v>
+      </c>
+      <c r="S69" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" t="s">
+        <v>87</v>
+      </c>
+      <c r="C70" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1242.9115804444446</v>
+      </c>
+      <c r="E70" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F70" s="2">
+        <v>1.059004111111111</v>
+      </c>
+      <c r="G70" s="2">
+        <v>299.96642388888887</v>
+      </c>
+      <c r="H70" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I70" s="2">
+        <v>5.6808013333333331</v>
+      </c>
+      <c r="J70" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K70" s="5">
+        <v>676.49806711111114</v>
+      </c>
+      <c r="L70" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M70" s="2">
+        <v>1459.1644423333332</v>
+      </c>
+      <c r="N70" s="2">
+        <v>1223.6673176666666</v>
+      </c>
+      <c r="O70" s="6">
+        <v>5486.7290039999998</v>
+      </c>
+      <c r="P70" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q70" s="2">
         <v>0.12781966666666669</v>
-      </c>
-      <c r="R67" s="4">
-        <v>1.4777777777777775E-5</v>
-      </c>
-      <c r="S67" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add reservoir evaporation to the mass balance in the AltWM Quick Check report. Flow.cpp, .h - Add FlowModel::m_totEvapFromReservoirsYr_m3, and store into it in Reservoir::GetResOutflowWP(). WaterRights.cpp - Include reservoir evap in the calculation of AET for the Quick Check report.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E56C982-32CE-4E4A-9937-BF0DBFA543DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FE337F-6BBB-40A4-9D0A-CD8FB746B243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="95">
   <si>
     <t>Year</t>
   </si>
@@ -305,6 +305,18 @@
   </si>
   <si>
     <t>Demo_Baseline_2010_C208</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18 C224+</t>
+  </si>
+  <si>
+    <t>2010-19</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-19 C225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demo_Baseline 2010-19 C225 </t>
   </si>
 </sst>
 </file>
@@ -803,7 +815,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -829,6 +841,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1186,11 +1201,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U70"/>
+  <dimension ref="A1:U78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3354,145 +3369,139 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="2"/>
+    <row r="38" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="8">
+        <v>2010</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1.443354</v>
+      </c>
+      <c r="G38" s="2">
+        <v>298.59677099999999</v>
+      </c>
+      <c r="H38" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I38" s="2">
+        <v>4.7859109999999996</v>
+      </c>
+      <c r="J38" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K38" s="2">
+        <v>735.242615</v>
+      </c>
+      <c r="L38" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="M38" s="2">
+        <v>1400.0203859999999</v>
+      </c>
+      <c r="N38" s="2">
+        <v>1351.616943</v>
+      </c>
+      <c r="O38" s="3">
+        <v>8159.8198240000002</v>
+      </c>
+      <c r="P38" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>-0.971356</v>
+      </c>
       <c r="R38" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" t="s">
-        <v>23</v>
+        <v>-2.7099999999999997E-4</v>
+      </c>
+      <c r="S38" s="8">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="17">
+        <v>44202</v>
       </c>
       <c r="D39" s="2">
-        <v>1138.6194117777777</v>
+        <v>1284.0238039999999</v>
       </c>
       <c r="E39" s="2">
-        <v>1901.5157334444443</v>
+        <v>1990.4650879999999</v>
       </c>
       <c r="F39" s="2">
-        <v>1.0119255555555557</v>
+        <v>1.443354</v>
       </c>
       <c r="G39" s="2">
-        <v>327.78053433333326</v>
+        <v>298.59677099999999</v>
       </c>
       <c r="H39" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I39" s="2"/>
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I39" s="2">
+        <v>4.7859109999999996</v>
+      </c>
       <c r="J39" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K39" s="2">
-        <v>769.26639155555551</v>
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K39" s="5">
+        <v>737.4375</v>
       </c>
       <c r="L39" s="2">
-        <v>83.47062044444445</v>
+        <v>93.234084999999993</v>
       </c>
       <c r="M39" s="2">
-        <v>1374.8233372222221</v>
+        <v>1400.0203859999999</v>
       </c>
       <c r="N39" s="2">
-        <v>1142.9502087777778</v>
+        <v>1351.616943</v>
       </c>
       <c r="O39" s="3">
-        <v>4918.1879612222219</v>
+        <v>8159.8198240000002</v>
       </c>
       <c r="P39" s="3">
-        <v>27227.338324777778</v>
-      </c>
-      <c r="Q39" s="2">
-        <v>-4.72741111111111E-2</v>
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>1.22353</v>
       </c>
       <c r="R39" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
-      <c r="S39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="2">
-        <v>1138.6194117777777</v>
-      </c>
-      <c r="E40" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F40" s="2">
-        <v>1.0119255555555557</v>
-      </c>
-      <c r="G40" s="2">
-        <v>327.78053433333326</v>
-      </c>
-      <c r="H40" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K40" s="2">
-        <v>769.26639155555551</v>
-      </c>
-      <c r="L40" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M40" s="2">
-        <v>1374.8233372222221</v>
-      </c>
-      <c r="N40" s="2">
-        <v>1142.9502087777778</v>
-      </c>
-      <c r="O40" s="3">
-        <v>4918.1879612222219</v>
-      </c>
-      <c r="P40" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q40" s="2">
-        <v>-4.72741111111111E-2</v>
-      </c>
-      <c r="R40" s="4">
-        <v>-3.8888888888888877E-5</v>
-      </c>
+        <v>3.4099999999999999E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="16"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="15"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
@@ -3532,13 +3541,13 @@
         <v>4918.1879612222219</v>
       </c>
       <c r="P41" s="3">
-        <v>27227.338324888889</v>
+        <v>27227.338324777778</v>
       </c>
       <c r="Q41" s="2">
         <v>-4.72741111111111E-2</v>
       </c>
       <c r="R41" s="4">
-        <v>1.4151111111111109E-3</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
       <c r="S41" t="s">
         <v>23</v>
@@ -3549,13 +3558,13 @@
         <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="2">
-        <v>1135.8478461111113</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E42" s="2">
         <v>1901.5157334444443</v>
@@ -3574,28 +3583,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K42" s="2">
-        <v>769.26112866666654</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L42" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M42" s="2">
-        <v>1378.3211942222222</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N42" s="2">
-        <v>1141.5044894444445</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O42" s="3">
-        <v>4878.4023980000002</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P42" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q42" s="2">
-        <v>4.7711666666666668</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R42" s="4">
-        <v>1.3650000000000001E-3</v>
+        <v>-3.8888888888888877E-5</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
@@ -3603,13 +3612,13 @@
         <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
       </c>
       <c r="D43" s="2">
-        <v>1161.1572335555554</v>
+        <v>1138.6194117777777</v>
       </c>
       <c r="E43" s="2">
         <v>1901.5157334444443</v>
@@ -3628,28 +3637,28 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K43" s="2">
-        <v>769.37008311111106</v>
+        <v>769.26639155555551</v>
       </c>
       <c r="L43" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M43" s="2">
-        <v>1383.6045464444442</v>
+        <v>1374.8233372222221</v>
       </c>
       <c r="N43" s="2">
-        <v>1161.284607111111</v>
+        <v>1142.9502087777778</v>
       </c>
       <c r="O43" s="3">
-        <v>4883.9277073333324</v>
+        <v>4918.1879612222219</v>
       </c>
       <c r="P43" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q43" s="2">
-        <v>4.6342037777777776</v>
+        <v>-4.72741111111111E-2</v>
       </c>
       <c r="R43" s="4">
-        <v>7.9151111111111106E-3</v>
+        <v>1.4151111111111109E-3</v>
       </c>
       <c r="S43" t="s">
         <v>23</v>
@@ -3660,13 +3669,13 @@
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="2">
-        <v>1161.1644491111113</v>
+        <v>1135.8478461111113</v>
       </c>
       <c r="E44" s="2">
         <v>1901.5157334444443</v>
@@ -3675,43 +3684,38 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G44" s="2">
-        <v>354.15221155555554</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H44" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I44" s="2">
-        <v>4.6817598888888901</v>
-      </c>
+      <c r="I44" s="2"/>
       <c r="J44" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K44" s="2">
-        <v>769.36972377777772</v>
+        <v>769.26112866666654</v>
       </c>
       <c r="L44" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M44" s="2">
-        <v>1437.0445828888887</v>
+        <v>1378.3211942222222</v>
       </c>
       <c r="N44" s="2">
-        <v>1161.2873196666667</v>
+        <v>1141.5044894444445</v>
       </c>
       <c r="O44" s="3">
-        <v>4883.9277073333324</v>
+        <v>4878.4023980000002</v>
       </c>
       <c r="P44" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q44" s="2">
-        <v>27.015940777777772</v>
+        <v>4.7711666666666668</v>
       </c>
       <c r="R44" s="4">
-        <v>2.9230000000000003E-3</v>
-      </c>
-      <c r="S44" t="s">
-        <v>23</v>
+        <v>1.3650000000000001E-3</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
@@ -3719,13 +3723,13 @@
         <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1572335555554</v>
       </c>
       <c r="E45" s="2">
         <v>1901.5157334444443</v>
@@ -3734,28 +3738,26 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G45" s="2">
-        <v>337.20870333333335</v>
+        <v>327.78053433333326</v>
       </c>
       <c r="H45" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I45" s="2">
-        <v>4.6813607777777788</v>
-      </c>
+      <c r="I45" s="2"/>
       <c r="J45" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K45" s="2">
-        <v>769.36992711111111</v>
+        <v>769.37008311111106</v>
       </c>
       <c r="L45" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M45" s="2">
-        <v>1403.060424888889</v>
+        <v>1383.6045464444442</v>
       </c>
       <c r="N45" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.284607111111</v>
       </c>
       <c r="O45" s="3">
         <v>4883.9277073333324</v>
@@ -3764,10 +3766,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q45" s="2">
-        <v>9.9787694444444455</v>
+        <v>4.6342037777777776</v>
       </c>
       <c r="R45" s="4">
-        <v>-3.7111111111111107E-5</v>
+        <v>7.9151111111111106E-3</v>
       </c>
       <c r="S45" t="s">
         <v>23</v>
@@ -3778,13 +3780,13 @@
         <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="2">
-        <v>1161.1599054444443</v>
+        <v>1161.1644491111113</v>
       </c>
       <c r="E46" s="2">
         <v>1901.5157334444443</v>
@@ -3793,28 +3795,28 @@
         <v>1.0119255555555557</v>
       </c>
       <c r="G46" s="2">
-        <v>347.23312744444445</v>
+        <v>354.15221155555554</v>
       </c>
       <c r="H46" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I46" s="2">
-        <v>4.6813607777777788</v>
+        <v>4.6817598888888901</v>
       </c>
       <c r="J46" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K46" s="2">
-        <v>769.36992711111111</v>
+        <v>769.36972377777772</v>
       </c>
       <c r="L46" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M46" s="2">
-        <v>1403.060424888889</v>
+        <v>1437.0445828888887</v>
       </c>
       <c r="N46" s="2">
-        <v>1161.2856514444443</v>
+        <v>1161.2873196666667</v>
       </c>
       <c r="O46" s="3">
         <v>4883.9277073333324</v>
@@ -3823,10 +3825,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q46" s="2">
-        <v>-4.5654777777777787E-2</v>
-      </c>
-      <c r="R46" s="7">
-        <v>5.926666666666668E-4</v>
+        <v>27.015940777777772</v>
+      </c>
+      <c r="R46" s="4">
+        <v>2.9230000000000003E-3</v>
       </c>
       <c r="S46" t="s">
         <v>23</v>
@@ -3837,55 +3839,55 @@
         <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="2">
-        <v>1200.1875406666668</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E47" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F47" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G47" s="5">
-        <v>291.69008066666663</v>
+        <v>1.0119255555555557</v>
+      </c>
+      <c r="G47" s="2">
+        <v>337.20870333333335</v>
       </c>
       <c r="H47" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I47" s="5">
-        <v>13.853347222222222</v>
+      <c r="I47" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J47" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K47" s="5">
-        <v>691.23065866666673</v>
+      <c r="K47" s="2">
+        <v>769.36992711111111</v>
       </c>
       <c r="L47" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M47" s="5">
-        <v>1431.1979711111112</v>
-      </c>
-      <c r="N47" s="5">
-        <v>1206.0454778888889</v>
-      </c>
-      <c r="O47" s="6">
-        <v>4695.8937716666669</v>
+      <c r="M47" s="2">
+        <v>1403.060424888889</v>
+      </c>
+      <c r="N47" s="2">
+        <v>1161.2856514444443</v>
+      </c>
+      <c r="O47" s="3">
+        <v>4883.9277073333324</v>
       </c>
       <c r="P47" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q47" s="5">
-        <v>2.0880971111111108</v>
+      <c r="Q47" s="2">
+        <v>9.9787694444444455</v>
       </c>
       <c r="R47" s="4">
-        <v>3.9399999999999998E-4</v>
+        <v>-3.7111111111111107E-5</v>
       </c>
       <c r="S47" t="s">
         <v>23</v>
@@ -3896,72 +3898,72 @@
         <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
         <v>23</v>
       </c>
       <c r="D48" s="2">
-        <v>1186.9521077777779</v>
+        <v>1161.1599054444443</v>
       </c>
       <c r="E48" s="2">
         <v>1901.5157334444443</v>
       </c>
       <c r="F48" s="2">
-        <v>0.97970299999999988</v>
+        <v>1.0119255555555557</v>
       </c>
       <c r="G48" s="2">
-        <v>280.33542888888883</v>
+        <v>347.23312744444445</v>
       </c>
       <c r="H48" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I48" s="5">
-        <v>12.968491888888888</v>
+      <c r="I48" s="2">
+        <v>4.6813607777777788</v>
       </c>
       <c r="J48" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K48" s="2">
-        <v>645.94098588888892</v>
+        <v>769.36992711111111</v>
       </c>
       <c r="L48" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M48" s="2">
-        <v>1465.1962754444444</v>
+        <v>1403.060424888889</v>
       </c>
       <c r="N48" s="2">
-        <v>1191.1222331111112</v>
+        <v>1161.2856514444443</v>
       </c>
       <c r="O48" s="3">
-        <v>4695.8937716666669</v>
+        <v>4883.9277073333324</v>
       </c>
       <c r="P48" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q48" s="2">
-        <v>1.3484236666666667</v>
-      </c>
-      <c r="R48" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S48" s="8" t="s">
+        <v>-4.5654777777777787E-2</v>
+      </c>
+      <c r="R48" s="7">
+        <v>5.926666666666668E-4</v>
+      </c>
+      <c r="S48" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A49" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="8" t="s">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" t="s">
         <v>23</v>
       </c>
       <c r="D49" s="2">
-        <v>1186.9497747777777</v>
+        <v>1200.1875406666668</v>
       </c>
       <c r="E49" s="2">
         <v>1901.5157334444443</v>
@@ -3969,58 +3971,58 @@
       <c r="F49" s="2">
         <v>0.97970299999999988</v>
       </c>
-      <c r="G49" s="2">
-        <v>280.33542888888883</v>
+      <c r="G49" s="5">
+        <v>291.69008066666663</v>
       </c>
       <c r="H49" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I49" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I49" s="5">
+        <v>13.853347222222222</v>
       </c>
       <c r="J49" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K49" s="2">
-        <v>645.93823922222225</v>
+      <c r="K49" s="5">
+        <v>691.23065866666673</v>
       </c>
       <c r="L49" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M49" s="2">
-        <v>1455.3145886666666</v>
-      </c>
-      <c r="N49" s="2">
-        <v>1191.1280516666666</v>
-      </c>
-      <c r="O49" s="3">
-        <v>4661.9885795555556</v>
+      <c r="M49" s="5">
+        <v>1431.1979711111112</v>
+      </c>
+      <c r="N49" s="5">
+        <v>1206.0454778888889</v>
+      </c>
+      <c r="O49" s="6">
+        <v>4695.8937716666669</v>
       </c>
       <c r="P49" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q49" s="2">
-        <v>-0.95070599999999983</v>
+      <c r="Q49" s="5">
+        <v>2.0880971111111108</v>
       </c>
       <c r="R49" s="4">
-        <v>-2.8933333333333328E-4</v>
-      </c>
-      <c r="S49" s="8" t="s">
+        <v>3.9399999999999998E-4</v>
+      </c>
+      <c r="S49" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" s="8" t="s">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" t="s">
         <v>23</v>
       </c>
       <c r="D50" s="2">
-        <v>1186.9497747777777</v>
+        <v>1186.9521077777779</v>
       </c>
       <c r="E50" s="2">
         <v>1901.5157334444443</v>
@@ -4034,35 +4036,35 @@
       <c r="H50" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I50" s="2">
-        <v>5.3913398888888899</v>
+      <c r="I50" s="5">
+        <v>12.968491888888888</v>
       </c>
       <c r="J50" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K50" s="2">
-        <v>645.93823922222225</v>
+        <v>645.94098588888892</v>
       </c>
       <c r="L50" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M50" s="2">
-        <v>1455.3145886666666</v>
+        <v>1465.1962754444444</v>
       </c>
       <c r="N50" s="2">
-        <v>1191.1280516666666</v>
+        <v>1191.1222331111112</v>
       </c>
       <c r="O50" s="3">
-        <v>4661.9885795555556</v>
+        <v>4695.8937716666669</v>
       </c>
       <c r="P50" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q50" s="2">
-        <v>-0.95070599999999983</v>
+        <v>1.3484236666666667</v>
       </c>
       <c r="R50" s="4">
-        <v>-3.0444444444444448E-4</v>
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S50" s="8" t="s">
         <v>23</v>
@@ -4073,13 +4075,13 @@
         <v>16</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D51" s="2">
-        <v>1186.8557127777776</v>
+        <v>1186.9497747777777</v>
       </c>
       <c r="E51" s="2">
         <v>1901.5157334444443</v>
@@ -4094,22 +4096,22 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I51" s="2">
-        <v>5.3870291111111106</v>
+        <v>5.3913398888888899</v>
       </c>
       <c r="J51" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K51" s="2">
-        <v>645.93811044444442</v>
+        <v>645.93823922222225</v>
       </c>
       <c r="L51" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M51" s="2">
-        <v>1455.2552082222223</v>
+        <v>1455.3145886666666</v>
       </c>
       <c r="N51" s="2">
-        <v>1191.0329453333334</v>
+        <v>1191.1280516666666</v>
       </c>
       <c r="O51" s="3">
         <v>4661.9885795555556</v>
@@ -4118,11 +4120,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q51" s="2">
-        <v>-1.0069492222222223</v>
-      </c>
-      <c r="R51" s="7">
-        <f t="shared" ref="E51:R53" si="0">AVERAGE(R42:R50)</f>
-        <v>1.3632839506172842E-3</v>
+        <v>-0.95070599999999983</v>
+      </c>
+      <c r="R51" s="4">
+        <v>-2.8933333333333328E-4</v>
       </c>
       <c r="S51" s="8" t="s">
         <v>23</v>
@@ -4133,261 +4134,262 @@
         <v>16</v>
       </c>
       <c r="B52" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1186.9497747777777</v>
+      </c>
+      <c r="E52" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G52" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H52" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I52" s="2">
+        <v>5.3913398888888899</v>
+      </c>
+      <c r="J52" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K52" s="2">
+        <v>645.93823922222225</v>
+      </c>
+      <c r="L52" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M52" s="2">
+        <v>1455.3145886666666</v>
+      </c>
+      <c r="N52" s="2">
+        <v>1191.1280516666666</v>
+      </c>
+      <c r="O52" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P52" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q52" s="2">
+        <v>-0.95070599999999983</v>
+      </c>
+      <c r="R52" s="4">
+        <v>-3.0444444444444448E-4</v>
+      </c>
+      <c r="S52" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1186.8557127777776</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1901.5157334444443</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G53" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H53" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I53" s="2">
+        <v>5.3870291111111106</v>
+      </c>
+      <c r="J53" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K53" s="2">
+        <v>645.93811044444442</v>
+      </c>
+      <c r="L53" s="2">
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M53" s="2">
+        <v>1455.2552082222223</v>
+      </c>
+      <c r="N53" s="2">
+        <v>1191.0329453333334</v>
+      </c>
+      <c r="O53" s="3">
+        <v>4661.9885795555556</v>
+      </c>
+      <c r="P53" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q53" s="2">
+        <v>-1.0069492222222223</v>
+      </c>
+      <c r="R53" s="7">
+        <f t="shared" ref="E53:R55" si="0">AVERAGE(R44:R52)</f>
+        <v>1.3632839506172842E-3</v>
+      </c>
+      <c r="S53" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D52" s="2">
-        <f>AVERAGE(D43:D51)</f>
+      <c r="C54" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="2">
+        <f>AVERAGE(D45:D53)</f>
         <v>1176.9484893703707</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E54" s="2">
         <f t="shared" si="0"/>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F54" s="2">
         <f t="shared" si="0"/>
         <v>0.99402413580246907</v>
       </c>
-      <c r="G52" s="5">
+      <c r="G54" s="5">
         <f t="shared" si="0"/>
         <v>308.82293032098761</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H54" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I52" s="5">
+      <c r="I54" s="5">
         <f t="shared" si="0"/>
         <v>7.1295036805555574</v>
       </c>
-      <c r="J52" s="2">
+      <c r="J54" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K52" s="5">
+      <c r="K54" s="5">
         <f t="shared" si="0"/>
         <v>705.82954383950619</v>
       </c>
-      <c r="L52" s="2">
+      <c r="L54" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M52" s="5">
+      <c r="M54" s="5">
         <f t="shared" si="0"/>
         <v>1432.1165123580245</v>
       </c>
-      <c r="N52" s="2">
+      <c r="N54" s="2">
         <f t="shared" si="0"/>
         <v>1179.5111099259257</v>
       </c>
-      <c r="O52" s="6">
+      <c r="O54" s="6">
         <f t="shared" si="0"/>
         <v>4768.1626790370356</v>
       </c>
-      <c r="P52" s="3">
+      <c r="P54" s="3">
         <f t="shared" si="0"/>
         <v>27227.338324888893</v>
       </c>
-      <c r="Q52" s="2">
+      <c r="Q54" s="2">
         <f t="shared" si="0"/>
         <v>4.6790465308641975</v>
       </c>
-      <c r="R52" s="4">
+      <c r="R54" s="4">
         <f t="shared" si="0"/>
         <v>1.363093278463649E-3</v>
       </c>
-      <c r="S52" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B53" s="8" t="s">
+      <c r="S54" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D53" s="2">
-        <f>AVERAGE(D44:D52)</f>
+      <c r="C55" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="2">
+        <f>AVERAGE(D46:D54)</f>
         <v>1178.7030733497943</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E55" s="2">
         <f t="shared" si="0"/>
         <v>1901.5157334444443</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F55" s="2">
         <f t="shared" si="0"/>
         <v>0.99203508916323713</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G55" s="2">
         <f t="shared" si="0"/>
         <v>306.71652987517137</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H55" s="2">
         <f t="shared" si="0"/>
         <v>9.775355222222224</v>
       </c>
-      <c r="I53" s="2">
+      <c r="I55" s="2">
         <f t="shared" si="0"/>
         <v>7.1295036805555565</v>
       </c>
-      <c r="J53" s="2">
+      <c r="J55" s="2">
         <f t="shared" si="0"/>
         <v>8.145128999999999</v>
       </c>
-      <c r="K53" s="2">
+      <c r="K55" s="2">
         <f t="shared" si="0"/>
         <v>698.76948392043903</v>
       </c>
-      <c r="L53" s="2">
+      <c r="L55" s="2">
         <f t="shared" si="0"/>
         <v>83.470620444444435</v>
       </c>
-      <c r="M53" s="2">
+      <c r="M55" s="2">
         <f t="shared" si="0"/>
         <v>1437.5067307928668</v>
       </c>
-      <c r="N53" s="2">
+      <c r="N55" s="2">
         <f t="shared" si="0"/>
         <v>1181.53627690535</v>
       </c>
-      <c r="O53" s="3">
+      <c r="O55" s="3">
         <f t="shared" si="0"/>
         <v>4755.299898115225</v>
       </c>
-      <c r="P53" s="3">
+      <c r="P55" s="3">
         <f t="shared" si="0"/>
         <v>27227.338324888893</v>
       </c>
-      <c r="Q53" s="2">
+      <c r="Q55" s="2">
         <f t="shared" si="0"/>
         <v>4.684029058984911</v>
       </c>
-      <c r="R53" s="4">
+      <c r="R55" s="4">
         <v>-2.0755555555555555E-4</v>
-      </c>
-      <c r="S53" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D54" s="2">
-        <v>1186.9773491111109</v>
-      </c>
-      <c r="E54" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F54" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G54" s="2">
-        <v>280.33542888888883</v>
-      </c>
-      <c r="H54" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I54" s="2">
-        <v>5.3870271111111121</v>
-      </c>
-      <c r="J54" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K54" s="2">
-        <v>645.93808322222219</v>
-      </c>
-      <c r="L54" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M54" s="2">
-        <v>1455.5792641111111</v>
-      </c>
-      <c r="N54" s="2">
-        <v>1191.1918266666667</v>
-      </c>
-      <c r="O54" s="3">
-        <v>4661.9885253333332</v>
-      </c>
-      <c r="P54" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q54" s="2">
-        <v>-0.64567288888888896</v>
-      </c>
-      <c r="R54" s="4">
-        <v>-2.0744444444444445E-4</v>
-      </c>
-      <c r="S54" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D55" s="2">
-        <v>1186.9773355555556</v>
-      </c>
-      <c r="E55" s="2">
-        <v>1901.5157334444443</v>
-      </c>
-      <c r="F55" s="2">
-        <v>0.97970299999999988</v>
-      </c>
-      <c r="G55" s="2">
-        <v>280.33542888888883</v>
-      </c>
-      <c r="H55" s="2">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I55" s="2">
-        <v>5.3870271111111121</v>
-      </c>
-      <c r="J55" s="2">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K55" s="2">
-        <v>645.93833411111109</v>
-      </c>
-      <c r="L55" s="2">
-        <v>83.47062044444445</v>
-      </c>
-      <c r="M55" s="2">
-        <v>1455.5790065555557</v>
-      </c>
-      <c r="N55" s="2">
-        <v>1191.1918131111113</v>
-      </c>
-      <c r="O55" s="3">
-        <v>4661.9885253333332</v>
-      </c>
-      <c r="P55" s="3">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q55" s="2">
-        <v>-0.64567966666666665</v>
-      </c>
-      <c r="R55" s="4">
-        <v>-2.0744444444444445E-4</v>
       </c>
       <c r="S55" s="8" t="s">
         <v>23</v>
@@ -4398,13 +4400,13 @@
         <v>16</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D56" s="2">
-        <v>1186.9773355555556</v>
+        <v>1186.9773491111109</v>
       </c>
       <c r="E56" s="2">
         <v>1901.5157334444443</v>
@@ -4425,16 +4427,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K56" s="2">
-        <v>645.9383002222221</v>
+        <v>645.93808322222219</v>
       </c>
       <c r="L56" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M56" s="2">
-        <v>1455.5790607777778</v>
+        <v>1455.5792641111111</v>
       </c>
       <c r="N56" s="2">
-        <v>1191.1918131111113</v>
+        <v>1191.1918266666667</v>
       </c>
       <c r="O56" s="3">
         <v>4661.9885253333332</v>
@@ -4443,10 +4445,10 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q56" s="2">
-        <v>-0.64565933333333325</v>
+        <v>-0.64567288888888896</v>
       </c>
       <c r="R56" s="4">
-        <v>-1.7433333333333333E-4</v>
+        <v>-2.0744444444444445E-4</v>
       </c>
       <c r="S56" s="8" t="s">
         <v>23</v>
@@ -4457,13 +4459,13 @@
         <v>16</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D57" s="2">
-        <v>1187.0067003333331</v>
+        <v>1186.9773355555556</v>
       </c>
       <c r="E57" s="2">
         <v>1901.5157334444443</v>
@@ -4484,16 +4486,16 @@
         <v>8.145128999999999</v>
       </c>
       <c r="K57" s="2">
-        <v>645.93713388888887</v>
+        <v>645.93833411111109</v>
       </c>
       <c r="L57" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M57" s="2">
-        <v>1455.6553682222225</v>
+        <v>1455.5790065555557</v>
       </c>
       <c r="N57" s="2">
-        <v>1191.1764458888888</v>
+        <v>1191.1918131111113</v>
       </c>
       <c r="O57" s="3">
         <v>4661.9885253333332</v>
@@ -4502,27 +4504,27 @@
         <v>27227.338324888889</v>
       </c>
       <c r="Q57" s="2">
-        <v>-0.61525011111111105</v>
+        <v>-0.64567966666666665</v>
       </c>
       <c r="R57" s="4">
-        <v>-1.5888888888888889E-4</v>
+        <v>-2.0744444444444445E-4</v>
       </c>
       <c r="S57" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>16</v>
-      </c>
-      <c r="B58" t="s">
-        <v>65</v>
+      <c r="A58" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D58" s="2">
-        <v>1187.0063613333334</v>
+        <v>1186.9773355555556</v>
       </c>
       <c r="E58" s="2">
         <v>1901.5157334444443</v>
@@ -4537,51 +4539,51 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I58" s="2">
-        <v>5.3870315555555557</v>
+        <v>5.3870271111111121</v>
       </c>
       <c r="J58" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K58" s="2">
-        <v>645.93916833333344</v>
+        <v>645.9383002222221</v>
       </c>
       <c r="L58" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M58" s="2">
-        <v>1455.7051053333334</v>
+        <v>1455.5790607777778</v>
       </c>
       <c r="N58" s="2">
-        <v>1191.1759305555559</v>
+        <v>1191.1918131111113</v>
       </c>
       <c r="O58" s="3">
-        <v>4661.988498222222</v>
+        <v>4661.9885253333332</v>
       </c>
       <c r="P58" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q58" s="2">
-        <v>-0.56365988888888896</v>
+        <v>-0.64565933333333325</v>
       </c>
       <c r="R58" s="4">
-        <v>-1.5933333333333332E-4</v>
+        <v>-1.7433333333333333E-4</v>
       </c>
       <c r="S58" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>16</v>
-      </c>
-      <c r="B59" t="s">
-        <v>67</v>
+      <c r="A59" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D59" s="5">
-        <v>1208.5438095555555</v>
+      <c r="D59" s="2">
+        <v>1187.0067003333331</v>
       </c>
       <c r="E59" s="2">
         <v>1901.5157334444443</v>
@@ -4596,48 +4598,51 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I59" s="2">
-        <v>5.3172314444444444</v>
+        <v>5.3870271111111121</v>
       </c>
       <c r="J59" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K59" s="2">
-        <v>645.97183577777787</v>
+        <v>645.93713388888887</v>
       </c>
       <c r="L59" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M59" s="5">
-        <v>1460.2614338888889</v>
-      </c>
-      <c r="N59" s="5">
-        <v>1208.0519340000001</v>
+      <c r="M59" s="2">
+        <v>1455.6553682222225</v>
+      </c>
+      <c r="N59" s="2">
+        <v>1191.1764458888888</v>
       </c>
       <c r="O59" s="3">
-        <v>4662.6060926666669</v>
+        <v>4661.9885253333332</v>
       </c>
       <c r="P59" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q59" s="2">
-        <v>-0.5663084444444445</v>
+        <v>-0.61525011111111105</v>
       </c>
       <c r="R59" s="4">
-        <v>-2.0655555555555556E-4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+        <v>-1.5888888888888889E-4</v>
+      </c>
+      <c r="S59" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>16</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>74</v>
+      <c r="B60" t="s">
+        <v>65</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D60" s="2">
-        <v>1207.0222438888889</v>
+        <v>1187.0063613333334</v>
       </c>
       <c r="E60" s="2">
         <v>1901.5157334444443</v>
@@ -4652,48 +4657,51 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I60" s="2">
-        <v>5.3316344444444441</v>
+        <v>5.3870315555555557</v>
       </c>
       <c r="J60" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K60" s="2">
-        <v>645.95907266666666</v>
+        <v>645.93916833333344</v>
       </c>
       <c r="L60" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M60" s="2">
-        <v>1460.4185112222222</v>
+        <v>1455.7051053333334</v>
       </c>
       <c r="N60" s="2">
-        <v>1206.2352837777776</v>
+        <v>1191.1759305555559</v>
       </c>
       <c r="O60" s="3">
-        <v>4662.5755209999998</v>
+        <v>4661.988498222222</v>
       </c>
       <c r="P60" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q60" s="2">
-        <v>-0.73148200000000008</v>
+        <v>-0.56365988888888896</v>
       </c>
       <c r="R60" s="4">
-        <v>-2.5755555555555558E-4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+        <v>-1.5933333333333332E-4</v>
+      </c>
+      <c r="S60" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>16</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>75</v>
+      <c r="B61" t="s">
+        <v>67</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D61" s="2">
-        <v>1206.5233695555557</v>
+      <c r="D61" s="5">
+        <v>1208.5438095555555</v>
       </c>
       <c r="E61" s="2">
         <v>1901.5157334444443</v>
@@ -4708,51 +4716,48 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I61" s="2">
-        <v>5.3531247777777775</v>
+        <v>5.3172314444444444</v>
       </c>
       <c r="J61" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K61" s="2">
-        <v>645.94818811111122</v>
+        <v>645.97183577777787</v>
       </c>
       <c r="L61" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M61" s="2">
-        <v>1460.5092637777777</v>
-      </c>
-      <c r="N61" s="2">
-        <v>1205.5020886666666</v>
+      <c r="M61" s="5">
+        <v>1460.2614338888889</v>
+      </c>
+      <c r="N61" s="5">
+        <v>1208.0519340000001</v>
       </c>
       <c r="O61" s="3">
-        <v>4662.5708008888896</v>
+        <v>4662.6060926666669</v>
       </c>
       <c r="P61" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q61" s="2">
-        <v>-0.90742522222222222</v>
+        <v>-0.5663084444444445</v>
       </c>
       <c r="R61" s="4">
-        <v>-2.5788888888888888E-4</v>
-      </c>
-      <c r="S61" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+        <v>-2.0655555555555556E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>16</v>
       </c>
-      <c r="B62" t="s">
-        <v>76</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="B62" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D62" s="2">
-        <v>1080.801350777778</v>
+        <v>1207.0222438888889</v>
       </c>
       <c r="E62" s="2">
         <v>1901.5157334444443</v>
@@ -4767,51 +4772,48 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I62" s="2">
-        <v>5.7424886666666666</v>
+        <v>5.3316344444444441</v>
       </c>
       <c r="J62" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K62" s="2">
-        <v>645.86557344444441</v>
+        <v>645.95907266666666</v>
       </c>
       <c r="L62" s="2">
         <v>83.47062044444445</v>
       </c>
-      <c r="M62" s="5">
-        <v>1430.3511555555554</v>
+      <c r="M62" s="2">
+        <v>1460.4185112222222</v>
       </c>
       <c r="N62" s="2">
-        <v>1110.4303452222223</v>
+        <v>1206.2352837777776</v>
       </c>
       <c r="O62" s="3">
-        <v>4638.5936415555561</v>
+        <v>4662.5755209999998</v>
       </c>
       <c r="P62" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q62" s="2">
-        <v>-0.8872363333333334</v>
+        <v>-0.73148200000000008</v>
       </c>
       <c r="R62" s="4">
-        <v>-2.5788888888888888E-4</v>
-      </c>
-      <c r="S62" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+        <v>-2.5755555555555558E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>16</v>
       </c>
-      <c r="B63" t="s">
-        <v>77</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B63" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D63" s="2">
-        <v>1080.801350777778</v>
+        <v>1206.5233695555557</v>
       </c>
       <c r="E63" s="2">
         <v>1901.5157334444443</v>
@@ -4826,34 +4828,34 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I63" s="2">
-        <v>5.7424886666666666</v>
+        <v>5.3531247777777775</v>
       </c>
       <c r="J63" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K63" s="2">
-        <v>645.86557344444441</v>
+        <v>645.94818811111122</v>
       </c>
       <c r="L63" s="2">
         <v>83.47062044444445</v>
       </c>
       <c r="M63" s="2">
-        <v>1430.3511555555554</v>
+        <v>1460.5092637777777</v>
       </c>
       <c r="N63" s="2">
-        <v>1110.4303452222223</v>
+        <v>1205.5020886666666</v>
       </c>
       <c r="O63" s="3">
-        <v>4638.5936415555561</v>
+        <v>4662.5708008888896</v>
       </c>
       <c r="P63" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q63" s="2">
-        <v>-0.8872363333333334</v>
+        <v>-0.90742522222222222</v>
       </c>
       <c r="R63" s="4">
-        <v>4.2666666666666656E-5</v>
+        <v>-2.5788888888888888E-4</v>
       </c>
       <c r="S63" t="s">
         <v>23</v>
@@ -4864,19 +4866,19 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
         <v>23</v>
       </c>
-      <c r="D64" s="5">
-        <v>897.84913466666671</v>
-      </c>
-      <c r="E64" s="5">
-        <v>1763.5263265555557</v>
+      <c r="D64" s="2">
+        <v>1080.801350777778</v>
+      </c>
+      <c r="E64" s="2">
+        <v>1901.5157334444443</v>
       </c>
       <c r="F64" s="2">
-        <v>1.0174076666666665</v>
+        <v>0.97970299999999988</v>
       </c>
       <c r="G64" s="2">
         <v>280.33542888888883</v>
@@ -4884,170 +4886,170 @@
       <c r="H64" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I64" s="5">
-        <v>7.299440555555555</v>
+      <c r="I64" s="2">
+        <v>5.7424886666666666</v>
       </c>
       <c r="J64" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K64" s="2">
-        <v>646.63056122222224</v>
-      </c>
-      <c r="L64" s="5">
-        <v>60.018756111111117</v>
+        <v>645.86557344444441</v>
+      </c>
+      <c r="L64" s="2">
+        <v>83.47062044444445</v>
       </c>
       <c r="M64" s="5">
-        <v>1342.5421007777777</v>
-      </c>
-      <c r="N64" s="5">
-        <v>902.73358833333339</v>
-      </c>
-      <c r="O64" s="6">
-        <v>5459.5160589999996</v>
+        <v>1430.3511555555554</v>
+      </c>
+      <c r="N64" s="2">
+        <v>1110.4303452222223</v>
+      </c>
+      <c r="O64" s="3">
+        <v>4638.5936415555561</v>
       </c>
       <c r="P64" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q64" s="2">
-        <v>0.26704155555555559</v>
+        <v>-0.8872363333333334</v>
       </c>
       <c r="R64" s="4">
-        <v>6.222222222222222E-5</v>
+        <v>-2.5788888888888888E-4</v>
       </c>
       <c r="S64" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C65" t="s">
         <v>23</v>
       </c>
-      <c r="D65" s="5">
-        <v>1000.3124864444443</v>
+      <c r="D65" s="2">
+        <v>1080.801350777778</v>
       </c>
       <c r="E65" s="2">
-        <v>1763.5263265555557</v>
+        <v>1901.5157334444443</v>
       </c>
       <c r="F65" s="2">
-        <v>0.999942</v>
-      </c>
-      <c r="G65" s="5">
-        <v>305.6782124444444</v>
+        <v>0.97970299999999988</v>
+      </c>
+      <c r="G65" s="2">
+        <v>280.33542888888883</v>
       </c>
       <c r="H65" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I65" s="2">
-        <v>6.8948233333333331</v>
+        <v>5.7424886666666666</v>
       </c>
       <c r="J65" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K65" s="5">
-        <v>673.17452677777771</v>
+      <c r="K65" s="2">
+        <v>645.86557344444441</v>
       </c>
       <c r="L65" s="2">
-        <v>60.018756111111117</v>
-      </c>
-      <c r="M65" s="5">
-        <v>1321.9402533333332</v>
-      </c>
-      <c r="N65" s="5">
-        <v>1024.1975572222223</v>
-      </c>
-      <c r="O65" s="6">
-        <v>4583.9874403333333</v>
+        <v>83.47062044444445</v>
+      </c>
+      <c r="M65" s="2">
+        <v>1430.3511555555554</v>
+      </c>
+      <c r="N65" s="2">
+        <v>1110.4303452222223</v>
+      </c>
+      <c r="O65" s="3">
+        <v>4638.5936415555561</v>
       </c>
       <c r="P65" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q65" s="2">
-        <v>0.28907633333333327</v>
-      </c>
-      <c r="R65" s="15">
+        <v>-0.8872363333333334</v>
+      </c>
+      <c r="R65" s="4">
+        <v>4.2666666666666656E-5</v>
+      </c>
+      <c r="S65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="5">
+        <v>897.84913466666671</v>
+      </c>
+      <c r="E66" s="5">
+        <v>1763.5263265555557</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1.0174076666666665</v>
+      </c>
+      <c r="G66" s="2">
+        <v>280.33542888888883</v>
+      </c>
+      <c r="H66" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I66" s="5">
+        <v>7.299440555555555</v>
+      </c>
+      <c r="J66" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K66" s="2">
+        <v>646.63056122222224</v>
+      </c>
+      <c r="L66" s="5">
+        <v>60.018756111111117</v>
+      </c>
+      <c r="M66" s="5">
+        <v>1342.5421007777777</v>
+      </c>
+      <c r="N66" s="5">
+        <v>902.73358833333339</v>
+      </c>
+      <c r="O66" s="6">
+        <v>5459.5160589999996</v>
+      </c>
+      <c r="P66" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q66" s="2">
+        <v>0.26704155555555559</v>
+      </c>
+      <c r="R66" s="4">
         <v>6.222222222222222E-5</v>
       </c>
-      <c r="S65" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>16</v>
-      </c>
-      <c r="B66" t="s">
-        <v>82</v>
-      </c>
-      <c r="C66" t="s">
-        <v>23</v>
-      </c>
-      <c r="D66" s="13">
+      <c r="S66" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" s="5">
         <v>1000.3124864444443</v>
-      </c>
-      <c r="E66" s="13">
-        <v>1763.5263265555557</v>
-      </c>
-      <c r="F66" s="13">
-        <v>0.999942</v>
-      </c>
-      <c r="G66" s="13">
-        <v>305.6782124444444</v>
-      </c>
-      <c r="H66" s="13">
-        <v>9.775355222222224</v>
-      </c>
-      <c r="I66" s="13">
-        <v>6.8948233333333331</v>
-      </c>
-      <c r="J66" s="13">
-        <v>8.145128999999999</v>
-      </c>
-      <c r="K66" s="13">
-        <v>673.17452677777771</v>
-      </c>
-      <c r="L66" s="13">
-        <v>60.018756111111117</v>
-      </c>
-      <c r="M66" s="13">
-        <v>1321.9402533333332</v>
-      </c>
-      <c r="N66" s="13">
-        <v>1024.1975572222223</v>
-      </c>
-      <c r="O66" s="14">
-        <v>4583.9874403333333</v>
-      </c>
-      <c r="P66" s="14">
-        <v>27227.338324888889</v>
-      </c>
-      <c r="Q66" s="13">
-        <v>0.28907633333333327</v>
-      </c>
-      <c r="R66" s="4">
-        <v>5.7555555555555559E-5</v>
-      </c>
-      <c r="S66" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>16</v>
-      </c>
-      <c r="B67" t="s">
-        <v>84</v>
-      </c>
-      <c r="C67" t="s">
-        <v>23</v>
-      </c>
-      <c r="D67" s="5">
-        <v>1070.3662515555557</v>
       </c>
       <c r="E67" s="2">
         <v>1763.5263265555557</v>
@@ -5055,123 +5057,123 @@
       <c r="F67" s="2">
         <v>0.999942</v>
       </c>
-      <c r="G67" s="2">
+      <c r="G67" s="5">
         <v>305.6782124444444</v>
       </c>
       <c r="H67" s="2">
         <v>9.775355222222224</v>
       </c>
       <c r="I67" s="2">
-        <v>6.8224234444444436</v>
+        <v>6.8948233333333331</v>
       </c>
       <c r="J67" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K67" s="2">
-        <v>672.51038266666671</v>
+      <c r="K67" s="5">
+        <v>673.17452677777771</v>
       </c>
       <c r="L67" s="2">
         <v>60.018756111111117</v>
       </c>
       <c r="M67" s="5">
-        <v>1335.0520562222218</v>
+        <v>1321.9402533333332</v>
       </c>
       <c r="N67" s="5">
-        <v>1081.7151217777778</v>
-      </c>
-      <c r="O67" s="3">
-        <v>4576.182644333333</v>
+        <v>1024.1975572222223</v>
+      </c>
+      <c r="O67" s="6">
+        <v>4583.9874403333333</v>
       </c>
       <c r="P67" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q67" s="2">
-        <v>0.27293466666666671</v>
-      </c>
-      <c r="R67" s="4">
-        <v>2.3444444444444448E-5</v>
+        <v>0.28907633333333327</v>
+      </c>
+      <c r="R67" s="15">
+        <v>6.222222222222222E-5</v>
       </c>
       <c r="S67" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C68" t="s">
         <v>23</v>
       </c>
-      <c r="D68" s="5">
-        <v>1246.3303018888889</v>
-      </c>
-      <c r="E68" s="5">
-        <v>1890.2624783333331</v>
-      </c>
-      <c r="F68" s="2">
-        <v>0.94846033333333346</v>
-      </c>
-      <c r="G68" s="2">
+      <c r="D68" s="13">
+        <v>1000.3124864444443</v>
+      </c>
+      <c r="E68" s="13">
+        <v>1763.5263265555557</v>
+      </c>
+      <c r="F68" s="13">
+        <v>0.999942</v>
+      </c>
+      <c r="G68" s="13">
         <v>305.6782124444444</v>
       </c>
-      <c r="H68" s="2">
+      <c r="H68" s="13">
         <v>9.775355222222224</v>
       </c>
-      <c r="I68" s="5">
-        <v>6.3587768888888885</v>
-      </c>
-      <c r="J68" s="2">
+      <c r="I68" s="13">
+        <v>6.8948233333333331</v>
+      </c>
+      <c r="J68" s="13">
         <v>8.145128999999999</v>
       </c>
-      <c r="K68" s="5">
-        <v>628.90788111111101</v>
-      </c>
-      <c r="L68" s="5">
-        <v>82.308506444444433</v>
-      </c>
-      <c r="M68" s="5">
-        <v>1456.3722873333334</v>
-      </c>
-      <c r="N68" s="5">
-        <v>1283.7495253333334</v>
-      </c>
-      <c r="O68" s="6">
-        <v>3986.0738390000001</v>
-      </c>
-      <c r="P68" s="3">
+      <c r="K68" s="13">
+        <v>673.17452677777771</v>
+      </c>
+      <c r="L68" s="13">
+        <v>60.018756111111117</v>
+      </c>
+      <c r="M68" s="13">
+        <v>1321.9402533333332</v>
+      </c>
+      <c r="N68" s="13">
+        <v>1024.1975572222223</v>
+      </c>
+      <c r="O68" s="14">
+        <v>4583.9874403333333</v>
+      </c>
+      <c r="P68" s="14">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q68" s="2">
-        <v>0.12974411111111114</v>
+      <c r="Q68" s="13">
+        <v>0.28907633333333327</v>
       </c>
       <c r="R68" s="4">
-        <v>2.1888888888888887E-5</v>
+        <v>5.7555555555555559E-5</v>
       </c>
       <c r="S68" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C69" t="s">
         <v>23</v>
       </c>
       <c r="D69" s="5">
-        <v>1380.5085448888888</v>
+        <v>1070.3662515555557</v>
       </c>
       <c r="E69" s="2">
-        <v>1890.2624783333331</v>
+        <v>1763.5263265555557</v>
       </c>
       <c r="F69" s="2">
-        <v>0.94846033333333346</v>
+        <v>0.999942</v>
       </c>
       <c r="G69" s="2">
         <v>305.6782124444444</v>
@@ -5180,90 +5182,458 @@
         <v>9.775355222222224</v>
       </c>
       <c r="I69" s="2">
-        <v>6.1288343333333337</v>
+        <v>6.8224234444444436</v>
       </c>
       <c r="J69" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K69" s="2">
-        <v>628.9703199999999</v>
+        <v>672.51038266666671</v>
       </c>
       <c r="L69" s="2">
-        <v>82.308506444444433</v>
+        <v>60.018756111111117</v>
       </c>
       <c r="M69" s="5">
-        <v>1487.9843207777781</v>
+        <v>1335.0520562222218</v>
       </c>
       <c r="N69" s="5">
-        <v>1386.0215385555557</v>
-      </c>
-      <c r="O69" s="6">
-        <v>4013.3543294444444</v>
+        <v>1081.7151217777778</v>
+      </c>
+      <c r="O69" s="3">
+        <v>4576.182644333333</v>
       </c>
       <c r="P69" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q69" s="2">
-        <v>0.12792911111111113</v>
+        <v>0.27293466666666671</v>
       </c>
       <c r="R69" s="4">
-        <v>1.4777777777777775E-5</v>
+        <v>2.3444444444444448E-5</v>
       </c>
       <c r="S69" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>16</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C70" t="s">
         <v>23</v>
       </c>
-      <c r="D70" s="2">
-        <v>1242.9115804444446</v>
-      </c>
-      <c r="E70" s="2">
+      <c r="D70" s="5">
+        <v>1246.3303018888889</v>
+      </c>
+      <c r="E70" s="5">
         <v>1890.2624783333331</v>
       </c>
       <c r="F70" s="2">
-        <v>1.059004111111111</v>
+        <v>0.94846033333333346</v>
       </c>
       <c r="G70" s="2">
-        <v>299.96642388888887</v>
+        <v>305.6782124444444</v>
       </c>
       <c r="H70" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I70" s="2">
-        <v>5.6808013333333331</v>
+      <c r="I70" s="5">
+        <v>6.3587768888888885</v>
       </c>
       <c r="J70" s="2">
         <v>8.145128999999999</v>
       </c>
       <c r="K70" s="5">
-        <v>676.49806711111114</v>
-      </c>
-      <c r="L70" s="2">
+        <v>628.90788111111101</v>
+      </c>
+      <c r="L70" s="5">
         <v>82.308506444444433</v>
       </c>
-      <c r="M70" s="2">
-        <v>1459.1644423333332</v>
-      </c>
-      <c r="N70" s="2">
-        <v>1223.6673176666666</v>
+      <c r="M70" s="5">
+        <v>1456.3722873333334</v>
+      </c>
+      <c r="N70" s="5">
+        <v>1283.7495253333334</v>
       </c>
       <c r="O70" s="6">
-        <v>5486.7290039999998</v>
+        <v>3986.0738390000001</v>
       </c>
       <c r="P70" s="3">
         <v>27227.338324888889</v>
       </c>
       <c r="Q70" s="2">
+        <v>0.12974411111111114</v>
+      </c>
+      <c r="R70" s="4">
+        <v>2.1888888888888887E-5</v>
+      </c>
+      <c r="S70" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>16</v>
+      </c>
+      <c r="B71" t="s">
+        <v>86</v>
+      </c>
+      <c r="C71" t="s">
+        <v>23</v>
+      </c>
+      <c r="D71" s="5">
+        <v>1380.5085448888888</v>
+      </c>
+      <c r="E71" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F71" s="2">
+        <v>0.94846033333333346</v>
+      </c>
+      <c r="G71" s="2">
+        <v>305.6782124444444</v>
+      </c>
+      <c r="H71" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I71" s="2">
+        <v>6.1288343333333337</v>
+      </c>
+      <c r="J71" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K71" s="2">
+        <v>628.9703199999999</v>
+      </c>
+      <c r="L71" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M71" s="5">
+        <v>1487.9843207777781</v>
+      </c>
+      <c r="N71" s="5">
+        <v>1386.0215385555557</v>
+      </c>
+      <c r="O71" s="6">
+        <v>4013.3543294444444</v>
+      </c>
+      <c r="P71" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q71" s="2">
+        <v>0.12792911111111113</v>
+      </c>
+      <c r="R71" s="4">
+        <v>1.4777777777777775E-5</v>
+      </c>
+      <c r="S71" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" t="s">
+        <v>87</v>
+      </c>
+      <c r="C72" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1242.9115804444446</v>
+      </c>
+      <c r="E72" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F72" s="2">
+        <v>1.059004111111111</v>
+      </c>
+      <c r="G72" s="2">
+        <v>299.96642388888887</v>
+      </c>
+      <c r="H72" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I72" s="2">
+        <v>5.6808013333333331</v>
+      </c>
+      <c r="J72" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K72" s="5">
+        <v>676.49806711111114</v>
+      </c>
+      <c r="L72" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M72" s="2">
+        <v>1459.1644423333332</v>
+      </c>
+      <c r="N72" s="2">
+        <v>1223.6673176666666</v>
+      </c>
+      <c r="O72" s="6">
+        <v>5486.7290039999998</v>
+      </c>
+      <c r="P72" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q72" s="2">
         <v>0.12781966666666669</v>
+      </c>
+      <c r="R72" s="4">
+        <v>1.5000000000000004E-5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73" t="s">
+        <v>91</v>
+      </c>
+      <c r="C73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1243.2278510000001</v>
+      </c>
+      <c r="E73" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F73" s="2">
+        <v>1.059004111111111</v>
+      </c>
+      <c r="G73" s="2">
+        <v>299.96146311111113</v>
+      </c>
+      <c r="H73" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I73" s="5">
+        <v>9.777777777777777E-6</v>
+      </c>
+      <c r="J73" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K73" s="2">
+        <v>674.44692644444456</v>
+      </c>
+      <c r="L73" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M73" s="2">
+        <v>1458.7926432222221</v>
+      </c>
+      <c r="N73" s="2">
+        <v>1224.0023193333334</v>
+      </c>
+      <c r="O73" s="3">
+        <v>5486.7054580000004</v>
+      </c>
+      <c r="P73" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q73" s="5">
+        <v>3.4093633333333333</v>
+      </c>
+      <c r="R73" s="7">
+        <v>1.0044444444444445E-3</v>
+      </c>
+      <c r="S73" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" t="s">
+        <v>93</v>
+      </c>
+      <c r="C74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1243.2278509999999</v>
+      </c>
+      <c r="E74" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F74" s="2">
+        <v>1.059004111111111</v>
+      </c>
+      <c r="G74" s="2">
+        <v>299.96151055555561</v>
+      </c>
+      <c r="H74" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I74" s="2">
+        <v>5.6491045555555557</v>
+      </c>
+      <c r="J74" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K74" s="5">
+        <v>674.44512255555549</v>
+      </c>
+      <c r="L74" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M74" s="2">
+        <v>1458.7950304444444</v>
+      </c>
+      <c r="N74" s="2">
+        <v>1224.0023193333334</v>
+      </c>
+      <c r="O74" s="3">
+        <v>5486.7059732222224</v>
+      </c>
+      <c r="P74" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q74" s="5">
+        <v>-2.2391961111111112</v>
+      </c>
+      <c r="R74" s="7">
+        <v>-6.7688888888888887E-4</v>
+      </c>
+      <c r="S74" t="s">
+        <v>23</v>
+      </c>
+      <c r="T74" s="2">
+        <f>SUM(D74:I74)</f>
+        <v>3449.9353037777769</v>
+      </c>
+      <c r="U74" s="2">
+        <f>SUM(J74:N74)</f>
+        <v>3447.6961077777778</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D76" s="2">
+        <f>D74-D72</f>
+        <v>0.31627055555532024</v>
+      </c>
+      <c r="E76" s="2">
+        <f t="shared" ref="E76:R76" si="1">E74-E72</f>
+        <v>0</v>
+      </c>
+      <c r="F76" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G76" s="2">
+        <f t="shared" si="1"/>
+        <v>-4.9133333332633811E-3</v>
+      </c>
+      <c r="H76" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I76" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.1696777777777463E-2</v>
+      </c>
+      <c r="J76" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K76" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.0529445555556549</v>
+      </c>
+      <c r="L76" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M76" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.36941188888886245</v>
+      </c>
+      <c r="N76" s="2">
+        <f t="shared" si="1"/>
+        <v>0.33500166666681253</v>
+      </c>
+      <c r="O76" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.3030777777421463E-2</v>
+      </c>
+      <c r="P76" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q76" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.3670157777777781</v>
+      </c>
+      <c r="R76" s="4">
+        <f t="shared" si="1"/>
+        <v>-6.9188888888888891E-4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>16</v>
+      </c>
+      <c r="B78" t="s">
+        <v>93</v>
+      </c>
+      <c r="C78" t="s">
+        <v>92</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1230.0044677999999</v>
+      </c>
+      <c r="E78" s="2">
+        <v>1848.1456909000001</v>
+      </c>
+      <c r="F78" s="2">
+        <v>1.0573501000000001</v>
+      </c>
+      <c r="G78" s="2">
+        <v>299.4371582</v>
+      </c>
+      <c r="H78" s="2">
+        <v>9.7418259000000003</v>
+      </c>
+      <c r="I78" s="2">
+        <v>5.7446602000000002</v>
+      </c>
+      <c r="J78" s="2">
+        <v>8.1171118999999994</v>
+      </c>
+      <c r="K78" s="2">
+        <v>673.08737180000003</v>
+      </c>
+      <c r="L78" s="2">
+        <v>81.12013859999999</v>
+      </c>
+      <c r="M78" s="2">
+        <v>1432.6230836</v>
+      </c>
+      <c r="N78" s="2">
+        <v>1196.8767700000001</v>
+      </c>
+      <c r="O78" s="3">
+        <v>5429.4087645999998</v>
+      </c>
+      <c r="P78" s="3">
+        <v>27140.258789299998</v>
+      </c>
+      <c r="Q78" s="2">
+        <v>-2.3066774000000003</v>
+      </c>
+      <c r="R78" s="4">
+        <v>-7.1000000000000002E-4</v>
+      </c>
+      <c r="S78" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Save recent additions to CW3MdigitalHandbook.docx.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FE337F-6BBB-40A4-9D0A-CD8FB746B243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9C7FEA-2998-4EAF-B919-986FAF75F89F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="468" yWindow="1092" windowWidth="22392" windowHeight="10356" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="96">
   <si>
     <t>Year</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t xml:space="preserve">Demo_Baseline 2010-19 C225 </t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-19 C226</t>
   </si>
 </sst>
 </file>
@@ -1201,11 +1204,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U78"/>
+  <dimension ref="A1:U79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S39" sqref="S39"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O81" sqref="O81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5515,67 +5518,78 @@
         <v>3447.6961077777778</v>
       </c>
     </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>16</v>
+      </c>
+      <c r="B75" t="s">
+        <v>95</v>
+      </c>
+      <c r="C75" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1243.2278509999999</v>
+      </c>
+      <c r="E75" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F75" s="2">
+        <v>1.059004111111111</v>
+      </c>
+      <c r="G75" s="2">
+        <v>299.96151055555561</v>
+      </c>
+      <c r="H75" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I75" s="2">
+        <v>5.6491045555555557</v>
+      </c>
+      <c r="J75" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K75" s="5">
+        <v>676.83127177777783</v>
+      </c>
+      <c r="L75" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M75" s="2">
+        <v>1458.7950304444444</v>
+      </c>
+      <c r="N75" s="2">
+        <v>1224.0023193333334</v>
+      </c>
+      <c r="O75" s="3">
+        <v>5486.7059732222224</v>
+      </c>
+      <c r="P75" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q75" s="5">
+        <v>0.14695311111111112</v>
+      </c>
+      <c r="R75" s="4">
+        <v>2.0111111111111117E-5</v>
+      </c>
+    </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D76" s="2">
-        <f>D74-D72</f>
-        <v>0.31627055555532024</v>
-      </c>
-      <c r="E76" s="2">
-        <f t="shared" ref="E76:R76" si="1">E74-E72</f>
-        <v>0</v>
-      </c>
-      <c r="F76" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G76" s="2">
-        <f t="shared" si="1"/>
-        <v>-4.9133333332633811E-3</v>
-      </c>
-      <c r="H76" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I76" s="2">
-        <f t="shared" si="1"/>
-        <v>-3.1696777777777463E-2</v>
-      </c>
-      <c r="J76" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K76" s="2">
-        <f t="shared" si="1"/>
-        <v>-2.0529445555556549</v>
-      </c>
-      <c r="L76" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M76" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.36941188888886245</v>
-      </c>
-      <c r="N76" s="2">
-        <f t="shared" si="1"/>
-        <v>0.33500166666681253</v>
-      </c>
-      <c r="O76" s="2">
-        <f t="shared" si="1"/>
-        <v>-2.3030777777421463E-2</v>
-      </c>
-      <c r="P76" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q76" s="2">
-        <f t="shared" si="1"/>
-        <v>-2.3670157777777781</v>
-      </c>
-      <c r="R76" s="4">
-        <f t="shared" si="1"/>
-        <v>-6.9188888888888891E-4</v>
-      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
+      <c r="Q76" s="5"/>
+      <c r="R76" s="4"/>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
@@ -5633,6 +5647,65 @@
         <v>-7.1000000000000002E-4</v>
       </c>
       <c r="S78" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>16</v>
+      </c>
+      <c r="B79" t="s">
+        <v>95</v>
+      </c>
+      <c r="C79" t="s">
+        <v>92</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1230.0044677999999</v>
+      </c>
+      <c r="E79" s="2">
+        <v>1848.1456909000001</v>
+      </c>
+      <c r="F79" s="2">
+        <v>1.0573501000000001</v>
+      </c>
+      <c r="G79" s="2">
+        <v>299.4371582</v>
+      </c>
+      <c r="H79" s="2">
+        <v>9.7418259000000003</v>
+      </c>
+      <c r="I79" s="2">
+        <v>5.7446602000000002</v>
+      </c>
+      <c r="J79" s="2">
+        <v>8.1171118999999994</v>
+      </c>
+      <c r="K79" s="5">
+        <v>675.4841553</v>
+      </c>
+      <c r="L79" s="2">
+        <v>81.12013859999999</v>
+      </c>
+      <c r="M79" s="2">
+        <v>1432.6230836</v>
+      </c>
+      <c r="N79" s="2">
+        <v>1196.8767700000001</v>
+      </c>
+      <c r="O79" s="3">
+        <v>5429.4087645999998</v>
+      </c>
+      <c r="P79" s="3">
+        <v>27140.258789299998</v>
+      </c>
+      <c r="Q79" s="5">
+        <v>9.0106100000000008E-2</v>
+      </c>
+      <c r="R79" s="7">
+        <v>3.5000000000000063E-6</v>
+      </c>
+      <c r="S79" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Release CW3M_Installer_McKenzie_0.4.4.exe. More of the stream temperature logic is working now.  A lot of details about the flow and stream temperature models have been added to the digital handbook. The McKenzie flow and stream temperature models were calibrated one more time.  Preliminary estimates of the stream flow and thermal energy budgets for the McKenzie basin have been made, and added to the digital handbook.  Files and folders related to running PEST on the BLU and Marys drainages have been added.  Files for the McKenzie and North Santiam basins are in this release, but the files for the Clackamas basin and other parts of the WRB have been left out.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9C7FEA-2998-4EAF-B919-986FAF75F89F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776DE35A-CD5C-44D9-9B78-1665243BCEB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="468" yWindow="1092" windowWidth="22392" windowHeight="10356" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,8 +326,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="170" formatCode="0.000%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -774,7 +775,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -817,8 +818,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -849,8 +851,9 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -890,6 +893,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -1208,7 +1212,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O81" sqref="O81"/>
+      <selection pane="bottomLeft" activeCell="R75" sqref="R75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5570,7 +5574,7 @@
       <c r="Q75" s="5">
         <v>0.14695311111111112</v>
       </c>
-      <c r="R75" s="4">
+      <c r="R75" s="18">
         <v>2.0111111111111117E-5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make changes to facilitate comparing CW3M output with Shade-a-lator output. Set up 4 scenario folders in ScenarioData: SAL36CC Test, SAL75CC Test, SAL36FC Test, and SAL75FC Test.  These are all cloned from Demo_Baseline. SimulationScenarios.xml - Add the four new Shade-a-lator test scenarios. Scenario.h - Add members to class Shade_a_latorData: m_endDate, m_canopyDensity_pct, m_heightThreshold_m, and m_futureHeight_m. Scenario.cpp - Add logic to ScenarioManager::LoadXml() to read the new Shade_a_latorData members. FlowContext.h - Add member m_SALmode to class FlowContext.h. Flow.cpp - Move the logic to read the SAL output file from FlowModel::EndStep() to FlowModel::StartStep.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776DE35A-CD5C-44D9-9B78-1665243BCEB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170AB969-9CD1-4DA0-A751-6B246D990262}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="468" yWindow="1092" windowWidth="22392" windowHeight="10356" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="97">
   <si>
     <t>Year</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>Demo_Baseline_2010-19 C226</t>
+  </si>
+  <si>
+    <t>Baseline_1979-current C286</t>
   </si>
 </sst>
 </file>
@@ -328,7 +331,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="170" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -851,7 +854,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1212,18 +1215,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R75" sqref="R75"/>
+      <selection pane="bottomLeft" activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="33.77734375" customWidth="1"/>
-    <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1282,7 +1285,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>-4.8000000000000001E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1564,7 +1567,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1735,7 +1738,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1792,7 +1795,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1849,7 +1852,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1906,7 +1909,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1970,7 +1973,7 @@
         <v>-1.3600000000000005E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2030,7 +2033,7 @@
       </c>
       <c r="U14" s="4"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2090,7 +2093,7 @@
       </c>
       <c r="U15" s="4"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2149,7 +2152,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2208,7 +2211,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2267,7 +2270,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>46</v>
       </c>
@@ -2323,7 +2326,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2382,7 +2385,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2441,7 +2444,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2500,7 +2503,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>55</v>
       </c>
@@ -2556,7 +2559,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>56</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -2671,7 +2674,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -2730,7 +2733,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -2789,7 +2792,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2848,7 +2851,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -2907,7 +2910,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -2966,7 +2969,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -3025,7 +3028,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -3084,7 +3087,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>78</v>
       </c>
@@ -3140,7 +3143,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -3199,7 +3202,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -3258,7 +3261,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -3317,7 +3320,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="37" spans="1:19" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>16</v>
       </c>
@@ -3376,7 +3379,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="38" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>16</v>
       </c>
@@ -3435,7 +3438,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="39" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="17">
         <v>44202</v>
       </c>
@@ -3485,7 +3488,7 @@
         <v>3.4099999999999999E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="16"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
@@ -3503,7 +3506,7 @@
       <c r="Q40" s="13"/>
       <c r="R40" s="15"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -3560,7 +3563,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -3614,7 +3617,7 @@
         <v>-3.8888888888888877E-5</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -3671,7 +3674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -3725,7 +3728,7 @@
         <v>1.3650000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -3782,7 +3785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -3841,7 +3844,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -3900,7 +3903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -3959,7 +3962,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -4018,7 +4021,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -4077,7 +4080,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>16</v>
       </c>
@@ -4136,7 +4139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>16</v>
       </c>
@@ -4195,7 +4198,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>16</v>
       </c>
@@ -4255,7 +4258,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>16</v>
       </c>
@@ -4329,7 +4332,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>16</v>
       </c>
@@ -4402,7 +4405,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>16</v>
       </c>
@@ -4461,7 +4464,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>16</v>
       </c>
@@ -4520,7 +4523,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>16</v>
       </c>
@@ -4579,7 +4582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>16</v>
       </c>
@@ -4638,7 +4641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -4697,7 +4700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -4753,7 +4756,7 @@
         <v>-2.0655555555555556E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -4809,7 +4812,7 @@
         <v>-2.5755555555555558E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -4868,7 +4871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -4927,7 +4930,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -4986,7 +4989,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -5045,7 +5048,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -5104,7 +5107,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -5163,7 +5166,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -5222,7 +5225,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -5281,7 +5284,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -5340,7 +5343,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -5396,7 +5399,7 @@
         <v>1.5000000000000004E-5</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -5455,7 +5458,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -5522,7 +5525,7 @@
         <v>3447.6961077777778</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -5553,7 +5556,7 @@
       <c r="J75" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K75" s="5">
+      <c r="K75" s="13">
         <v>676.83127177777783</v>
       </c>
       <c r="L75" s="2">
@@ -5571,31 +5574,70 @@
       <c r="P75" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q75" s="5">
+      <c r="Q75" s="13">
         <v>0.14695311111111112</v>
       </c>
       <c r="R75" s="18">
         <v>2.0111111111111117E-5</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
-      <c r="N76" s="2"/>
-      <c r="O76" s="3"/>
-      <c r="P76" s="3"/>
-      <c r="Q76" s="5"/>
-      <c r="R76" s="4"/>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>16</v>
+      </c>
+      <c r="B76" t="s">
+        <v>96</v>
+      </c>
+      <c r="C76" t="s">
+        <v>23</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1112.7018771111111</v>
+      </c>
+      <c r="E76" s="5">
+        <v>1763.5263265555557</v>
+      </c>
+      <c r="F76" s="2">
+        <v>1.1070731111111112</v>
+      </c>
+      <c r="G76" s="2">
+        <v>295.25833466666666</v>
+      </c>
+      <c r="H76" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I76" s="2">
+        <v>6.5172971111111115</v>
+      </c>
+      <c r="J76" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K76" s="5">
+        <v>686.8172538888889</v>
+      </c>
+      <c r="L76" s="5">
+        <v>60.018756111111117</v>
+      </c>
+      <c r="M76" s="5">
+        <v>1361.733412</v>
+      </c>
+      <c r="N76" s="5">
+        <v>1072.4035372222222</v>
+      </c>
+      <c r="O76" s="6">
+        <v>6355.1079644444444</v>
+      </c>
+      <c r="P76" s="3">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q76" s="13">
+        <v>0.23182455555555562</v>
+      </c>
+      <c r="R76" s="4">
+        <v>4.1777777777777767E-5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -5654,7 +5696,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>16</v>
       </c>
@@ -5725,7 +5767,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5739,14 +5781,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.21875" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="18" max="18" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -5802,7 +5844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5859,7 +5901,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -5918,7 +5960,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -5977,7 +6019,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
@@ -5994,7 +6036,7 @@
       <c r="Q5" s="13"/>
       <c r="R5" s="15"/>
     </row>
-    <row r="6" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Try to clean up the repository status.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7007C5F-BC7E-4087-99AC-9760B6A829FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591A5130-59ED-4B45-922E-5DEC6914270D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
-    <sheet name="SAL75CC 2020" sheetId="3" r:id="rId2"/>
-    <sheet name="2000-09" sheetId="2" r:id="rId3"/>
+    <sheet name="C330 v C309" sheetId="4" r:id="rId2"/>
+    <sheet name="SAL75CC 2020" sheetId="3" r:id="rId3"/>
+    <sheet name="2000-09" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="108">
   <si>
     <t>Year</t>
   </si>
@@ -335,6 +336,27 @@
   </si>
   <si>
     <t>Demo_Baseline_C326</t>
+  </si>
+  <si>
+    <t>SAL75CC_Test_C326+</t>
+  </si>
+  <si>
+    <t>Demo-Baseline 2010-20 C330</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-20_C301</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_C309</t>
+  </si>
+  <si>
+    <t>C330</t>
+  </si>
+  <si>
+    <t>C309</t>
+  </si>
+  <si>
+    <t>C330-C309</t>
   </si>
 </sst>
 </file>
@@ -1223,11 +1245,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U80"/>
+  <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O77" sqref="O77"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86:XFD86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5705,139 +5727,442 @@
         <v>2.1777777777777772E-5</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" s="3"/>
-      <c r="P78" s="3"/>
-      <c r="Q78" s="2"/>
-      <c r="R78" s="4"/>
-    </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="78" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>16</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B78" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78" s="13">
+        <v>1209.7411295555555</v>
+      </c>
+      <c r="E78" s="13">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F78" s="13">
+        <v>1.0618724444444443</v>
+      </c>
+      <c r="G78" s="13">
+        <v>299.96341288888891</v>
+      </c>
+      <c r="H78" s="13">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I78" s="13">
+        <v>6.1721304444444449</v>
+      </c>
+      <c r="J78" s="13">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K78" s="13">
+        <v>677.92138000000011</v>
+      </c>
+      <c r="L78" s="13">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M78" s="13">
+        <v>1466.654920777778</v>
+      </c>
+      <c r="N78" s="13">
+        <v>1182.084838888889</v>
+      </c>
+      <c r="O78" s="14">
+        <v>5611.1297472222222</v>
+      </c>
+      <c r="P78" s="14">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q78" s="13">
+        <v>0.13839622222222225</v>
+      </c>
+      <c r="R78" s="15">
+        <v>2.1777777777777772E-5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" s="13">
+        <v>1211.2905952222222</v>
+      </c>
+      <c r="E79" s="13">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F79" s="13">
+        <v>1.0618724444444443</v>
+      </c>
+      <c r="G79" s="5">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H79" s="13">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I79" s="13">
+        <v>6.0642897777777778</v>
+      </c>
+      <c r="J79" s="13">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K79" s="5">
+        <v>693.59226477777781</v>
+      </c>
+      <c r="L79" s="13">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M79" s="5">
+        <v>1421.0889756666668</v>
+      </c>
+      <c r="N79" s="13">
+        <v>1183.8691948888891</v>
+      </c>
+      <c r="O79" s="14">
+        <v>5611.1297472222222</v>
+      </c>
+      <c r="P79" s="14">
+        <v>27227.338324888889</v>
+      </c>
+      <c r="Q79" s="13">
+        <v>0.13742122222222222</v>
+      </c>
+      <c r="R79" s="15">
+        <v>2.1777777777777772E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D80" s="13">
+        <v>1210.7227647777777</v>
+      </c>
+      <c r="E80" s="13">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F80" s="13">
+        <v>0.79770599999999992</v>
+      </c>
+      <c r="G80" s="13">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H80" s="13">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I80" s="13">
+        <v>6.0671333333333344</v>
+      </c>
+      <c r="J80" s="13">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K80" s="13">
+        <v>693.57959655555555</v>
+      </c>
+      <c r="L80" s="13">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M80" s="13">
+        <v>1420.9534639999999</v>
+      </c>
+      <c r="N80" s="13">
+        <v>1183.1882459999999</v>
+      </c>
+      <c r="O80" s="6">
+        <v>3355.463243333334</v>
+      </c>
+      <c r="P80" s="14">
+        <v>27227.338324777778</v>
+      </c>
+      <c r="Q80" s="13">
+        <v>0.1374461111111111</v>
+      </c>
+      <c r="R80" s="15">
+        <v>2.1888888888888884E-5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="13"/>
+      <c r="N81" s="13"/>
+      <c r="O81" s="14"/>
+      <c r="P81" s="14"/>
+      <c r="Q81" s="13"/>
+      <c r="R81" s="15"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+      <c r="M82" s="2"/>
+      <c r="N82" s="2"/>
+      <c r="O82" s="3"/>
+      <c r="P82" s="3"/>
+      <c r="Q82" s="2"/>
+      <c r="R82" s="4"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>16</v>
+      </c>
+      <c r="B83" t="s">
         <v>93</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C83" t="s">
         <v>92</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D83" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E83" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F83" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G79" s="2">
+      <c r="G83" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H79" s="2">
+      <c r="H83" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I79" s="2">
+      <c r="I83" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J79" s="2">
+      <c r="J83" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K79" s="2">
+      <c r="K83" s="2">
         <v>673.08737180000003</v>
       </c>
-      <c r="L79" s="2">
+      <c r="L83" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M79" s="2">
+      <c r="M83" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N79" s="2">
+      <c r="N83" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O79" s="3">
+      <c r="O83" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P79" s="3">
+      <c r="P83" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q79" s="2">
+      <c r="Q83" s="2">
         <v>-2.3066774000000003</v>
       </c>
-      <c r="R79" s="4">
+      <c r="R83" s="4">
         <v>-7.1000000000000002E-4</v>
       </c>
-      <c r="S79" t="s">
+      <c r="S83" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>16</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B84" t="s">
         <v>95</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C84" t="s">
         <v>92</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D84" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E84" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F80" s="2">
+      <c r="F84" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G80" s="2">
+      <c r="G84" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H80" s="2">
+      <c r="H84" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I80" s="2">
+      <c r="I84" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J80" s="2">
+      <c r="J84" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K80" s="5">
+      <c r="K84" s="5">
         <v>675.4841553</v>
       </c>
-      <c r="L80" s="2">
+      <c r="L84" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M80" s="2">
+      <c r="M84" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N80" s="2">
+      <c r="N84" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O80" s="3">
+      <c r="O84" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P80" s="3">
+      <c r="P84" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q80" s="5">
+      <c r="Q84" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R80" s="7">
+      <c r="R84" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S80" t="s">
+      <c r="S84" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C87">
+        <v>2010</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="E87" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="F87" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="G87" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="H87" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I87" s="2">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="J87" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K87" s="2">
+        <v>755.98974599999997</v>
+      </c>
+      <c r="L87" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="M87" s="2">
+        <v>1371.442139</v>
+      </c>
+      <c r="N87" s="2">
+        <v>1333.3842770000001</v>
+      </c>
+      <c r="O87" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="P87" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q87" s="2">
+        <v>1.1251089999999999</v>
+      </c>
+      <c r="R87" s="4">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="S87">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88" t="s">
+        <v>102</v>
+      </c>
+      <c r="C88">
+        <v>2010</v>
+      </c>
+      <c r="D88" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="E88" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="F88" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="G88" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="H88" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="I88" s="2">
+        <v>4.971921</v>
+      </c>
+      <c r="J88" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="K88" s="2">
+        <v>755.736267</v>
+      </c>
+      <c r="L88" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="M88" s="2">
+        <v>1371.6888429999999</v>
+      </c>
+      <c r="N88" s="2">
+        <v>1333.3907469999999</v>
+      </c>
+      <c r="O88" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="P88" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="Q88" s="2">
+        <v>1.124727</v>
+      </c>
+      <c r="R88" s="4">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="S88">
+        <v>2010</v>
       </c>
     </row>
   </sheetData>
@@ -5847,11 +6172,2068 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25FC4C8C-80C5-4523-80C6-0A9555BDD035}">
+  <dimension ref="A1:Q40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:P27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2010</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4.971921</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I3" s="2">
+        <v>755.736267</v>
+      </c>
+      <c r="J3" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1371.6888429999999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1333.3907469999999</v>
+      </c>
+      <c r="M3" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N3" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1.124727</v>
+      </c>
+      <c r="P3" s="4">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2011</v>
+      </c>
+      <c r="B4">
+        <v>1333.3907469999999</v>
+      </c>
+      <c r="C4">
+        <v>1796.097168</v>
+      </c>
+      <c r="D4">
+        <v>0.64938200000000001</v>
+      </c>
+      <c r="E4">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F4">
+        <v>10.363204</v>
+      </c>
+      <c r="G4">
+        <v>5.5908110000000004</v>
+      </c>
+      <c r="H4">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I4">
+        <v>710.03326400000003</v>
+      </c>
+      <c r="J4">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K4">
+        <v>1410.5351559999999</v>
+      </c>
+      <c r="L4">
+        <v>1197.6400149999999</v>
+      </c>
+      <c r="M4">
+        <v>2649.6083979999999</v>
+      </c>
+      <c r="N4">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O4">
+        <v>-2.056495</v>
+      </c>
+      <c r="P4">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q4">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2012</v>
+      </c>
+      <c r="B5">
+        <v>1197.6400149999999</v>
+      </c>
+      <c r="C5">
+        <v>2439.6132809999999</v>
+      </c>
+      <c r="D5">
+        <v>0.87193900000000002</v>
+      </c>
+      <c r="E5">
+        <v>270.98791499999999</v>
+      </c>
+      <c r="F5">
+        <v>10.101295</v>
+      </c>
+      <c r="G5">
+        <v>4.8161160000000001</v>
+      </c>
+      <c r="H5">
+        <v>8.4196930000000005</v>
+      </c>
+      <c r="I5">
+        <v>697.88244599999996</v>
+      </c>
+      <c r="J5">
+        <v>120.810104</v>
+      </c>
+      <c r="K5">
+        <v>1767.345703</v>
+      </c>
+      <c r="L5">
+        <v>1331.1992190000001</v>
+      </c>
+      <c r="M5">
+        <v>3559.713135</v>
+      </c>
+      <c r="N5">
+        <v>28093.638672000001</v>
+      </c>
+      <c r="O5">
+        <v>1.6266039999999999</v>
+      </c>
+      <c r="P5">
+        <v>4.15E-4</v>
+      </c>
+      <c r="Q5">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2013</v>
+      </c>
+      <c r="B6">
+        <v>1331.1992190000001</v>
+      </c>
+      <c r="C6">
+        <v>1379.9248050000001</v>
+      </c>
+      <c r="D6">
+        <v>0.67753099999999999</v>
+      </c>
+      <c r="E6">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F6">
+        <v>9.8130170000000003</v>
+      </c>
+      <c r="G6">
+        <v>5.9064420000000002</v>
+      </c>
+      <c r="H6">
+        <v>8.1756840000000004</v>
+      </c>
+      <c r="I6">
+        <v>777.21038799999997</v>
+      </c>
+      <c r="J6">
+        <v>59.869819999999997</v>
+      </c>
+      <c r="K6">
+        <v>1112.5089109999999</v>
+      </c>
+      <c r="L6">
+        <v>1040.0164789999999</v>
+      </c>
+      <c r="M6">
+        <v>1653.8325199999999</v>
+      </c>
+      <c r="N6">
+        <v>27320.419922000001</v>
+      </c>
+      <c r="O6">
+        <v>1.2741000000000001E-2</v>
+      </c>
+      <c r="P6">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="Q6">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2014</v>
+      </c>
+      <c r="B7">
+        <v>1040.0164789999999</v>
+      </c>
+      <c r="C7">
+        <v>2346.181885</v>
+      </c>
+      <c r="D7">
+        <v>0.62700500000000003</v>
+      </c>
+      <c r="E7">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F7">
+        <v>9.5482680000000002</v>
+      </c>
+      <c r="G7">
+        <v>5.5257620000000003</v>
+      </c>
+      <c r="H7">
+        <v>7.9551129999999999</v>
+      </c>
+      <c r="I7">
+        <v>723.81976299999997</v>
+      </c>
+      <c r="J7">
+        <v>77.950027000000006</v>
+      </c>
+      <c r="K7">
+        <v>1658.4123540000001</v>
+      </c>
+      <c r="L7">
+        <v>1204.138672</v>
+      </c>
+      <c r="M7">
+        <v>1679.5195309999999</v>
+      </c>
+      <c r="N7">
+        <v>26614.640625</v>
+      </c>
+      <c r="O7">
+        <v>0.12900200000000001</v>
+      </c>
+      <c r="P7">
+        <v>3.4999999999999997E-5</v>
+      </c>
+      <c r="Q7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2015</v>
+      </c>
+      <c r="B8">
+        <v>1204.138672</v>
+      </c>
+      <c r="C8">
+        <v>1549.783081</v>
+      </c>
+      <c r="D8">
+        <v>0.891343</v>
+      </c>
+      <c r="E8">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F8">
+        <v>9.3388390000000001</v>
+      </c>
+      <c r="G8">
+        <v>8.5774699999999999</v>
+      </c>
+      <c r="H8">
+        <v>7.7806230000000003</v>
+      </c>
+      <c r="I8">
+        <v>666.04467799999998</v>
+      </c>
+      <c r="J8">
+        <v>50.906196999999999</v>
+      </c>
+      <c r="K8">
+        <v>1123.669067</v>
+      </c>
+      <c r="L8">
+        <v>1194.6411129999999</v>
+      </c>
+      <c r="M8">
+        <v>4403.6020509999998</v>
+      </c>
+      <c r="N8">
+        <v>26057.529297000001</v>
+      </c>
+      <c r="O8">
+        <v>6.4745999999999998E-2</v>
+      </c>
+      <c r="P8">
+        <v>2.0999999999999999E-5</v>
+      </c>
+      <c r="Q8">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2016</v>
+      </c>
+      <c r="B9">
+        <v>1194.6411129999999</v>
+      </c>
+      <c r="C9">
+        <v>1990.084595</v>
+      </c>
+      <c r="D9">
+        <v>0.92508100000000004</v>
+      </c>
+      <c r="E9">
+        <v>270.98791499999999</v>
+      </c>
+      <c r="F9">
+        <v>9.3833330000000004</v>
+      </c>
+      <c r="G9">
+        <v>5.6312860000000002</v>
+      </c>
+      <c r="H9">
+        <v>7.8212489999999999</v>
+      </c>
+      <c r="I9">
+        <v>662.38037099999997</v>
+      </c>
+      <c r="J9">
+        <v>94.515556000000004</v>
+      </c>
+      <c r="K9">
+        <v>1480.9849850000001</v>
+      </c>
+      <c r="L9">
+        <v>1225.4578859999999</v>
+      </c>
+      <c r="M9">
+        <v>4338.1889650000003</v>
+      </c>
+      <c r="N9">
+        <v>26184.960938</v>
+      </c>
+      <c r="O9">
+        <v>-0.49327599999999999</v>
+      </c>
+      <c r="P9">
+        <v>-1.4200000000000001E-4</v>
+      </c>
+      <c r="Q9">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2017</v>
+      </c>
+      <c r="B10">
+        <v>1225.4578859999999</v>
+      </c>
+      <c r="C10">
+        <v>2105.5676269999999</v>
+      </c>
+      <c r="D10">
+        <v>0.55353600000000003</v>
+      </c>
+      <c r="E10">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F10">
+        <v>9.3968910000000001</v>
+      </c>
+      <c r="G10">
+        <v>5.0438409999999996</v>
+      </c>
+      <c r="H10">
+        <v>7.8289910000000003</v>
+      </c>
+      <c r="I10">
+        <v>700.13690199999996</v>
+      </c>
+      <c r="J10">
+        <v>89.795829999999995</v>
+      </c>
+      <c r="K10">
+        <v>1734.2989500000001</v>
+      </c>
+      <c r="L10">
+        <v>1085.996948</v>
+      </c>
+      <c r="M10">
+        <v>1670.2463379999999</v>
+      </c>
+      <c r="N10">
+        <v>26228.105468999998</v>
+      </c>
+      <c r="O10">
+        <v>1.790313</v>
+      </c>
+      <c r="P10">
+        <v>4.95E-4</v>
+      </c>
+      <c r="Q10">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2018</v>
+      </c>
+      <c r="B11">
+        <v>1085.996948</v>
+      </c>
+      <c r="C11">
+        <v>1414.644775</v>
+      </c>
+      <c r="D11">
+        <v>0.53712000000000004</v>
+      </c>
+      <c r="E11">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F11">
+        <v>9.4224359999999994</v>
+      </c>
+      <c r="G11">
+        <v>8.5405510000000007</v>
+      </c>
+      <c r="H11">
+        <v>7.850276</v>
+      </c>
+      <c r="I11">
+        <v>548.97229000000004</v>
+      </c>
+      <c r="J11">
+        <v>66.255104000000003</v>
+      </c>
+      <c r="K11">
+        <v>1129.137207</v>
+      </c>
+      <c r="L11">
+        <v>1036.213135</v>
+      </c>
+      <c r="M11">
+        <v>1971.369385</v>
+      </c>
+      <c r="N11">
+        <v>26304.007812</v>
+      </c>
+      <c r="O11">
+        <v>-0.96134699999999995</v>
+      </c>
+      <c r="P11">
+        <v>-3.4499999999999998E-4</v>
+      </c>
+      <c r="Q11">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2019</v>
+      </c>
+      <c r="B12">
+        <v>1036.213135</v>
+      </c>
+      <c r="C12">
+        <v>1469.0946039999999</v>
+      </c>
+      <c r="D12">
+        <v>0.72606300000000001</v>
+      </c>
+      <c r="E12">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F12">
+        <v>9.4400619999999993</v>
+      </c>
+      <c r="G12">
+        <v>7.4573460000000003</v>
+      </c>
+      <c r="H12">
+        <v>7.8649579999999997</v>
+      </c>
+      <c r="I12">
+        <v>677.703125</v>
+      </c>
+      <c r="J12">
+        <v>70.424828000000005</v>
+      </c>
+      <c r="K12">
+        <v>1163.58374</v>
+      </c>
+      <c r="L12">
+        <v>873.25817900000004</v>
+      </c>
+      <c r="M12">
+        <v>2767.766846</v>
+      </c>
+      <c r="N12">
+        <v>26356.542968999998</v>
+      </c>
+      <c r="O12">
+        <v>-0.34390900000000002</v>
+      </c>
+      <c r="P12">
+        <v>-1.2300000000000001E-4</v>
+      </c>
+      <c r="Q12">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2020</v>
+      </c>
+      <c r="B13">
+        <v>873.25817900000004</v>
+      </c>
+      <c r="C13">
+        <v>1888.009155</v>
+      </c>
+      <c r="D13">
+        <v>0.76152200000000003</v>
+      </c>
+      <c r="E13">
+        <v>270.98791499999999</v>
+      </c>
+      <c r="F13">
+        <v>9.4790550000000007</v>
+      </c>
+      <c r="G13">
+        <v>7.2725099999999996</v>
+      </c>
+      <c r="H13">
+        <v>7.9010379999999998</v>
+      </c>
+      <c r="I13">
+        <v>696.08813499999997</v>
+      </c>
+      <c r="J13">
+        <v>90.618942000000004</v>
+      </c>
+      <c r="K13">
+        <v>1264.7332759999999</v>
+      </c>
+      <c r="L13">
+        <v>989.89398200000005</v>
+      </c>
+      <c r="M13">
+        <v>3506.4147950000001</v>
+      </c>
+      <c r="N13">
+        <v>26471.685547000001</v>
+      </c>
+      <c r="O13">
+        <v>-0.53296299999999996</v>
+      </c>
+      <c r="P13">
+        <v>-1.75E-4</v>
+      </c>
+      <c r="Q13">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2">
+        <f>AVERAGE(B3:B11)</f>
+        <v>1210.7227647777777</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" ref="C14:P14" si="0">AVERAGE(C3:C11)</f>
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.79770599999999992</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>270.41205844444437</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>6.0671333333333344</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="0"/>
+        <v>693.57959655555555</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="0"/>
+        <v>82.308506444444433</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="0"/>
+        <v>1420.9534639999999</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="0"/>
+        <v>1183.1882459999999</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="0"/>
+        <v>3355.463243333334</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324777778</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1374461111111111</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="0"/>
+        <v>2.1888888888888884E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" t="s">
+        <v>13</v>
+      </c>
+      <c r="P17" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2010</v>
+      </c>
+      <c r="B18">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C18">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D18">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E18">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F18">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G18">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H18">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I18">
+        <v>755.98974599999997</v>
+      </c>
+      <c r="J18">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K18">
+        <v>1371.442139</v>
+      </c>
+      <c r="L18">
+        <v>1333.3842770000001</v>
+      </c>
+      <c r="M18">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N18">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O18">
+        <v>1.1251089999999999</v>
+      </c>
+      <c r="P18">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q18">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2011</v>
+      </c>
+      <c r="B19">
+        <v>1333.3842770000001</v>
+      </c>
+      <c r="C19">
+        <v>1796.097168</v>
+      </c>
+      <c r="D19">
+        <v>0.94261200000000001</v>
+      </c>
+      <c r="E19">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F19">
+        <v>10.363204</v>
+      </c>
+      <c r="G19">
+        <v>5.5840180000000004</v>
+      </c>
+      <c r="H19">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I19">
+        <v>709.59491000000003</v>
+      </c>
+      <c r="J19">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K19">
+        <v>1410.7021480000001</v>
+      </c>
+      <c r="L19">
+        <v>1198.1911620000001</v>
+      </c>
+      <c r="M19">
+        <v>4586.8471680000002</v>
+      </c>
+      <c r="N19">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O19">
+        <v>-2.0566779999999998</v>
+      </c>
+      <c r="P19">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q19">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2012</v>
+      </c>
+      <c r="B20">
+        <v>1198.1911620000001</v>
+      </c>
+      <c r="C20">
+        <v>2439.6132809999999</v>
+      </c>
+      <c r="D20">
+        <v>1.4083209999999999</v>
+      </c>
+      <c r="E20">
+        <v>270.98791499999999</v>
+      </c>
+      <c r="F20">
+        <v>10.101295</v>
+      </c>
+      <c r="G20">
+        <v>4.8155799999999997</v>
+      </c>
+      <c r="H20">
+        <v>8.4196930000000005</v>
+      </c>
+      <c r="I20">
+        <v>698.32501200000002</v>
+      </c>
+      <c r="J20">
+        <v>120.810104</v>
+      </c>
+      <c r="K20">
+        <v>1767.443726</v>
+      </c>
+      <c r="L20">
+        <v>1331.7452390000001</v>
+      </c>
+      <c r="M20">
+        <v>7521.1850590000004</v>
+      </c>
+      <c r="N20">
+        <v>28093.638672000001</v>
+      </c>
+      <c r="O20">
+        <v>1.62622</v>
+      </c>
+      <c r="P20">
+        <v>4.1399999999999998E-4</v>
+      </c>
+      <c r="Q20">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2013</v>
+      </c>
+      <c r="B21">
+        <v>1331.7452390000001</v>
+      </c>
+      <c r="C21">
+        <v>1379.9248050000001</v>
+      </c>
+      <c r="D21">
+        <v>0.81979199999999997</v>
+      </c>
+      <c r="E21">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F21">
+        <v>9.8130170000000003</v>
+      </c>
+      <c r="G21">
+        <v>5.9076300000000002</v>
+      </c>
+      <c r="H21">
+        <v>8.1756840000000004</v>
+      </c>
+      <c r="I21">
+        <v>776.65783699999997</v>
+      </c>
+      <c r="J21">
+        <v>59.869819999999997</v>
+      </c>
+      <c r="K21">
+        <v>1112.962769</v>
+      </c>
+      <c r="L21">
+        <v>1040.8048100000001</v>
+      </c>
+      <c r="M21">
+        <v>3262.7998050000001</v>
+      </c>
+      <c r="N21">
+        <v>27320.419922000001</v>
+      </c>
+      <c r="O21">
+        <v>1.2907E-2</v>
+      </c>
+      <c r="P21">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="Q21">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2014</v>
+      </c>
+      <c r="B22">
+        <v>1040.8048100000001</v>
+      </c>
+      <c r="C22">
+        <v>2346.181885</v>
+      </c>
+      <c r="D22">
+        <v>0.856595</v>
+      </c>
+      <c r="E22">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F22">
+        <v>9.5482680000000002</v>
+      </c>
+      <c r="G22">
+        <v>5.5137869999999998</v>
+      </c>
+      <c r="H22">
+        <v>7.9551129999999999</v>
+      </c>
+      <c r="I22">
+        <v>723.80175799999995</v>
+      </c>
+      <c r="J22">
+        <v>77.950027000000006</v>
+      </c>
+      <c r="K22">
+        <v>1658.7143550000001</v>
+      </c>
+      <c r="L22">
+        <v>1204.8604740000001</v>
+      </c>
+      <c r="M22">
+        <v>3795.5959469999998</v>
+      </c>
+      <c r="N22">
+        <v>26614.640625</v>
+      </c>
+      <c r="O22">
+        <v>0.128855</v>
+      </c>
+      <c r="P22">
+        <v>3.4999999999999997E-5</v>
+      </c>
+      <c r="Q22">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2015</v>
+      </c>
+      <c r="B23">
+        <v>1204.8604740000001</v>
+      </c>
+      <c r="C23">
+        <v>1549.783081</v>
+      </c>
+      <c r="D23">
+        <v>1.2800210000000001</v>
+      </c>
+      <c r="E23">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F23">
+        <v>9.3388390000000001</v>
+      </c>
+      <c r="G23">
+        <v>8.5799669999999999</v>
+      </c>
+      <c r="H23">
+        <v>7.7806230000000003</v>
+      </c>
+      <c r="I23">
+        <v>666.39453100000003</v>
+      </c>
+      <c r="J23">
+        <v>50.906196999999999</v>
+      </c>
+      <c r="K23">
+        <v>1123.6132809999999</v>
+      </c>
+      <c r="L23">
+        <v>1195.4602050000001</v>
+      </c>
+      <c r="M23">
+        <v>8177.5766599999997</v>
+      </c>
+      <c r="N23">
+        <v>26057.529297000001</v>
+      </c>
+      <c r="O23">
+        <v>6.4928E-2</v>
+      </c>
+      <c r="P23">
+        <v>2.0999999999999999E-5</v>
+      </c>
+      <c r="Q23">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2016</v>
+      </c>
+      <c r="B24">
+        <v>1195.4602050000001</v>
+      </c>
+      <c r="C24">
+        <v>1990.084595</v>
+      </c>
+      <c r="D24">
+        <v>1.131345</v>
+      </c>
+      <c r="E24">
+        <v>270.98791499999999</v>
+      </c>
+      <c r="F24">
+        <v>9.3833330000000004</v>
+      </c>
+      <c r="G24">
+        <v>5.6367320000000003</v>
+      </c>
+      <c r="H24">
+        <v>7.8212489999999999</v>
+      </c>
+      <c r="I24">
+        <v>662.680969</v>
+      </c>
+      <c r="J24">
+        <v>94.515556000000004</v>
+      </c>
+      <c r="K24">
+        <v>1480.8908690000001</v>
+      </c>
+      <c r="L24">
+        <v>1226.2822269999999</v>
+      </c>
+      <c r="M24">
+        <v>7506.1694340000004</v>
+      </c>
+      <c r="N24">
+        <v>26184.960938</v>
+      </c>
+      <c r="O24">
+        <v>-0.493255</v>
+      </c>
+      <c r="P24">
+        <v>-1.4200000000000001E-4</v>
+      </c>
+      <c r="Q24">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2017</v>
+      </c>
+      <c r="B25">
+        <v>1226.2822269999999</v>
+      </c>
+      <c r="C25">
+        <v>2105.5676269999999</v>
+      </c>
+      <c r="D25">
+        <v>0.74674399999999996</v>
+      </c>
+      <c r="E25">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F25">
+        <v>9.3968910000000001</v>
+      </c>
+      <c r="G25">
+        <v>5.0378579999999999</v>
+      </c>
+      <c r="H25">
+        <v>7.8289910000000003</v>
+      </c>
+      <c r="I25">
+        <v>700.01544200000001</v>
+      </c>
+      <c r="J25">
+        <v>89.795829999999995</v>
+      </c>
+      <c r="K25">
+        <v>1734.5657960000001</v>
+      </c>
+      <c r="L25">
+        <v>1086.863159</v>
+      </c>
+      <c r="M25">
+        <v>3097.1513669999999</v>
+      </c>
+      <c r="N25">
+        <v>26228.105468999998</v>
+      </c>
+      <c r="O25">
+        <v>1.790343</v>
+      </c>
+      <c r="P25">
+        <v>4.95E-4</v>
+      </c>
+      <c r="Q25">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2018</v>
+      </c>
+      <c r="B26">
+        <v>1086.863159</v>
+      </c>
+      <c r="C26">
+        <v>1414.644775</v>
+      </c>
+      <c r="D26">
+        <v>0.92500499999999997</v>
+      </c>
+      <c r="E26">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F26">
+        <v>9.4224359999999994</v>
+      </c>
+      <c r="G26">
+        <v>8.5311920000000008</v>
+      </c>
+      <c r="H26">
+        <v>7.850276</v>
+      </c>
+      <c r="I26">
+        <v>548.87017800000001</v>
+      </c>
+      <c r="J26">
+        <v>66.255104000000003</v>
+      </c>
+      <c r="K26">
+        <v>1129.465698</v>
+      </c>
+      <c r="L26">
+        <v>1037.2312010000001</v>
+      </c>
+      <c r="M26">
+        <v>4279.7534180000002</v>
+      </c>
+      <c r="N26">
+        <v>26304.007813</v>
+      </c>
+      <c r="O26">
+        <v>-0.96163799999999999</v>
+      </c>
+      <c r="P26">
+        <v>-3.4499999999999998E-4</v>
+      </c>
+      <c r="Q26">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <f>AVERAGE(B18:B26)</f>
+        <v>1211.2905952222222</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" ref="C27" si="1">AVERAGE(C18:C26)</f>
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" ref="D27" si="2">AVERAGE(D18:D26)</f>
+        <v>1.0618724444444443</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" ref="E27" si="3">AVERAGE(E18:E26)</f>
+        <v>270.41205844444437</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" ref="F27" si="4">AVERAGE(F18:F26)</f>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" ref="G27" si="5">AVERAGE(G18:G26)</f>
+        <v>6.0642897777777778</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" ref="H27" si="6">AVERAGE(H18:H26)</f>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" ref="I27" si="7">AVERAGE(I18:I26)</f>
+        <v>693.59226477777781</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" ref="J27" si="8">AVERAGE(J18:J26)</f>
+        <v>82.308506444444433</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" ref="K27" si="9">AVERAGE(K18:K26)</f>
+        <v>1421.0889756666668</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" ref="L27" si="10">AVERAGE(L18:L26)</f>
+        <v>1183.8691948888891</v>
+      </c>
+      <c r="M27" s="3">
+        <f t="shared" ref="M27" si="11">AVERAGE(M18:M26)</f>
+        <v>5611.1297472222222</v>
+      </c>
+      <c r="N27" s="3">
+        <f t="shared" ref="N27" si="12">AVERAGE(N18:N26)</f>
+        <v>27227.338324888889</v>
+      </c>
+      <c r="O27" s="2">
+        <f t="shared" ref="O27" si="13">AVERAGE(O18:O26)</f>
+        <v>0.13742122222222222</v>
+      </c>
+      <c r="P27" s="4">
+        <f t="shared" ref="P27" si="14">AVERAGE(P18:P26)</f>
+        <v>2.1777777777777772E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="4"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30" t="s">
+        <v>10</v>
+      </c>
+      <c r="M30" t="s">
+        <v>11</v>
+      </c>
+      <c r="N30" t="s">
+        <v>12</v>
+      </c>
+      <c r="O30" t="s">
+        <v>13</v>
+      </c>
+      <c r="P30" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2010</v>
+      </c>
+      <c r="B31" s="2">
+        <f>B3-B18</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" ref="C31:P31" si="15">C3-C18</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="15"/>
+        <v>7.7000000000104762E-5</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="15"/>
+        <v>-0.25347899999997026</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="15"/>
+        <v>0.24670399999990877</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="15"/>
+        <v>6.4699999998083513E-3</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="2">
+        <f t="shared" si="15"/>
+        <v>-3.8199999999988243E-4</v>
+      </c>
+      <c r="P31" s="2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2011</v>
+      </c>
+      <c r="B32" s="2">
+        <f>B4-B19</f>
+        <v>6.4699999998083513E-3</v>
+      </c>
+      <c r="C32" s="2">
+        <f>C4-C19</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <f>D4-D19</f>
+        <v>-0.29322999999999999</v>
+      </c>
+      <c r="E32" s="2">
+        <f>E4-E19</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <f>F4-F19</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <f>G4-G19</f>
+        <v>6.793000000000049E-3</v>
+      </c>
+      <c r="H32" s="2">
+        <f>H4-H19</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <f>I4-I19</f>
+        <v>0.43835400000000391</v>
+      </c>
+      <c r="J32" s="2">
+        <f>J4-J19</f>
+        <v>0</v>
+      </c>
+      <c r="K32" s="2">
+        <f>K4-K19</f>
+        <v>-0.1669920000001639</v>
+      </c>
+      <c r="L32" s="2">
+        <f>L4-L19</f>
+        <v>-0.55114700000012817</v>
+      </c>
+      <c r="M32" s="2">
+        <f>M4-M19</f>
+        <v>-1937.2387700000004</v>
+      </c>
+      <c r="N32" s="2">
+        <f>N4-N19</f>
+        <v>0</v>
+      </c>
+      <c r="O32" s="2">
+        <f>O4-O19</f>
+        <v>1.8299999999982219E-4</v>
+      </c>
+      <c r="P32" s="2">
+        <f>P4-P19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2012</v>
+      </c>
+      <c r="B33" s="2">
+        <f>B5-B20</f>
+        <v>-0.55114700000012817</v>
+      </c>
+      <c r="C33" s="2">
+        <f>C5-C20</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <f>D5-D20</f>
+        <v>-0.53638199999999991</v>
+      </c>
+      <c r="E33" s="2">
+        <f>E5-E20</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <f>F5-F20</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="2">
+        <f>G5-G20</f>
+        <v>5.36000000000314E-4</v>
+      </c>
+      <c r="H33" s="2">
+        <f>H5-H20</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <f>I5-I20</f>
+        <v>-0.44256600000005619</v>
+      </c>
+      <c r="J33" s="2">
+        <f>J5-J20</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="2">
+        <f>K5-K20</f>
+        <v>-9.8023000000011962E-2</v>
+      </c>
+      <c r="L33" s="2">
+        <f>L5-L20</f>
+        <v>-0.54601999999999862</v>
+      </c>
+      <c r="M33" s="2">
+        <f>M5-M20</f>
+        <v>-3961.4719240000004</v>
+      </c>
+      <c r="N33" s="2">
+        <f>N5-N20</f>
+        <v>0</v>
+      </c>
+      <c r="O33" s="2">
+        <f>O5-O20</f>
+        <v>3.8399999999993994E-4</v>
+      </c>
+      <c r="P33" s="2">
+        <f>P5-P20</f>
+        <v>1.0000000000000243E-6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2013</v>
+      </c>
+      <c r="B34" s="2">
+        <f>B6-B21</f>
+        <v>-0.54601999999999862</v>
+      </c>
+      <c r="C34" s="2">
+        <f>C6-C21</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <f>D6-D21</f>
+        <v>-0.14226099999999997</v>
+      </c>
+      <c r="E34" s="2">
+        <f>E6-E21</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <f>F6-F21</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <f>G6-G21</f>
+        <v>-1.1879999999999669E-3</v>
+      </c>
+      <c r="H34" s="2">
+        <f>H6-H21</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <f>I6-I21</f>
+        <v>0.55255099999999402</v>
+      </c>
+      <c r="J34" s="2">
+        <f>J6-J21</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="2">
+        <f>K6-K21</f>
+        <v>-0.45385800000008203</v>
+      </c>
+      <c r="L34" s="2">
+        <f>L6-L21</f>
+        <v>-0.7883310000001984</v>
+      </c>
+      <c r="M34" s="2">
+        <f>M6-M21</f>
+        <v>-1608.9672850000002</v>
+      </c>
+      <c r="N34" s="2">
+        <f>N6-N21</f>
+        <v>0</v>
+      </c>
+      <c r="O34" s="2">
+        <f>O6-O21</f>
+        <v>-1.6599999999999948E-4</v>
+      </c>
+      <c r="P34" s="2">
+        <f>P6-P21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2014</v>
+      </c>
+      <c r="B35" s="2">
+        <f>B7-B22</f>
+        <v>-0.7883310000001984</v>
+      </c>
+      <c r="C35" s="2">
+        <f>C7-C22</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <f>D7-D22</f>
+        <v>-0.22958999999999996</v>
+      </c>
+      <c r="E35" s="2">
+        <f>E7-E22</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <f>F7-F22</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <f>G7-G22</f>
+        <v>1.1975000000000513E-2</v>
+      </c>
+      <c r="H35" s="2">
+        <f>H7-H22</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="2">
+        <f>I7-I22</f>
+        <v>1.800500000001648E-2</v>
+      </c>
+      <c r="J35" s="2">
+        <f>J7-J22</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
+        <f>K7-K22</f>
+        <v>-0.30200100000001839</v>
+      </c>
+      <c r="L35" s="2">
+        <f>L7-L22</f>
+        <v>-0.72180200000002515</v>
+      </c>
+      <c r="M35" s="2">
+        <f>M7-M22</f>
+        <v>-2116.0764159999999</v>
+      </c>
+      <c r="N35" s="2">
+        <f>N7-N22</f>
+        <v>0</v>
+      </c>
+      <c r="O35" s="2">
+        <f>O7-O22</f>
+        <v>1.4700000000000824E-4</v>
+      </c>
+      <c r="P35" s="2">
+        <f>P7-P22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2015</v>
+      </c>
+      <c r="B36" s="2">
+        <f>B8-B23</f>
+        <v>-0.72180200000002515</v>
+      </c>
+      <c r="C36" s="2">
+        <f>C8-C23</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <f>D8-D23</f>
+        <v>-0.38867800000000008</v>
+      </c>
+      <c r="E36" s="2">
+        <f>E8-E23</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <f>F8-F23</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
+        <f>G8-G23</f>
+        <v>-2.4969999999999715E-3</v>
+      </c>
+      <c r="H36" s="2">
+        <f>H8-H23</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="2">
+        <f>I8-I23</f>
+        <v>-0.34985300000005282</v>
+      </c>
+      <c r="J36" s="2">
+        <f>J8-J23</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="2">
+        <f>K8-K23</f>
+        <v>5.5786000000125568E-2</v>
+      </c>
+      <c r="L36" s="2">
+        <f>L8-L23</f>
+        <v>-0.81909200000018245</v>
+      </c>
+      <c r="M36" s="2">
+        <f>M8-M23</f>
+        <v>-3773.9746089999999</v>
+      </c>
+      <c r="N36" s="2">
+        <f>N8-N23</f>
+        <v>0</v>
+      </c>
+      <c r="O36" s="2">
+        <f>O8-O23</f>
+        <v>-1.820000000000016E-4</v>
+      </c>
+      <c r="P36" s="2">
+        <f>P8-P23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2016</v>
+      </c>
+      <c r="B37" s="2">
+        <f>B9-B24</f>
+        <v>-0.81909200000018245</v>
+      </c>
+      <c r="C37" s="2">
+        <f>C9-C24</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <f>D9-D24</f>
+        <v>-0.206264</v>
+      </c>
+      <c r="E37" s="2">
+        <f>E9-E24</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <f>F9-F24</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <f>G9-G24</f>
+        <v>-5.4460000000000619E-3</v>
+      </c>
+      <c r="H37" s="2">
+        <f>H9-H24</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="2">
+        <f>I9-I24</f>
+        <v>-0.30059800000003634</v>
+      </c>
+      <c r="J37" s="2">
+        <f>J9-J24</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="2">
+        <f>K9-K24</f>
+        <v>9.4115999999985434E-2</v>
+      </c>
+      <c r="L37" s="2">
+        <f>L9-L24</f>
+        <v>-0.82434100000000399</v>
+      </c>
+      <c r="M37" s="2">
+        <f>M9-M24</f>
+        <v>-3167.9804690000001</v>
+      </c>
+      <c r="N37" s="2">
+        <f>N9-N24</f>
+        <v>0</v>
+      </c>
+      <c r="O37" s="2">
+        <f>O9-O24</f>
+        <v>-2.0999999999993246E-5</v>
+      </c>
+      <c r="P37" s="2">
+        <f>P9-P24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2017</v>
+      </c>
+      <c r="B38" s="2">
+        <f>B10-B25</f>
+        <v>-0.82434100000000399</v>
+      </c>
+      <c r="C38" s="2">
+        <f>C10-C25</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <f>D10-D25</f>
+        <v>-0.19320799999999994</v>
+      </c>
+      <c r="E38" s="2">
+        <f>E10-E25</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <f>F10-F25</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <f>G10-G25</f>
+        <v>5.9829999999996275E-3</v>
+      </c>
+      <c r="H38" s="2">
+        <f>H10-H25</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="2">
+        <f>I10-I25</f>
+        <v>0.12145999999995638</v>
+      </c>
+      <c r="J38" s="2">
+        <f>J10-J25</f>
+        <v>0</v>
+      </c>
+      <c r="K38" s="2">
+        <f>K10-K25</f>
+        <v>-0.26684599999998682</v>
+      </c>
+      <c r="L38" s="2">
+        <f>L10-L25</f>
+        <v>-0.86621100000002116</v>
+      </c>
+      <c r="M38" s="2">
+        <f>M10-M25</f>
+        <v>-1426.905029</v>
+      </c>
+      <c r="N38" s="2">
+        <f>N10-N25</f>
+        <v>0</v>
+      </c>
+      <c r="O38" s="2">
+        <f>O10-O25</f>
+        <v>-2.9999999999974492E-5</v>
+      </c>
+      <c r="P38" s="2">
+        <f>P10-P25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2018</v>
+      </c>
+      <c r="B39" s="2">
+        <f>B11-B26</f>
+        <v>-0.86621100000002116</v>
+      </c>
+      <c r="C39" s="2">
+        <f>C11-C26</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
+        <f>D11-D26</f>
+        <v>-0.38788499999999992</v>
+      </c>
+      <c r="E39" s="2">
+        <f>E11-E26</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <f>F11-F26</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <f>G11-G26</f>
+        <v>9.3589999999998952E-3</v>
+      </c>
+      <c r="H39" s="2">
+        <f>H11-H26</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="2">
+        <f>I11-I26</f>
+        <v>0.10211200000003373</v>
+      </c>
+      <c r="J39" s="2">
+        <f>J11-J26</f>
+        <v>0</v>
+      </c>
+      <c r="K39" s="2">
+        <f>K11-K26</f>
+        <v>-0.32849099999998543</v>
+      </c>
+      <c r="L39" s="2">
+        <f>L11-L26</f>
+        <v>-1.0180660000000898</v>
+      </c>
+      <c r="M39" s="2">
+        <f>M11-M26</f>
+        <v>-2308.3840330000003</v>
+      </c>
+      <c r="N39" s="2">
+        <f>N11-N26</f>
+        <v>-1.0000003385357559E-6</v>
+      </c>
+      <c r="O39" s="2">
+        <f>O11-O26</f>
+        <v>2.9100000000004123E-4</v>
+      </c>
+      <c r="P39" s="2">
+        <f>P11-P26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B40" s="2">
+        <f>AVERAGE(B31:B39)</f>
+        <v>-0.56783044444452768</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" ref="C40:P40" si="16">AVERAGE(C31:C39)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="16"/>
+        <v>-0.26416644444444443</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="16"/>
+        <v>2.8435555555556113E-3</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="16"/>
+        <v>-1.2668222222234564E-2</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="16"/>
+        <v>-0.13551166666669209</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="16"/>
+        <v>-0.6809488888889822</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="16"/>
+        <v>-2255.6665038888896</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="16"/>
+        <v>-1.111111487261951E-7</v>
+      </c>
+      <c r="O40" s="2">
+        <f t="shared" si="16"/>
+        <v>2.4888888888884481E-5</v>
+      </c>
+      <c r="P40" s="2">
+        <f t="shared" si="16"/>
+        <v>1.1111111111111381E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD84CEC-7113-4714-90A2-84947C9E014D}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6037,12 +8419,71 @@
         <v>2020</v>
       </c>
     </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="2">
+        <v>873.22174099999995</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1888.009155</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.4834149999999999</v>
+      </c>
+      <c r="G4" s="2">
+        <v>270.98791499999999</v>
+      </c>
+      <c r="H4" s="2">
+        <v>11.634945</v>
+      </c>
+      <c r="I4" s="2">
+        <v>7.84185</v>
+      </c>
+      <c r="J4" s="2">
+        <v>9.6980299999999993</v>
+      </c>
+      <c r="K4" s="2">
+        <v>765.64221199999997</v>
+      </c>
+      <c r="L4" s="2">
+        <v>99.961585999999997</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1191.4267580000001</v>
+      </c>
+      <c r="N4" s="2">
+        <v>987.38439900000003</v>
+      </c>
+      <c r="O4" s="3">
+        <v>8747.7519530000009</v>
+      </c>
+      <c r="P4" s="3">
+        <v>32251.826172000001</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0.93396400000000002</v>
+      </c>
+      <c r="R4" s="4">
+        <v>3.0600000000000001E-4</v>
+      </c>
+      <c r="S4">
+        <v>2020</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD88AF4-3325-45AB-9D19-94573DCD22C4}">
   <dimension ref="A1:S6"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fix the irrigation anomaly. EvapTrans.cpp - Separate the 3 ET cases in EvapTrans::Init(), StartYear(), and StartStep().
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50F3703-BDF1-49B2-AEA2-5E57EA835DAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC226355-57DF-4F20-8B12-8A68F1FEFC8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
-    <sheet name="C330 comparisons" sheetId="3" r:id="rId2"/>
-    <sheet name="2000-09" sheetId="2" r:id="rId3"/>
+    <sheet name="2000-09" sheetId="2" r:id="rId2"/>
+    <sheet name="C330 comparisons" sheetId="3" r:id="rId3"/>
+    <sheet name="irrigation anomaly" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="109">
   <si>
     <t>Year</t>
   </si>
@@ -338,6 +339,27 @@
   </si>
   <si>
     <t>C318</t>
+  </si>
+  <si>
+    <t>C319+</t>
+  </si>
+  <si>
+    <t>C319+, except without the change in ReachRouting.cpp</t>
+  </si>
+  <si>
+    <t>C319+, except without the change in ReachRouting.cpp, and in Flow.xml the new &lt;evap_trans&gt; WetlandsET block has been commented out</t>
+  </si>
+  <si>
+    <t>C319+, with a correction in EvapTrans::SetMethod()</t>
+  </si>
+  <si>
+    <t>C319+, with corrections at EvapTrans.cpp: 169, 499, and 1561, but not yet at 1182</t>
+  </si>
+  <si>
+    <t>C319+, with corrections at EvapTrans.cpp: 169, 499, and 1561, 1182, and in EvapTrans::StartYear() and StartStep()</t>
+  </si>
+  <si>
+    <t>C333</t>
   </si>
 </sst>
 </file>
@@ -5850,1531 +5872,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD84CEC-7113-4714-90A2-84947C9E014D}">
-  <dimension ref="A1:Q38"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37:N38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="12" width="8.88671875" style="2"/>
-    <col min="13" max="14" width="8.88671875" style="3"/>
-    <col min="15" max="15" width="8.88671875" style="2"/>
-    <col min="16" max="16" width="9.21875" style="4" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2010</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1284.0238039999999</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1990.4650879999999</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.4464170000000001</v>
-      </c>
-      <c r="E3" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F3" s="2">
-        <v>10.610913999999999</v>
-      </c>
-      <c r="G3" s="2">
-        <v>4.9718439999999999</v>
-      </c>
-      <c r="H3" s="2">
-        <v>8.8404570000000007</v>
-      </c>
-      <c r="I3" s="2">
-        <v>755.977844</v>
-      </c>
-      <c r="J3" s="2">
-        <v>93.234084999999993</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1371.4539789999999</v>
-      </c>
-      <c r="L3" s="2">
-        <v>1333.384399</v>
-      </c>
-      <c r="M3" s="3">
-        <v>8273.0888670000004</v>
-      </c>
-      <c r="N3" s="3">
-        <v>29450.638672000001</v>
-      </c>
-      <c r="O3" s="2">
-        <v>1.12517</v>
-      </c>
-      <c r="P3" s="4">
-        <v>3.1599999999999998E-4</v>
-      </c>
-      <c r="Q3">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2011</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1333.384399</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1796.097168</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.94261200000000001</v>
-      </c>
-      <c r="E4" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F4" s="2">
-        <v>10.363204</v>
-      </c>
-      <c r="G4" s="2">
-        <v>5.5840180000000004</v>
-      </c>
-      <c r="H4" s="2">
-        <v>8.6340749999999993</v>
-      </c>
-      <c r="I4" s="2">
-        <v>709.58264199999996</v>
-      </c>
-      <c r="J4" s="2">
-        <v>87.439835000000002</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1410.7139890000001</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1198.1915280000001</v>
-      </c>
-      <c r="M4" s="3">
-        <v>4586.8471680000002</v>
-      </c>
-      <c r="N4" s="3">
-        <v>28792.103515999999</v>
-      </c>
-      <c r="O4" s="2">
-        <v>-2.0568610000000001</v>
-      </c>
-      <c r="P4" s="4">
-        <v>-6.02E-4</v>
-      </c>
-      <c r="Q4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2010</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1284.0238039999999</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1990.4650879999999</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.4464170000000001</v>
-      </c>
-      <c r="E9" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F9" s="2">
-        <v>10.610913999999999</v>
-      </c>
-      <c r="G9" s="2">
-        <v>4.971921</v>
-      </c>
-      <c r="H9" s="2">
-        <v>8.8404570000000007</v>
-      </c>
-      <c r="I9" s="2">
-        <v>755.736267</v>
-      </c>
-      <c r="J9" s="2">
-        <v>93.234084999999993</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1371.6888429999999</v>
-      </c>
-      <c r="L9" s="2">
-        <v>1333.3907469999999</v>
-      </c>
-      <c r="M9" s="3">
-        <v>8273.0888670000004</v>
-      </c>
-      <c r="N9" s="3">
-        <v>29450.638672000001</v>
-      </c>
-      <c r="O9" s="2">
-        <v>1.124727</v>
-      </c>
-      <c r="P9" s="4">
-        <v>3.1599999999999998E-4</v>
-      </c>
-      <c r="Q9">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2011</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1333.3907469999999</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1796.097168</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.64938200000000001</v>
-      </c>
-      <c r="E10" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F10" s="2">
-        <v>10.363204</v>
-      </c>
-      <c r="G10" s="2">
-        <v>5.5908110000000004</v>
-      </c>
-      <c r="H10" s="2">
-        <v>8.6340749999999993</v>
-      </c>
-      <c r="I10" s="2">
-        <v>710.03326400000003</v>
-      </c>
-      <c r="J10" s="2">
-        <v>87.439835000000002</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1410.5351559999999</v>
-      </c>
-      <c r="L10" s="2">
-        <v>1197.6400149999999</v>
-      </c>
-      <c r="M10" s="3">
-        <v>2649.6083979999999</v>
-      </c>
-      <c r="N10" s="3">
-        <v>28792.103515999999</v>
-      </c>
-      <c r="O10" s="2">
-        <v>-2.056495</v>
-      </c>
-      <c r="P10" s="4">
-        <v>-6.02E-4</v>
-      </c>
-      <c r="Q10">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2012</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1197.6400149999999</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2439.6132809999999</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.87193900000000002</v>
-      </c>
-      <c r="E11" s="2">
-        <v>270.98791499999999</v>
-      </c>
-      <c r="F11" s="2">
-        <v>10.101295</v>
-      </c>
-      <c r="G11" s="2">
-        <v>4.8161160000000001</v>
-      </c>
-      <c r="H11" s="2">
-        <v>8.4196930000000005</v>
-      </c>
-      <c r="I11" s="2">
-        <v>697.88244599999996</v>
-      </c>
-      <c r="J11" s="2">
-        <v>120.810104</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1767.345703</v>
-      </c>
-      <c r="L11" s="2">
-        <v>1331.1992190000001</v>
-      </c>
-      <c r="M11" s="3">
-        <v>3559.713135</v>
-      </c>
-      <c r="N11" s="3">
-        <v>28093.638672000001</v>
-      </c>
-      <c r="O11" s="2">
-        <v>1.6266039999999999</v>
-      </c>
-      <c r="P11" s="4">
-        <v>4.15E-4</v>
-      </c>
-      <c r="Q11">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2013</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1331.1992190000001</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1379.9248050000001</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.67753099999999999</v>
-      </c>
-      <c r="E12" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F12" s="2">
-        <v>9.8130170000000003</v>
-      </c>
-      <c r="G12" s="2">
-        <v>5.9064420000000002</v>
-      </c>
-      <c r="H12" s="2">
-        <v>8.1756840000000004</v>
-      </c>
-      <c r="I12" s="2">
-        <v>777.21038799999997</v>
-      </c>
-      <c r="J12" s="2">
-        <v>59.869819999999997</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1112.5089109999999</v>
-      </c>
-      <c r="L12" s="2">
-        <v>1040.0164789999999</v>
-      </c>
-      <c r="M12" s="3">
-        <v>1653.8325199999999</v>
-      </c>
-      <c r="N12" s="3">
-        <v>27320.419922000001</v>
-      </c>
-      <c r="O12" s="2">
-        <v>1.2741000000000001E-2</v>
-      </c>
-      <c r="P12" s="4">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="Q12">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2014</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1040.0164789999999</v>
-      </c>
-      <c r="C13" s="2">
-        <v>2346.181885</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.62700500000000003</v>
-      </c>
-      <c r="E13" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F13" s="2">
-        <v>9.5482680000000002</v>
-      </c>
-      <c r="G13" s="2">
-        <v>5.5257620000000003</v>
-      </c>
-      <c r="H13" s="2">
-        <v>7.9551129999999999</v>
-      </c>
-      <c r="I13" s="2">
-        <v>723.81976299999997</v>
-      </c>
-      <c r="J13" s="2">
-        <v>77.950027000000006</v>
-      </c>
-      <c r="K13" s="2">
-        <v>1658.4123540000001</v>
-      </c>
-      <c r="L13" s="2">
-        <v>1204.138672</v>
-      </c>
-      <c r="M13" s="3">
-        <v>1679.5195309999999</v>
-      </c>
-      <c r="N13" s="3">
-        <v>26614.640625</v>
-      </c>
-      <c r="O13" s="2">
-        <v>0.12900200000000001</v>
-      </c>
-      <c r="P13" s="4">
-        <v>3.4999999999999997E-5</v>
-      </c>
-      <c r="Q13">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2015</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1204.138672</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1549.783081</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.891343</v>
-      </c>
-      <c r="E14" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F14" s="2">
-        <v>9.3388390000000001</v>
-      </c>
-      <c r="G14" s="2">
-        <v>8.5774699999999999</v>
-      </c>
-      <c r="H14" s="2">
-        <v>7.7806230000000003</v>
-      </c>
-      <c r="I14" s="2">
-        <v>666.04467799999998</v>
-      </c>
-      <c r="J14" s="2">
-        <v>50.906196999999999</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1123.669067</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1194.6411129999999</v>
-      </c>
-      <c r="M14" s="3">
-        <v>4403.6020509999998</v>
-      </c>
-      <c r="N14" s="3">
-        <v>26057.529297000001</v>
-      </c>
-      <c r="O14" s="2">
-        <v>6.4745999999999998E-2</v>
-      </c>
-      <c r="P14" s="4">
-        <v>2.0999999999999999E-5</v>
-      </c>
-      <c r="Q14">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2016</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1194.6411129999999</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1990.084595</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.92508100000000004</v>
-      </c>
-      <c r="E15" s="2">
-        <v>270.98791499999999</v>
-      </c>
-      <c r="F15" s="2">
-        <v>9.3833330000000004</v>
-      </c>
-      <c r="G15" s="2">
-        <v>5.6312860000000002</v>
-      </c>
-      <c r="H15" s="2">
-        <v>7.8212489999999999</v>
-      </c>
-      <c r="I15" s="2">
-        <v>662.38037099999997</v>
-      </c>
-      <c r="J15" s="2">
-        <v>94.515556000000004</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1480.9849850000001</v>
-      </c>
-      <c r="L15" s="2">
-        <v>1225.4578859999999</v>
-      </c>
-      <c r="M15" s="3">
-        <v>4338.1889650000003</v>
-      </c>
-      <c r="N15" s="3">
-        <v>26184.960938</v>
-      </c>
-      <c r="O15" s="2">
-        <v>-0.49327599999999999</v>
-      </c>
-      <c r="P15" s="4">
-        <v>-1.4200000000000001E-4</v>
-      </c>
-      <c r="Q15">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>2017</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1225.4578859999999</v>
-      </c>
-      <c r="C16" s="2">
-        <v>2105.5676269999999</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.55353600000000003</v>
-      </c>
-      <c r="E16" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F16" s="2">
-        <v>9.3968910000000001</v>
-      </c>
-      <c r="G16" s="2">
-        <v>5.0438409999999996</v>
-      </c>
-      <c r="H16" s="2">
-        <v>7.8289910000000003</v>
-      </c>
-      <c r="I16" s="2">
-        <v>700.13690199999996</v>
-      </c>
-      <c r="J16" s="2">
-        <v>89.795829999999995</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1734.2989500000001</v>
-      </c>
-      <c r="L16" s="2">
-        <v>1085.996948</v>
-      </c>
-      <c r="M16" s="3">
-        <v>1670.2463379999999</v>
-      </c>
-      <c r="N16" s="3">
-        <v>26228.105468999998</v>
-      </c>
-      <c r="O16" s="2">
-        <v>1.790313</v>
-      </c>
-      <c r="P16" s="4">
-        <v>4.95E-4</v>
-      </c>
-      <c r="Q16">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>2018</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1085.996948</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1414.644775</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.53712000000000004</v>
-      </c>
-      <c r="E17" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F17" s="2">
-        <v>9.4224359999999994</v>
-      </c>
-      <c r="G17" s="2">
-        <v>8.5405510000000007</v>
-      </c>
-      <c r="H17" s="2">
-        <v>7.850276</v>
-      </c>
-      <c r="I17" s="2">
-        <v>548.97229000000004</v>
-      </c>
-      <c r="J17" s="2">
-        <v>66.255104000000003</v>
-      </c>
-      <c r="K17" s="2">
-        <v>1129.137207</v>
-      </c>
-      <c r="L17" s="2">
-        <v>1036.213135</v>
-      </c>
-      <c r="M17" s="3">
-        <v>1971.369385</v>
-      </c>
-      <c r="N17" s="3">
-        <v>26304.007812</v>
-      </c>
-      <c r="O17" s="2">
-        <v>-0.96134699999999995</v>
-      </c>
-      <c r="P17" s="4">
-        <v>-3.4499999999999998E-4</v>
-      </c>
-      <c r="Q17">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>2019</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1036.213135</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1469.0946039999999</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.72606300000000001</v>
-      </c>
-      <c r="E18" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F18" s="2">
-        <v>9.4400619999999993</v>
-      </c>
-      <c r="G18" s="2">
-        <v>7.4573460000000003</v>
-      </c>
-      <c r="H18" s="2">
-        <v>7.8649579999999997</v>
-      </c>
-      <c r="I18" s="2">
-        <v>677.703125</v>
-      </c>
-      <c r="J18" s="2">
-        <v>70.424828000000005</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1163.58374</v>
-      </c>
-      <c r="L18" s="2">
-        <v>873.25817900000004</v>
-      </c>
-      <c r="M18" s="3">
-        <v>2767.766846</v>
-      </c>
-      <c r="N18" s="3">
-        <v>26356.542968999998</v>
-      </c>
-      <c r="O18" s="2">
-        <v>-0.34390900000000002</v>
-      </c>
-      <c r="P18" s="4">
-        <v>-1.2300000000000001E-4</v>
-      </c>
-      <c r="Q18">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>2020</v>
-      </c>
-      <c r="B19" s="2">
-        <v>873.25817900000004</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1888.009155</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.76152200000000003</v>
-      </c>
-      <c r="E19" s="2">
-        <v>270.98791499999999</v>
-      </c>
-      <c r="F19" s="2">
-        <v>9.4790550000000007</v>
-      </c>
-      <c r="G19" s="2">
-        <v>7.2725099999999996</v>
-      </c>
-      <c r="H19" s="2">
-        <v>7.9010379999999998</v>
-      </c>
-      <c r="I19" s="2">
-        <v>696.08813499999997</v>
-      </c>
-      <c r="J19" s="2">
-        <v>90.618942000000004</v>
-      </c>
-      <c r="K19" s="2">
-        <v>1264.7332759999999</v>
-      </c>
-      <c r="L19" s="2">
-        <v>989.89398200000005</v>
-      </c>
-      <c r="M19" s="3">
-        <v>3506.4147950000001</v>
-      </c>
-      <c r="N19" s="3">
-        <v>26471.685547000001</v>
-      </c>
-      <c r="O19" s="2">
-        <v>-0.53296299999999996</v>
-      </c>
-      <c r="P19" s="4">
-        <v>-1.75E-4</v>
-      </c>
-      <c r="Q19">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" t="s">
-        <v>6</v>
-      </c>
-      <c r="I23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J23" t="s">
-        <v>8</v>
-      </c>
-      <c r="K23" t="s">
-        <v>9</v>
-      </c>
-      <c r="L23" t="s">
-        <v>10</v>
-      </c>
-      <c r="M23" t="s">
-        <v>11</v>
-      </c>
-      <c r="N23" t="s">
-        <v>12</v>
-      </c>
-      <c r="O23" t="s">
-        <v>13</v>
-      </c>
-      <c r="P23" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>2010</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1284.0238039999999</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1990.4650879999999</v>
-      </c>
-      <c r="D24" s="2">
-        <v>1.4464170000000001</v>
-      </c>
-      <c r="E24" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F24" s="2">
-        <v>10.610913999999999</v>
-      </c>
-      <c r="G24" s="2">
-        <v>4.9718439999999999</v>
-      </c>
-      <c r="H24" s="2">
-        <v>8.8404570000000007</v>
-      </c>
-      <c r="I24" s="2">
-        <v>755.98974599999997</v>
-      </c>
-      <c r="J24" s="2">
-        <v>93.234084999999993</v>
-      </c>
-      <c r="K24" s="2">
-        <v>1371.442139</v>
-      </c>
-      <c r="L24" s="2">
-        <v>1333.3842770000001</v>
-      </c>
-      <c r="M24" s="3">
-        <v>8273.0888670000004</v>
-      </c>
-      <c r="N24" s="3">
-        <v>29450.638672000001</v>
-      </c>
-      <c r="O24" s="2">
-        <v>1.1251089999999999</v>
-      </c>
-      <c r="P24">
-        <v>3.1599999999999998E-4</v>
-      </c>
-      <c r="Q24">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>2011</v>
-      </c>
-      <c r="B25" s="2">
-        <v>1333.3842770000001</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1796.097168</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.94261200000000001</v>
-      </c>
-      <c r="E25" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F25" s="2">
-        <v>10.363204</v>
-      </c>
-      <c r="G25" s="2">
-        <v>5.5840180000000004</v>
-      </c>
-      <c r="H25" s="2">
-        <v>8.6340749999999993</v>
-      </c>
-      <c r="I25" s="2">
-        <v>709.59491000000003</v>
-      </c>
-      <c r="J25" s="2">
-        <v>87.439835000000002</v>
-      </c>
-      <c r="K25" s="2">
-        <v>1410.7021480000001</v>
-      </c>
-      <c r="L25" s="2">
-        <v>1198.1911620000001</v>
-      </c>
-      <c r="M25" s="3">
-        <v>4586.8471680000002</v>
-      </c>
-      <c r="N25" s="3">
-        <v>28792.103515999999</v>
-      </c>
-      <c r="O25" s="2">
-        <v>-2.0566779999999998</v>
-      </c>
-      <c r="P25">
-        <v>-6.02E-4</v>
-      </c>
-      <c r="Q25">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>2012</v>
-      </c>
-      <c r="B26" s="2">
-        <v>1198.1911620000001</v>
-      </c>
-      <c r="C26" s="2">
-        <v>2439.6132809999999</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1.4083209999999999</v>
-      </c>
-      <c r="E26" s="2">
-        <v>270.98791499999999</v>
-      </c>
-      <c r="F26" s="2">
-        <v>10.101295</v>
-      </c>
-      <c r="G26" s="2">
-        <v>4.8155799999999997</v>
-      </c>
-      <c r="H26" s="2">
-        <v>8.4196930000000005</v>
-      </c>
-      <c r="I26" s="2">
-        <v>698.32501200000002</v>
-      </c>
-      <c r="J26" s="2">
-        <v>120.810104</v>
-      </c>
-      <c r="K26" s="2">
-        <v>1767.443726</v>
-      </c>
-      <c r="L26" s="2">
-        <v>1331.7452390000001</v>
-      </c>
-      <c r="M26" s="3">
-        <v>7521.1850590000004</v>
-      </c>
-      <c r="N26" s="3">
-        <v>28093.638672000001</v>
-      </c>
-      <c r="O26" s="2">
-        <v>1.62622</v>
-      </c>
-      <c r="P26">
-        <v>4.1399999999999998E-4</v>
-      </c>
-      <c r="Q26">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>2013</v>
-      </c>
-      <c r="B27" s="2">
-        <v>1331.7452390000001</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1379.9248050000001</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.81979199999999997</v>
-      </c>
-      <c r="E27" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F27" s="2">
-        <v>9.8130170000000003</v>
-      </c>
-      <c r="G27" s="2">
-        <v>5.9076300000000002</v>
-      </c>
-      <c r="H27" s="2">
-        <v>8.1756840000000004</v>
-      </c>
-      <c r="I27" s="2">
-        <v>776.65783699999997</v>
-      </c>
-      <c r="J27" s="2">
-        <v>59.869819999999997</v>
-      </c>
-      <c r="K27" s="2">
-        <v>1112.962769</v>
-      </c>
-      <c r="L27" s="2">
-        <v>1040.8048100000001</v>
-      </c>
-      <c r="M27" s="3">
-        <v>3262.7998050000001</v>
-      </c>
-      <c r="N27" s="3">
-        <v>27320.419922000001</v>
-      </c>
-      <c r="O27" s="2">
-        <v>1.2907E-2</v>
-      </c>
-      <c r="P27">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="Q27">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>2014</v>
-      </c>
-      <c r="B28" s="2">
-        <v>1040.8048100000001</v>
-      </c>
-      <c r="C28" s="2">
-        <v>2346.181885</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.856595</v>
-      </c>
-      <c r="E28" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F28" s="2">
-        <v>9.5482680000000002</v>
-      </c>
-      <c r="G28" s="2">
-        <v>5.5137869999999998</v>
-      </c>
-      <c r="H28" s="2">
-        <v>7.9551129999999999</v>
-      </c>
-      <c r="I28" s="2">
-        <v>723.80175799999995</v>
-      </c>
-      <c r="J28" s="2">
-        <v>77.950027000000006</v>
-      </c>
-      <c r="K28" s="2">
-        <v>1658.7143550000001</v>
-      </c>
-      <c r="L28" s="2">
-        <v>1204.8604740000001</v>
-      </c>
-      <c r="M28" s="3">
-        <v>3795.5959469999998</v>
-      </c>
-      <c r="N28" s="3">
-        <v>26614.640625</v>
-      </c>
-      <c r="O28" s="2">
-        <v>0.128855</v>
-      </c>
-      <c r="P28">
-        <v>3.4999999999999997E-5</v>
-      </c>
-      <c r="Q28">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>2015</v>
-      </c>
-      <c r="B29" s="2">
-        <v>1204.8604740000001</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1549.783081</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1.2800210000000001</v>
-      </c>
-      <c r="E29" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F29" s="2">
-        <v>9.3388390000000001</v>
-      </c>
-      <c r="G29" s="2">
-        <v>8.5799669999999999</v>
-      </c>
-      <c r="H29" s="2">
-        <v>7.7806230000000003</v>
-      </c>
-      <c r="I29" s="2">
-        <v>666.39453100000003</v>
-      </c>
-      <c r="J29" s="2">
-        <v>50.906196999999999</v>
-      </c>
-      <c r="K29" s="2">
-        <v>1123.6132809999999</v>
-      </c>
-      <c r="L29" s="2">
-        <v>1195.4602050000001</v>
-      </c>
-      <c r="M29" s="3">
-        <v>8177.5766599999997</v>
-      </c>
-      <c r="N29" s="3">
-        <v>26057.529297000001</v>
-      </c>
-      <c r="O29" s="2">
-        <v>6.4928E-2</v>
-      </c>
-      <c r="P29">
-        <v>2.0999999999999999E-5</v>
-      </c>
-      <c r="Q29">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>2016</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1195.4602050000001</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1990.084595</v>
-      </c>
-      <c r="D30" s="2">
-        <v>1.131345</v>
-      </c>
-      <c r="E30" s="2">
-        <v>270.98791499999999</v>
-      </c>
-      <c r="F30" s="2">
-        <v>9.3833330000000004</v>
-      </c>
-      <c r="G30" s="2">
-        <v>5.6367320000000003</v>
-      </c>
-      <c r="H30" s="2">
-        <v>7.8212489999999999</v>
-      </c>
-      <c r="I30" s="2">
-        <v>662.680969</v>
-      </c>
-      <c r="J30" s="2">
-        <v>94.515556000000004</v>
-      </c>
-      <c r="K30" s="2">
-        <v>1480.8908690000001</v>
-      </c>
-      <c r="L30" s="2">
-        <v>1226.2822269999999</v>
-      </c>
-      <c r="M30" s="3">
-        <v>7506.1694340000004</v>
-      </c>
-      <c r="N30" s="3">
-        <v>26184.960938</v>
-      </c>
-      <c r="O30" s="2">
-        <v>-0.493255</v>
-      </c>
-      <c r="P30">
-        <v>-1.4200000000000001E-4</v>
-      </c>
-      <c r="Q30">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>2017</v>
-      </c>
-      <c r="B31" s="2">
-        <v>1226.2822269999999</v>
-      </c>
-      <c r="C31" s="2">
-        <v>2105.5676269999999</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.74674399999999996</v>
-      </c>
-      <c r="E31" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F31" s="2">
-        <v>9.3968910000000001</v>
-      </c>
-      <c r="G31" s="2">
-        <v>5.0378579999999999</v>
-      </c>
-      <c r="H31" s="2">
-        <v>7.8289910000000003</v>
-      </c>
-      <c r="I31" s="2">
-        <v>700.01544200000001</v>
-      </c>
-      <c r="J31" s="2">
-        <v>89.795829999999995</v>
-      </c>
-      <c r="K31" s="2">
-        <v>1734.5657960000001</v>
-      </c>
-      <c r="L31" s="2">
-        <v>1086.863159</v>
-      </c>
-      <c r="M31" s="3">
-        <v>3097.1513669999999</v>
-      </c>
-      <c r="N31" s="3">
-        <v>26228.105468999998</v>
-      </c>
-      <c r="O31" s="2">
-        <v>1.790343</v>
-      </c>
-      <c r="P31">
-        <v>4.95E-4</v>
-      </c>
-      <c r="Q31">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>2018</v>
-      </c>
-      <c r="B32" s="2">
-        <v>1086.863159</v>
-      </c>
-      <c r="C32" s="2">
-        <v>1414.644775</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.92500499999999997</v>
-      </c>
-      <c r="E32" s="2">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F32" s="2">
-        <v>9.4224359999999994</v>
-      </c>
-      <c r="G32" s="2">
-        <v>8.5311920000000008</v>
-      </c>
-      <c r="H32" s="2">
-        <v>7.850276</v>
-      </c>
-      <c r="I32" s="2">
-        <v>548.87017800000001</v>
-      </c>
-      <c r="J32" s="2">
-        <v>66.255104000000003</v>
-      </c>
-      <c r="K32" s="2">
-        <v>1129.465698</v>
-      </c>
-      <c r="L32" s="2">
-        <v>1037.2312010000001</v>
-      </c>
-      <c r="M32" s="3">
-        <v>4279.7534180000002</v>
-      </c>
-      <c r="N32" s="3">
-        <v>26304.007813</v>
-      </c>
-      <c r="O32" s="2">
-        <v>-0.96163799999999999</v>
-      </c>
-      <c r="P32">
-        <v>-3.4499999999999998E-4</v>
-      </c>
-      <c r="Q32">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E36" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" t="s">
-        <v>36</v>
-      </c>
-      <c r="H36" t="s">
-        <v>6</v>
-      </c>
-      <c r="I36" t="s">
-        <v>7</v>
-      </c>
-      <c r="J36" t="s">
-        <v>8</v>
-      </c>
-      <c r="K36" t="s">
-        <v>9</v>
-      </c>
-      <c r="L36" t="s">
-        <v>10</v>
-      </c>
-      <c r="M36" t="s">
-        <v>11</v>
-      </c>
-      <c r="N36" t="s">
-        <v>12</v>
-      </c>
-      <c r="O36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P36" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>2010</v>
-      </c>
-      <c r="B37">
-        <v>1284.0238039999999</v>
-      </c>
-      <c r="C37">
-        <v>1990.4650879999999</v>
-      </c>
-      <c r="D37">
-        <v>1.4464170000000001</v>
-      </c>
-      <c r="E37">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F37">
-        <v>10.610913999999999</v>
-      </c>
-      <c r="G37">
-        <v>4.9718439999999999</v>
-      </c>
-      <c r="H37">
-        <v>8.8404570000000007</v>
-      </c>
-      <c r="I37">
-        <v>755.977844</v>
-      </c>
-      <c r="J37">
-        <v>93.234084999999993</v>
-      </c>
-      <c r="K37">
-        <v>1371.4539789999999</v>
-      </c>
-      <c r="L37">
-        <v>1333.384399</v>
-      </c>
-      <c r="M37" s="3">
-        <v>8273.0888670000004</v>
-      </c>
-      <c r="N37" s="3">
-        <v>29450.638672000001</v>
-      </c>
-      <c r="O37">
-        <v>1.12517</v>
-      </c>
-      <c r="P37">
-        <v>3.1599999999999998E-4</v>
-      </c>
-      <c r="Q37">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>2011</v>
-      </c>
-      <c r="B38">
-        <v>1333.384399</v>
-      </c>
-      <c r="C38">
-        <v>1796.097168</v>
-      </c>
-      <c r="D38">
-        <v>0.94261200000000001</v>
-      </c>
-      <c r="E38">
-        <v>270.24752799999999</v>
-      </c>
-      <c r="F38">
-        <v>10.363204</v>
-      </c>
-      <c r="G38">
-        <v>5.5840180000000004</v>
-      </c>
-      <c r="H38">
-        <v>8.6340749999999993</v>
-      </c>
-      <c r="I38">
-        <v>709.58264199999996</v>
-      </c>
-      <c r="J38">
-        <v>87.439835000000002</v>
-      </c>
-      <c r="K38">
-        <v>1410.7139890000001</v>
-      </c>
-      <c r="L38">
-        <v>1198.1915280000001</v>
-      </c>
-      <c r="M38" s="3">
-        <v>4586.8471680000002</v>
-      </c>
-      <c r="N38" s="3">
-        <v>28792.103515999999</v>
-      </c>
-      <c r="O38">
-        <v>-2.0568610000000001</v>
-      </c>
-      <c r="P38">
-        <v>-6.02E-4</v>
-      </c>
-      <c r="Q38">
-        <v>2011</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD88AF4-3325-45AB-9D19-94573DCD22C4}">
   <dimension ref="A1:S6"/>
   <sheetViews>
@@ -7693,4 +6190,3020 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD84CEC-7113-4714-90A2-84947C9E014D}">
+  <dimension ref="A1:Q38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M37" sqref="M37:N38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="12" width="8.88671875" style="2"/>
+    <col min="13" max="14" width="8.88671875" style="3"/>
+    <col min="15" max="15" width="8.88671875" style="2"/>
+    <col min="16" max="16" width="9.21875" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2010</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I3" s="2">
+        <v>755.977844</v>
+      </c>
+      <c r="J3" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1371.4539789999999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1333.384399</v>
+      </c>
+      <c r="M3" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N3" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1.12517</v>
+      </c>
+      <c r="P3" s="4">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2011</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1333.384399</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1796.097168</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.94261200000000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F4" s="2">
+        <v>10.363204</v>
+      </c>
+      <c r="G4" s="2">
+        <v>5.5840180000000004</v>
+      </c>
+      <c r="H4" s="2">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I4" s="2">
+        <v>709.58264199999996</v>
+      </c>
+      <c r="J4" s="2">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1410.7139890000001</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1198.1915280000001</v>
+      </c>
+      <c r="M4" s="3">
+        <v>4586.8471680000002</v>
+      </c>
+      <c r="N4" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O4" s="2">
+        <v>-2.0568610000000001</v>
+      </c>
+      <c r="P4" s="4">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q4">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2010</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F9" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4.971921</v>
+      </c>
+      <c r="H9" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I9" s="2">
+        <v>755.736267</v>
+      </c>
+      <c r="J9" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1371.6888429999999</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1333.3907469999999</v>
+      </c>
+      <c r="M9" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N9" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1.124727</v>
+      </c>
+      <c r="P9" s="4">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q9">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2011</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1333.3907469999999</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1796.097168</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.64938200000000001</v>
+      </c>
+      <c r="E10" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F10" s="2">
+        <v>10.363204</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5.5908110000000004</v>
+      </c>
+      <c r="H10" s="2">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I10" s="2">
+        <v>710.03326400000003</v>
+      </c>
+      <c r="J10" s="2">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1410.5351559999999</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1197.6400149999999</v>
+      </c>
+      <c r="M10" s="3">
+        <v>2649.6083979999999</v>
+      </c>
+      <c r="N10" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O10" s="2">
+        <v>-2.056495</v>
+      </c>
+      <c r="P10" s="4">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q10">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2012</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1197.6400149999999</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2439.6132809999999</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.87193900000000002</v>
+      </c>
+      <c r="E11" s="2">
+        <v>270.98791499999999</v>
+      </c>
+      <c r="F11" s="2">
+        <v>10.101295</v>
+      </c>
+      <c r="G11" s="2">
+        <v>4.8161160000000001</v>
+      </c>
+      <c r="H11" s="2">
+        <v>8.4196930000000005</v>
+      </c>
+      <c r="I11" s="2">
+        <v>697.88244599999996</v>
+      </c>
+      <c r="J11" s="2">
+        <v>120.810104</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1767.345703</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1331.1992190000001</v>
+      </c>
+      <c r="M11" s="3">
+        <v>3559.713135</v>
+      </c>
+      <c r="N11" s="3">
+        <v>28093.638672000001</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1.6266039999999999</v>
+      </c>
+      <c r="P11" s="4">
+        <v>4.15E-4</v>
+      </c>
+      <c r="Q11">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2013</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1331.1992190000001</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1379.9248050000001</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.67753099999999999</v>
+      </c>
+      <c r="E12" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F12" s="2">
+        <v>9.8130170000000003</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5.9064420000000002</v>
+      </c>
+      <c r="H12" s="2">
+        <v>8.1756840000000004</v>
+      </c>
+      <c r="I12" s="2">
+        <v>777.21038799999997</v>
+      </c>
+      <c r="J12" s="2">
+        <v>59.869819999999997</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1112.5089109999999</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1040.0164789999999</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1653.8325199999999</v>
+      </c>
+      <c r="N12" s="3">
+        <v>27320.419922000001</v>
+      </c>
+      <c r="O12" s="2">
+        <v>1.2741000000000001E-2</v>
+      </c>
+      <c r="P12" s="4">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="Q12">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2014</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1040.0164789999999</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2346.181885</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.62700500000000003</v>
+      </c>
+      <c r="E13" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F13" s="2">
+        <v>9.5482680000000002</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5.5257620000000003</v>
+      </c>
+      <c r="H13" s="2">
+        <v>7.9551129999999999</v>
+      </c>
+      <c r="I13" s="2">
+        <v>723.81976299999997</v>
+      </c>
+      <c r="J13" s="2">
+        <v>77.950027000000006</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1658.4123540000001</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1204.138672</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1679.5195309999999</v>
+      </c>
+      <c r="N13" s="3">
+        <v>26614.640625</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.12900200000000001</v>
+      </c>
+      <c r="P13" s="4">
+        <v>3.4999999999999997E-5</v>
+      </c>
+      <c r="Q13">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2015</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1204.138672</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1549.783081</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.891343</v>
+      </c>
+      <c r="E14" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F14" s="2">
+        <v>9.3388390000000001</v>
+      </c>
+      <c r="G14" s="2">
+        <v>8.5774699999999999</v>
+      </c>
+      <c r="H14" s="2">
+        <v>7.7806230000000003</v>
+      </c>
+      <c r="I14" s="2">
+        <v>666.04467799999998</v>
+      </c>
+      <c r="J14" s="2">
+        <v>50.906196999999999</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1123.669067</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1194.6411129999999</v>
+      </c>
+      <c r="M14" s="3">
+        <v>4403.6020509999998</v>
+      </c>
+      <c r="N14" s="3">
+        <v>26057.529297000001</v>
+      </c>
+      <c r="O14" s="2">
+        <v>6.4745999999999998E-2</v>
+      </c>
+      <c r="P14" s="4">
+        <v>2.0999999999999999E-5</v>
+      </c>
+      <c r="Q14">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2016</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1194.6411129999999</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1990.084595</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.92508100000000004</v>
+      </c>
+      <c r="E15" s="2">
+        <v>270.98791499999999</v>
+      </c>
+      <c r="F15" s="2">
+        <v>9.3833330000000004</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5.6312860000000002</v>
+      </c>
+      <c r="H15" s="2">
+        <v>7.8212489999999999</v>
+      </c>
+      <c r="I15" s="2">
+        <v>662.38037099999997</v>
+      </c>
+      <c r="J15" s="2">
+        <v>94.515556000000004</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1480.9849850000001</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1225.4578859999999</v>
+      </c>
+      <c r="M15" s="3">
+        <v>4338.1889650000003</v>
+      </c>
+      <c r="N15" s="3">
+        <v>26184.960938</v>
+      </c>
+      <c r="O15" s="2">
+        <v>-0.49327599999999999</v>
+      </c>
+      <c r="P15" s="4">
+        <v>-1.4200000000000001E-4</v>
+      </c>
+      <c r="Q15">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2017</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1225.4578859999999</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2105.5676269999999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.55353600000000003</v>
+      </c>
+      <c r="E16" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F16" s="2">
+        <v>9.3968910000000001</v>
+      </c>
+      <c r="G16" s="2">
+        <v>5.0438409999999996</v>
+      </c>
+      <c r="H16" s="2">
+        <v>7.8289910000000003</v>
+      </c>
+      <c r="I16" s="2">
+        <v>700.13690199999996</v>
+      </c>
+      <c r="J16" s="2">
+        <v>89.795829999999995</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1734.2989500000001</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1085.996948</v>
+      </c>
+      <c r="M16" s="3">
+        <v>1670.2463379999999</v>
+      </c>
+      <c r="N16" s="3">
+        <v>26228.105468999998</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1.790313</v>
+      </c>
+      <c r="P16" s="4">
+        <v>4.95E-4</v>
+      </c>
+      <c r="Q16">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2018</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1085.996948</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1414.644775</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.53712000000000004</v>
+      </c>
+      <c r="E17" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F17" s="2">
+        <v>9.4224359999999994</v>
+      </c>
+      <c r="G17" s="2">
+        <v>8.5405510000000007</v>
+      </c>
+      <c r="H17" s="2">
+        <v>7.850276</v>
+      </c>
+      <c r="I17" s="2">
+        <v>548.97229000000004</v>
+      </c>
+      <c r="J17" s="2">
+        <v>66.255104000000003</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1129.137207</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1036.213135</v>
+      </c>
+      <c r="M17" s="3">
+        <v>1971.369385</v>
+      </c>
+      <c r="N17" s="3">
+        <v>26304.007812</v>
+      </c>
+      <c r="O17" s="2">
+        <v>-0.96134699999999995</v>
+      </c>
+      <c r="P17" s="4">
+        <v>-3.4499999999999998E-4</v>
+      </c>
+      <c r="Q17">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2019</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1036.213135</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1469.0946039999999</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.72606300000000001</v>
+      </c>
+      <c r="E18" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F18" s="2">
+        <v>9.4400619999999993</v>
+      </c>
+      <c r="G18" s="2">
+        <v>7.4573460000000003</v>
+      </c>
+      <c r="H18" s="2">
+        <v>7.8649579999999997</v>
+      </c>
+      <c r="I18" s="2">
+        <v>677.703125</v>
+      </c>
+      <c r="J18" s="2">
+        <v>70.424828000000005</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1163.58374</v>
+      </c>
+      <c r="L18" s="2">
+        <v>873.25817900000004</v>
+      </c>
+      <c r="M18" s="3">
+        <v>2767.766846</v>
+      </c>
+      <c r="N18" s="3">
+        <v>26356.542968999998</v>
+      </c>
+      <c r="O18" s="2">
+        <v>-0.34390900000000002</v>
+      </c>
+      <c r="P18" s="4">
+        <v>-1.2300000000000001E-4</v>
+      </c>
+      <c r="Q18">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2020</v>
+      </c>
+      <c r="B19" s="2">
+        <v>873.25817900000004</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1888.009155</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.76152200000000003</v>
+      </c>
+      <c r="E19" s="2">
+        <v>270.98791499999999</v>
+      </c>
+      <c r="F19" s="2">
+        <v>9.4790550000000007</v>
+      </c>
+      <c r="G19" s="2">
+        <v>7.2725099999999996</v>
+      </c>
+      <c r="H19" s="2">
+        <v>7.9010379999999998</v>
+      </c>
+      <c r="I19" s="2">
+        <v>696.08813499999997</v>
+      </c>
+      <c r="J19" s="2">
+        <v>90.618942000000004</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1264.7332759999999</v>
+      </c>
+      <c r="L19" s="2">
+        <v>989.89398200000005</v>
+      </c>
+      <c r="M19" s="3">
+        <v>3506.4147950000001</v>
+      </c>
+      <c r="N19" s="3">
+        <v>26471.685547000001</v>
+      </c>
+      <c r="O19" s="2">
+        <v>-0.53296299999999996</v>
+      </c>
+      <c r="P19" s="4">
+        <v>-1.75E-4</v>
+      </c>
+      <c r="Q19">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23" t="s">
+        <v>13</v>
+      </c>
+      <c r="P23" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2010</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E24" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F24" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G24" s="2">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H24" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I24" s="2">
+        <v>755.98974599999997</v>
+      </c>
+      <c r="J24" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1371.442139</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1333.3842770000001</v>
+      </c>
+      <c r="M24" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N24" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O24" s="2">
+        <v>1.1251089999999999</v>
+      </c>
+      <c r="P24">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q24">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2011</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1333.3842770000001</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1796.097168</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.94261200000000001</v>
+      </c>
+      <c r="E25" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F25" s="2">
+        <v>10.363204</v>
+      </c>
+      <c r="G25" s="2">
+        <v>5.5840180000000004</v>
+      </c>
+      <c r="H25" s="2">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I25" s="2">
+        <v>709.59491000000003</v>
+      </c>
+      <c r="J25" s="2">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1410.7021480000001</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1198.1911620000001</v>
+      </c>
+      <c r="M25" s="3">
+        <v>4586.8471680000002</v>
+      </c>
+      <c r="N25" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O25" s="2">
+        <v>-2.0566779999999998</v>
+      </c>
+      <c r="P25">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q25">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2012</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1198.1911620000001</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2439.6132809999999</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1.4083209999999999</v>
+      </c>
+      <c r="E26" s="2">
+        <v>270.98791499999999</v>
+      </c>
+      <c r="F26" s="2">
+        <v>10.101295</v>
+      </c>
+      <c r="G26" s="2">
+        <v>4.8155799999999997</v>
+      </c>
+      <c r="H26" s="2">
+        <v>8.4196930000000005</v>
+      </c>
+      <c r="I26" s="2">
+        <v>698.32501200000002</v>
+      </c>
+      <c r="J26" s="2">
+        <v>120.810104</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1767.443726</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1331.7452390000001</v>
+      </c>
+      <c r="M26" s="3">
+        <v>7521.1850590000004</v>
+      </c>
+      <c r="N26" s="3">
+        <v>28093.638672000001</v>
+      </c>
+      <c r="O26" s="2">
+        <v>1.62622</v>
+      </c>
+      <c r="P26">
+        <v>4.1399999999999998E-4</v>
+      </c>
+      <c r="Q26">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2013</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1331.7452390000001</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1379.9248050000001</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.81979199999999997</v>
+      </c>
+      <c r="E27" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F27" s="2">
+        <v>9.8130170000000003</v>
+      </c>
+      <c r="G27" s="2">
+        <v>5.9076300000000002</v>
+      </c>
+      <c r="H27" s="2">
+        <v>8.1756840000000004</v>
+      </c>
+      <c r="I27" s="2">
+        <v>776.65783699999997</v>
+      </c>
+      <c r="J27" s="2">
+        <v>59.869819999999997</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1112.962769</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1040.8048100000001</v>
+      </c>
+      <c r="M27" s="3">
+        <v>3262.7998050000001</v>
+      </c>
+      <c r="N27" s="3">
+        <v>27320.419922000001</v>
+      </c>
+      <c r="O27" s="2">
+        <v>1.2907E-2</v>
+      </c>
+      <c r="P27">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="Q27">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2014</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1040.8048100000001</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2346.181885</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.856595</v>
+      </c>
+      <c r="E28" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F28" s="2">
+        <v>9.5482680000000002</v>
+      </c>
+      <c r="G28" s="2">
+        <v>5.5137869999999998</v>
+      </c>
+      <c r="H28" s="2">
+        <v>7.9551129999999999</v>
+      </c>
+      <c r="I28" s="2">
+        <v>723.80175799999995</v>
+      </c>
+      <c r="J28" s="2">
+        <v>77.950027000000006</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1658.7143550000001</v>
+      </c>
+      <c r="L28" s="2">
+        <v>1204.8604740000001</v>
+      </c>
+      <c r="M28" s="3">
+        <v>3795.5959469999998</v>
+      </c>
+      <c r="N28" s="3">
+        <v>26614.640625</v>
+      </c>
+      <c r="O28" s="2">
+        <v>0.128855</v>
+      </c>
+      <c r="P28">
+        <v>3.4999999999999997E-5</v>
+      </c>
+      <c r="Q28">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2015</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1204.8604740000001</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1549.783081</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1.2800210000000001</v>
+      </c>
+      <c r="E29" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F29" s="2">
+        <v>9.3388390000000001</v>
+      </c>
+      <c r="G29" s="2">
+        <v>8.5799669999999999</v>
+      </c>
+      <c r="H29" s="2">
+        <v>7.7806230000000003</v>
+      </c>
+      <c r="I29" s="2">
+        <v>666.39453100000003</v>
+      </c>
+      <c r="J29" s="2">
+        <v>50.906196999999999</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1123.6132809999999</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1195.4602050000001</v>
+      </c>
+      <c r="M29" s="3">
+        <v>8177.5766599999997</v>
+      </c>
+      <c r="N29" s="3">
+        <v>26057.529297000001</v>
+      </c>
+      <c r="O29" s="2">
+        <v>6.4928E-2</v>
+      </c>
+      <c r="P29">
+        <v>2.0999999999999999E-5</v>
+      </c>
+      <c r="Q29">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2016</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1195.4602050000001</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1990.084595</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1.131345</v>
+      </c>
+      <c r="E30" s="2">
+        <v>270.98791499999999</v>
+      </c>
+      <c r="F30" s="2">
+        <v>9.3833330000000004</v>
+      </c>
+      <c r="G30" s="2">
+        <v>5.6367320000000003</v>
+      </c>
+      <c r="H30" s="2">
+        <v>7.8212489999999999</v>
+      </c>
+      <c r="I30" s="2">
+        <v>662.680969</v>
+      </c>
+      <c r="J30" s="2">
+        <v>94.515556000000004</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1480.8908690000001</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1226.2822269999999</v>
+      </c>
+      <c r="M30" s="3">
+        <v>7506.1694340000004</v>
+      </c>
+      <c r="N30" s="3">
+        <v>26184.960938</v>
+      </c>
+      <c r="O30" s="2">
+        <v>-0.493255</v>
+      </c>
+      <c r="P30">
+        <v>-1.4200000000000001E-4</v>
+      </c>
+      <c r="Q30">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2017</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1226.2822269999999</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2105.5676269999999</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.74674399999999996</v>
+      </c>
+      <c r="E31" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F31" s="2">
+        <v>9.3968910000000001</v>
+      </c>
+      <c r="G31" s="2">
+        <v>5.0378579999999999</v>
+      </c>
+      <c r="H31" s="2">
+        <v>7.8289910000000003</v>
+      </c>
+      <c r="I31" s="2">
+        <v>700.01544200000001</v>
+      </c>
+      <c r="J31" s="2">
+        <v>89.795829999999995</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1734.5657960000001</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1086.863159</v>
+      </c>
+      <c r="M31" s="3">
+        <v>3097.1513669999999</v>
+      </c>
+      <c r="N31" s="3">
+        <v>26228.105468999998</v>
+      </c>
+      <c r="O31" s="2">
+        <v>1.790343</v>
+      </c>
+      <c r="P31">
+        <v>4.95E-4</v>
+      </c>
+      <c r="Q31">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2018</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1086.863159</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1414.644775</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.92500499999999997</v>
+      </c>
+      <c r="E32" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F32" s="2">
+        <v>9.4224359999999994</v>
+      </c>
+      <c r="G32" s="2">
+        <v>8.5311920000000008</v>
+      </c>
+      <c r="H32" s="2">
+        <v>7.850276</v>
+      </c>
+      <c r="I32" s="2">
+        <v>548.87017800000001</v>
+      </c>
+      <c r="J32" s="2">
+        <v>66.255104000000003</v>
+      </c>
+      <c r="K32" s="2">
+        <v>1129.465698</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1037.2312010000001</v>
+      </c>
+      <c r="M32" s="3">
+        <v>4279.7534180000002</v>
+      </c>
+      <c r="N32" s="3">
+        <v>26304.007813</v>
+      </c>
+      <c r="O32" s="2">
+        <v>-0.96163799999999999</v>
+      </c>
+      <c r="P32">
+        <v>-3.4499999999999998E-4</v>
+      </c>
+      <c r="Q32">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" t="s">
+        <v>36</v>
+      </c>
+      <c r="H36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" t="s">
+        <v>8</v>
+      </c>
+      <c r="K36" t="s">
+        <v>9</v>
+      </c>
+      <c r="L36" t="s">
+        <v>10</v>
+      </c>
+      <c r="M36" t="s">
+        <v>11</v>
+      </c>
+      <c r="N36" t="s">
+        <v>12</v>
+      </c>
+      <c r="O36" t="s">
+        <v>13</v>
+      </c>
+      <c r="P36" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2010</v>
+      </c>
+      <c r="B37">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C37">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D37">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E37">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F37">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G37">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H37">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I37">
+        <v>755.977844</v>
+      </c>
+      <c r="J37">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K37">
+        <v>1371.4539789999999</v>
+      </c>
+      <c r="L37">
+        <v>1333.384399</v>
+      </c>
+      <c r="M37" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N37" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O37">
+        <v>1.12517</v>
+      </c>
+      <c r="P37">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q37">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2011</v>
+      </c>
+      <c r="B38">
+        <v>1333.384399</v>
+      </c>
+      <c r="C38">
+        <v>1796.097168</v>
+      </c>
+      <c r="D38">
+        <v>0.94261200000000001</v>
+      </c>
+      <c r="E38">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F38">
+        <v>10.363204</v>
+      </c>
+      <c r="G38">
+        <v>5.5840180000000004</v>
+      </c>
+      <c r="H38">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I38">
+        <v>709.58264199999996</v>
+      </c>
+      <c r="J38">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K38">
+        <v>1410.7139890000001</v>
+      </c>
+      <c r="L38">
+        <v>1198.1915280000001</v>
+      </c>
+      <c r="M38" s="3">
+        <v>4586.8471680000002</v>
+      </c>
+      <c r="N38" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O38">
+        <v>-2.0568610000000001</v>
+      </c>
+      <c r="P38">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q38">
+        <v>2011</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B026C72-90A7-4456-B791-A2F0295E05B9}">
+  <dimension ref="A1:Q52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2010</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I3" s="2">
+        <v>755.977844</v>
+      </c>
+      <c r="J3" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1371.4539789999999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1333.384399</v>
+      </c>
+      <c r="M3" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N3" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1.12517</v>
+      </c>
+      <c r="P3" s="4">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2011</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1333.384399</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1796.097168</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.64938200000000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F4" s="2">
+        <v>10.363204</v>
+      </c>
+      <c r="G4" s="2">
+        <v>5.5907879999999999</v>
+      </c>
+      <c r="H4" s="2">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I4" s="2">
+        <v>709.99151600000005</v>
+      </c>
+      <c r="J4" s="2">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1410.570068</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1197.6401370000001</v>
+      </c>
+      <c r="M4" s="3">
+        <v>2649.6049800000001</v>
+      </c>
+      <c r="N4" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O4" s="2">
+        <v>-2.0568390000000001</v>
+      </c>
+      <c r="P4" s="4">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q4">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2010</v>
+      </c>
+      <c r="B9">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C9">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D9">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E9">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F9">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G9">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H9">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I9">
+        <v>755.977844</v>
+      </c>
+      <c r="J9">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K9">
+        <v>1371.4539789999999</v>
+      </c>
+      <c r="L9">
+        <v>1333.384399</v>
+      </c>
+      <c r="M9" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N9" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O9">
+        <v>1.12517</v>
+      </c>
+      <c r="P9">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q9">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2011</v>
+      </c>
+      <c r="B10">
+        <v>1333.384399</v>
+      </c>
+      <c r="C10">
+        <v>1796.097168</v>
+      </c>
+      <c r="D10">
+        <v>0.94261200000000001</v>
+      </c>
+      <c r="E10">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F10">
+        <v>10.363204</v>
+      </c>
+      <c r="G10">
+        <v>5.5840180000000004</v>
+      </c>
+      <c r="H10">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I10">
+        <v>709.58264199999996</v>
+      </c>
+      <c r="J10">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K10">
+        <v>1410.7139890000001</v>
+      </c>
+      <c r="L10">
+        <v>1198.1915280000001</v>
+      </c>
+      <c r="M10" s="3">
+        <v>4586.8471680000002</v>
+      </c>
+      <c r="N10" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O10">
+        <v>-2.0568610000000001</v>
+      </c>
+      <c r="P10">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q10">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" t="s">
+        <v>12</v>
+      </c>
+      <c r="O14" t="s">
+        <v>13</v>
+      </c>
+      <c r="P14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2010</v>
+      </c>
+      <c r="B15">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C15">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D15">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E15">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F15">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G15">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H15">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I15">
+        <v>755.977844</v>
+      </c>
+      <c r="J15">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K15">
+        <v>1371.4539789999999</v>
+      </c>
+      <c r="L15">
+        <v>1333.384399</v>
+      </c>
+      <c r="M15" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N15" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O15">
+        <v>1.12517</v>
+      </c>
+      <c r="P15">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q15">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2011</v>
+      </c>
+      <c r="B16">
+        <v>1333.384399</v>
+      </c>
+      <c r="C16">
+        <v>1796.097168</v>
+      </c>
+      <c r="D16">
+        <v>0.94261200000000001</v>
+      </c>
+      <c r="E16">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F16">
+        <v>10.363204</v>
+      </c>
+      <c r="G16">
+        <v>5.5840180000000004</v>
+      </c>
+      <c r="H16">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I16">
+        <v>709.58264199999996</v>
+      </c>
+      <c r="J16">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K16">
+        <v>1410.7139890000001</v>
+      </c>
+      <c r="L16">
+        <v>1198.1915280000001</v>
+      </c>
+      <c r="M16" s="3">
+        <v>4586.8471680000002</v>
+      </c>
+      <c r="N16" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O16">
+        <v>-2.0568610000000001</v>
+      </c>
+      <c r="P16">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q16">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20" t="s">
+        <v>13</v>
+      </c>
+      <c r="P20" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2010</v>
+      </c>
+      <c r="B21">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C21">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D21">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E21">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F21">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G21">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H21">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I21">
+        <v>755.977844</v>
+      </c>
+      <c r="J21">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K21">
+        <v>1371.4539789999999</v>
+      </c>
+      <c r="L21">
+        <v>1333.384399</v>
+      </c>
+      <c r="M21" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N21" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O21">
+        <v>1.12517</v>
+      </c>
+      <c r="P21">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q21">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2011</v>
+      </c>
+      <c r="B22">
+        <v>1333.384399</v>
+      </c>
+      <c r="C22">
+        <v>1796.097168</v>
+      </c>
+      <c r="D22">
+        <v>0.64938200000000001</v>
+      </c>
+      <c r="E22">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F22">
+        <v>10.363204</v>
+      </c>
+      <c r="G22">
+        <v>5.5907879999999999</v>
+      </c>
+      <c r="H22">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I22">
+        <v>709.99151600000005</v>
+      </c>
+      <c r="J22">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K22">
+        <v>1410.570068</v>
+      </c>
+      <c r="L22">
+        <v>1197.6401370000001</v>
+      </c>
+      <c r="M22" s="3">
+        <v>2649.6049800000001</v>
+      </c>
+      <c r="N22" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O22">
+        <v>-2.0568390000000001</v>
+      </c>
+      <c r="P22">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q22">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" t="s">
+        <v>9</v>
+      </c>
+      <c r="L26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" t="s">
+        <v>11</v>
+      </c>
+      <c r="N26" t="s">
+        <v>12</v>
+      </c>
+      <c r="O26" t="s">
+        <v>13</v>
+      </c>
+      <c r="P26" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2010</v>
+      </c>
+      <c r="B27">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C27">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D27">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E27">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F27">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G27">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H27">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I27">
+        <v>755.977844</v>
+      </c>
+      <c r="J27">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K27">
+        <v>1371.4539789999999</v>
+      </c>
+      <c r="L27">
+        <v>1333.384399</v>
+      </c>
+      <c r="M27" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N27" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O27">
+        <v>1.12517</v>
+      </c>
+      <c r="P27">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q27">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2011</v>
+      </c>
+      <c r="B28">
+        <v>1333.384399</v>
+      </c>
+      <c r="C28">
+        <v>1796.097168</v>
+      </c>
+      <c r="D28">
+        <v>0.94261200000000001</v>
+      </c>
+      <c r="E28">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F28">
+        <v>10.363204</v>
+      </c>
+      <c r="G28">
+        <v>5.5840180000000004</v>
+      </c>
+      <c r="H28">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I28">
+        <v>709.58264199999996</v>
+      </c>
+      <c r="J28">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K28">
+        <v>1410.7139890000001</v>
+      </c>
+      <c r="L28">
+        <v>1198.1915280000001</v>
+      </c>
+      <c r="M28" s="3">
+        <v>4586.8471680000002</v>
+      </c>
+      <c r="N28" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O28">
+        <v>-2.0568610000000001</v>
+      </c>
+      <c r="P28">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q28">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" t="s">
+        <v>36</v>
+      </c>
+      <c r="H32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I32" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" t="s">
+        <v>8</v>
+      </c>
+      <c r="K32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L32" t="s">
+        <v>10</v>
+      </c>
+      <c r="M32" t="s">
+        <v>11</v>
+      </c>
+      <c r="N32" t="s">
+        <v>12</v>
+      </c>
+      <c r="O32" t="s">
+        <v>13</v>
+      </c>
+      <c r="P32" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2010</v>
+      </c>
+      <c r="B33">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C33">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D33">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E33">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F33">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G33">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H33">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I33">
+        <v>755.977844</v>
+      </c>
+      <c r="J33">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K33">
+        <v>1371.4539789999999</v>
+      </c>
+      <c r="L33">
+        <v>1333.384399</v>
+      </c>
+      <c r="M33" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N33" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O33">
+        <v>1.12517</v>
+      </c>
+      <c r="P33">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q33">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2011</v>
+      </c>
+      <c r="B34">
+        <v>1333.384399</v>
+      </c>
+      <c r="C34">
+        <v>1796.097168</v>
+      </c>
+      <c r="D34">
+        <v>0.64938200000000001</v>
+      </c>
+      <c r="E34">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F34">
+        <v>10.363204</v>
+      </c>
+      <c r="G34">
+        <v>5.5907879999999999</v>
+      </c>
+      <c r="H34">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I34">
+        <v>709.99151600000005</v>
+      </c>
+      <c r="J34">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K34">
+        <v>1410.570068</v>
+      </c>
+      <c r="L34">
+        <v>1197.6401370000001</v>
+      </c>
+      <c r="M34" s="3">
+        <v>2649.6049800000001</v>
+      </c>
+      <c r="N34" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O34">
+        <v>-2.0568390000000001</v>
+      </c>
+      <c r="P34">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q34">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" t="s">
+        <v>36</v>
+      </c>
+      <c r="H38" t="s">
+        <v>6</v>
+      </c>
+      <c r="I38" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" t="s">
+        <v>8</v>
+      </c>
+      <c r="K38" t="s">
+        <v>9</v>
+      </c>
+      <c r="L38" t="s">
+        <v>10</v>
+      </c>
+      <c r="M38" t="s">
+        <v>11</v>
+      </c>
+      <c r="N38" t="s">
+        <v>12</v>
+      </c>
+      <c r="O38" t="s">
+        <v>13</v>
+      </c>
+      <c r="P38" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2010</v>
+      </c>
+      <c r="B39">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C39">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D39">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E39">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F39">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G39">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H39">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I39">
+        <v>755.977844</v>
+      </c>
+      <c r="J39">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K39">
+        <v>1371.4539789999999</v>
+      </c>
+      <c r="L39">
+        <v>1333.384399</v>
+      </c>
+      <c r="M39">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N39">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O39">
+        <v>1.12517</v>
+      </c>
+      <c r="P39">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q39">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2011</v>
+      </c>
+      <c r="B40">
+        <v>1333.384399</v>
+      </c>
+      <c r="C40">
+        <v>1796.097168</v>
+      </c>
+      <c r="D40">
+        <v>0.64938200000000001</v>
+      </c>
+      <c r="E40">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F40">
+        <v>10.363204</v>
+      </c>
+      <c r="G40">
+        <v>5.5907879999999999</v>
+      </c>
+      <c r="H40">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I40">
+        <v>709.99151600000005</v>
+      </c>
+      <c r="J40">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K40">
+        <v>1410.570068</v>
+      </c>
+      <c r="L40">
+        <v>1197.6401370000001</v>
+      </c>
+      <c r="M40">
+        <v>2649.6049800000001</v>
+      </c>
+      <c r="N40">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O40">
+        <v>-2.0568390000000001</v>
+      </c>
+      <c r="P40">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q40">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" t="s">
+        <v>36</v>
+      </c>
+      <c r="H44" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" t="s">
+        <v>8</v>
+      </c>
+      <c r="K44" t="s">
+        <v>9</v>
+      </c>
+      <c r="L44" t="s">
+        <v>10</v>
+      </c>
+      <c r="M44" t="s">
+        <v>11</v>
+      </c>
+      <c r="N44" t="s">
+        <v>12</v>
+      </c>
+      <c r="O44" t="s">
+        <v>13</v>
+      </c>
+      <c r="P44" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2010</v>
+      </c>
+      <c r="B45">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C45">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D45">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E45">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F45">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G45">
+        <v>4.9718439999999999</v>
+      </c>
+      <c r="H45">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I45">
+        <v>755.977844</v>
+      </c>
+      <c r="J45">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K45">
+        <v>1371.4539789999999</v>
+      </c>
+      <c r="L45">
+        <v>1333.384399</v>
+      </c>
+      <c r="M45">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N45">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O45">
+        <v>1.12517</v>
+      </c>
+      <c r="P45">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q45">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2011</v>
+      </c>
+      <c r="B46">
+        <v>1333.384399</v>
+      </c>
+      <c r="C46">
+        <v>1796.097168</v>
+      </c>
+      <c r="D46">
+        <v>0.94261200000000001</v>
+      </c>
+      <c r="E46">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F46">
+        <v>10.363204</v>
+      </c>
+      <c r="G46">
+        <v>5.5840180000000004</v>
+      </c>
+      <c r="H46">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I46">
+        <v>709.58264199999996</v>
+      </c>
+      <c r="J46">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K46">
+        <v>1410.7139890000001</v>
+      </c>
+      <c r="L46">
+        <v>1198.1915280000001</v>
+      </c>
+      <c r="M46">
+        <v>4586.8471680000002</v>
+      </c>
+      <c r="N46">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O46">
+        <v>-2.0568610000000001</v>
+      </c>
+      <c r="P46">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q46">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>36</v>
+      </c>
+      <c r="H50" t="s">
+        <v>6</v>
+      </c>
+      <c r="I50" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" t="s">
+        <v>8</v>
+      </c>
+      <c r="K50" t="s">
+        <v>9</v>
+      </c>
+      <c r="L50" t="s">
+        <v>10</v>
+      </c>
+      <c r="M50" t="s">
+        <v>11</v>
+      </c>
+      <c r="N50" t="s">
+        <v>12</v>
+      </c>
+      <c r="O50" t="s">
+        <v>13</v>
+      </c>
+      <c r="P50" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2010</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E51" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F51" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G51" s="2">
+        <v>4.971921</v>
+      </c>
+      <c r="H51" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I51" s="2">
+        <v>755.736267</v>
+      </c>
+      <c r="J51" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K51" s="2">
+        <v>1371.6888429999999</v>
+      </c>
+      <c r="L51" s="2">
+        <v>1333.3907469999999</v>
+      </c>
+      <c r="M51" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N51" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O51" s="2">
+        <v>1.124727</v>
+      </c>
+      <c r="P51" s="4">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q51">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2011</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1333.3907469999999</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1796.097168</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.94261200000000001</v>
+      </c>
+      <c r="E52" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F52" s="2">
+        <v>10.363204</v>
+      </c>
+      <c r="G52" s="2">
+        <v>5.584041</v>
+      </c>
+      <c r="H52" s="2">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I52" s="2">
+        <v>709.62438999999995</v>
+      </c>
+      <c r="J52" s="2">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K52" s="2">
+        <v>1410.6791989999999</v>
+      </c>
+      <c r="L52" s="2">
+        <v>1198.191284</v>
+      </c>
+      <c r="M52" s="3">
+        <v>4586.8505859999996</v>
+      </c>
+      <c r="N52" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O52" s="2">
+        <v>-2.0565169999999999</v>
+      </c>
+      <c r="P52" s="4">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q52">
+        <v>2011</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Clean up EvapTrans. CW3MdigitalHandbook.docx - Add "Time steps, autonomous processes, and global methods" subsection. EvapTrans.cpp - Rewrite EvapTrans::Init(), InitRun(), StartYear(), StartStep() and Step() in recognition that they get entered repeatedly due to the multiple <evap_trans> blocks in the Flow XML file. Flow.cpp, GlobalMethods.h - Add static m_dateEvapTransLastExecuted to class EvapTrans.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC226355-57DF-4F20-8B12-8A68F1FEFC8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B564A357-F80A-4D80-BEDD-3CD0EDD0495A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="112">
   <si>
     <t>Year</t>
   </si>
@@ -360,6 +360,15 @@
   </si>
   <si>
     <t>C333</t>
+  </si>
+  <si>
+    <t>Demo-Baseline 2010-20 C333</t>
+  </si>
+  <si>
+    <t>Demo-Baseline 2010-20 C330</t>
+  </si>
+  <si>
+    <t>C333+</t>
   </si>
 </sst>
 </file>
@@ -1248,11 +1257,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U80"/>
+  <dimension ref="A1:U82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O77" sqref="O77"/>
+      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5731,137 +5740,249 @@
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" s="3"/>
-      <c r="P78" s="3"/>
-      <c r="Q78" s="2"/>
-      <c r="R78" s="4"/>
+      <c r="A78" t="s">
+        <v>16</v>
+      </c>
+      <c r="B78" t="s">
+        <v>110</v>
+      </c>
+      <c r="C78" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1210.7227647777777</v>
+      </c>
+      <c r="E78" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F78" s="2">
+        <v>0.79770599999999992</v>
+      </c>
+      <c r="G78" s="5">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H78" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I78" s="5">
+        <v>6.0671333333333344</v>
+      </c>
+      <c r="J78" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K78" s="5">
+        <v>693.57959655555555</v>
+      </c>
+      <c r="L78" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M78" s="5">
+        <v>1420.9534639999999</v>
+      </c>
+      <c r="N78" s="5">
+        <v>1183.1882459999999</v>
+      </c>
+      <c r="O78" s="6">
+        <v>3355.463243333334</v>
+      </c>
+      <c r="P78" s="3">
+        <v>27227.338324777778</v>
+      </c>
+      <c r="Q78" s="2">
+        <v>0.1374461111111111</v>
+      </c>
+      <c r="R78" s="4">
+        <v>2.1888888888888884E-5</v>
+      </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>16</v>
       </c>
       <c r="B79" t="s">
+        <v>109</v>
+      </c>
+      <c r="C79" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1211.291843</v>
+      </c>
+      <c r="E79" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F79" s="2">
+        <v>1.0618724444444443</v>
+      </c>
+      <c r="G79" s="13">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H79" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I79" s="2">
+        <v>6.0643295555555561</v>
+      </c>
+      <c r="J79" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K79" s="13">
+        <v>693.57013622222212</v>
+      </c>
+      <c r="L79" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M79" s="13">
+        <v>1421.1105007777778</v>
+      </c>
+      <c r="N79" s="2">
+        <v>1183.8711479999999</v>
+      </c>
+      <c r="O79" s="6">
+        <v>5611.1337891111116</v>
+      </c>
+      <c r="P79" s="3">
+        <v>27227.338324777778</v>
+      </c>
+      <c r="Q79" s="2">
+        <v>0.13748355555555555</v>
+      </c>
+      <c r="R79" s="4">
+        <v>2.1888888888888877E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+      <c r="O80" s="3"/>
+      <c r="P80" s="3"/>
+      <c r="Q80" s="2"/>
+      <c r="R80" s="4"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81" t="s">
         <v>93</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C81" t="s">
         <v>92</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D81" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E81" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F81" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G79" s="2">
+      <c r="G81" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H79" s="2">
+      <c r="H81" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I79" s="2">
+      <c r="I81" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J79" s="2">
+      <c r="J81" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K79" s="2">
+      <c r="K81" s="2">
         <v>673.08737180000003</v>
       </c>
-      <c r="L79" s="2">
+      <c r="L81" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M79" s="2">
+      <c r="M81" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N79" s="2">
+      <c r="N81" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O79" s="3">
+      <c r="O81" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P79" s="3">
+      <c r="P81" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q79" s="2">
+      <c r="Q81" s="2">
         <v>-2.3066774000000003</v>
       </c>
-      <c r="R79" s="4">
+      <c r="R81" s="4">
         <v>-7.1000000000000002E-4</v>
       </c>
-      <c r="S79" t="s">
+      <c r="S81" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>16</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B82" t="s">
         <v>95</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C82" t="s">
         <v>92</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D82" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E82" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F80" s="2">
+      <c r="F82" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G80" s="2">
+      <c r="G82" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H80" s="2">
+      <c r="H82" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I80" s="2">
+      <c r="I82" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J80" s="2">
+      <c r="J82" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K80" s="5">
+      <c r="K82" s="5">
         <v>675.4841553</v>
       </c>
-      <c r="L80" s="2">
+      <c r="L82" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M80" s="2">
+      <c r="M82" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N80" s="2">
+      <c r="N82" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O80" s="3">
+      <c r="O82" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P80" s="3">
+      <c r="P82" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q80" s="5">
+      <c r="Q82" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R80" s="7">
+      <c r="R82" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S80" t="s">
+      <c r="S82" t="s">
         <v>92</v>
       </c>
     </row>
@@ -6197,7 +6318,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M37" sqref="M37:N38"/>
+      <selection activeCell="A20" sqref="A20:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7013,6 +7134,71 @@
         <v>2020</v>
       </c>
     </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
+        <f>AVERAGE(B9:B17)</f>
+        <v>1210.7227647777777</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" ref="C20:P20" si="0">AVERAGE(C9:C17)</f>
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.79770599999999992</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>270.41205844444437</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="0"/>
+        <v>9.775355222222224</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>6.0671333333333344</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="0"/>
+        <v>8.145128999999999</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="0"/>
+        <v>693.57959655555555</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="0"/>
+        <v>82.308506444444433</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="0"/>
+        <v>1420.9534639999999</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="0"/>
+        <v>1183.1882459999999</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="0"/>
+        <v>3355.463243333334</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="0"/>
+        <v>27227.338324777778</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1374461111111111</v>
+      </c>
+      <c r="P20" s="4">
+        <f t="shared" si="0"/>
+        <v>2.1888888888888884E-5</v>
+      </c>
+    </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>100</v>
@@ -7719,13 +7905,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B026C72-90A7-4456-B791-A2F0295E05B9}">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="16" max="16" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -9203,6 +9392,170 @@
         <v>2011</v>
       </c>
     </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" t="s">
+        <v>4</v>
+      </c>
+      <c r="F56" t="s">
+        <v>5</v>
+      </c>
+      <c r="G56" t="s">
+        <v>36</v>
+      </c>
+      <c r="H56" t="s">
+        <v>6</v>
+      </c>
+      <c r="I56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J56" t="s">
+        <v>8</v>
+      </c>
+      <c r="K56" t="s">
+        <v>9</v>
+      </c>
+      <c r="L56" t="s">
+        <v>10</v>
+      </c>
+      <c r="M56" t="s">
+        <v>11</v>
+      </c>
+      <c r="N56" t="s">
+        <v>12</v>
+      </c>
+      <c r="O56" t="s">
+        <v>13</v>
+      </c>
+      <c r="P56" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>2010</v>
+      </c>
+      <c r="B57" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E57" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F57" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G57" s="2">
+        <v>4.971921</v>
+      </c>
+      <c r="H57" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I57" s="2">
+        <v>755.736267</v>
+      </c>
+      <c r="J57" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K57" s="2">
+        <v>1371.6888429999999</v>
+      </c>
+      <c r="L57" s="2">
+        <v>1333.3907469999999</v>
+      </c>
+      <c r="M57" s="3">
+        <v>8273.0888670000004</v>
+      </c>
+      <c r="N57" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O57" s="2">
+        <v>1.124727</v>
+      </c>
+      <c r="P57" s="4">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q57">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>2011</v>
+      </c>
+      <c r="B58" s="2">
+        <v>1333.3907469999999</v>
+      </c>
+      <c r="C58" s="2">
+        <v>1796.097168</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.94261200000000001</v>
+      </c>
+      <c r="E58" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F58" s="2">
+        <v>10.363204</v>
+      </c>
+      <c r="G58" s="2">
+        <v>5.584041</v>
+      </c>
+      <c r="H58" s="2">
+        <v>8.6340749999999993</v>
+      </c>
+      <c r="I58" s="2">
+        <v>709.62438999999995</v>
+      </c>
+      <c r="J58" s="2">
+        <v>87.439835000000002</v>
+      </c>
+      <c r="K58" s="2">
+        <v>1410.6791989999999</v>
+      </c>
+      <c r="L58" s="2">
+        <v>1198.191284</v>
+      </c>
+      <c r="M58" s="3">
+        <v>4586.8505859999996</v>
+      </c>
+      <c r="N58" s="3">
+        <v>28792.103515999999</v>
+      </c>
+      <c r="O58" s="2">
+        <v>-2.0565169999999999</v>
+      </c>
+      <c r="P58" s="4">
+        <v>-6.02E-4</v>
+      </c>
+      <c r="Q58">
+        <v>2011</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Integrate WetlandET into EvapTrans::GetHruET(). ETEquation.cpp, .h - Add ActualET(). Calculate wetland PET IDU-by-IDU rather than all at once for the whole HRU. Rewrite WetlandET() to be called for each IDU individually, rather than once for the whole HRU. Minor cleanups to PenmanMonteith(). EvapTrans.cpp, GlobalMethods.h - Use m_colF_THETA and m_colVPD_SCALAR from Flow.h instead of from GlobalMethods.h. Restructure GetHruET() to include wetland ET. Flow.cpp, Flow.h - Adopt a naming convention for attribute symbols: IDU attribute symbols have no prefix, Reach and HRU attribute symbols start with "Reach" or "Hru", respectively. Add HRU::Att(), AttInt(), and AttFloat(). Add FlowModel::SetAttFloat(). Add FlowModel::m_colF_THETA and m_colVPD_SCALAR. Make all the Att() and SetAtt() methods inline. ReachRouting.cpp - Implement the new naming convention for attribute symbols.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D15A55C-8512-45EB-8F5A-8BB8B7F7DC86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65DADEC-7F60-4F61-831E-B398D97D70DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="116">
   <si>
     <t>Year</t>
   </si>
@@ -375,6 +375,12 @@
   </si>
   <si>
     <t>C335+</t>
+  </si>
+  <si>
+    <t>C339</t>
+  </si>
+  <si>
+    <t>C340</t>
   </si>
 </sst>
 </file>
@@ -6377,10 +6383,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD84CEC-7113-4714-90A2-84947C9E014D}">
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8022,49 +8028,49 @@
       <c r="A43">
         <v>2010</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="2">
         <v>1284.0238039999999</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="2">
         <v>1990.4650879999999</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="2">
         <v>1.4464170000000001</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="2">
         <v>270.24752799999999</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="2">
         <v>4.971921</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="2">
         <v>755.736267</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="2">
         <v>93.234084999999993</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="2">
         <v>1371.6888429999999</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="2">
         <v>1333.3907469999999</v>
       </c>
-      <c r="M43">
+      <c r="M43" s="3">
         <v>8273.0888670000004</v>
       </c>
-      <c r="N43">
+      <c r="N43" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="O43">
+      <c r="O43" s="2">
         <v>1.124727</v>
       </c>
-      <c r="P43">
+      <c r="P43" s="4">
         <v>3.1599999999999998E-4</v>
       </c>
       <c r="Q43">
@@ -8122,6 +8128,245 @@
       </c>
       <c r="Q44">
         <v>2011</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" t="s">
+        <v>36</v>
+      </c>
+      <c r="H47" t="s">
+        <v>6</v>
+      </c>
+      <c r="I47" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" t="s">
+        <v>8</v>
+      </c>
+      <c r="K47" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" t="s">
+        <v>10</v>
+      </c>
+      <c r="M47" t="s">
+        <v>11</v>
+      </c>
+      <c r="N47" t="s">
+        <v>12</v>
+      </c>
+      <c r="O47" t="s">
+        <v>13</v>
+      </c>
+      <c r="P47" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2010</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E48" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F48" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G48" s="2">
+        <v>4.9719860000000002</v>
+      </c>
+      <c r="H48" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I48" s="2">
+        <v>755.73742700000003</v>
+      </c>
+      <c r="J48" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K48" s="2">
+        <v>1371.6883539999999</v>
+      </c>
+      <c r="L48" s="2">
+        <v>1333.3901370000001</v>
+      </c>
+      <c r="M48" s="3">
+        <v>8273.0849610000005</v>
+      </c>
+      <c r="N48" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O48" s="2">
+        <v>1.124722</v>
+      </c>
+      <c r="P48" s="4">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q48">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>36</v>
+      </c>
+      <c r="H51" t="s">
+        <v>6</v>
+      </c>
+      <c r="I51" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" t="s">
+        <v>8</v>
+      </c>
+      <c r="K51" t="s">
+        <v>9</v>
+      </c>
+      <c r="L51" t="s">
+        <v>10</v>
+      </c>
+      <c r="M51" t="s">
+        <v>11</v>
+      </c>
+      <c r="N51" t="s">
+        <v>12</v>
+      </c>
+      <c r="O51" t="s">
+        <v>13</v>
+      </c>
+      <c r="P51" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2010</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E52" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F52" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G52" s="2">
+        <v>4.9719850000000001</v>
+      </c>
+      <c r="H52" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I52" s="2">
+        <v>755.73742700000003</v>
+      </c>
+      <c r="J52" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K52" s="2">
+        <v>1371.6883539999999</v>
+      </c>
+      <c r="L52" s="2">
+        <v>1333.3901370000001</v>
+      </c>
+      <c r="M52" s="3">
+        <v>8273.0849610000005</v>
+      </c>
+      <c r="N52" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O52" s="2">
+        <v>1.1247229999999999</v>
+      </c>
+      <c r="P52" s="4">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="Q52">
+        <v>2010</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get the simulations running for the Little NSantiam and Blowout Cr watersheds. HBV.csv - Add entries for LittleNSantiam50 and Blowout51. FLOWreports_McKenzie.xml - Add a column for Q back to the "FLOW Wetland 17 analysis" report. Add some files to the SkillAssessment folder that had been overlooked.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D77351-07EA-4A0F-9882-01A8AEEDFB08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967AFED2-6E49-4BB0-B0A1-8699302E7249}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="118">
   <si>
     <t>Year</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t>Demo-Baseline 2010-18 C340</t>
+  </si>
+  <si>
+    <t>C345</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
     </sheetView>
@@ -6442,10 +6445,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD84CEC-7113-4714-90A2-84947C9E014D}">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8425,6 +8428,117 @@
         <v>3.1599999999999998E-4</v>
       </c>
       <c r="Q52">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" t="s">
+        <v>5</v>
+      </c>
+      <c r="G55" t="s">
+        <v>36</v>
+      </c>
+      <c r="H55" t="s">
+        <v>6</v>
+      </c>
+      <c r="I55" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" t="s">
+        <v>8</v>
+      </c>
+      <c r="K55" t="s">
+        <v>9</v>
+      </c>
+      <c r="L55" t="s">
+        <v>10</v>
+      </c>
+      <c r="M55" t="s">
+        <v>11</v>
+      </c>
+      <c r="N55" t="s">
+        <v>12</v>
+      </c>
+      <c r="O55" t="s">
+        <v>13</v>
+      </c>
+      <c r="P55" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>2010</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1284.0238039999999</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1.4464170000000001</v>
+      </c>
+      <c r="E56" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F56" s="2">
+        <v>10.610913999999999</v>
+      </c>
+      <c r="G56" s="2">
+        <v>4.9719850000000001</v>
+      </c>
+      <c r="H56" s="2">
+        <v>8.8404570000000007</v>
+      </c>
+      <c r="I56" s="2">
+        <v>755.73742700000003</v>
+      </c>
+      <c r="J56" s="2">
+        <v>93.234084999999993</v>
+      </c>
+      <c r="K56" s="2">
+        <v>1371.4332280000001</v>
+      </c>
+      <c r="L56" s="2">
+        <v>1333.389404</v>
+      </c>
+      <c r="M56" s="3">
+        <v>8273.0849610000005</v>
+      </c>
+      <c r="N56" s="3">
+        <v>29450.638672000001</v>
+      </c>
+      <c r="O56" s="2">
+        <v>0.86886399999999997</v>
+      </c>
+      <c r="P56" s="4">
+        <v>2.4399999999999999E-4</v>
+      </c>
+      <c r="Q56">
         <v>2010</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flow.cpp, .h - Remove misnamed IDU attribute column number m_colHruPrecipYr; it duplicates m_colPRECIP_YR. The attribute itself is named Precip_yr; the use of lower case letters causes some confusion. ReachRouting.cpp - Move the use of GetReachDischargeWP() until after the calculation of m_q2wetl, to ensure that the subreach outflow and q2wetl used in GetReachDischargeWP are from the same timestep.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E80AFF-0FA2-41E4-821F-8259C5A85DD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E07C21-52E3-4B39-A0C6-22ADA039A17C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="121">
   <si>
     <t>Year</t>
   </si>
@@ -393,6 +393,9 @@
   </si>
   <si>
     <t>Baseline_2000-09_C356</t>
+  </si>
+  <si>
+    <t>Baseline_2000-09_C364</t>
   </si>
 </sst>
 </file>
@@ -6133,7 +6136,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6431,21 +6434,60 @@
       </c>
     </row>
     <row r="6" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="15"/>
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="5">
+        <v>710.48948979999989</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1790.8486085</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1.0913157999999998</v>
+      </c>
+      <c r="G6" s="13">
+        <v>270.46964409999998</v>
+      </c>
+      <c r="H6" s="13">
+        <v>9.3450500000000005</v>
+      </c>
+      <c r="I6" s="5">
+        <v>9.9604478000000007</v>
+      </c>
+      <c r="J6" s="13">
+        <v>7.7868856999999991</v>
+      </c>
+      <c r="K6" s="13">
+        <v>681.48979490000011</v>
+      </c>
+      <c r="L6" s="13">
+        <v>84.457442000000015</v>
+      </c>
+      <c r="M6" s="13">
+        <v>1242.3430969999999</v>
+      </c>
+      <c r="N6" s="5">
+        <v>775.89280400000007</v>
+      </c>
+      <c r="O6" s="14">
+        <v>6120.3169676999996</v>
+      </c>
+      <c r="P6" s="14">
+        <v>26051.2640627</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>-0.23453229999999983</v>
+      </c>
+      <c r="R6" s="15">
+        <v>-1.3900000000000007E-4</v>
+      </c>
     </row>
     <row r="7" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D7" s="13"/>
@@ -6524,10 +6566,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD84CEC-7113-4714-90A2-84947C9E014D}">
-  <dimension ref="A1:Q59"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:Q61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8676,6 +8718,59 @@
         <v>2.2499999999999999E-4</v>
       </c>
       <c r="Q59">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>2010</v>
+      </c>
+      <c r="B61" s="2">
+        <v>840.40521200000001</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1990.4650879999999</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.98794499999999996</v>
+      </c>
+      <c r="E61" s="2">
+        <v>270.24752799999999</v>
+      </c>
+      <c r="F61" s="2">
+        <v>10.773111999999999</v>
+      </c>
+      <c r="G61" s="2">
+        <v>6.1254460000000002</v>
+      </c>
+      <c r="H61" s="2">
+        <v>8.9755880000000001</v>
+      </c>
+      <c r="I61" s="2">
+        <v>666.909851</v>
+      </c>
+      <c r="J61" s="2">
+        <v>84.283332999999999</v>
+      </c>
+      <c r="K61" s="2">
+        <v>1390.6453859999999</v>
+      </c>
+      <c r="L61" s="2">
+        <v>969.10101299999997</v>
+      </c>
+      <c r="M61" s="3">
+        <v>4564.9228519999997</v>
+      </c>
+      <c r="N61" s="3">
+        <v>29885.382812</v>
+      </c>
+      <c r="O61" s="2">
+        <v>0.91083899999999995</v>
+      </c>
+      <c r="P61" s="4">
+        <v>2.92E-4</v>
+      </c>
+      <c r="Q61">
         <v>2010</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Save the layer data and the IC file after spinning up C366 for 2000-09.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E07C21-52E3-4B39-A0C6-22ADA039A17C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E550F6C9-B952-476A-B53D-3942A7CA238C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="122">
   <si>
     <t>Year</t>
   </si>
@@ -396,6 +396,9 @@
   </si>
   <si>
     <t>Baseline_2000-09_C364</t>
+  </si>
+  <si>
+    <t>Baseline_2000-09_C366</t>
   </si>
 </sst>
 </file>
@@ -6133,10 +6136,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD88AF4-3325-45AB-9D19-94573DCD22C4}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="K7" sqref="K7:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6490,72 +6493,128 @@
       </c>
     </row>
     <row r="7" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="15"/>
-    </row>
-    <row r="8" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C8" s="1" t="s">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="5">
+        <v>898.93680410000002</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1790.8486085</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.0508375999999999</v>
+      </c>
+      <c r="G7" s="2">
+        <v>270.46964409999998</v>
+      </c>
+      <c r="H7" s="2">
+        <v>9.3795183999999985</v>
+      </c>
+      <c r="I7" s="5">
+        <v>8.2381033000000006</v>
+      </c>
+      <c r="J7" s="2">
+        <v>7.8156088999999991</v>
+      </c>
+      <c r="K7" s="5">
+        <v>669.21583260000011</v>
+      </c>
+      <c r="L7" s="5">
+        <v>82.082697999999993</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1318.0059082</v>
+      </c>
+      <c r="N7" s="5">
+        <v>901.35064690000002</v>
+      </c>
+      <c r="O7" s="6">
+        <v>6196.2257811999998</v>
+      </c>
+      <c r="P7" s="6">
+        <v>26143.669140599999</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>-0.45282139999999982</v>
+      </c>
+      <c r="R7" s="4">
+        <v>-2.0030000000000004E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="15"/>
+    </row>
+    <row r="9" spans="1:19" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="P9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="Q9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="R9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Get the NSantiam Demo-Baseline simulation running right again. Flow.xml _ Uncomment the 8 springs in the NSantiam basin. FLOWreports_NSantiam.xml - Replace references to Q with references to Q_DISCHARG.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E550F6C9-B952-476A-B53D-3942A7CA238C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0EFE21-CF2F-4C35-973C-8E68FEE7974D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="125">
   <si>
     <t>Year</t>
   </si>
@@ -399,6 +399,15 @@
   </si>
   <si>
     <t>Baseline_2000-09_C366</t>
+  </si>
+  <si>
+    <t>Demo-Baseline 2010-18 C367</t>
+  </si>
+  <si>
+    <t>Demo_Baseline2010-18 C353 0.4.12</t>
+  </si>
+  <si>
+    <t>Demo-Baseline 2010-18 C367 with the 2010 IC file and 3 DBF files from before C363</t>
   </si>
 </sst>
 </file>
@@ -899,7 +908,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -931,6 +940,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1287,11 +1297,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U84"/>
+  <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
+      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5994,137 +6004,322 @@
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
-      <c r="L82" s="2"/>
-      <c r="M82" s="2"/>
-      <c r="N82" s="2"/>
-      <c r="O82" s="3"/>
-      <c r="P82" s="3"/>
-      <c r="Q82" s="2"/>
-      <c r="R82" s="4"/>
+      <c r="A82" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" t="s">
+        <v>123</v>
+      </c>
+      <c r="C82" t="s">
+        <v>23</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1211.2893745555557</v>
+      </c>
+      <c r="E82" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F82" s="2">
+        <v>1.0618724444444443</v>
+      </c>
+      <c r="G82" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H82" s="2">
+        <v>9.775355222222224</v>
+      </c>
+      <c r="I82" s="2">
+        <v>6.0645103333333337</v>
+      </c>
+      <c r="J82" s="2">
+        <v>8.145128999999999</v>
+      </c>
+      <c r="K82" s="2">
+        <v>693.57211644444442</v>
+      </c>
+      <c r="L82" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M82" s="2">
+        <v>1420.7684055555555</v>
+      </c>
+      <c r="N82" s="2">
+        <v>1183.8681234444446</v>
+      </c>
+      <c r="O82" s="3">
+        <v>5611.0926921111113</v>
+      </c>
+      <c r="P82" s="3">
+        <v>27227.338324777778</v>
+      </c>
+      <c r="Q82" s="2">
+        <v>-0.2033686666666667</v>
+      </c>
+      <c r="R82" s="4">
+        <v>-7.5666666666666685E-5</v>
+      </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>16</v>
       </c>
       <c r="B83" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="C83" t="s">
-        <v>92</v>
-      </c>
-      <c r="D83" s="2">
-        <v>1230.0044677999999</v>
+        <v>23</v>
+      </c>
+      <c r="D83" s="5">
+        <v>941.6316866666665</v>
       </c>
       <c r="E83" s="2">
-        <v>1848.1456909000001</v>
+        <v>1890.2624783333331</v>
       </c>
       <c r="F83" s="2">
-        <v>1.0573501000000001</v>
+        <v>1.0110783333333333</v>
       </c>
       <c r="G83" s="2">
-        <v>299.4371582</v>
-      </c>
-      <c r="H83" s="2">
-        <v>9.7418259000000003</v>
-      </c>
-      <c r="I83" s="2">
-        <v>5.7446602000000002</v>
-      </c>
-      <c r="J83" s="2">
-        <v>8.1171118999999994</v>
-      </c>
-      <c r="K83" s="2">
-        <v>673.08737180000003</v>
-      </c>
-      <c r="L83" s="2">
-        <v>81.12013859999999</v>
-      </c>
-      <c r="M83" s="2">
-        <v>1432.6230836</v>
-      </c>
-      <c r="N83" s="2">
-        <v>1196.8767700000001</v>
-      </c>
-      <c r="O83" s="3">
-        <v>5429.4087645999998</v>
-      </c>
-      <c r="P83" s="3">
-        <v>27140.258789299998</v>
-      </c>
-      <c r="Q83" s="2">
-        <v>-2.3066774000000003</v>
-      </c>
-      <c r="R83" s="4">
-        <v>-7.1000000000000002E-4</v>
-      </c>
-      <c r="S83" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H83" s="5">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I83" s="5">
+        <v>7.3469983333333335</v>
+      </c>
+      <c r="J83" s="5">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K83" s="5">
+        <v>662.97213411111125</v>
+      </c>
+      <c r="L83" s="5">
+        <v>79.247251333333338</v>
+      </c>
+      <c r="M83" s="5">
+        <v>1427.5617810000001</v>
+      </c>
+      <c r="N83" s="5">
+        <v>942.10510922222215</v>
+      </c>
+      <c r="O83" s="6">
+        <v>5443.1432835555561</v>
+      </c>
+      <c r="P83" s="6">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q83" s="5">
+        <v>-0.4197893333333334</v>
+      </c>
+      <c r="R83" s="7">
+        <v>-1.4999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>16</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C84" t="s">
+        <v>23</v>
+      </c>
+      <c r="D84" s="19">
+        <v>1047.3404814444443</v>
+      </c>
+      <c r="E84" s="2">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F84" s="5">
+        <v>1.3226727777777778</v>
+      </c>
+      <c r="G84" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H84" s="2">
+        <v>9.7822335555555568</v>
+      </c>
+      <c r="I84" s="5">
+        <v>6.8577086666666673</v>
+      </c>
+      <c r="J84" s="2">
+        <v>8.1508595555555541</v>
+      </c>
+      <c r="K84" s="2">
+        <v>693.59288199999992</v>
+      </c>
+      <c r="L84" s="2">
+        <v>82.308506444444433</v>
+      </c>
+      <c r="M84" s="5">
+        <v>1416.5313586666666</v>
+      </c>
+      <c r="N84" s="5">
+        <v>1025.2008329999999</v>
+      </c>
+      <c r="O84" s="6">
+        <v>5579.9969345555546</v>
+      </c>
+      <c r="P84" s="6">
+        <v>27942.445963666669</v>
+      </c>
+      <c r="Q84" s="2">
+        <v>-0.19319399999999998</v>
+      </c>
+      <c r="R84" s="4">
+        <v>-7.8111111111111114E-5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
+      <c r="Q85" s="2"/>
+      <c r="R85" s="4"/>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2"/>
+      <c r="N86" s="2"/>
+      <c r="O86" s="3"/>
+      <c r="P86" s="3"/>
+      <c r="Q86" s="2"/>
+      <c r="R86" s="4"/>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" t="s">
+        <v>93</v>
+      </c>
+      <c r="C87" t="s">
+        <v>92</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1230.0044677999999</v>
+      </c>
+      <c r="E87" s="2">
+        <v>1848.1456909000001</v>
+      </c>
+      <c r="F87" s="2">
+        <v>1.0573501000000001</v>
+      </c>
+      <c r="G87" s="2">
+        <v>299.4371582</v>
+      </c>
+      <c r="H87" s="2">
+        <v>9.7418259000000003</v>
+      </c>
+      <c r="I87" s="2">
+        <v>5.7446602000000002</v>
+      </c>
+      <c r="J87" s="2">
+        <v>8.1171118999999994</v>
+      </c>
+      <c r="K87" s="2">
+        <v>673.08737180000003</v>
+      </c>
+      <c r="L87" s="2">
+        <v>81.12013859999999</v>
+      </c>
+      <c r="M87" s="2">
+        <v>1432.6230836</v>
+      </c>
+      <c r="N87" s="2">
+        <v>1196.8767700000001</v>
+      </c>
+      <c r="O87" s="3">
+        <v>5429.4087645999998</v>
+      </c>
+      <c r="P87" s="3">
+        <v>27140.258789299998</v>
+      </c>
+      <c r="Q87" s="2">
+        <v>-2.3066774000000003</v>
+      </c>
+      <c r="R87" s="4">
+        <v>-7.1000000000000002E-4</v>
+      </c>
+      <c r="S87" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88" t="s">
         <v>95</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C88" t="s">
         <v>92</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D88" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E88" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F84" s="2">
+      <c r="F88" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G84" s="2">
+      <c r="G88" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H84" s="2">
+      <c r="H88" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I84" s="2">
+      <c r="I88" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J84" s="2">
+      <c r="J88" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K84" s="5">
+      <c r="K88" s="5">
         <v>675.4841553</v>
       </c>
-      <c r="L84" s="2">
+      <c r="L88" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M84" s="2">
+      <c r="M88" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N84" s="2">
+      <c r="N88" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O84" s="3">
+      <c r="O88" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P84" s="3">
+      <c r="P88" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q84" s="5">
+      <c r="Q88" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R84" s="7">
+      <c r="R88" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S84" t="s">
+      <c r="S88" t="s">
         <v>92</v>
       </c>
     </row>
@@ -6138,7 +6333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD88AF4-3325-45AB-9D19-94573DCD22C4}">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7:P7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Commit new McKenzie spinup results. CW3M_McKenzie.envx - Add "spinup='0'" to <settings>. McKenzie/flow2010.ic - From spinup over 2000-09. HRU_McKenzie.dbf, IDU_McKenzie.dbf, Reach_McKenzie.dbf - From spinup over 2000-09.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0EFE21-CF2F-4C35-973C-8E68FEE7974D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49369E2-3171-4D08-ABB4-C6A49BB44054}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="126">
   <si>
     <t>Year</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>Demo-Baseline 2010-18 C367 with the 2010 IC file and 3 DBF files from before C363</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_C372+</t>
   </si>
 </sst>
 </file>
@@ -1297,11 +1300,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U88"/>
+  <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
+      <selection pane="bottomLeft" activeCell="J92" sqref="J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6172,104 +6175,101 @@
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
-      <c r="L85" s="2"/>
-      <c r="M85" s="2"/>
-      <c r="N85" s="2"/>
-      <c r="O85" s="3"/>
-      <c r="P85" s="3"/>
-      <c r="Q85" s="2"/>
-      <c r="R85" s="4"/>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
-      <c r="K86" s="2"/>
-      <c r="L86" s="2"/>
-      <c r="M86" s="2"/>
-      <c r="N86" s="2"/>
-      <c r="O86" s="3"/>
-      <c r="P86" s="3"/>
-      <c r="Q86" s="2"/>
-      <c r="R86" s="4"/>
+      <c r="A85" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" t="s">
+        <v>125</v>
+      </c>
+      <c r="C85" t="s">
+        <v>23</v>
+      </c>
+      <c r="D85" s="5">
+        <v>930.3491414444444</v>
+      </c>
+      <c r="E85" s="13">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F85" s="2">
+        <v>1.0534737777777776</v>
+      </c>
+      <c r="G85" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H85" s="2">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I85" s="5">
+        <v>7.3367124444444443</v>
+      </c>
+      <c r="J85" s="2">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K85" s="5">
+        <v>668.41088177777783</v>
+      </c>
+      <c r="L85" s="5">
+        <v>80.17382866666668</v>
+      </c>
+      <c r="M85" s="13">
+        <v>1419.6366374444444</v>
+      </c>
+      <c r="N85" s="5">
+        <v>932.39704044444443</v>
+      </c>
+      <c r="O85" s="6">
+        <v>5977.3932020000002</v>
+      </c>
+      <c r="P85" s="3">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q85" s="2">
+        <v>-0.43724066666666661</v>
+      </c>
+      <c r="R85" s="7">
+        <v>-1.5666666666666669E-4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
+      <c r="K86" s="13"/>
+      <c r="L86" s="13"/>
+      <c r="M86" s="13"/>
+      <c r="N86" s="13"/>
+      <c r="O86" s="14"/>
+      <c r="P86" s="14"/>
+      <c r="Q86" s="13"/>
+      <c r="R86" s="15"/>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>16</v>
-      </c>
-      <c r="B87" t="s">
-        <v>93</v>
-      </c>
-      <c r="C87" t="s">
-        <v>92</v>
-      </c>
-      <c r="D87" s="2">
-        <v>1230.0044677999999</v>
-      </c>
-      <c r="E87" s="2">
-        <v>1848.1456909000001</v>
-      </c>
-      <c r="F87" s="2">
-        <v>1.0573501000000001</v>
-      </c>
-      <c r="G87" s="2">
-        <v>299.4371582</v>
-      </c>
-      <c r="H87" s="2">
-        <v>9.7418259000000003</v>
-      </c>
-      <c r="I87" s="2">
-        <v>5.7446602000000002</v>
-      </c>
-      <c r="J87" s="2">
-        <v>8.1171118999999994</v>
-      </c>
-      <c r="K87" s="2">
-        <v>673.08737180000003</v>
-      </c>
-      <c r="L87" s="2">
-        <v>81.12013859999999</v>
-      </c>
-      <c r="M87" s="2">
-        <v>1432.6230836</v>
-      </c>
-      <c r="N87" s="2">
-        <v>1196.8767700000001</v>
-      </c>
-      <c r="O87" s="3">
-        <v>5429.4087645999998</v>
-      </c>
-      <c r="P87" s="3">
-        <v>27140.258789299998</v>
-      </c>
-      <c r="Q87" s="2">
-        <v>-2.3066774000000003</v>
-      </c>
-      <c r="R87" s="4">
-        <v>-7.1000000000000002E-4</v>
-      </c>
-      <c r="S87" t="s">
-        <v>92</v>
-      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="3"/>
+      <c r="Q87" s="2"/>
+      <c r="R87" s="4"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>16</v>
       </c>
       <c r="B88" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C88" t="s">
         <v>92</v>
@@ -6295,8 +6295,8 @@
       <c r="J88" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K88" s="5">
-        <v>675.4841553</v>
+      <c r="K88" s="2">
+        <v>673.08737180000003</v>
       </c>
       <c r="L88" s="2">
         <v>81.12013859999999</v>
@@ -6313,14 +6313,83 @@
       <c r="P88" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q88" s="5">
-        <v>9.0106100000000008E-2</v>
-      </c>
-      <c r="R88" s="7">
-        <v>3.5000000000000063E-6</v>
+      <c r="Q88" s="2">
+        <v>-2.3066774000000003</v>
+      </c>
+      <c r="R88" s="4">
+        <v>-7.1000000000000002E-4</v>
       </c>
       <c r="S88" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" t="s">
+        <v>95</v>
+      </c>
+      <c r="C89" t="s">
+        <v>92</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1230.0044677999999</v>
+      </c>
+      <c r="E89" s="2">
+        <v>1848.1456909000001</v>
+      </c>
+      <c r="F89" s="2">
+        <v>1.0573501000000001</v>
+      </c>
+      <c r="G89" s="2">
+        <v>299.4371582</v>
+      </c>
+      <c r="H89" s="2">
+        <v>9.7418259000000003</v>
+      </c>
+      <c r="I89" s="2">
+        <v>5.7446602000000002</v>
+      </c>
+      <c r="J89" s="2">
+        <v>8.1171118999999994</v>
+      </c>
+      <c r="K89" s="5">
+        <v>675.4841553</v>
+      </c>
+      <c r="L89" s="2">
+        <v>81.12013859999999</v>
+      </c>
+      <c r="M89" s="2">
+        <v>1432.6230836</v>
+      </c>
+      <c r="N89" s="2">
+        <v>1196.8767700000001</v>
+      </c>
+      <c r="O89" s="3">
+        <v>5429.4087645999998</v>
+      </c>
+      <c r="P89" s="3">
+        <v>27140.258789299998</v>
+      </c>
+      <c r="Q89" s="5">
+        <v>9.0106100000000008E-2</v>
+      </c>
+      <c r="R89" s="7">
+        <v>3.5000000000000063E-6</v>
+      </c>
+      <c r="S89" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D91" s="2">
+        <f>SUM(D85:I85)</f>
+        <v>3109.2584012222219</v>
+      </c>
+      <c r="J91" s="2">
+        <f>SUM(J85:N85)</f>
+        <v>3108.8211602222223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WORK-IN-PROGRESS. Still trying to get MAXSNOW to work right and to get NSantiam stream temperatures to work better. FLOWreports_NSantiam.xml - Add 3 columns to the MAXSNOW report. GlobalMethods.h - Remove ReachRouting::PutLateralWP() + 1 overload as unnecessary. ReachRouting.cpp - Fix a problem that was preventing getting good values for w2a_slp[hbvcalib] and w2a_int[hbvcalib]. Replace calls to PutLateralWP() with explicit in-line code.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49369E2-3171-4D08-ABB4-C6A49BB44054}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8370EA5-3917-4F0C-BE09-F433AA7E6704}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="127">
   <si>
     <t>Year</t>
   </si>
@@ -411,6 +411,9 @@
   </si>
   <si>
     <t>Demo_Baseline_2010-18_C372+</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_C375+</t>
   </si>
 </sst>
 </file>
@@ -1300,11 +1303,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U91"/>
+  <dimension ref="A1:U93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J92" sqref="J92"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87:XFD87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6231,163 +6234,242 @@
       </c>
     </row>
     <row r="86" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
-      <c r="K86" s="13"/>
-      <c r="L86" s="13"/>
-      <c r="M86" s="13"/>
-      <c r="N86" s="13"/>
-      <c r="O86" s="14"/>
-      <c r="P86" s="14"/>
-      <c r="Q86" s="13"/>
-      <c r="R86" s="15"/>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
-      <c r="K87" s="2"/>
-      <c r="L87" s="2"/>
-      <c r="M87" s="2"/>
-      <c r="N87" s="2"/>
-      <c r="O87" s="3"/>
-      <c r="P87" s="3"/>
-      <c r="Q87" s="2"/>
-      <c r="R87" s="4"/>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+      <c r="A86" t="s">
         <v>16</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B86" t="s">
+        <v>126</v>
+      </c>
+      <c r="C86" t="s">
+        <v>23</v>
+      </c>
+      <c r="D86" s="13">
+        <v>930.3491414444444</v>
+      </c>
+      <c r="E86" s="13">
+        <v>1890.2624783333331</v>
+      </c>
+      <c r="F86" s="13">
+        <v>1.0534737777777776</v>
+      </c>
+      <c r="G86" s="13">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H86" s="13">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I86" s="13">
+        <v>7.3367124444444443</v>
+      </c>
+      <c r="J86" s="13">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K86" s="13">
+        <v>668.41088177777783</v>
+      </c>
+      <c r="L86" s="13">
+        <v>80.17382866666668</v>
+      </c>
+      <c r="M86" s="13">
+        <v>1419.6366374444444</v>
+      </c>
+      <c r="N86" s="13">
+        <v>932.39704044444443</v>
+      </c>
+      <c r="O86" s="14">
+        <v>5977.3932020000002</v>
+      </c>
+      <c r="P86" s="14">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q86" s="13">
+        <v>-0.43724066666666661</v>
+      </c>
+      <c r="R86" s="15">
+        <v>-1.5666666666666669E-4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87"/>
+      <c r="B87"/>
+      <c r="C87"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="13"/>
+      <c r="M87" s="13"/>
+      <c r="N87" s="13"/>
+      <c r="O87" s="14"/>
+      <c r="P87" s="14"/>
+      <c r="Q87" s="13"/>
+      <c r="R87" s="15"/>
+    </row>
+    <row r="88" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88"/>
+      <c r="B88"/>
+      <c r="C88"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+      <c r="K88" s="13"/>
+      <c r="L88" s="13"/>
+      <c r="M88" s="13"/>
+      <c r="N88" s="13"/>
+      <c r="O88" s="14"/>
+      <c r="P88" s="14"/>
+      <c r="Q88" s="13"/>
+      <c r="R88" s="15"/>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="2"/>
+      <c r="L89" s="2"/>
+      <c r="M89" s="2"/>
+      <c r="N89" s="2"/>
+      <c r="O89" s="3"/>
+      <c r="P89" s="3"/>
+      <c r="Q89" s="2"/>
+      <c r="R89" s="4"/>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>16</v>
+      </c>
+      <c r="B90" t="s">
         <v>93</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C90" t="s">
         <v>92</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D90" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E90" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F88" s="2">
+      <c r="F90" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G88" s="2">
+      <c r="G90" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H88" s="2">
+      <c r="H90" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I88" s="2">
+      <c r="I90" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J88" s="2">
+      <c r="J90" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K88" s="2">
+      <c r="K90" s="2">
         <v>673.08737180000003</v>
       </c>
-      <c r="L88" s="2">
+      <c r="L90" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M88" s="2">
+      <c r="M90" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N88" s="2">
+      <c r="N90" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O88" s="3">
+      <c r="O90" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P88" s="3">
+      <c r="P90" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q88" s="2">
+      <c r="Q90" s="2">
         <v>-2.3066774000000003</v>
       </c>
-      <c r="R88" s="4">
+      <c r="R90" s="4">
         <v>-7.1000000000000002E-4</v>
       </c>
-      <c r="S88" t="s">
+      <c r="S90" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>16</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B91" t="s">
         <v>95</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C91" t="s">
         <v>92</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D91" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E91" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F89" s="2">
+      <c r="F91" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G89" s="2">
+      <c r="G91" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H89" s="2">
+      <c r="H91" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I89" s="2">
+      <c r="I91" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J89" s="2">
+      <c r="J91" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K89" s="5">
+      <c r="K91" s="5">
         <v>675.4841553</v>
       </c>
-      <c r="L89" s="2">
+      <c r="L91" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M89" s="2">
+      <c r="M91" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N89" s="2">
+      <c r="N91" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O89" s="3">
+      <c r="O91" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P89" s="3">
+      <c r="P91" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q89" s="5">
+      <c r="Q91" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R89" s="7">
+      <c r="R91" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S89" t="s">
+      <c r="S91" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D91" s="2">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D93" s="2">
         <f>SUM(D85:I85)</f>
         <v>3109.2584012222219</v>
       </c>
-      <c r="J91" s="2">
+      <c r="J93" s="2">
         <f>SUM(J85:N85)</f>
         <v>3108.8211602222223</v>
       </c>

</xml_diff>

<commit_message>
Flow.cpp - Move the call to RestoreStateVariables() from FlowModel::Run() to FlowModel::InitRun().
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8410FDAC-83A1-467B-A509-D93CBEAF1983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47643053-97A3-419D-99BF-57DC84F6B10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="129">
   <si>
     <t>Year</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>Demo_Baseline_2010-18_C409</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-19 C466</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -756,6 +759,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -918,7 +927,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -954,6 +963,8 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1310,11 +1321,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U98"/>
+  <dimension ref="A1:U101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J92" sqref="J92"/>
+      <selection pane="bottomLeft" activeCell="V90" sqref="V90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5960,7 +5971,7 @@
         <v>2.1888888888888877E-5</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -6016,7 +6027,7 @@
         <v>2.1777777777777772E-5</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -6072,7 +6083,7 @@
         <v>-7.5666666666666685E-5</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -6128,7 +6139,7 @@
         <v>-1.4999999999999999E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -6184,7 +6195,7 @@
         <v>-7.8111111111111114E-5</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -6240,7 +6251,7 @@
         <v>-1.5666666666666669E-4</v>
       </c>
     </row>
-    <row r="86" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -6296,7 +6307,7 @@
         <v>-1.5666666666666669E-4</v>
       </c>
     </row>
-    <row r="87" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -6352,7 +6363,7 @@
         <v>-1.5677777777777779E-4</v>
       </c>
     </row>
-    <row r="88" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
@@ -6399,7 +6410,7 @@
       <c r="Q88" s="13"/>
       <c r="R88" s="15"/>
     </row>
-    <row r="89" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
@@ -6431,7 +6442,7 @@
       <c r="Q89" s="13"/>
       <c r="R89" s="15"/>
     </row>
-    <row r="90" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
@@ -6463,7 +6474,7 @@
       <c r="Q90" s="13"/>
       <c r="R90" s="15"/>
     </row>
-    <row r="91" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
@@ -6486,7 +6497,7 @@
       <c r="Q91" s="13"/>
       <c r="R91" s="15"/>
     </row>
-    <row r="92" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
@@ -6509,7 +6520,7 @@
       <c r="Q92" s="13"/>
       <c r="R92" s="15"/>
     </row>
-    <row r="93" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
@@ -6532,149 +6543,188 @@
       <c r="Q93" s="13"/>
       <c r="R93" s="15"/>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
-      <c r="J94" s="2"/>
-      <c r="K94" s="2"/>
-      <c r="L94" s="2"/>
-      <c r="M94" s="2"/>
-      <c r="N94" s="2"/>
-      <c r="O94" s="3"/>
-      <c r="P94" s="3"/>
-      <c r="Q94" s="2"/>
-      <c r="R94" s="4"/>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>16</v>
-      </c>
-      <c r="B95" t="s">
-        <v>93</v>
-      </c>
-      <c r="C95" t="s">
-        <v>92</v>
-      </c>
-      <c r="D95" s="2">
-        <v>1230.0044677999999</v>
-      </c>
-      <c r="E95" s="2">
-        <v>1848.1456909000001</v>
-      </c>
-      <c r="F95" s="2">
-        <v>1.0573501000000001</v>
-      </c>
-      <c r="G95" s="2">
-        <v>299.4371582</v>
-      </c>
-      <c r="H95" s="2">
-        <v>9.7418259000000003</v>
-      </c>
-      <c r="I95" s="2">
-        <v>5.7446602000000002</v>
-      </c>
-      <c r="J95" s="2">
-        <v>8.1171118999999994</v>
-      </c>
-      <c r="K95" s="2">
-        <v>673.08737180000003</v>
-      </c>
-      <c r="L95" s="2">
-        <v>81.12013859999999</v>
-      </c>
-      <c r="M95" s="2">
-        <v>1432.6230836</v>
-      </c>
-      <c r="N95" s="2">
-        <v>1196.8767700000001</v>
-      </c>
-      <c r="O95" s="3">
-        <v>5429.4087645999998</v>
-      </c>
-      <c r="P95" s="3">
-        <v>27140.258789299998</v>
-      </c>
-      <c r="Q95" s="2">
-        <v>-2.3066774000000003</v>
-      </c>
-      <c r="R95" s="4">
-        <v>-7.1000000000000002E-4</v>
-      </c>
-      <c r="S95" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D94" s="2">
+        <f>SUM(D85:I85)</f>
+        <v>3109.2584012222219</v>
+      </c>
+      <c r="J94" s="2">
+        <f>SUM(J85:N85)</f>
+        <v>3108.8211602222223</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>16</v>
       </c>
       <c r="B96" t="s">
+        <v>128</v>
+      </c>
+      <c r="C96" t="s">
+        <v>23</v>
+      </c>
+      <c r="D96" s="5">
+        <v>928.42462833333332</v>
+      </c>
+      <c r="E96" s="13">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F96" s="13">
+        <v>0.97914977777777779</v>
+      </c>
+      <c r="G96" s="13">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H96" s="13">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I96" s="13">
+        <v>7.3341234444444439</v>
+      </c>
+      <c r="J96" s="13">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K96" s="13">
+        <v>669.07213688888896</v>
+      </c>
+      <c r="L96" s="13">
+        <v>80.17382866666668</v>
+      </c>
+      <c r="M96" s="5">
+        <v>1393.0887585555556</v>
+      </c>
+      <c r="N96" s="13">
+        <v>930.93472622222225</v>
+      </c>
+      <c r="O96" s="14">
+        <v>5483.3967555555555</v>
+      </c>
+      <c r="P96" s="14">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q96" s="23">
+        <v>-25.78476622222222</v>
+      </c>
+      <c r="R96" s="24">
+        <v>-7.9697777777777788E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>16</v>
+      </c>
+      <c r="B100" t="s">
+        <v>93</v>
+      </c>
+      <c r="C100" t="s">
+        <v>92</v>
+      </c>
+      <c r="D100" s="2">
+        <v>1230.0044677999999</v>
+      </c>
+      <c r="E100" s="2">
+        <v>1848.1456909000001</v>
+      </c>
+      <c r="F100" s="2">
+        <v>1.0573501000000001</v>
+      </c>
+      <c r="G100" s="2">
+        <v>299.4371582</v>
+      </c>
+      <c r="H100" s="2">
+        <v>9.7418259000000003</v>
+      </c>
+      <c r="I100" s="2">
+        <v>5.7446602000000002</v>
+      </c>
+      <c r="J100" s="2">
+        <v>8.1171118999999994</v>
+      </c>
+      <c r="K100" s="2">
+        <v>673.08737180000003</v>
+      </c>
+      <c r="L100" s="2">
+        <v>81.12013859999999</v>
+      </c>
+      <c r="M100" s="2">
+        <v>1432.6230836</v>
+      </c>
+      <c r="N100" s="2">
+        <v>1196.8767700000001</v>
+      </c>
+      <c r="O100" s="3">
+        <v>5429.4087645999998</v>
+      </c>
+      <c r="P100" s="3">
+        <v>27140.258789299998</v>
+      </c>
+      <c r="Q100" s="2">
+        <v>-2.3066774000000003</v>
+      </c>
+      <c r="R100" s="4">
+        <v>-7.1000000000000002E-4</v>
+      </c>
+      <c r="S100" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>16</v>
+      </c>
+      <c r="B101" t="s">
         <v>95</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C101" t="s">
         <v>92</v>
       </c>
-      <c r="D96" s="2">
+      <c r="D101" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E96" s="2">
+      <c r="E101" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F96" s="2">
+      <c r="F101" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G96" s="2">
+      <c r="G101" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H96" s="2">
+      <c r="H101" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I96" s="2">
+      <c r="I101" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J96" s="2">
+      <c r="J101" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K96" s="5">
+      <c r="K101" s="5">
         <v>675.4841553</v>
       </c>
-      <c r="L96" s="2">
+      <c r="L101" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M96" s="2">
+      <c r="M101" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N96" s="2">
+      <c r="N101" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O96" s="3">
+      <c r="O101" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P96" s="3">
+      <c r="P101" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q96" s="5">
+      <c r="Q101" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R96" s="7">
+      <c r="R101" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S96" t="s">
+      <c r="S101" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="98" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D98" s="2">
-        <f>SUM(D85:I85)</f>
-        <v>3109.2584012222219</v>
-      </c>
-      <c r="J98" s="2">
-        <f>SUM(J85:N85)</f>
-        <v>3108.8211602222223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BLU/flow2010.ic, HRU_BLU.dbf, IDU_BLU.dbf, Reach_BLU.dbf - From spinning up version 470 over 2000-09. NSantiam/flow2010.ic, HRU_NSantiam.dbf, IDU_NSantiam.dbf, Reach_NSantiam.dbf - From spinning up version 470 over 2000-09. Delete DataCW3M/McKenzie/Flow_McKenzie.xml as obsolete, replaced some time ago by DataCW3M/Flow.xml and DataCW3M/McKenzie/FLOWreports_McKenzie.xml.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCD9768-974B-45A7-A94E-3C17DD8E8BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424F0DE4-A88F-4B81-BEF0-2ABA84A33725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="132">
   <si>
     <t>Year</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>Baseline_2000-09_C467</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_C470+</t>
   </si>
 </sst>
 </file>
@@ -1327,11 +1330,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U101"/>
+  <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q97" sqref="Q97:R97"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T88" sqref="T88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6369,78 +6372,102 @@
         <v>-1.5677777777777779E-4</v>
       </c>
     </row>
-    <row r="88" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="20">
-        <f>E87/$E90</f>
-        <v>0.86752539266866613</v>
-      </c>
-      <c r="F88" s="21">
-        <f>(F87)/$E90</f>
-        <v>4.8348589849734502E-4</v>
-      </c>
-      <c r="G88" s="20">
-        <f>G87/$E90</f>
-        <v>0.12410410187647543</v>
-      </c>
-      <c r="H88" s="21">
-        <f>H87/$E90</f>
-        <v>4.5180950961439771E-3</v>
-      </c>
-      <c r="I88" s="20">
-        <f>I87/$E90</f>
-        <v>3.3689244602171388E-3</v>
-      </c>
-      <c r="J88" s="20">
-        <f>J87/$E87</f>
-        <v>4.3394882895423969E-3</v>
-      </c>
-      <c r="K88" s="20">
-        <f t="shared" ref="K88:M88" si="1">K87/$E87</f>
-        <v>0.35395211306017388</v>
-      </c>
-      <c r="L88" s="20">
-        <f t="shared" si="1"/>
-        <v>4.241412480311036E-2</v>
-      </c>
-      <c r="M88" s="20">
-        <f t="shared" si="1"/>
-        <v>0.75068557970027316</v>
-      </c>
-      <c r="N88" s="13"/>
-      <c r="O88" s="14"/>
-      <c r="P88" s="14"/>
-      <c r="Q88" s="13"/>
-      <c r="R88" s="15"/>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88" t="s">
+        <v>131</v>
+      </c>
+      <c r="C88" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" s="2">
+        <v>927.75490977777781</v>
+      </c>
+      <c r="E88" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F88" s="2">
+        <v>1.0680628888888888</v>
+      </c>
+      <c r="G88" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H88" s="2">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I88" s="2">
+        <v>7.3354347777777793</v>
+      </c>
+      <c r="J88" s="2">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K88" s="2">
+        <v>668.9959784444444</v>
+      </c>
+      <c r="L88" s="2">
+        <v>80.5032391111111</v>
+      </c>
+      <c r="M88" s="5">
+        <v>1392.9367132222224</v>
+      </c>
+      <c r="N88" s="2">
+        <v>930.33574744444434</v>
+      </c>
+      <c r="O88" s="3">
+        <v>5813.9261067777779</v>
+      </c>
+      <c r="P88" s="3">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q88" s="23">
+        <v>-25.703044444444444</v>
+      </c>
+      <c r="R88" s="24">
+        <v>-7.9450000000000007E-3</v>
+      </c>
     </row>
     <row r="89" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
       <c r="D89" s="13"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="21"/>
-      <c r="G89" s="20"/>
-      <c r="H89" s="21"/>
-      <c r="I89" s="20"/>
+      <c r="E89" s="20">
+        <f>E87/$E91</f>
+        <v>0.86752539266866613</v>
+      </c>
+      <c r="F89" s="21">
+        <f>(F87)/$E91</f>
+        <v>4.8348589849734502E-4</v>
+      </c>
+      <c r="G89" s="20">
+        <f>G87/$E91</f>
+        <v>0.12410410187647543</v>
+      </c>
+      <c r="H89" s="21">
+        <f>H87/$E91</f>
+        <v>4.5180950961439771E-3</v>
+      </c>
+      <c r="I89" s="20">
+        <f>I87/$E91</f>
+        <v>3.3689244602171388E-3</v>
+      </c>
       <c r="J89" s="20">
-        <f>J87/$M87</f>
-        <v>5.7807002117651277E-3</v>
+        <f>J87/$E87</f>
+        <v>4.3394882895423969E-3</v>
       </c>
       <c r="K89" s="20">
-        <f t="shared" ref="K89:M89" si="2">K87/$M87</f>
-        <v>0.4715051449389725</v>
+        <f t="shared" ref="K89:M89" si="1">K87/$E87</f>
+        <v>0.35395211306017388</v>
       </c>
       <c r="L89" s="20">
-        <f t="shared" si="2"/>
-        <v>5.6500518925706657E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.241412480311036E-2</v>
       </c>
       <c r="M89" s="20">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.75068557970027316</v>
       </c>
       <c r="N89" s="13"/>
       <c r="O89" s="14"/>
@@ -6453,26 +6480,26 @@
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90" s="13"/>
-      <c r="E90" s="13">
-        <f>SUM(E87:I87)</f>
-        <v>2178.9131411111107</v>
-      </c>
-      <c r="F90" s="20">
-        <f>F88+H88</f>
-        <v>5.0015809946413218E-3</v>
-      </c>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13">
-        <f>SUM(J87:M87)</f>
-        <v>2176.4317833333334</v>
-      </c>
-      <c r="K90" s="13"/>
-      <c r="L90" s="13"/>
-      <c r="M90" s="13">
-        <f>(M87/1000)*3307080000/(365.25*24*60*60)</f>
-        <v>148.70340764865134</v>
+      <c r="E90" s="20"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="20"/>
+      <c r="H90" s="21"/>
+      <c r="I90" s="20"/>
+      <c r="J90" s="20">
+        <f>J87/$M87</f>
+        <v>5.7807002117651277E-3</v>
+      </c>
+      <c r="K90" s="20">
+        <f t="shared" ref="K90:M90" si="2">K87/$M87</f>
+        <v>0.4715051449389725</v>
+      </c>
+      <c r="L90" s="20">
+        <f t="shared" si="2"/>
+        <v>5.6500518925706657E-2</v>
+      </c>
+      <c r="M90" s="20">
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="N90" s="13"/>
       <c r="O90" s="14"/>
@@ -6485,18 +6512,27 @@
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91" s="13"/>
-      <c r="E91" s="13"/>
-      <c r="F91" s="20"/>
+      <c r="E91" s="13">
+        <f>SUM(E87:I87)</f>
+        <v>2178.9131411111107</v>
+      </c>
+      <c r="F91" s="20">
+        <f>F89+H89</f>
+        <v>5.0015809946413218E-3</v>
+      </c>
       <c r="G91" s="13"/>
       <c r="H91" s="13"/>
       <c r="I91" s="13"/>
-      <c r="J91" s="20">
-        <f>J90/E87</f>
-        <v>1.1513913058531</v>
+      <c r="J91" s="13">
+        <f>SUM(J87:M87)</f>
+        <v>2176.4317833333334</v>
       </c>
       <c r="K91" s="13"/>
       <c r="L91" s="13"/>
-      <c r="M91" s="13"/>
+      <c r="M91" s="13">
+        <f>(M87/1000)*3307080000/(365.25*24*60*60)</f>
+        <v>148.70340764865134</v>
+      </c>
       <c r="N91" s="13"/>
       <c r="O91" s="14"/>
       <c r="P91" s="14"/>
@@ -6513,9 +6549,9 @@
       <c r="G92" s="13"/>
       <c r="H92" s="13"/>
       <c r="I92" s="13"/>
-      <c r="J92" s="22">
-        <f>J90-E90</f>
-        <v>-2.481357777777248</v>
+      <c r="J92" s="20">
+        <f>J91/E87</f>
+        <v>1.1513913058531</v>
       </c>
       <c r="K92" s="13"/>
       <c r="L92" s="13"/>
@@ -6536,9 +6572,9 @@
       <c r="G93" s="13"/>
       <c r="H93" s="13"/>
       <c r="I93" s="13"/>
-      <c r="J93" s="21">
-        <f>J92/E90</f>
-        <v>-1.1388052745011715E-3</v>
+      <c r="J93" s="22">
+        <f>J91-E91</f>
+        <v>-2.481357777777248</v>
       </c>
       <c r="K93" s="13"/>
       <c r="L93" s="13"/>
@@ -6549,70 +6585,37 @@
       <c r="Q93" s="13"/>
       <c r="R93" s="15"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="D94" s="2">
+    <row r="94" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="21">
+        <f>J93/E91</f>
+        <v>-1.1388052745011715E-3</v>
+      </c>
+      <c r="K94" s="13"/>
+      <c r="L94" s="13"/>
+      <c r="M94" s="13"/>
+      <c r="N94" s="13"/>
+      <c r="O94" s="14"/>
+      <c r="P94" s="14"/>
+      <c r="Q94" s="13"/>
+      <c r="R94" s="15"/>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D95" s="2">
         <f>SUM(D85:I85)</f>
         <v>3109.2584012222219</v>
       </c>
-      <c r="J94" s="2">
+      <c r="J95" s="2">
         <f>SUM(J85:N85)</f>
         <v>3108.8211602222223</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>16</v>
-      </c>
-      <c r="B96" t="s">
-        <v>128</v>
-      </c>
-      <c r="C96" t="s">
-        <v>23</v>
-      </c>
-      <c r="D96" s="5">
-        <v>928.42462833333332</v>
-      </c>
-      <c r="E96" s="13">
-        <v>1890.2624918888889</v>
-      </c>
-      <c r="F96" s="13">
-        <v>0.97914977777777779</v>
-      </c>
-      <c r="G96" s="13">
-        <v>270.41205844444437</v>
-      </c>
-      <c r="H96" s="13">
-        <v>9.8445367777777779</v>
-      </c>
-      <c r="I96" s="13">
-        <v>7.3341234444444439</v>
-      </c>
-      <c r="J96" s="13">
-        <v>8.2027718888888881</v>
-      </c>
-      <c r="K96" s="13">
-        <v>669.07213688888896</v>
-      </c>
-      <c r="L96" s="13">
-        <v>80.17382866666668</v>
-      </c>
-      <c r="M96" s="5">
-        <v>1393.0887585555556</v>
-      </c>
-      <c r="N96" s="13">
-        <v>930.93472622222225</v>
-      </c>
-      <c r="O96" s="14">
-        <v>5483.3967555555555</v>
-      </c>
-      <c r="P96" s="14">
-        <v>27412.728515555555</v>
-      </c>
-      <c r="Q96" s="23">
-        <v>-25.78476622222222</v>
-      </c>
-      <c r="R96" s="24">
-        <v>-7.9697777777777788E-3</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.3">
@@ -6620,114 +6623,119 @@
         <v>16</v>
       </c>
       <c r="B97" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C97" t="s">
         <v>23</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D97" s="5">
+        <v>928.42462833333332</v>
+      </c>
+      <c r="E97" s="13">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F97" s="13">
+        <v>0.97914977777777779</v>
+      </c>
+      <c r="G97" s="13">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H97" s="13">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I97" s="13">
+        <v>7.3341234444444439</v>
+      </c>
+      <c r="J97" s="13">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K97" s="13">
+        <v>669.07213688888896</v>
+      </c>
+      <c r="L97" s="13">
+        <v>80.17382866666668</v>
+      </c>
+      <c r="M97" s="5">
+        <v>1393.0887585555556</v>
+      </c>
+      <c r="N97" s="13">
+        <v>930.93472622222225</v>
+      </c>
+      <c r="O97" s="14">
+        <v>5483.3967555555555</v>
+      </c>
+      <c r="P97" s="14">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q97" s="23">
+        <v>-25.78476622222222</v>
+      </c>
+      <c r="R97" s="24">
+        <v>-7.9697777777777788E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>16</v>
+      </c>
+      <c r="B98" t="s">
+        <v>129</v>
+      </c>
+      <c r="C98" t="s">
+        <v>23</v>
+      </c>
+      <c r="D98" s="2">
         <v>928.62194833333342</v>
       </c>
-      <c r="E97" s="2">
+      <c r="E98" s="2">
         <v>1890.2624918888889</v>
       </c>
-      <c r="F97" s="2">
+      <c r="F98" s="2">
         <v>1.0534737777777776</v>
       </c>
-      <c r="G97" s="2">
+      <c r="G98" s="2">
         <v>270.41205844444437</v>
       </c>
-      <c r="H97" s="2">
+      <c r="H98" s="2">
         <v>9.8445367777777779</v>
       </c>
-      <c r="I97" s="2">
+      <c r="I98" s="2">
         <v>7.3320814444444453</v>
       </c>
-      <c r="J97" s="2">
+      <c r="J98" s="2">
         <v>8.2027718888888881</v>
       </c>
-      <c r="K97" s="2">
+      <c r="K98" s="2">
         <v>669.06689466666683</v>
       </c>
-      <c r="L97" s="2">
+      <c r="L98" s="2">
         <v>80.17382866666668</v>
       </c>
-      <c r="M97" s="2">
+      <c r="M98" s="2">
         <v>1393.1514079999999</v>
       </c>
-      <c r="N97" s="2">
+      <c r="N98" s="2">
         <v>931.139784111111</v>
       </c>
-      <c r="O97" s="3">
+      <c r="O98" s="3">
         <v>5989.2639431111111</v>
       </c>
-      <c r="P97" s="3">
+      <c r="P98" s="3">
         <v>27412.728515555555</v>
       </c>
-      <c r="Q97" s="23">
+      <c r="Q98" s="23">
         <v>-25.791903222222221</v>
       </c>
-      <c r="R97" s="24">
+      <c r="R98" s="24">
         <v>-7.9711111111111128E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>16</v>
       </c>
-      <c r="B100" t="s">
-        <v>93</v>
-      </c>
-      <c r="C100" t="s">
-        <v>92</v>
-      </c>
-      <c r="D100" s="2">
-        <v>1230.0044677999999</v>
-      </c>
-      <c r="E100" s="2">
-        <v>1848.1456909000001</v>
-      </c>
-      <c r="F100" s="2">
-        <v>1.0573501000000001</v>
-      </c>
-      <c r="G100" s="2">
-        <v>299.4371582</v>
-      </c>
-      <c r="H100" s="2">
-        <v>9.7418259000000003</v>
-      </c>
-      <c r="I100" s="2">
-        <v>5.7446602000000002</v>
-      </c>
-      <c r="J100" s="2">
-        <v>8.1171118999999994</v>
-      </c>
-      <c r="K100" s="2">
-        <v>673.08737180000003</v>
-      </c>
-      <c r="L100" s="2">
-        <v>81.12013859999999</v>
-      </c>
-      <c r="M100" s="2">
-        <v>1432.6230836</v>
-      </c>
-      <c r="N100" s="2">
-        <v>1196.8767700000001</v>
-      </c>
-      <c r="O100" s="3">
-        <v>5429.4087645999998</v>
-      </c>
-      <c r="P100" s="3">
-        <v>27140.258789299998</v>
-      </c>
-      <c r="Q100" s="2">
-        <v>-2.3066774000000003</v>
-      </c>
-      <c r="R100" s="4">
-        <v>-7.1000000000000002E-4</v>
-      </c>
-      <c r="S100" t="s">
-        <v>92</v>
+      <c r="C99" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.3">
@@ -6735,7 +6743,7 @@
         <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C101" t="s">
         <v>92</v>
@@ -6761,8 +6769,8 @@
       <c r="J101" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K101" s="5">
-        <v>675.4841553</v>
+      <c r="K101" s="2">
+        <v>673.08737180000003</v>
       </c>
       <c r="L101" s="2">
         <v>81.12013859999999</v>
@@ -6779,13 +6787,72 @@
       <c r="P101" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q101" s="5">
+      <c r="Q101" s="2">
+        <v>-2.3066774000000003</v>
+      </c>
+      <c r="R101" s="4">
+        <v>-7.1000000000000002E-4</v>
+      </c>
+      <c r="S101" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>16</v>
+      </c>
+      <c r="B102" t="s">
+        <v>95</v>
+      </c>
+      <c r="C102" t="s">
+        <v>92</v>
+      </c>
+      <c r="D102" s="2">
+        <v>1230.0044677999999</v>
+      </c>
+      <c r="E102" s="2">
+        <v>1848.1456909000001</v>
+      </c>
+      <c r="F102" s="2">
+        <v>1.0573501000000001</v>
+      </c>
+      <c r="G102" s="2">
+        <v>299.4371582</v>
+      </c>
+      <c r="H102" s="2">
+        <v>9.7418259000000003</v>
+      </c>
+      <c r="I102" s="2">
+        <v>5.7446602000000002</v>
+      </c>
+      <c r="J102" s="2">
+        <v>8.1171118999999994</v>
+      </c>
+      <c r="K102" s="5">
+        <v>675.4841553</v>
+      </c>
+      <c r="L102" s="2">
+        <v>81.12013859999999</v>
+      </c>
+      <c r="M102" s="2">
+        <v>1432.6230836</v>
+      </c>
+      <c r="N102" s="2">
+        <v>1196.8767700000001</v>
+      </c>
+      <c r="O102" s="3">
+        <v>5429.4087645999998</v>
+      </c>
+      <c r="P102" s="3">
+        <v>27140.258789299998</v>
+      </c>
+      <c r="Q102" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R101" s="7">
+      <c r="R102" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S101" t="s">
+      <c r="S102" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WORK-IN-PROGRESS Flow.xml - Remove "area_col" from the <catchments> block, as unnecessary. The area, m2, attribute is always called "AREA". Flow.cpp, .h - Remove 2 obsolete members of class FlowModel. Move GroundWaterRechargeFraction() out of HBV and add it to Flow.cpp as a global subroutine. In HRU::WetlSurfH2Ofluxes(), calculate HRU::m_standingH2Oflag. HBV.cpp, .h - Declare GroundWaterRechargeFraction() as extern and remove it from class HBV. Continue debugging the wetland v. non-wetland logic.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424F0DE4-A88F-4B81-BEF0-2ABA84A33725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AAA690-26AB-478E-BFE8-128246C5A202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="133">
   <si>
     <t>Year</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>Demo_Baseline_2010-18_C470+</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_C474+</t>
   </si>
 </sst>
 </file>
@@ -1330,11 +1333,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U102"/>
+  <dimension ref="A1:U103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T88" sqref="T88"/>
+      <selection pane="bottomLeft" activeCell="V90" sqref="V90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6428,78 +6431,102 @@
         <v>-7.9450000000000007E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="C89"/>
-      <c r="D89" s="13"/>
-      <c r="E89" s="20">
-        <f>E87/$E91</f>
-        <v>0.86752539266866613</v>
-      </c>
-      <c r="F89" s="21">
-        <f>(F87)/$E91</f>
-        <v>4.8348589849734502E-4</v>
-      </c>
-      <c r="G89" s="20">
-        <f>G87/$E91</f>
-        <v>0.12410410187647543</v>
-      </c>
-      <c r="H89" s="21">
-        <f>H87/$E91</f>
-        <v>4.5180950961439771E-3</v>
-      </c>
-      <c r="I89" s="20">
-        <f>I87/$E91</f>
-        <v>3.3689244602171388E-3</v>
-      </c>
-      <c r="J89" s="20">
-        <f>J87/$E87</f>
-        <v>4.3394882895423969E-3</v>
-      </c>
-      <c r="K89" s="20">
-        <f t="shared" ref="K89:M89" si="1">K87/$E87</f>
-        <v>0.35395211306017388</v>
-      </c>
-      <c r="L89" s="20">
-        <f t="shared" si="1"/>
-        <v>4.241412480311036E-2</v>
-      </c>
-      <c r="M89" s="20">
-        <f t="shared" si="1"/>
-        <v>0.75068557970027316</v>
-      </c>
-      <c r="N89" s="13"/>
-      <c r="O89" s="14"/>
-      <c r="P89" s="14"/>
-      <c r="Q89" s="13"/>
-      <c r="R89" s="15"/>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" t="s">
+        <v>132</v>
+      </c>
+      <c r="C89" t="s">
+        <v>23</v>
+      </c>
+      <c r="D89" s="2">
+        <v>929.71728533333328</v>
+      </c>
+      <c r="E89" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F89" s="2">
+        <v>1.0680259999999999</v>
+      </c>
+      <c r="G89" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H89" s="2">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I89" s="2">
+        <v>7.7082955555555559</v>
+      </c>
+      <c r="J89" s="2">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K89" s="2">
+        <v>669.04810911111099</v>
+      </c>
+      <c r="L89" s="2">
+        <v>80.5032391111111</v>
+      </c>
+      <c r="M89" s="13">
+        <v>1418.8638372222224</v>
+      </c>
+      <c r="N89" s="2">
+        <v>932.63113755555548</v>
+      </c>
+      <c r="O89" s="3">
+        <v>5820.4378255555557</v>
+      </c>
+      <c r="P89" s="3">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q89" s="13">
+        <v>0.23640099999999997</v>
+      </c>
+      <c r="R89" s="15">
+        <v>4.7777777777777777E-5</v>
+      </c>
     </row>
     <row r="90" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90" s="13"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="20"/>
-      <c r="H90" s="21"/>
-      <c r="I90" s="20"/>
+      <c r="E90" s="20">
+        <f>E87/$E92</f>
+        <v>0.86752539266866613</v>
+      </c>
+      <c r="F90" s="21">
+        <f>(F87)/$E92</f>
+        <v>4.8348589849734502E-4</v>
+      </c>
+      <c r="G90" s="20">
+        <f>G87/$E92</f>
+        <v>0.12410410187647543</v>
+      </c>
+      <c r="H90" s="21">
+        <f>H87/$E92</f>
+        <v>4.5180950961439771E-3</v>
+      </c>
+      <c r="I90" s="20">
+        <f>I87/$E92</f>
+        <v>3.3689244602171388E-3</v>
+      </c>
       <c r="J90" s="20">
-        <f>J87/$M87</f>
-        <v>5.7807002117651277E-3</v>
+        <f>J87/$E87</f>
+        <v>4.3394882895423969E-3</v>
       </c>
       <c r="K90" s="20">
-        <f t="shared" ref="K90:M90" si="2">K87/$M87</f>
-        <v>0.4715051449389725</v>
+        <f t="shared" ref="K90:M90" si="1">K87/$E87</f>
+        <v>0.35395211306017388</v>
       </c>
       <c r="L90" s="20">
-        <f t="shared" si="2"/>
-        <v>5.6500518925706657E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.241412480311036E-2</v>
       </c>
       <c r="M90" s="20">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.75068557970027316</v>
       </c>
       <c r="N90" s="13"/>
       <c r="O90" s="14"/>
@@ -6512,26 +6539,26 @@
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91" s="13"/>
-      <c r="E91" s="13">
-        <f>SUM(E87:I87)</f>
-        <v>2178.9131411111107</v>
-      </c>
-      <c r="F91" s="20">
-        <f>F89+H89</f>
-        <v>5.0015809946413218E-3</v>
-      </c>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13">
-        <f>SUM(J87:M87)</f>
-        <v>2176.4317833333334</v>
-      </c>
-      <c r="K91" s="13"/>
-      <c r="L91" s="13"/>
-      <c r="M91" s="13">
-        <f>(M87/1000)*3307080000/(365.25*24*60*60)</f>
-        <v>148.70340764865134</v>
+      <c r="E91" s="20"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="20"/>
+      <c r="H91" s="21"/>
+      <c r="I91" s="20"/>
+      <c r="J91" s="20">
+        <f>J87/$M87</f>
+        <v>5.7807002117651277E-3</v>
+      </c>
+      <c r="K91" s="20">
+        <f t="shared" ref="K91:M91" si="2">K87/$M87</f>
+        <v>0.4715051449389725</v>
+      </c>
+      <c r="L91" s="20">
+        <f t="shared" si="2"/>
+        <v>5.6500518925706657E-2</v>
+      </c>
+      <c r="M91" s="20">
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="N91" s="13"/>
       <c r="O91" s="14"/>
@@ -6544,18 +6571,27 @@
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92" s="13"/>
-      <c r="E92" s="13"/>
-      <c r="F92" s="20"/>
+      <c r="E92" s="13">
+        <f>SUM(E87:I87)</f>
+        <v>2178.9131411111107</v>
+      </c>
+      <c r="F92" s="20">
+        <f>F90+H90</f>
+        <v>5.0015809946413218E-3</v>
+      </c>
       <c r="G92" s="13"/>
       <c r="H92" s="13"/>
       <c r="I92" s="13"/>
-      <c r="J92" s="20">
-        <f>J91/E87</f>
-        <v>1.1513913058531</v>
+      <c r="J92" s="13">
+        <f>SUM(J87:M87)</f>
+        <v>2176.4317833333334</v>
       </c>
       <c r="K92" s="13"/>
       <c r="L92" s="13"/>
-      <c r="M92" s="13"/>
+      <c r="M92" s="13">
+        <f>(M87/1000)*3307080000/(365.25*24*60*60)</f>
+        <v>148.70340764865134</v>
+      </c>
       <c r="N92" s="13"/>
       <c r="O92" s="14"/>
       <c r="P92" s="14"/>
@@ -6572,9 +6608,9 @@
       <c r="G93" s="13"/>
       <c r="H93" s="13"/>
       <c r="I93" s="13"/>
-      <c r="J93" s="22">
-        <f>J91-E91</f>
-        <v>-2.481357777777248</v>
+      <c r="J93" s="20">
+        <f>J92/E87</f>
+        <v>1.1513913058531</v>
       </c>
       <c r="K93" s="13"/>
       <c r="L93" s="13"/>
@@ -6595,9 +6631,9 @@
       <c r="G94" s="13"/>
       <c r="H94" s="13"/>
       <c r="I94" s="13"/>
-      <c r="J94" s="21">
-        <f>J93/E91</f>
-        <v>-1.1388052745011715E-3</v>
+      <c r="J94" s="22">
+        <f>J92-E92</f>
+        <v>-2.481357777777248</v>
       </c>
       <c r="K94" s="13"/>
       <c r="L94" s="13"/>
@@ -6608,70 +6644,37 @@
       <c r="Q94" s="13"/>
       <c r="R94" s="15"/>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="D95" s="2">
+    <row r="95" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95"/>
+      <c r="B95"/>
+      <c r="C95"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="21">
+        <f>J94/E92</f>
+        <v>-1.1388052745011715E-3</v>
+      </c>
+      <c r="K95" s="13"/>
+      <c r="L95" s="13"/>
+      <c r="M95" s="13"/>
+      <c r="N95" s="13"/>
+      <c r="O95" s="14"/>
+      <c r="P95" s="14"/>
+      <c r="Q95" s="13"/>
+      <c r="R95" s="15"/>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D96" s="2">
         <f>SUM(D85:I85)</f>
         <v>3109.2584012222219</v>
       </c>
-      <c r="J95" s="2">
+      <c r="J96" s="2">
         <f>SUM(J85:N85)</f>
         <v>3108.8211602222223</v>
-      </c>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>16</v>
-      </c>
-      <c r="B97" t="s">
-        <v>128</v>
-      </c>
-      <c r="C97" t="s">
-        <v>23</v>
-      </c>
-      <c r="D97" s="5">
-        <v>928.42462833333332</v>
-      </c>
-      <c r="E97" s="13">
-        <v>1890.2624918888889</v>
-      </c>
-      <c r="F97" s="13">
-        <v>0.97914977777777779</v>
-      </c>
-      <c r="G97" s="13">
-        <v>270.41205844444437</v>
-      </c>
-      <c r="H97" s="13">
-        <v>9.8445367777777779</v>
-      </c>
-      <c r="I97" s="13">
-        <v>7.3341234444444439</v>
-      </c>
-      <c r="J97" s="13">
-        <v>8.2027718888888881</v>
-      </c>
-      <c r="K97" s="13">
-        <v>669.07213688888896</v>
-      </c>
-      <c r="L97" s="13">
-        <v>80.17382866666668</v>
-      </c>
-      <c r="M97" s="5">
-        <v>1393.0887585555556</v>
-      </c>
-      <c r="N97" s="13">
-        <v>930.93472622222225</v>
-      </c>
-      <c r="O97" s="14">
-        <v>5483.3967555555555</v>
-      </c>
-      <c r="P97" s="14">
-        <v>27412.728515555555</v>
-      </c>
-      <c r="Q97" s="23">
-        <v>-25.78476622222222</v>
-      </c>
-      <c r="R97" s="24">
-        <v>-7.9697777777777788E-3</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.3">
@@ -6679,122 +6682,119 @@
         <v>16</v>
       </c>
       <c r="B98" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C98" t="s">
         <v>23</v>
       </c>
-      <c r="D98" s="2">
-        <v>928.62194833333342</v>
-      </c>
-      <c r="E98" s="2">
+      <c r="D98" s="5">
+        <v>928.42462833333332</v>
+      </c>
+      <c r="E98" s="13">
         <v>1890.2624918888889</v>
       </c>
-      <c r="F98" s="2">
-        <v>1.0534737777777776</v>
-      </c>
-      <c r="G98" s="2">
+      <c r="F98" s="13">
+        <v>0.97914977777777779</v>
+      </c>
+      <c r="G98" s="13">
         <v>270.41205844444437</v>
       </c>
-      <c r="H98" s="2">
+      <c r="H98" s="13">
         <v>9.8445367777777779</v>
       </c>
-      <c r="I98" s="2">
-        <v>7.3320814444444453</v>
-      </c>
-      <c r="J98" s="2">
+      <c r="I98" s="13">
+        <v>7.3341234444444439</v>
+      </c>
+      <c r="J98" s="13">
         <v>8.2027718888888881</v>
       </c>
-      <c r="K98" s="2">
-        <v>669.06689466666683</v>
-      </c>
-      <c r="L98" s="2">
+      <c r="K98" s="13">
+        <v>669.07213688888896</v>
+      </c>
+      <c r="L98" s="13">
         <v>80.17382866666668</v>
       </c>
-      <c r="M98" s="2">
-        <v>1393.1514079999999</v>
-      </c>
-      <c r="N98" s="2">
-        <v>931.139784111111</v>
-      </c>
-      <c r="O98" s="3">
-        <v>5989.2639431111111</v>
-      </c>
-      <c r="P98" s="3">
+      <c r="M98" s="5">
+        <v>1393.0887585555556</v>
+      </c>
+      <c r="N98" s="13">
+        <v>930.93472622222225</v>
+      </c>
+      <c r="O98" s="14">
+        <v>5483.3967555555555</v>
+      </c>
+      <c r="P98" s="14">
         <v>27412.728515555555</v>
       </c>
       <c r="Q98" s="23">
-        <v>-25.791903222222221</v>
+        <v>-25.78476622222222</v>
       </c>
       <c r="R98" s="24">
-        <v>-7.9711111111111128E-3</v>
+        <v>-7.9697777777777788E-3</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>16</v>
       </c>
+      <c r="B99" t="s">
+        <v>129</v>
+      </c>
       <c r="C99" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+      <c r="D99" s="2">
+        <v>928.62194833333342</v>
+      </c>
+      <c r="E99" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F99" s="2">
+        <v>1.0534737777777776</v>
+      </c>
+      <c r="G99" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H99" s="2">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I99" s="2">
+        <v>7.3320814444444453</v>
+      </c>
+      <c r="J99" s="2">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K99" s="2">
+        <v>669.06689466666683</v>
+      </c>
+      <c r="L99" s="2">
+        <v>80.17382866666668</v>
+      </c>
+      <c r="M99" s="2">
+        <v>1393.1514079999999</v>
+      </c>
+      <c r="N99" s="2">
+        <v>931.139784111111</v>
+      </c>
+      <c r="O99" s="3">
+        <v>5989.2639431111111</v>
+      </c>
+      <c r="P99" s="3">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q99" s="23">
+        <v>-25.791903222222221</v>
+      </c>
+      <c r="R99" s="24">
+        <v>-7.9711111111111128E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>16</v>
       </c>
-      <c r="B101" t="s">
-        <v>93</v>
-      </c>
-      <c r="C101" t="s">
-        <v>92</v>
-      </c>
-      <c r="D101" s="2">
-        <v>1230.0044677999999</v>
-      </c>
-      <c r="E101" s="2">
-        <v>1848.1456909000001</v>
-      </c>
-      <c r="F101" s="2">
-        <v>1.0573501000000001</v>
-      </c>
-      <c r="G101" s="2">
-        <v>299.4371582</v>
-      </c>
-      <c r="H101" s="2">
-        <v>9.7418259000000003</v>
-      </c>
-      <c r="I101" s="2">
-        <v>5.7446602000000002</v>
-      </c>
-      <c r="J101" s="2">
-        <v>8.1171118999999994</v>
-      </c>
-      <c r="K101" s="2">
-        <v>673.08737180000003</v>
-      </c>
-      <c r="L101" s="2">
-        <v>81.12013859999999</v>
-      </c>
-      <c r="M101" s="2">
-        <v>1432.6230836</v>
-      </c>
-      <c r="N101" s="2">
-        <v>1196.8767700000001</v>
-      </c>
-      <c r="O101" s="3">
-        <v>5429.4087645999998</v>
-      </c>
-      <c r="P101" s="3">
-        <v>27140.258789299998</v>
-      </c>
-      <c r="Q101" s="2">
-        <v>-2.3066774000000003</v>
-      </c>
-      <c r="R101" s="4">
-        <v>-7.1000000000000002E-4</v>
-      </c>
-      <c r="S101" t="s">
-        <v>92</v>
+      <c r="C100" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.3">
@@ -6802,7 +6802,7 @@
         <v>16</v>
       </c>
       <c r="B102" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C102" t="s">
         <v>92</v>
@@ -6828,8 +6828,8 @@
       <c r="J102" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K102" s="5">
-        <v>675.4841553</v>
+      <c r="K102" s="2">
+        <v>673.08737180000003</v>
       </c>
       <c r="L102" s="2">
         <v>81.12013859999999</v>
@@ -6846,13 +6846,72 @@
       <c r="P102" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q102" s="5">
+      <c r="Q102" s="2">
+        <v>-2.3066774000000003</v>
+      </c>
+      <c r="R102" s="4">
+        <v>-7.1000000000000002E-4</v>
+      </c>
+      <c r="S102" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>16</v>
+      </c>
+      <c r="B103" t="s">
+        <v>95</v>
+      </c>
+      <c r="C103" t="s">
+        <v>92</v>
+      </c>
+      <c r="D103" s="2">
+        <v>1230.0044677999999</v>
+      </c>
+      <c r="E103" s="2">
+        <v>1848.1456909000001</v>
+      </c>
+      <c r="F103" s="2">
+        <v>1.0573501000000001</v>
+      </c>
+      <c r="G103" s="2">
+        <v>299.4371582</v>
+      </c>
+      <c r="H103" s="2">
+        <v>9.7418259000000003</v>
+      </c>
+      <c r="I103" s="2">
+        <v>5.7446602000000002</v>
+      </c>
+      <c r="J103" s="2">
+        <v>8.1171118999999994</v>
+      </c>
+      <c r="K103" s="5">
+        <v>675.4841553</v>
+      </c>
+      <c r="L103" s="2">
+        <v>81.12013859999999</v>
+      </c>
+      <c r="M103" s="2">
+        <v>1432.6230836</v>
+      </c>
+      <c r="N103" s="2">
+        <v>1196.8767700000001</v>
+      </c>
+      <c r="O103" s="3">
+        <v>5429.4087645999998</v>
+      </c>
+      <c r="P103" s="3">
+        <v>27140.258789299998</v>
+      </c>
+      <c r="Q103" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R102" s="7">
+      <c r="R103" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S102" t="s">
+      <c r="S103" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flow.cpp - Add logic for WETL2Q.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AAA690-26AB-478E-BFE8-128246C5A202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730F74AB-7426-41BD-B2C6-4D3842FB3D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="134">
   <si>
     <t>Year</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>Demo_Baseline_2010-18_C474+</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_C478</t>
   </si>
 </sst>
 </file>
@@ -1333,11 +1336,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U103"/>
+  <dimension ref="A1:U104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V90" sqref="V90"/>
+      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6487,78 +6490,102 @@
         <v>4.7777777777777777E-5</v>
       </c>
     </row>
-    <row r="90" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90"/>
-      <c r="B90"/>
-      <c r="C90"/>
-      <c r="D90" s="13"/>
-      <c r="E90" s="20">
-        <f>E87/$E92</f>
-        <v>0.86752539266866613</v>
-      </c>
-      <c r="F90" s="21">
-        <f>(F87)/$E92</f>
-        <v>4.8348589849734502E-4</v>
-      </c>
-      <c r="G90" s="20">
-        <f>G87/$E92</f>
-        <v>0.12410410187647543</v>
-      </c>
-      <c r="H90" s="21">
-        <f>H87/$E92</f>
-        <v>4.5180950961439771E-3</v>
-      </c>
-      <c r="I90" s="20">
-        <f>I87/$E92</f>
-        <v>3.3689244602171388E-3</v>
-      </c>
-      <c r="J90" s="20">
-        <f>J87/$E87</f>
-        <v>4.3394882895423969E-3</v>
-      </c>
-      <c r="K90" s="20">
-        <f t="shared" ref="K90:M90" si="1">K87/$E87</f>
-        <v>0.35395211306017388</v>
-      </c>
-      <c r="L90" s="20">
-        <f t="shared" si="1"/>
-        <v>4.241412480311036E-2</v>
-      </c>
-      <c r="M90" s="20">
-        <f t="shared" si="1"/>
-        <v>0.75068557970027316</v>
-      </c>
-      <c r="N90" s="13"/>
-      <c r="O90" s="14"/>
-      <c r="P90" s="14"/>
-      <c r="Q90" s="13"/>
-      <c r="R90" s="15"/>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>16</v>
+      </c>
+      <c r="B90" t="s">
+        <v>133</v>
+      </c>
+      <c r="C90" t="s">
+        <v>23</v>
+      </c>
+      <c r="D90" s="2">
+        <v>929.20939122222217</v>
+      </c>
+      <c r="E90" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F90" s="2">
+        <v>1.0680628888888888</v>
+      </c>
+      <c r="G90" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H90" s="2">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I90" s="2">
+        <v>7.3098580000000011</v>
+      </c>
+      <c r="J90" s="2">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K90" s="2">
+        <v>669.03998488888885</v>
+      </c>
+      <c r="L90" s="2">
+        <v>80.503111000000018</v>
+      </c>
+      <c r="M90" s="13">
+        <v>1418.4739583333333</v>
+      </c>
+      <c r="N90" s="2">
+        <v>932.03712288888892</v>
+      </c>
+      <c r="O90" s="3">
+        <v>5819.6493598888883</v>
+      </c>
+      <c r="P90" s="3">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q90" s="13">
+        <v>0.15054966666666666</v>
+      </c>
+      <c r="R90" s="15">
+        <v>2.0333333333333334E-5</v>
+      </c>
     </row>
     <row r="91" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91" s="13"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="20"/>
-      <c r="H91" s="21"/>
-      <c r="I91" s="20"/>
+      <c r="E91" s="20">
+        <f>E87/$E93</f>
+        <v>0.86752539266866613</v>
+      </c>
+      <c r="F91" s="21">
+        <f>(F87)/$E93</f>
+        <v>4.8348589849734502E-4</v>
+      </c>
+      <c r="G91" s="20">
+        <f>G87/$E93</f>
+        <v>0.12410410187647543</v>
+      </c>
+      <c r="H91" s="21">
+        <f>H87/$E93</f>
+        <v>4.5180950961439771E-3</v>
+      </c>
+      <c r="I91" s="20">
+        <f>I87/$E93</f>
+        <v>3.3689244602171388E-3</v>
+      </c>
       <c r="J91" s="20">
-        <f>J87/$M87</f>
-        <v>5.7807002117651277E-3</v>
+        <f>J87/$E87</f>
+        <v>4.3394882895423969E-3</v>
       </c>
       <c r="K91" s="20">
-        <f t="shared" ref="K91:M91" si="2">K87/$M87</f>
-        <v>0.4715051449389725</v>
+        <f t="shared" ref="K91:M91" si="1">K87/$E87</f>
+        <v>0.35395211306017388</v>
       </c>
       <c r="L91" s="20">
-        <f t="shared" si="2"/>
-        <v>5.6500518925706657E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.241412480311036E-2</v>
       </c>
       <c r="M91" s="20">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.75068557970027316</v>
       </c>
       <c r="N91" s="13"/>
       <c r="O91" s="14"/>
@@ -6571,26 +6598,26 @@
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92" s="13"/>
-      <c r="E92" s="13">
-        <f>SUM(E87:I87)</f>
-        <v>2178.9131411111107</v>
-      </c>
-      <c r="F92" s="20">
-        <f>F90+H90</f>
-        <v>5.0015809946413218E-3</v>
-      </c>
-      <c r="G92" s="13"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13">
-        <f>SUM(J87:M87)</f>
-        <v>2176.4317833333334</v>
-      </c>
-      <c r="K92" s="13"/>
-      <c r="L92" s="13"/>
-      <c r="M92" s="13">
-        <f>(M87/1000)*3307080000/(365.25*24*60*60)</f>
-        <v>148.70340764865134</v>
+      <c r="E92" s="20"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="20"/>
+      <c r="H92" s="21"/>
+      <c r="I92" s="20"/>
+      <c r="J92" s="20">
+        <f>J87/$M87</f>
+        <v>5.7807002117651277E-3</v>
+      </c>
+      <c r="K92" s="20">
+        <f t="shared" ref="K92:M92" si="2">K87/$M87</f>
+        <v>0.4715051449389725</v>
+      </c>
+      <c r="L92" s="20">
+        <f t="shared" si="2"/>
+        <v>5.6500518925706657E-2</v>
+      </c>
+      <c r="M92" s="20">
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="N92" s="13"/>
       <c r="O92" s="14"/>
@@ -6603,18 +6630,27 @@
       <c r="B93"/>
       <c r="C93"/>
       <c r="D93" s="13"/>
-      <c r="E93" s="13"/>
-      <c r="F93" s="20"/>
+      <c r="E93" s="13">
+        <f>SUM(E87:I87)</f>
+        <v>2178.9131411111107</v>
+      </c>
+      <c r="F93" s="20">
+        <f>F91+H91</f>
+        <v>5.0015809946413218E-3</v>
+      </c>
       <c r="G93" s="13"/>
       <c r="H93" s="13"/>
       <c r="I93" s="13"/>
-      <c r="J93" s="20">
-        <f>J92/E87</f>
-        <v>1.1513913058531</v>
+      <c r="J93" s="13">
+        <f>SUM(J87:M87)</f>
+        <v>2176.4317833333334</v>
       </c>
       <c r="K93" s="13"/>
       <c r="L93" s="13"/>
-      <c r="M93" s="13"/>
+      <c r="M93" s="13">
+        <f>(M87/1000)*3307080000/(365.25*24*60*60)</f>
+        <v>148.70340764865134</v>
+      </c>
       <c r="N93" s="13"/>
       <c r="O93" s="14"/>
       <c r="P93" s="14"/>
@@ -6631,9 +6667,9 @@
       <c r="G94" s="13"/>
       <c r="H94" s="13"/>
       <c r="I94" s="13"/>
-      <c r="J94" s="22">
-        <f>J92-E92</f>
-        <v>-2.481357777777248</v>
+      <c r="J94" s="20">
+        <f>J93/E87</f>
+        <v>1.1513913058531</v>
       </c>
       <c r="K94" s="13"/>
       <c r="L94" s="13"/>
@@ -6654,9 +6690,9 @@
       <c r="G95" s="13"/>
       <c r="H95" s="13"/>
       <c r="I95" s="13"/>
-      <c r="J95" s="21">
-        <f>J94/E92</f>
-        <v>-1.1388052745011715E-3</v>
+      <c r="J95" s="22">
+        <f>J93-E93</f>
+        <v>-2.481357777777248</v>
       </c>
       <c r="K95" s="13"/>
       <c r="L95" s="13"/>
@@ -6667,70 +6703,37 @@
       <c r="Q95" s="13"/>
       <c r="R95" s="15"/>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="D96" s="2">
+    <row r="96" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96"/>
+      <c r="B96"/>
+      <c r="C96"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="21">
+        <f>J95/E93</f>
+        <v>-1.1388052745011715E-3</v>
+      </c>
+      <c r="K96" s="13"/>
+      <c r="L96" s="13"/>
+      <c r="M96" s="13"/>
+      <c r="N96" s="13"/>
+      <c r="O96" s="14"/>
+      <c r="P96" s="14"/>
+      <c r="Q96" s="13"/>
+      <c r="R96" s="15"/>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D97" s="2">
         <f>SUM(D85:I85)</f>
         <v>3109.2584012222219</v>
       </c>
-      <c r="J96" s="2">
+      <c r="J97" s="2">
         <f>SUM(J85:N85)</f>
         <v>3108.8211602222223</v>
-      </c>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>16</v>
-      </c>
-      <c r="B98" t="s">
-        <v>128</v>
-      </c>
-      <c r="C98" t="s">
-        <v>23</v>
-      </c>
-      <c r="D98" s="5">
-        <v>928.42462833333332</v>
-      </c>
-      <c r="E98" s="13">
-        <v>1890.2624918888889</v>
-      </c>
-      <c r="F98" s="13">
-        <v>0.97914977777777779</v>
-      </c>
-      <c r="G98" s="13">
-        <v>270.41205844444437</v>
-      </c>
-      <c r="H98" s="13">
-        <v>9.8445367777777779</v>
-      </c>
-      <c r="I98" s="13">
-        <v>7.3341234444444439</v>
-      </c>
-      <c r="J98" s="13">
-        <v>8.2027718888888881</v>
-      </c>
-      <c r="K98" s="13">
-        <v>669.07213688888896</v>
-      </c>
-      <c r="L98" s="13">
-        <v>80.17382866666668</v>
-      </c>
-      <c r="M98" s="5">
-        <v>1393.0887585555556</v>
-      </c>
-      <c r="N98" s="13">
-        <v>930.93472622222225</v>
-      </c>
-      <c r="O98" s="14">
-        <v>5483.3967555555555</v>
-      </c>
-      <c r="P98" s="14">
-        <v>27412.728515555555</v>
-      </c>
-      <c r="Q98" s="23">
-        <v>-25.78476622222222</v>
-      </c>
-      <c r="R98" s="24">
-        <v>-7.9697777777777788E-3</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.3">
@@ -6738,122 +6741,119 @@
         <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C99" t="s">
         <v>23</v>
       </c>
-      <c r="D99" s="2">
-        <v>928.62194833333342</v>
-      </c>
-      <c r="E99" s="2">
+      <c r="D99" s="5">
+        <v>928.42462833333332</v>
+      </c>
+      <c r="E99" s="13">
         <v>1890.2624918888889</v>
       </c>
-      <c r="F99" s="2">
-        <v>1.0534737777777776</v>
-      </c>
-      <c r="G99" s="2">
+      <c r="F99" s="13">
+        <v>0.97914977777777779</v>
+      </c>
+      <c r="G99" s="13">
         <v>270.41205844444437</v>
       </c>
-      <c r="H99" s="2">
+      <c r="H99" s="13">
         <v>9.8445367777777779</v>
       </c>
-      <c r="I99" s="2">
-        <v>7.3320814444444453</v>
-      </c>
-      <c r="J99" s="2">
+      <c r="I99" s="13">
+        <v>7.3341234444444439</v>
+      </c>
+      <c r="J99" s="13">
         <v>8.2027718888888881</v>
       </c>
-      <c r="K99" s="2">
-        <v>669.06689466666683</v>
-      </c>
-      <c r="L99" s="2">
+      <c r="K99" s="13">
+        <v>669.07213688888896</v>
+      </c>
+      <c r="L99" s="13">
         <v>80.17382866666668</v>
       </c>
-      <c r="M99" s="2">
-        <v>1393.1514079999999</v>
-      </c>
-      <c r="N99" s="2">
-        <v>931.139784111111</v>
-      </c>
-      <c r="O99" s="3">
-        <v>5989.2639431111111</v>
-      </c>
-      <c r="P99" s="3">
+      <c r="M99" s="5">
+        <v>1393.0887585555556</v>
+      </c>
+      <c r="N99" s="13">
+        <v>930.93472622222225</v>
+      </c>
+      <c r="O99" s="14">
+        <v>5483.3967555555555</v>
+      </c>
+      <c r="P99" s="14">
         <v>27412.728515555555</v>
       </c>
       <c r="Q99" s="23">
-        <v>-25.791903222222221</v>
+        <v>-25.78476622222222</v>
       </c>
       <c r="R99" s="24">
-        <v>-7.9711111111111128E-3</v>
+        <v>-7.9697777777777788E-3</v>
       </c>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>16</v>
       </c>
+      <c r="B100" t="s">
+        <v>129</v>
+      </c>
       <c r="C100" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+      <c r="D100" s="2">
+        <v>928.62194833333342</v>
+      </c>
+      <c r="E100" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F100" s="2">
+        <v>1.0534737777777776</v>
+      </c>
+      <c r="G100" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H100" s="2">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I100" s="2">
+        <v>7.3320814444444453</v>
+      </c>
+      <c r="J100" s="2">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K100" s="2">
+        <v>669.06689466666683</v>
+      </c>
+      <c r="L100" s="2">
+        <v>80.17382866666668</v>
+      </c>
+      <c r="M100" s="2">
+        <v>1393.1514079999999</v>
+      </c>
+      <c r="N100" s="2">
+        <v>931.139784111111</v>
+      </c>
+      <c r="O100" s="3">
+        <v>5989.2639431111111</v>
+      </c>
+      <c r="P100" s="3">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q100" s="23">
+        <v>-25.791903222222221</v>
+      </c>
+      <c r="R100" s="24">
+        <v>-7.9711111111111128E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>16</v>
       </c>
-      <c r="B102" t="s">
-        <v>93</v>
-      </c>
-      <c r="C102" t="s">
-        <v>92</v>
-      </c>
-      <c r="D102" s="2">
-        <v>1230.0044677999999</v>
-      </c>
-      <c r="E102" s="2">
-        <v>1848.1456909000001</v>
-      </c>
-      <c r="F102" s="2">
-        <v>1.0573501000000001</v>
-      </c>
-      <c r="G102" s="2">
-        <v>299.4371582</v>
-      </c>
-      <c r="H102" s="2">
-        <v>9.7418259000000003</v>
-      </c>
-      <c r="I102" s="2">
-        <v>5.7446602000000002</v>
-      </c>
-      <c r="J102" s="2">
-        <v>8.1171118999999994</v>
-      </c>
-      <c r="K102" s="2">
-        <v>673.08737180000003</v>
-      </c>
-      <c r="L102" s="2">
-        <v>81.12013859999999</v>
-      </c>
-      <c r="M102" s="2">
-        <v>1432.6230836</v>
-      </c>
-      <c r="N102" s="2">
-        <v>1196.8767700000001</v>
-      </c>
-      <c r="O102" s="3">
-        <v>5429.4087645999998</v>
-      </c>
-      <c r="P102" s="3">
-        <v>27140.258789299998</v>
-      </c>
-      <c r="Q102" s="2">
-        <v>-2.3066774000000003</v>
-      </c>
-      <c r="R102" s="4">
-        <v>-7.1000000000000002E-4</v>
-      </c>
-      <c r="S102" t="s">
-        <v>92</v>
+      <c r="C101" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.3">
@@ -6861,7 +6861,7 @@
         <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C103" t="s">
         <v>92</v>
@@ -6887,8 +6887,8 @@
       <c r="J103" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K103" s="5">
-        <v>675.4841553</v>
+      <c r="K103" s="2">
+        <v>673.08737180000003</v>
       </c>
       <c r="L103" s="2">
         <v>81.12013859999999</v>
@@ -6905,13 +6905,72 @@
       <c r="P103" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q103" s="5">
+      <c r="Q103" s="2">
+        <v>-2.3066774000000003</v>
+      </c>
+      <c r="R103" s="4">
+        <v>-7.1000000000000002E-4</v>
+      </c>
+      <c r="S103" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>16</v>
+      </c>
+      <c r="B104" t="s">
+        <v>95</v>
+      </c>
+      <c r="C104" t="s">
+        <v>92</v>
+      </c>
+      <c r="D104" s="2">
+        <v>1230.0044677999999</v>
+      </c>
+      <c r="E104" s="2">
+        <v>1848.1456909000001</v>
+      </c>
+      <c r="F104" s="2">
+        <v>1.0573501000000001</v>
+      </c>
+      <c r="G104" s="2">
+        <v>299.4371582</v>
+      </c>
+      <c r="H104" s="2">
+        <v>9.7418259000000003</v>
+      </c>
+      <c r="I104" s="2">
+        <v>5.7446602000000002</v>
+      </c>
+      <c r="J104" s="2">
+        <v>8.1171118999999994</v>
+      </c>
+      <c r="K104" s="5">
+        <v>675.4841553</v>
+      </c>
+      <c r="L104" s="2">
+        <v>81.12013859999999</v>
+      </c>
+      <c r="M104" s="2">
+        <v>1432.6230836</v>
+      </c>
+      <c r="N104" s="2">
+        <v>1196.8767700000001</v>
+      </c>
+      <c r="O104" s="3">
+        <v>5429.4087645999998</v>
+      </c>
+      <c r="P104" s="3">
+        <v>27140.258789299998</v>
+      </c>
+      <c r="Q104" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R103" s="7">
+      <c r="R104" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S103" t="s">
+      <c r="S104" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new shapefile pieces created by David Holman.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EC4743-2B32-44C6-B4BA-7E807A1E76D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35982294-E339-4F01-8706-08059CE55128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="139">
   <si>
     <t>Year</t>
   </si>
@@ -444,6 +444,12 @@
   </si>
   <si>
     <t>Demo_Baseline_2010-19 C550</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-19 C564</t>
+  </si>
+  <si>
+    <t>CW3M 1.1.0</t>
   </si>
 </sst>
 </file>
@@ -1349,7 +1355,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F117" sqref="F116:F117"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7022,6 +7028,62 @@
         <v>0.15698588888888887</v>
       </c>
       <c r="R103" s="15">
+        <v>2.8555555555555569E-5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>138</v>
+      </c>
+      <c r="B104" t="s">
+        <v>137</v>
+      </c>
+      <c r="C104" t="s">
+        <v>23</v>
+      </c>
+      <c r="D104" s="2">
+        <v>929.46765811111118</v>
+      </c>
+      <c r="E104" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F104" s="2">
+        <v>1.0681051111111111</v>
+      </c>
+      <c r="G104" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H104" s="2">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I104" s="2">
+        <v>7.3214413333333335</v>
+      </c>
+      <c r="J104" s="2">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K104" s="2">
+        <v>668.82741966666663</v>
+      </c>
+      <c r="L104" s="2">
+        <v>80.524254777777799</v>
+      </c>
+      <c r="M104" s="2">
+        <v>1418.6363662222223</v>
+      </c>
+      <c r="N104" s="2">
+        <v>932.34245466666675</v>
+      </c>
+      <c r="O104" s="3">
+        <v>5824.0347221111115</v>
+      </c>
+      <c r="P104" s="3">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q104" s="2">
+        <v>0.15697544444444445</v>
+      </c>
+      <c r="R104" s="4">
         <v>2.8555555555555569E-5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Activate wetland 10, which has 2 IDUs (IDs 33827 and 33807), totaling 21 acres adjacent to Springfield. HRU_McKenzie.dbf - Set wetland 10 IDUs as WETNESS=0. IDU_McKenzie.dbf - Set VEGCLASS for the 2 IDUs as 6246 PEMC, and propagate to LULC_B and LULC_A. Also, add new attribute TEMP_WETL.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35982294-E339-4F01-8706-08059CE55128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BC19A1-7C41-4CB5-8C66-0F1E5081FEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="140">
   <si>
     <t>Year</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>CW3M 1.1.0</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18 C600</t>
   </si>
 </sst>
 </file>
@@ -1351,11 +1354,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U108"/>
+  <dimension ref="A1:U113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7087,123 +7090,247 @@
         <v>2.8555555555555569E-5</v>
       </c>
     </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>138</v>
+      </c>
+      <c r="B105" t="s">
+        <v>139</v>
+      </c>
+      <c r="C105" t="s">
+        <v>23</v>
+      </c>
+      <c r="D105" s="2">
+        <v>929.46866188888873</v>
+      </c>
+      <c r="E105" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F105" s="2">
+        <v>1.0681051111111111</v>
+      </c>
+      <c r="G105" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H105" s="2">
+        <v>9.8445367777777779</v>
+      </c>
+      <c r="I105" s="2">
+        <v>7.3212358888888884</v>
+      </c>
+      <c r="J105" s="2">
+        <v>8.2027718888888881</v>
+      </c>
+      <c r="K105" s="2">
+        <v>668.60776777777789</v>
+      </c>
+      <c r="L105" s="2">
+        <v>80.524254777777799</v>
+      </c>
+      <c r="M105" s="2">
+        <v>1418.8558755555559</v>
+      </c>
+      <c r="N105" s="2">
+        <v>932.34357366666654</v>
+      </c>
+      <c r="O105" s="3">
+        <v>5824.0346137777778</v>
+      </c>
+      <c r="P105" s="3">
+        <v>27412.728515555555</v>
+      </c>
+      <c r="Q105" s="2">
+        <v>0.15715366666666666</v>
+      </c>
+      <c r="R105" s="4">
+        <v>2.8666666666666671E-5</v>
+      </c>
+    </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
+      <c r="K106" s="2"/>
+      <c r="L106" s="2"/>
+      <c r="M106" s="2"/>
+      <c r="N106" s="2"/>
+      <c r="O106" s="3"/>
+      <c r="P106" s="3"/>
+      <c r="Q106" s="2"/>
+      <c r="R106" s="4"/>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="2"/>
+      <c r="K107" s="2"/>
+      <c r="L107" s="2"/>
+      <c r="M107" s="2"/>
+      <c r="N107" s="2"/>
+      <c r="O107" s="3"/>
+      <c r="P107" s="3"/>
+      <c r="Q107" s="2"/>
+      <c r="R107" s="4"/>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+      <c r="K108" s="2"/>
+      <c r="L108" s="2"/>
+      <c r="M108" s="2"/>
+      <c r="N108" s="2"/>
+      <c r="O108" s="3"/>
+      <c r="P108" s="3"/>
+      <c r="Q108" s="2"/>
+      <c r="R108" s="4"/>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+      <c r="K109" s="2"/>
+      <c r="L109" s="2"/>
+      <c r="M109" s="2"/>
+      <c r="N109" s="2"/>
+      <c r="O109" s="3"/>
+      <c r="P109" s="3"/>
+      <c r="Q109" s="2"/>
+      <c r="R109" s="4"/>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>16</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B111" t="s">
         <v>93</v>
       </c>
-      <c r="D106" s="2">
+      <c r="D111" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E106" s="2">
+      <c r="E111" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F106" s="2">
+      <c r="F111" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G106" s="2">
+      <c r="G111" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H106" s="2">
+      <c r="H111" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I106" s="2">
+      <c r="I111" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J106" s="2">
+      <c r="J111" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K106" s="2">
+      <c r="K111" s="2">
         <v>673.08737180000003</v>
       </c>
-      <c r="L106" s="2">
+      <c r="L111" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M106" s="2">
+      <c r="M111" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N106" s="2">
+      <c r="N111" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O106" s="3">
+      <c r="O111" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P106" s="3">
+      <c r="P111" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q106" s="2">
+      <c r="Q111" s="2">
         <v>-2.3066774000000003</v>
       </c>
-      <c r="R106" s="4">
+      <c r="R111" s="4">
         <v>-7.1000000000000002E-4</v>
       </c>
-      <c r="S106" t="s">
+      <c r="S111" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>16</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B112" t="s">
         <v>95</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C112" t="s">
         <v>92</v>
       </c>
-      <c r="D107" s="2">
+      <c r="D112" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E107" s="2">
+      <c r="E112" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F107" s="2">
+      <c r="F112" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G107" s="2">
+      <c r="G112" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H107" s="2">
+      <c r="H112" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I107" s="2">
+      <c r="I112" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J107" s="2">
+      <c r="J112" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K107" s="5">
+      <c r="K112" s="5">
         <v>675.4841553</v>
       </c>
-      <c r="L107" s="2">
+      <c r="L112" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M107" s="2">
+      <c r="M112" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N107" s="2">
+      <c r="N112" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O107" s="3">
+      <c r="O112" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P107" s="3">
+      <c r="P112" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q107" s="5">
+      <c r="Q112" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R107" s="7">
+      <c r="R112" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S107" t="s">
+      <c r="S112" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C108" t="s">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C113" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Log entries for 616-619. Allow for leading comments in CSV files, using ';' in column 1. ScenarioData/Demo_Baseline/prescribedLULCs.csv - Add leading comments. APs.cpp - In InitRunPrescribedLULCs(), replace the ReadAscii() call with a call to ReadCSVwithLeadingComments(). Vdataobj.cpp, .h - Add SkipLeadingComments() and ReadCSVwithLeadingComments().
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC08E9C-8B36-4557-96E0-166E9A78BFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503617A3-1983-40CD-AB36-0F999E1467D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="146">
   <si>
     <t>Year</t>
   </si>
@@ -465,6 +465,12 @@
   </si>
   <si>
     <t>Demo Baseline</t>
+  </si>
+  <si>
+    <t>CW3M C618</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_C618</t>
   </si>
 </sst>
 </file>
@@ -1366,11 +1372,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U113"/>
+  <dimension ref="A1:U114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
+      <selection pane="bottomLeft" activeCell="R109" sqref="R109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7327,87 +7333,84 @@
       </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
-      <c r="I109" s="2"/>
-      <c r="J109" s="2"/>
-      <c r="K109" s="2"/>
-      <c r="L109" s="2"/>
-      <c r="M109" s="2"/>
-      <c r="N109" s="2"/>
-      <c r="O109" s="3"/>
-      <c r="P109" s="3"/>
-      <c r="Q109" s="2"/>
-      <c r="R109" s="4"/>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>16</v>
-      </c>
-      <c r="B111" t="s">
-        <v>93</v>
-      </c>
-      <c r="D111" s="2">
-        <v>1230.0044677999999</v>
-      </c>
-      <c r="E111" s="2">
-        <v>1848.1456909000001</v>
-      </c>
-      <c r="F111" s="2">
-        <v>1.0573501000000001</v>
-      </c>
-      <c r="G111" s="2">
-        <v>299.4371582</v>
-      </c>
-      <c r="H111" s="2">
-        <v>9.7418259000000003</v>
-      </c>
-      <c r="I111" s="2">
-        <v>5.7446602000000002</v>
-      </c>
-      <c r="J111" s="2">
-        <v>8.1171118999999994</v>
-      </c>
-      <c r="K111" s="2">
-        <v>673.08737180000003</v>
-      </c>
-      <c r="L111" s="2">
-        <v>81.12013859999999</v>
-      </c>
-      <c r="M111" s="2">
-        <v>1432.6230836</v>
-      </c>
-      <c r="N111" s="2">
-        <v>1196.8767700000001</v>
-      </c>
-      <c r="O111" s="3">
-        <v>5429.4087645999998</v>
-      </c>
-      <c r="P111" s="3">
-        <v>27140.258789299998</v>
-      </c>
-      <c r="Q111" s="2">
-        <v>-2.3066774000000003</v>
-      </c>
-      <c r="R111" s="4">
-        <v>-7.1000000000000002E-4</v>
-      </c>
-      <c r="S111" t="s">
-        <v>92</v>
-      </c>
+      <c r="A109" t="s">
+        <v>144</v>
+      </c>
+      <c r="B109" t="s">
+        <v>145</v>
+      </c>
+      <c r="C109" t="s">
+        <v>23</v>
+      </c>
+      <c r="D109" s="2">
+        <v>930.00079344444441</v>
+      </c>
+      <c r="E109" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F109" s="2">
+        <v>1.1355297777777777</v>
+      </c>
+      <c r="G109" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H109" s="2">
+        <v>9.8446185555555559</v>
+      </c>
+      <c r="I109" s="2">
+        <v>7.306026666666666</v>
+      </c>
+      <c r="J109" s="2">
+        <v>8.202840444444444</v>
+      </c>
+      <c r="K109" s="2">
+        <v>667.3960911111111</v>
+      </c>
+      <c r="L109" s="2">
+        <v>80.428346444444458</v>
+      </c>
+      <c r="M109" s="2">
+        <v>1419.9760742222222</v>
+      </c>
+      <c r="N109" s="2">
+        <v>933.11573622222204</v>
+      </c>
+      <c r="O109" s="3">
+        <v>6418.2839627777767</v>
+      </c>
+      <c r="P109" s="3">
+        <v>27412.947482666666</v>
+      </c>
+      <c r="Q109" s="2">
+        <v>0.15756933333333334</v>
+      </c>
+      <c r="R109" s="4">
+        <v>2.7555555555555555E-5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="J110" s="2"/>
+      <c r="K110" s="2"/>
+      <c r="L110" s="2"/>
+      <c r="M110" s="2"/>
+      <c r="N110" s="2"/>
+      <c r="O110" s="3"/>
+      <c r="P110" s="3"/>
+      <c r="Q110" s="2"/>
+      <c r="R110" s="4"/>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>16</v>
       </c>
       <c r="B112" t="s">
-        <v>95</v>
-      </c>
-      <c r="C112" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D112" s="2">
         <v>1230.0044677999999</v>
@@ -7430,8 +7433,8 @@
       <c r="J112" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K112" s="5">
-        <v>675.4841553</v>
+      <c r="K112" s="2">
+        <v>673.08737180000003</v>
       </c>
       <c r="L112" s="2">
         <v>81.12013859999999</v>
@@ -7448,18 +7451,77 @@
       <c r="P112" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q112" s="5">
-        <v>9.0106100000000008E-2</v>
-      </c>
-      <c r="R112" s="7">
-        <v>3.5000000000000063E-6</v>
+      <c r="Q112" s="2">
+        <v>-2.3066774000000003</v>
+      </c>
+      <c r="R112" s="4">
+        <v>-7.1000000000000002E-4</v>
       </c>
       <c r="S112" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>16</v>
+      </c>
+      <c r="B113" t="s">
+        <v>95</v>
+      </c>
       <c r="C113" t="s">
+        <v>92</v>
+      </c>
+      <c r="D113" s="2">
+        <v>1230.0044677999999</v>
+      </c>
+      <c r="E113" s="2">
+        <v>1848.1456909000001</v>
+      </c>
+      <c r="F113" s="2">
+        <v>1.0573501000000001</v>
+      </c>
+      <c r="G113" s="2">
+        <v>299.4371582</v>
+      </c>
+      <c r="H113" s="2">
+        <v>9.7418259000000003</v>
+      </c>
+      <c r="I113" s="2">
+        <v>5.7446602000000002</v>
+      </c>
+      <c r="J113" s="2">
+        <v>8.1171118999999994</v>
+      </c>
+      <c r="K113" s="5">
+        <v>675.4841553</v>
+      </c>
+      <c r="L113" s="2">
+        <v>81.12013859999999</v>
+      </c>
+      <c r="M113" s="2">
+        <v>1432.6230836</v>
+      </c>
+      <c r="N113" s="2">
+        <v>1196.8767700000001</v>
+      </c>
+      <c r="O113" s="3">
+        <v>5429.4087645999998</v>
+      </c>
+      <c r="P113" s="3">
+        <v>27140.258789299998</v>
+      </c>
+      <c r="Q113" s="5">
+        <v>9.0106100000000008E-2</v>
+      </c>
+      <c r="R113" s="7">
+        <v>3.5000000000000063E-6</v>
+      </c>
+      <c r="S113" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C114" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Release CW3M 1.2.1. This release includes a new calibration of the Wiley Creek watershed in the South Santiam basin.  Code was added to support leading comments in CSV files; the new Prescribed LULCs process uses this code.  Added logic to populate the WETL_CAP attribute automatically when initializing wetland objects, if WETL_CAP values are not already present.  Activated wetland 15 in the wetland model with Q_CAP = 300 cms and QSPILL_FRC = 0.9 for its outlet reach (COMID 23772753).  Added a No_wetlands_demo scenario. CW3M_McKenzie_Script.iss - Update version number. Add No_wetlands_demo scenario data. Reconcile to CW3M_Script.iss. CW3M_Script.iss - Add Observations\Willamette folder. Add No_wetlands_demo scenario data. Reconcile to CW3M_McKenzie_Script.iss.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88CF314-BF72-4C00-833A-66384A52A761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95D8E75-2EAB-48DB-956D-2CF0D50277D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="151">
   <si>
     <t>Year</t>
   </si>
@@ -477,6 +477,15 @@
   </si>
   <si>
     <t>Demo_Baseline_2010-18_C646</t>
+  </si>
+  <si>
+    <t>CW3M C650</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_C650</t>
+  </si>
+  <si>
+    <t>No_wetlands_demo_2010-18_C650</t>
   </si>
 </sst>
 </file>
@@ -1378,11 +1387,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U115"/>
+  <dimension ref="A1:U118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N110" sqref="N110"/>
+      <selection pane="bottomLeft" activeCell="A113" sqref="A113:XFD114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7450,140 +7459,269 @@
         <v>-6.8888888888889176E-6</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="D111" s="2"/>
-      <c r="E111" s="2"/>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
-      <c r="I111" s="2"/>
-      <c r="J111" s="2"/>
-      <c r="K111" s="2"/>
-      <c r="L111" s="2"/>
-      <c r="M111" s="2"/>
-      <c r="N111" s="2"/>
-      <c r="O111" s="3"/>
-      <c r="P111" s="3"/>
-      <c r="Q111" s="2"/>
-      <c r="R111" s="4"/>
+    <row r="111" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>148</v>
+      </c>
+      <c r="B111" t="s">
+        <v>149</v>
+      </c>
+      <c r="C111" t="s">
+        <v>23</v>
+      </c>
+      <c r="D111" s="13">
+        <v>936.4586451111112</v>
+      </c>
+      <c r="E111" s="13">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F111" s="13">
+        <v>1.1353011111111111</v>
+      </c>
+      <c r="G111" s="13">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H111" s="13">
+        <v>9.8446185555555559</v>
+      </c>
+      <c r="I111" s="13">
+        <v>7.3262146666666679</v>
+      </c>
+      <c r="J111" s="13">
+        <v>8.202840444444444</v>
+      </c>
+      <c r="K111" s="13">
+        <v>664.89181855555546</v>
+      </c>
+      <c r="L111" s="13">
+        <v>80.365177222222229</v>
+      </c>
+      <c r="M111" s="13">
+        <v>1422.6016167777777</v>
+      </c>
+      <c r="N111" s="13">
+        <v>939.5350204444444</v>
+      </c>
+      <c r="O111" s="14">
+        <v>6416.2319064444446</v>
+      </c>
+      <c r="P111" s="14">
+        <v>27412.947482666666</v>
+      </c>
+      <c r="Q111" s="13">
+        <v>0.15714333333333327</v>
+      </c>
+      <c r="R111" s="15">
+        <v>4.0333333333333261E-5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>148</v>
+      </c>
+      <c r="B112" t="s">
+        <v>150</v>
+      </c>
+      <c r="C112" t="s">
+        <v>23</v>
+      </c>
+      <c r="D112" s="2">
+        <v>934.65285922222233</v>
+      </c>
+      <c r="E112" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F112" s="2">
+        <v>1.0305982222222221</v>
+      </c>
+      <c r="G112" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H112" s="2">
+        <v>9.860652222222221</v>
+      </c>
+      <c r="I112" s="2">
+        <v>7.342017444444445</v>
+      </c>
+      <c r="J112" s="2">
+        <v>8.2161996666666663</v>
+      </c>
+      <c r="K112" s="2">
+        <v>664.22806799999989</v>
+      </c>
+      <c r="L112" s="2">
+        <v>80.302231777777777</v>
+      </c>
+      <c r="M112" s="2">
+        <v>1423.3923340000001</v>
+      </c>
+      <c r="N112" s="2">
+        <v>937.57914911111118</v>
+      </c>
+      <c r="O112" s="6">
+        <v>5596.6441785555553</v>
+      </c>
+      <c r="P112" s="6">
+        <v>27457.329643999998</v>
+      </c>
+      <c r="Q112" s="2">
+        <v>0.15730522222222224</v>
+      </c>
+      <c r="R112" s="4">
+        <v>2.9444444444444438E-5</v>
+      </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+      <c r="K113" s="2"/>
+      <c r="L113" s="2"/>
+      <c r="M113" s="2"/>
+      <c r="N113" s="2"/>
+      <c r="O113" s="6"/>
+      <c r="P113" s="6"/>
+      <c r="Q113" s="2"/>
+      <c r="R113" s="4"/>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+      <c r="L114" s="2"/>
+      <c r="M114" s="2"/>
+      <c r="N114" s="2"/>
+      <c r="O114" s="6"/>
+      <c r="P114" s="6"/>
+      <c r="Q114" s="2"/>
+      <c r="R114" s="4"/>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>16</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B116" t="s">
         <v>93</v>
       </c>
-      <c r="D113" s="2">
+      <c r="D116" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E113" s="2">
+      <c r="E116" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F113" s="2">
+      <c r="F116" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G113" s="2">
+      <c r="G116" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H113" s="2">
+      <c r="H116" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I113" s="2">
+      <c r="I116" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J113" s="2">
+      <c r="J116" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K113" s="2">
+      <c r="K116" s="2">
         <v>673.08737180000003</v>
       </c>
-      <c r="L113" s="2">
+      <c r="L116" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M113" s="2">
+      <c r="M116" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N113" s="2">
+      <c r="N116" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O113" s="3">
+      <c r="O116" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P113" s="3">
+      <c r="P116" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q113" s="2">
+      <c r="Q116" s="2">
         <v>-2.3066774000000003</v>
       </c>
-      <c r="R113" s="4">
+      <c r="R116" s="4">
         <v>-7.1000000000000002E-4</v>
       </c>
-      <c r="S113" t="s">
+      <c r="S116" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>16</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B117" t="s">
         <v>95</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C117" t="s">
         <v>92</v>
       </c>
-      <c r="D114" s="2">
+      <c r="D117" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E114" s="2">
+      <c r="E117" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F114" s="2">
+      <c r="F117" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G114" s="2">
+      <c r="G117" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H114" s="2">
+      <c r="H117" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I114" s="2">
+      <c r="I117" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J114" s="2">
+      <c r="J117" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K114" s="5">
+      <c r="K117" s="5">
         <v>675.4841553</v>
       </c>
-      <c r="L114" s="2">
+      <c r="L117" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M114" s="2">
+      <c r="M117" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N114" s="2">
+      <c r="N117" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O114" s="3">
+      <c r="O117" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P114" s="3">
+      <c r="P117" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q114" s="5">
+      <c r="Q117" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R114" s="7">
+      <c r="R117" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S114" t="s">
+      <c r="S117" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C115" t="s">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C118" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit recent data updates.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95D8E75-2EAB-48DB-956D-2CF0D50277D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE3031A-0C47-40B6-9A7B-B8950E1D5890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="155">
   <si>
     <t>Year</t>
   </si>
@@ -486,6 +486,18 @@
   </si>
   <si>
     <t>No_wetlands_demo_2010-18_C650</t>
+  </si>
+  <si>
+    <t>CW3M C733</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_C733</t>
+  </si>
+  <si>
+    <t>has David Richey's new water rights data</t>
+  </si>
+  <si>
+    <t>Demo_Baseline_2010-18_C733 + old water rights</t>
   </si>
 </sst>
 </file>
@@ -633,7 +645,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -831,6 +843,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -993,7 +1011,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1031,6 +1049,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1387,11 +1406,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U118"/>
+  <dimension ref="A1:U120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A113" sqref="A113:XFD114"/>
+      <selection pane="bottomLeft" activeCell="O97" sqref="O97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7572,156 +7591,288 @@
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
-      <c r="F113" s="2"/>
-      <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
-      <c r="I113" s="2"/>
-      <c r="J113" s="2"/>
-      <c r="K113" s="2"/>
-      <c r="L113" s="2"/>
-      <c r="M113" s="2"/>
-      <c r="N113" s="2"/>
-      <c r="O113" s="6"/>
-      <c r="P113" s="6"/>
-      <c r="Q113" s="2"/>
-      <c r="R113" s="4"/>
-    </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D114" s="2"/>
-      <c r="E114" s="2"/>
-      <c r="F114" s="2"/>
-      <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
-      <c r="I114" s="2"/>
-      <c r="J114" s="2"/>
-      <c r="K114" s="2"/>
-      <c r="L114" s="2"/>
-      <c r="M114" s="2"/>
-      <c r="N114" s="2"/>
-      <c r="O114" s="6"/>
-      <c r="P114" s="6"/>
-      <c r="Q114" s="2"/>
-      <c r="R114" s="4"/>
+      <c r="A113" t="s">
+        <v>151</v>
+      </c>
+      <c r="B113" t="s">
+        <v>152</v>
+      </c>
+      <c r="C113" t="s">
+        <v>23</v>
+      </c>
+      <c r="D113" s="2">
+        <v>936.2841594444443</v>
+      </c>
+      <c r="E113" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F113" s="5">
+        <v>0.59877088888888885</v>
+      </c>
+      <c r="G113" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H113" s="5">
+        <v>0</v>
+      </c>
+      <c r="I113" s="2">
+        <v>7.3199817777777776</v>
+      </c>
+      <c r="J113" s="5">
+        <v>0</v>
+      </c>
+      <c r="K113" s="2">
+        <v>662.87599011111115</v>
+      </c>
+      <c r="L113" s="2">
+        <v>80.365177222222229</v>
+      </c>
+      <c r="M113" s="2">
+        <v>1422.4611409999998</v>
+      </c>
+      <c r="N113" s="2">
+        <v>939.33221444444439</v>
+      </c>
+      <c r="O113" s="6">
+        <v>4565.8835446666662</v>
+      </c>
+      <c r="P113" s="25">
+        <v>1017.8816121111109</v>
+      </c>
+      <c r="Q113" s="2">
+        <v>0.15706044444444447</v>
+      </c>
+      <c r="R113" s="4">
+        <v>4.0444444444444593E-5</v>
+      </c>
+      <c r="S113" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>151</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C114" t="s">
+        <v>23</v>
+      </c>
+      <c r="D114" s="2">
+        <f>AVERAGE(D105:D113)</f>
+        <v>932.52751403703689</v>
+      </c>
+      <c r="E114" s="2">
+        <f t="shared" ref="E114:R114" si="3">AVERAGE(E105:E113)</f>
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F114" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0491967654320991</v>
+      </c>
+      <c r="G114" s="2">
+        <f t="shared" si="3"/>
+        <v>270.41205844444443</v>
+      </c>
+      <c r="H114" s="2">
+        <f t="shared" si="3"/>
+        <v>8.7525930740740741</v>
+      </c>
+      <c r="I114" s="2">
+        <f t="shared" si="3"/>
+        <v>7.3194422222222233</v>
+      </c>
+      <c r="J114" s="2">
+        <f t="shared" si="3"/>
+        <v>7.2929307283950617</v>
+      </c>
+      <c r="K114" s="2">
+        <f t="shared" si="3"/>
+        <v>666.25400646913602</v>
+      </c>
+      <c r="L114" s="2">
+        <f t="shared" si="3"/>
+        <v>80.414587382716064</v>
+      </c>
+      <c r="M114" s="2">
+        <f t="shared" si="3"/>
+        <v>1420.9680507407409</v>
+      </c>
+      <c r="N114" s="2">
+        <f t="shared" si="3"/>
+        <v>935.55100653086402</v>
+      </c>
+      <c r="O114" s="6">
+        <f t="shared" si="3"/>
+        <v>5988.6604757530858</v>
+      </c>
+      <c r="P114" s="6">
+        <f t="shared" si="3"/>
+        <v>24485.1996158642</v>
+      </c>
+      <c r="Q114" s="2">
+        <f t="shared" si="3"/>
+        <v>0.15728533333333333</v>
+      </c>
+      <c r="R114" s="4">
+        <f t="shared" si="3"/>
+        <v>2.6925925925925932E-5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B115" s="1"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+      <c r="L115" s="2"/>
+      <c r="M115" s="2"/>
+      <c r="N115" s="2"/>
+      <c r="O115" s="14"/>
+      <c r="P115" s="14"/>
+      <c r="Q115" s="2"/>
+      <c r="R115" s="4"/>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+      <c r="B116" s="1"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2"/>
+      <c r="L116" s="2"/>
+      <c r="M116" s="2"/>
+      <c r="N116" s="2"/>
+      <c r="O116" s="14"/>
+      <c r="P116" s="14"/>
+      <c r="Q116" s="2"/>
+      <c r="R116" s="4"/>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>16</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B118" t="s">
         <v>93</v>
       </c>
-      <c r="D116" s="2">
+      <c r="D118" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E116" s="2">
+      <c r="E118" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F116" s="2">
+      <c r="F118" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G116" s="2">
+      <c r="G118" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H116" s="2">
+      <c r="H118" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I116" s="2">
+      <c r="I118" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J116" s="2">
+      <c r="J118" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K116" s="2">
+      <c r="K118" s="2">
         <v>673.08737180000003</v>
       </c>
-      <c r="L116" s="2">
+      <c r="L118" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M116" s="2">
+      <c r="M118" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N116" s="2">
+      <c r="N118" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O116" s="3">
+      <c r="O118" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P116" s="3">
+      <c r="P118" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q116" s="2">
+      <c r="Q118" s="2">
         <v>-2.3066774000000003</v>
       </c>
-      <c r="R116" s="4">
+      <c r="R118" s="4">
         <v>-7.1000000000000002E-4</v>
       </c>
-      <c r="S116" t="s">
+      <c r="S118" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>16</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B119" t="s">
         <v>95</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C119" t="s">
         <v>92</v>
       </c>
-      <c r="D117" s="2">
+      <c r="D119" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E117" s="2">
+      <c r="E119" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F117" s="2">
+      <c r="F119" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G117" s="2">
+      <c r="G119" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H117" s="2">
+      <c r="H119" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I117" s="2">
+      <c r="I119" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J117" s="2">
+      <c r="J119" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K117" s="5">
+      <c r="K119" s="5">
         <v>675.4841553</v>
       </c>
-      <c r="L117" s="2">
+      <c r="L119" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M117" s="2">
+      <c r="M119" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N117" s="2">
+      <c r="N119" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O117" s="3">
+      <c r="O119" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P117" s="3">
+      <c r="P119" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q117" s="5">
+      <c r="Q119" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R117" s="7">
+      <c r="R119" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S117" t="s">
+      <c r="S119" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C118" t="s">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C120" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
wr_pods_McKenzie.csv - Change the POUID field for 5 municipal water rights to -22 to connect them to the Eugene-Springfield UGA.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE3031A-0C47-40B6-9A7B-B8950E1D5890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AD8CC5-0FFD-4F2A-8B53-44AAC2BA8E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="159">
   <si>
     <t>Year</t>
   </si>
@@ -498,6 +498,18 @@
   </si>
   <si>
     <t>Demo_Baseline_2010-18_C733 + old water rights</t>
+  </si>
+  <si>
+    <t>CW3M C744</t>
+  </si>
+  <si>
+    <t>Demo_Baseline 2010-18 C744</t>
+  </si>
+  <si>
+    <t>CW3M C745</t>
+  </si>
+  <si>
+    <t>Demo_Baseline 2010-18 C745</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1023,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1050,6 +1062,21 @@
     <xf numFmtId="2" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1406,11 +1433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U120"/>
+  <dimension ref="A1:U121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O97" sqref="O97"/>
+      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A117" sqref="A117:XFD117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7649,178 +7676,213 @@
         <v>153</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+    <row r="114" spans="1:19" s="26" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A114" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D114" s="2">
+      <c r="D114" s="28">
         <f>AVERAGE(D105:D113)</f>
         <v>932.52751403703689</v>
       </c>
-      <c r="E114" s="2">
+      <c r="E114" s="28">
         <f t="shared" ref="E114:R114" si="3">AVERAGE(E105:E113)</f>
         <v>1890.2624918888889</v>
       </c>
-      <c r="F114" s="2">
+      <c r="F114" s="28">
         <f t="shared" si="3"/>
         <v>1.0491967654320991</v>
       </c>
-      <c r="G114" s="2">
+      <c r="G114" s="28">
         <f t="shared" si="3"/>
         <v>270.41205844444443</v>
       </c>
-      <c r="H114" s="2">
+      <c r="H114" s="28">
         <f t="shared" si="3"/>
         <v>8.7525930740740741</v>
       </c>
-      <c r="I114" s="2">
+      <c r="I114" s="28">
         <f t="shared" si="3"/>
         <v>7.3194422222222233</v>
       </c>
-      <c r="J114" s="2">
+      <c r="J114" s="28">
         <f t="shared" si="3"/>
         <v>7.2929307283950617</v>
       </c>
-      <c r="K114" s="2">
+      <c r="K114" s="28">
         <f t="shared" si="3"/>
         <v>666.25400646913602</v>
       </c>
-      <c r="L114" s="2">
+      <c r="L114" s="28">
         <f t="shared" si="3"/>
         <v>80.414587382716064</v>
       </c>
-      <c r="M114" s="2">
+      <c r="M114" s="28">
         <f t="shared" si="3"/>
         <v>1420.9680507407409</v>
       </c>
-      <c r="N114" s="2">
+      <c r="N114" s="28">
         <f t="shared" si="3"/>
         <v>935.55100653086402</v>
       </c>
-      <c r="O114" s="6">
+      <c r="O114" s="29">
         <f t="shared" si="3"/>
         <v>5988.6604757530858</v>
       </c>
-      <c r="P114" s="6">
+      <c r="P114" s="29">
         <f t="shared" si="3"/>
         <v>24485.1996158642</v>
       </c>
-      <c r="Q114" s="2">
+      <c r="Q114" s="28">
         <f t="shared" si="3"/>
         <v>0.15728533333333333</v>
       </c>
-      <c r="R114" s="4">
+      <c r="R114" s="30">
         <f t="shared" si="3"/>
         <v>2.6925925925925932E-5</v>
       </c>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B115" s="1"/>
-      <c r="D115" s="2"/>
-      <c r="E115" s="2"/>
-      <c r="F115" s="2"/>
-      <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
-      <c r="I115" s="2"/>
-      <c r="J115" s="2"/>
-      <c r="K115" s="2"/>
-      <c r="L115" s="2"/>
-      <c r="M115" s="2"/>
-      <c r="N115" s="2"/>
-      <c r="O115" s="14"/>
-      <c r="P115" s="14"/>
-      <c r="Q115" s="2"/>
-      <c r="R115" s="4"/>
+      <c r="A115" t="s">
+        <v>155</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C115" t="s">
+        <v>23</v>
+      </c>
+      <c r="D115" s="2">
+        <v>936.2754043333332</v>
+      </c>
+      <c r="E115" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F115" s="2">
+        <v>0.59877088888888885</v>
+      </c>
+      <c r="G115" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H115" s="2">
+        <v>0</v>
+      </c>
+      <c r="I115" s="2">
+        <v>0.21622155555555556</v>
+      </c>
+      <c r="J115" s="2">
+        <v>0</v>
+      </c>
+      <c r="K115" s="2">
+        <v>662.7248604444444</v>
+      </c>
+      <c r="L115" s="2">
+        <v>80.365177222222229</v>
+      </c>
+      <c r="M115" s="2">
+        <v>1415.5095484444446</v>
+      </c>
+      <c r="N115" s="2">
+        <v>939.32236066666655</v>
+      </c>
+      <c r="O115" s="14">
+        <v>4509.0119630000008</v>
+      </c>
+      <c r="P115" s="14">
+        <v>1017.8816121111109</v>
+      </c>
+      <c r="Q115" s="2">
+        <v>0.15699988888888899</v>
+      </c>
+      <c r="R115" s="4">
+        <v>4.0666666666666716E-5</v>
+      </c>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B116" s="1"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
-      <c r="J116" s="2"/>
-      <c r="K116" s="2"/>
-      <c r="L116" s="2"/>
-      <c r="M116" s="2"/>
-      <c r="N116" s="2"/>
-      <c r="O116" s="14"/>
-      <c r="P116" s="14"/>
-      <c r="Q116" s="2"/>
-      <c r="R116" s="4"/>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>16</v>
-      </c>
-      <c r="B118" t="s">
-        <v>93</v>
-      </c>
-      <c r="D118" s="2">
-        <v>1230.0044677999999</v>
-      </c>
-      <c r="E118" s="2">
-        <v>1848.1456909000001</v>
-      </c>
-      <c r="F118" s="2">
-        <v>1.0573501000000001</v>
-      </c>
-      <c r="G118" s="2">
-        <v>299.4371582</v>
-      </c>
-      <c r="H118" s="2">
-        <v>9.7418259000000003</v>
-      </c>
-      <c r="I118" s="2">
-        <v>5.7446602000000002</v>
-      </c>
-      <c r="J118" s="2">
-        <v>8.1171118999999994</v>
-      </c>
-      <c r="K118" s="2">
-        <v>673.08737180000003</v>
-      </c>
-      <c r="L118" s="2">
-        <v>81.12013859999999</v>
-      </c>
-      <c r="M118" s="2">
-        <v>1432.6230836</v>
-      </c>
-      <c r="N118" s="2">
-        <v>1196.8767700000001</v>
-      </c>
-      <c r="O118" s="3">
-        <v>5429.4087645999998</v>
-      </c>
-      <c r="P118" s="3">
-        <v>27140.258789299998</v>
-      </c>
-      <c r="Q118" s="2">
-        <v>-2.3066774000000003</v>
-      </c>
-      <c r="R118" s="4">
-        <v>-7.1000000000000002E-4</v>
-      </c>
-      <c r="S118" t="s">
-        <v>92</v>
-      </c>
+      <c r="A116" t="s">
+        <v>157</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C116" t="s">
+        <v>23</v>
+      </c>
+      <c r="D116" s="2">
+        <v>936.26689999999996</v>
+      </c>
+      <c r="E116" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F116" s="2">
+        <v>0.59877088888888885</v>
+      </c>
+      <c r="G116" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H116" s="2">
+        <v>0</v>
+      </c>
+      <c r="I116" s="2">
+        <v>0.21622155555555556</v>
+      </c>
+      <c r="J116" s="2">
+        <v>8.1971030000000003</v>
+      </c>
+      <c r="K116" s="2">
+        <v>664.36562777777772</v>
+      </c>
+      <c r="L116" s="2">
+        <v>80.365177222222229</v>
+      </c>
+      <c r="M116" s="2">
+        <v>1405.6726752222223</v>
+      </c>
+      <c r="N116" s="2">
+        <v>939.31270344444442</v>
+      </c>
+      <c r="O116" s="14">
+        <v>4509.0119630000008</v>
+      </c>
+      <c r="P116" s="6">
+        <v>27393.764540111111</v>
+      </c>
+      <c r="Q116" s="2">
+        <v>0.15684377777777789</v>
+      </c>
+      <c r="R116" s="4">
+        <v>3.9888888888888786E-5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B117" s="1"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
+      <c r="K117" s="2"/>
+      <c r="L117" s="2"/>
+      <c r="M117" s="2"/>
+      <c r="N117" s="2"/>
+      <c r="O117" s="14"/>
+      <c r="P117" s="6"/>
+      <c r="Q117" s="2"/>
+      <c r="R117" s="4"/>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>16</v>
       </c>
       <c r="B119" t="s">
-        <v>95</v>
-      </c>
-      <c r="C119" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D119" s="2">
         <v>1230.0044677999999</v>
@@ -7843,8 +7905,8 @@
       <c r="J119" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K119" s="5">
-        <v>675.4841553</v>
+      <c r="K119" s="2">
+        <v>673.08737180000003</v>
       </c>
       <c r="L119" s="2">
         <v>81.12013859999999</v>
@@ -7861,18 +7923,77 @@
       <c r="P119" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q119" s="5">
-        <v>9.0106100000000008E-2</v>
-      </c>
-      <c r="R119" s="7">
-        <v>3.5000000000000063E-6</v>
+      <c r="Q119" s="2">
+        <v>-2.3066774000000003</v>
+      </c>
+      <c r="R119" s="4">
+        <v>-7.1000000000000002E-4</v>
       </c>
       <c r="S119" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>16</v>
+      </c>
+      <c r="B120" t="s">
+        <v>95</v>
+      </c>
       <c r="C120" t="s">
+        <v>92</v>
+      </c>
+      <c r="D120" s="2">
+        <v>1230.0044677999999</v>
+      </c>
+      <c r="E120" s="2">
+        <v>1848.1456909000001</v>
+      </c>
+      <c r="F120" s="2">
+        <v>1.0573501000000001</v>
+      </c>
+      <c r="G120" s="2">
+        <v>299.4371582</v>
+      </c>
+      <c r="H120" s="2">
+        <v>9.7418259000000003</v>
+      </c>
+      <c r="I120" s="2">
+        <v>5.7446602000000002</v>
+      </c>
+      <c r="J120" s="2">
+        <v>8.1171118999999994</v>
+      </c>
+      <c r="K120" s="5">
+        <v>675.4841553</v>
+      </c>
+      <c r="L120" s="2">
+        <v>81.12013859999999</v>
+      </c>
+      <c r="M120" s="2">
+        <v>1432.6230836</v>
+      </c>
+      <c r="N120" s="2">
+        <v>1196.8767700000001</v>
+      </c>
+      <c r="O120" s="3">
+        <v>5429.4087645999998</v>
+      </c>
+      <c r="P120" s="3">
+        <v>27140.258789299998</v>
+      </c>
+      <c r="Q120" s="5">
+        <v>9.0106100000000008E-2</v>
+      </c>
+      <c r="R120" s="7">
+        <v>3.5000000000000063E-6</v>
+      </c>
+      <c r="S120" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C121" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Do a new McKenzie spinup over 2000-09; it does produce some warning messages. flow2010.ic, HRU_McKenzie.dbf, IDU_McKenzie.dbf, Reach_McKenzie.dbf - From the new spinup. Flow.cpp - Initialize HRU members m_infiltrationFromStandingH2O_m3 and m_addedVolume_m3 when the HRU objects are instantiated. In FlowModel::InitializeSpinup(), reset IRRIGATION to 0 for all IDUs and set m_areaIrrigated, m_fracIrrigated, HruIRRIG_SOIL, and HruAREA_IRRIG all to zero.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2296B658-D4E0-4D7F-BF88-0AA28FED0A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF73238-859C-4A2C-AA4F-1515ACA66B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="irrigation anomaly" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="163">
   <si>
     <t>Year</t>
   </si>
@@ -517,6 +516,12 @@
   </si>
   <si>
     <t>Demo_Baseline 2010-18 C748</t>
+  </si>
+  <si>
+    <t>CW3M C749+</t>
+  </si>
+  <si>
+    <t>Demo_Baseline 2010-18 C749+</t>
   </si>
 </sst>
 </file>
@@ -1443,8 +1448,8 @@
   <dimension ref="A1:U122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A117" sqref="A117:XFD117"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7923,22 +7928,60 @@
       </c>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B118" s="1"/>
-      <c r="D118" s="2"/>
-      <c r="E118" s="2"/>
-      <c r="F118" s="2"/>
-      <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
-      <c r="I118" s="2"/>
-      <c r="J118" s="2"/>
-      <c r="K118" s="2"/>
-      <c r="L118" s="2"/>
-      <c r="M118" s="2"/>
-      <c r="N118" s="2"/>
-      <c r="O118" s="14"/>
-      <c r="P118" s="14"/>
-      <c r="Q118" s="2"/>
-      <c r="R118" s="4"/>
+      <c r="A118" t="s">
+        <v>161</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C118" t="s">
+        <v>23</v>
+      </c>
+      <c r="D118" s="2">
+        <v>934.75066466666669</v>
+      </c>
+      <c r="E118" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F118" s="2">
+        <v>0.59877088888888885</v>
+      </c>
+      <c r="G118" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H118" s="2">
+        <v>0</v>
+      </c>
+      <c r="I118" s="2">
+        <v>0.21623588888888889</v>
+      </c>
+      <c r="J118" s="2">
+        <v>8.1971030000000003</v>
+      </c>
+      <c r="K118" s="2">
+        <v>664.36423055555542</v>
+      </c>
+      <c r="L118" s="2">
+        <v>80.365177222222229</v>
+      </c>
+      <c r="M118" s="2">
+        <v>1405.6821015555554</v>
+      </c>
+      <c r="N118" s="2">
+        <v>937.57624644444456</v>
+      </c>
+      <c r="O118" s="14">
+        <v>4509.0119630000008</v>
+      </c>
+      <c r="P118" s="14">
+        <v>27393.764540111111</v>
+      </c>
+      <c r="Q118" s="2">
+        <v>-5.5362888888888566E-2</v>
+      </c>
+      <c r="R118" s="4">
+        <v>-2.3000000000000041E-5</v>
+      </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120" t="s">

</xml_diff>

<commit_message>
Adjust the thresholds for warning messages to avoid nuisance warnings.  Now McKenzie Demo_Baseline 2010-18 runs to completion without stopping for warning messages. ReachRouting.cpp - Adjust thresholds for warning messages. HBV.cpp - Remove an obsolete comment.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9539C017-5622-40A0-B026-D4E815E9C632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C2BBBF-E0F1-49FA-B676-2D6A220A5000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="166">
   <si>
     <t>Year</t>
   </si>
@@ -528,6 +528,9 @@
   </si>
   <si>
     <t>Demo_Baseline 2010-18</t>
+  </si>
+  <si>
+    <t>CW3M C755</t>
   </si>
 </sst>
 </file>
@@ -1455,7 +1458,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
+      <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8032,7 +8035,7 @@
       <c r="N119" s="2">
         <v>938.96002866666663</v>
       </c>
-      <c r="O119" s="3">
+      <c r="O119" s="6">
         <v>3872.6727430000005</v>
       </c>
       <c r="P119" s="3">
@@ -8046,21 +8049,60 @@
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D120" s="2"/>
-      <c r="E120" s="2"/>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="2"/>
-      <c r="J120" s="2"/>
-      <c r="K120" s="2"/>
-      <c r="L120" s="2"/>
-      <c r="M120" s="2"/>
-      <c r="N120" s="2"/>
-      <c r="O120" s="3"/>
-      <c r="P120" s="3"/>
-      <c r="Q120" s="2"/>
-      <c r="R120" s="4"/>
+      <c r="A120" t="s">
+        <v>165</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C120" t="s">
+        <v>23</v>
+      </c>
+      <c r="D120" s="2">
+        <v>937.16306566666651</v>
+      </c>
+      <c r="E120" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F120" s="2">
+        <v>0.59877111111111114</v>
+      </c>
+      <c r="G120" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H120" s="2">
+        <v>0</v>
+      </c>
+      <c r="I120" s="2">
+        <v>0.32774833333333331</v>
+      </c>
+      <c r="J120" s="2">
+        <v>8.1971030000000003</v>
+      </c>
+      <c r="K120" s="2">
+        <v>664.68198655555557</v>
+      </c>
+      <c r="L120" s="2">
+        <v>80.258565666666669</v>
+      </c>
+      <c r="M120" s="2">
+        <v>1406.0243868888888</v>
+      </c>
+      <c r="N120" s="2">
+        <v>939.43141688888863</v>
+      </c>
+      <c r="O120" s="6">
+        <v>4507.2032877777783</v>
+      </c>
+      <c r="P120" s="3">
+        <v>27393.764540111111</v>
+      </c>
+      <c r="Q120" s="5">
+        <v>-0.17067655555555517</v>
+      </c>
+      <c r="R120" s="7">
+        <v>-6.2999999999999878E-5</v>
+      </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D121" s="2"/>

</xml_diff>

<commit_message>
WORK-IN-PROGRESS. Begin separating FLOODDEPTH from WETNESS.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C2BBBF-E0F1-49FA-B676-2D6A220A5000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35589A4-B926-4C84-80F5-3108176CD754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="168">
   <si>
     <t>Year</t>
   </si>
@@ -531,6 +531,12 @@
   </si>
   <si>
     <t>CW3M C755</t>
+  </si>
+  <si>
+    <t>CW3M C759+</t>
+  </si>
+  <si>
+    <t>CW3M C760</t>
   </si>
 </sst>
 </file>
@@ -1454,16 +1460,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U125"/>
+  <dimension ref="A1:U127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
+      <selection pane="bottomLeft" activeCell="Q143" sqref="Q143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" customWidth="1"/>
     <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -8105,156 +8111,284 @@
       </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D121" s="2"/>
-      <c r="E121" s="2"/>
-      <c r="F121" s="2"/>
-      <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
-      <c r="I121" s="2"/>
-      <c r="J121" s="2"/>
-      <c r="K121" s="2"/>
-      <c r="L121" s="2"/>
-      <c r="M121" s="2"/>
-      <c r="N121" s="2"/>
-      <c r="O121" s="3"/>
-      <c r="P121" s="3"/>
-      <c r="Q121" s="2"/>
-      <c r="R121" s="4"/>
+      <c r="A121" t="s">
+        <v>166</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C121" t="s">
+        <v>23</v>
+      </c>
+      <c r="D121" s="5">
+        <v>967.11334899999986</v>
+      </c>
+      <c r="E121" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F121" s="2">
+        <v>0.60024222222222212</v>
+      </c>
+      <c r="G121" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H121" s="2">
+        <v>0</v>
+      </c>
+      <c r="I121" s="2">
+        <v>0.3355455555555556</v>
+      </c>
+      <c r="J121" s="2">
+        <v>8.1971030000000003</v>
+      </c>
+      <c r="K121" s="2">
+        <v>663.56383599999992</v>
+      </c>
+      <c r="L121" s="2">
+        <v>80.24788955555556</v>
+      </c>
+      <c r="M121" s="2">
+        <v>1402.5904268888889</v>
+      </c>
+      <c r="N121" s="2">
+        <v>973.94152822222225</v>
+      </c>
+      <c r="O121" s="6">
+        <v>4286.9395074444437</v>
+      </c>
+      <c r="P121" s="3">
+        <v>27393.764540111111</v>
+      </c>
+      <c r="Q121" s="2">
+        <v>-0.18290366666666658</v>
+      </c>
+      <c r="R121" s="4">
+        <v>-1.4922222222222219E-4</v>
+      </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D122" s="2"/>
-      <c r="E122" s="2"/>
-      <c r="F122" s="2"/>
-      <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
-      <c r="I122" s="2"/>
-      <c r="J122" s="2"/>
-      <c r="K122" s="2"/>
-      <c r="L122" s="2"/>
-      <c r="M122" s="2"/>
-      <c r="N122" s="2"/>
-      <c r="O122" s="3"/>
-      <c r="P122" s="3"/>
-      <c r="Q122" s="2"/>
-      <c r="R122" s="4"/>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+      <c r="A122" t="s">
+        <v>167</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C122" t="s">
+        <v>23</v>
+      </c>
+      <c r="D122" s="2">
+        <f>AVERAGE(D113:D121)</f>
+        <v>939.09364460905351</v>
+      </c>
+      <c r="E122" s="2">
+        <f t="shared" ref="E122:R122" si="4">AVERAGE(E113:E121)</f>
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F122" s="2">
+        <f t="shared" si="4"/>
+        <v>0.64758003566529487</v>
+      </c>
+      <c r="G122" s="2">
+        <f t="shared" si="4"/>
+        <v>270.41205844444443</v>
+      </c>
+      <c r="H122" s="5">
+        <f t="shared" si="4"/>
+        <v>0.97251034156378602</v>
+      </c>
+      <c r="I122" s="5">
+        <f t="shared" si="4"/>
+        <v>1.8195075802469138</v>
+      </c>
+      <c r="J122" s="5">
+        <f t="shared" si="4"/>
+        <v>6.2750609698216726</v>
+      </c>
+      <c r="K122" s="2">
+        <f t="shared" si="4"/>
+        <v>664.02176757064478</v>
+      </c>
+      <c r="L122" s="2">
+        <f t="shared" si="4"/>
+        <v>80.32572049931413</v>
+      </c>
+      <c r="M122" s="5">
+        <f t="shared" si="4"/>
+        <v>1410.2472608106993</v>
+      </c>
+      <c r="N122" s="5">
+        <f t="shared" si="4"/>
+        <v>942.35013246639232</v>
+      </c>
+      <c r="O122" s="6">
+        <f t="shared" si="4"/>
+        <v>4584.1563789602187</v>
+      </c>
+      <c r="P122" s="25">
+        <f t="shared" si="4"/>
+        <v>21209.283342305902</v>
+      </c>
+      <c r="Q122" s="2">
+        <f t="shared" si="4"/>
+        <v>1.2149370370370585E-2</v>
+      </c>
+      <c r="R122" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.5008230452674883E-5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B123" s="16"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
+      <c r="F123" s="13"/>
+      <c r="G123" s="13"/>
+      <c r="H123" s="13"/>
+      <c r="I123" s="13"/>
+      <c r="J123" s="13"/>
+      <c r="K123" s="13"/>
+      <c r="L123" s="13"/>
+      <c r="M123" s="13"/>
+      <c r="N123" s="13"/>
+      <c r="O123" s="14"/>
+      <c r="P123" s="14"/>
+      <c r="Q123" s="13"/>
+      <c r="R123" s="15"/>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2"/>
+      <c r="K124" s="2"/>
+      <c r="L124" s="2"/>
+      <c r="M124" s="2"/>
+      <c r="N124" s="2"/>
+      <c r="O124" s="3"/>
+      <c r="P124" s="3"/>
+      <c r="Q124" s="2"/>
+      <c r="R124" s="4"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>16</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B125" t="s">
         <v>93</v>
       </c>
-      <c r="D123" s="2">
+      <c r="D125" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E123" s="2">
+      <c r="E125" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F123" s="2">
+      <c r="F125" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G123" s="2">
+      <c r="G125" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H123" s="2">
+      <c r="H125" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I123" s="2">
+      <c r="I125" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J123" s="2">
+      <c r="J125" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K123" s="2">
+      <c r="K125" s="2">
         <v>673.08737180000003</v>
       </c>
-      <c r="L123" s="2">
+      <c r="L125" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M123" s="2">
+      <c r="M125" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N123" s="2">
+      <c r="N125" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O123" s="3">
+      <c r="O125" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P123" s="3">
+      <c r="P125" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q123" s="2">
+      <c r="Q125" s="2">
         <v>-2.3066774000000003</v>
       </c>
-      <c r="R123" s="4">
+      <c r="R125" s="4">
         <v>-7.1000000000000002E-4</v>
       </c>
-      <c r="S123" t="s">
+      <c r="S125" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>16</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B126" t="s">
         <v>95</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C126" t="s">
         <v>92</v>
       </c>
-      <c r="D124" s="2">
+      <c r="D126" s="2">
         <v>1230.0044677999999</v>
       </c>
-      <c r="E124" s="2">
+      <c r="E126" s="2">
         <v>1848.1456909000001</v>
       </c>
-      <c r="F124" s="2">
+      <c r="F126" s="2">
         <v>1.0573501000000001</v>
       </c>
-      <c r="G124" s="2">
+      <c r="G126" s="2">
         <v>299.4371582</v>
       </c>
-      <c r="H124" s="2">
+      <c r="H126" s="2">
         <v>9.7418259000000003</v>
       </c>
-      <c r="I124" s="2">
+      <c r="I126" s="2">
         <v>5.7446602000000002</v>
       </c>
-      <c r="J124" s="2">
+      <c r="J126" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K124" s="5">
+      <c r="K126" s="5">
         <v>675.4841553</v>
       </c>
-      <c r="L124" s="2">
+      <c r="L126" s="2">
         <v>81.12013859999999</v>
       </c>
-      <c r="M124" s="2">
+      <c r="M126" s="2">
         <v>1432.6230836</v>
       </c>
-      <c r="N124" s="2">
+      <c r="N126" s="2">
         <v>1196.8767700000001</v>
       </c>
-      <c r="O124" s="3">
+      <c r="O126" s="3">
         <v>5429.4087645999998</v>
       </c>
-      <c r="P124" s="3">
+      <c r="P126" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q124" s="5">
+      <c r="Q126" s="5">
         <v>9.0106100000000008E-2</v>
       </c>
-      <c r="R124" s="7">
+      <c r="R126" s="7">
         <v>3.5000000000000063E-6</v>
       </c>
-      <c r="S124" t="s">
+      <c r="S126" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C125" t="s">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C127" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New McKenzie spinup. McKenzie/flow2010.ic, HRU_McKenzie.dbf, Reach_McKenzie.dbf - output from spinup over 2000-09. IDU_McKenzie.dbf was saved on Box in CW3M/DataCW3MfilesTooBigForGitHub. ReachRouting.cpp - #include misc.h instead of UNITCONV.H, because close_enough() has been moved to misc.cpp.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96865CD-6F23-425F-A343-F30C2B52FCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C611B793-632A-4CA5-902F-D7A7CF994380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="171">
   <si>
     <t>Year</t>
   </si>
@@ -543,6 +543,9 @@
   </si>
   <si>
     <t>CW3M C787+</t>
+  </si>
+  <si>
+    <t>CW3M C792+</t>
   </si>
 </sst>
 </file>
@@ -1466,11 +1469,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U127"/>
+  <dimension ref="A1:U128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q123" sqref="Q123:R123"/>
+      <selection pane="bottomLeft" activeCell="Q124" sqref="Q124:R124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8299,88 +8302,85 @@
         <v>6.0733333333333342E-4</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D124" s="2"/>
-      <c r="E124" s="2"/>
-      <c r="F124" s="2"/>
-      <c r="G124" s="2"/>
-      <c r="H124" s="2"/>
-      <c r="I124" s="2"/>
-      <c r="J124" s="2"/>
-      <c r="K124" s="2"/>
-      <c r="L124" s="2"/>
-      <c r="M124" s="2"/>
-      <c r="N124" s="2"/>
-      <c r="O124" s="3"/>
-      <c r="P124" s="3"/>
-      <c r="Q124" s="2"/>
-      <c r="R124" s="4"/>
+    <row r="124" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>170</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C124" t="s">
+        <v>23</v>
+      </c>
+      <c r="D124" s="13">
+        <v>948.8487955555554</v>
+      </c>
+      <c r="E124" s="13">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F124" s="13">
+        <v>0.58118922222222236</v>
+      </c>
+      <c r="G124" s="13">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H124" s="13">
+        <v>0</v>
+      </c>
+      <c r="I124" s="13">
+        <v>0.21021766666666669</v>
+      </c>
+      <c r="J124" s="13">
+        <v>8.1970344444444443</v>
+      </c>
+      <c r="K124" s="13">
+        <v>663.99315055555553</v>
+      </c>
+      <c r="L124" s="13">
+        <v>80.101195444444443</v>
+      </c>
+      <c r="M124" s="13">
+        <v>1409.0905896666666</v>
+      </c>
+      <c r="N124" s="13">
+        <v>951.36199944444445</v>
+      </c>
+      <c r="O124" s="14">
+        <v>4003.2288682222224</v>
+      </c>
+      <c r="P124" s="14">
+        <v>27393.541449666667</v>
+      </c>
+      <c r="Q124" s="5">
+        <v>2.4292164444444446</v>
+      </c>
+      <c r="R124" s="7">
+        <v>6.7188888888888897E-4</v>
+      </c>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>16</v>
-      </c>
-      <c r="B125" t="s">
-        <v>93</v>
-      </c>
-      <c r="D125" s="2">
-        <v>1230.0044677999999</v>
-      </c>
-      <c r="E125" s="2">
-        <v>1848.1456909000001</v>
-      </c>
-      <c r="F125" s="2">
-        <v>1.0573501000000001</v>
-      </c>
-      <c r="G125" s="2">
-        <v>299.4371582</v>
-      </c>
-      <c r="H125" s="2">
-        <v>9.7418259000000003</v>
-      </c>
-      <c r="I125" s="2">
-        <v>5.7446602000000002</v>
-      </c>
-      <c r="J125" s="2">
-        <v>8.1171118999999994</v>
-      </c>
-      <c r="K125" s="2">
-        <v>673.08737180000003</v>
-      </c>
-      <c r="L125" s="2">
-        <v>81.12013859999999</v>
-      </c>
-      <c r="M125" s="2">
-        <v>1432.6230836</v>
-      </c>
-      <c r="N125" s="2">
-        <v>1196.8767700000001</v>
-      </c>
-      <c r="O125" s="3">
-        <v>5429.4087645999998</v>
-      </c>
-      <c r="P125" s="3">
-        <v>27140.258789299998</v>
-      </c>
-      <c r="Q125" s="2">
-        <v>-2.3066774000000003</v>
-      </c>
-      <c r="R125" s="4">
-        <v>-7.1000000000000002E-4</v>
-      </c>
-      <c r="S125" t="s">
-        <v>92</v>
-      </c>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2"/>
+      <c r="K125" s="2"/>
+      <c r="L125" s="2"/>
+      <c r="M125" s="2"/>
+      <c r="N125" s="2"/>
+      <c r="O125" s="3"/>
+      <c r="P125" s="3"/>
+      <c r="Q125" s="2"/>
+      <c r="R125" s="4"/>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>16</v>
       </c>
       <c r="B126" t="s">
-        <v>95</v>
-      </c>
-      <c r="C126" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D126" s="2">
         <v>1230.0044677999999</v>
@@ -8403,8 +8403,8 @@
       <c r="J126" s="2">
         <v>8.1171118999999994</v>
       </c>
-      <c r="K126" s="5">
-        <v>675.4841553</v>
+      <c r="K126" s="2">
+        <v>673.08737180000003</v>
       </c>
       <c r="L126" s="2">
         <v>81.12013859999999</v>
@@ -8421,18 +8421,77 @@
       <c r="P126" s="3">
         <v>27140.258789299998</v>
       </c>
-      <c r="Q126" s="5">
-        <v>9.0106100000000008E-2</v>
-      </c>
-      <c r="R126" s="7">
-        <v>3.5000000000000063E-6</v>
+      <c r="Q126" s="2">
+        <v>-2.3066774000000003</v>
+      </c>
+      <c r="R126" s="4">
+        <v>-7.1000000000000002E-4</v>
       </c>
       <c r="S126" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>16</v>
+      </c>
+      <c r="B127" t="s">
+        <v>95</v>
+      </c>
       <c r="C127" t="s">
+        <v>92</v>
+      </c>
+      <c r="D127" s="2">
+        <v>1230.0044677999999</v>
+      </c>
+      <c r="E127" s="2">
+        <v>1848.1456909000001</v>
+      </c>
+      <c r="F127" s="2">
+        <v>1.0573501000000001</v>
+      </c>
+      <c r="G127" s="2">
+        <v>299.4371582</v>
+      </c>
+      <c r="H127" s="2">
+        <v>9.7418259000000003</v>
+      </c>
+      <c r="I127" s="2">
+        <v>5.7446602000000002</v>
+      </c>
+      <c r="J127" s="2">
+        <v>8.1171118999999994</v>
+      </c>
+      <c r="K127" s="5">
+        <v>675.4841553</v>
+      </c>
+      <c r="L127" s="2">
+        <v>81.12013859999999</v>
+      </c>
+      <c r="M127" s="2">
+        <v>1432.6230836</v>
+      </c>
+      <c r="N127" s="2">
+        <v>1196.8767700000001</v>
+      </c>
+      <c r="O127" s="3">
+        <v>5429.4087645999998</v>
+      </c>
+      <c r="P127" s="3">
+        <v>27140.258789299998</v>
+      </c>
+      <c r="Q127" s="5">
+        <v>9.0106100000000008E-2</v>
+      </c>
+      <c r="R127" s="7">
+        <v>3.5000000000000063E-6</v>
+      </c>
+      <c r="S127" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C128" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit old mods on the Dell desktop dated 4/16/22 to IDU_McKenzie.dbf and IDU_NSantiam.dbf.  I don't know what the mods are. ETEquation::WetlandET() - Prevent the temperature of standing water from going below DEFAULT_MIN_SKIN_TEMP_DEGC. Flow.cpp, HBV.cpp - Loosen two close_enough criteria. WaterMaster.h - #define FIRST_ARTIFICIAL_WATERRIGHTID 1000000
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF01E5A-F857-4287-872D-1E66AC69E24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECADB757-007A-46BB-BDCB-E1D5D36823CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1513,7 +1513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AJ126" sqref="AJ126"/>
     </sheetView>

</xml_diff>

<commit_message>
CW3M_Installer_1.3.0.exe comes from this version, which resulted from phase 3 of the LCOG McKenzie Wetlands project.  It incorporates David Richey’s updated water rights data for the complete Willamette River basin, in DataCW3M/wr_pods_McKenzie.csv and …/wr_pous_McKenzie.csv.  Two columns, UGB and CW3M_YEAR, have been added to the points-of-diversion file.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_McKenzie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECADB757-007A-46BB-BDCB-E1D5D36823CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CA1EF2-6746-45CF-A628-EF5F6F47FB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010 and 2010-18" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="187">
   <si>
     <t>Year</t>
   </si>
@@ -588,6 +588,12 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>CW3M C814</t>
+  </si>
+  <si>
+    <t>Baseline 2010-19</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1107,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1112,7 +1118,6 @@
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1123,13 +1128,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
@@ -1514,8 +1513,8 @@
   <dimension ref="A1:AJ131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ126" sqref="AJ126"/>
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2708,7 +2707,7 @@
       <c r="N20" s="2">
         <v>1207.1636960000001</v>
       </c>
-      <c r="O20" s="9">
+      <c r="O20" s="8">
         <v>6722.8808589999999</v>
       </c>
       <c r="P20" s="3">
@@ -3659,73 +3658,73 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="37" spans="1:19" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37">
         <v>2010</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="2">
         <v>1284.0238039999999</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="2">
         <v>1990.4650879999999</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="2">
         <v>1.443354</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G37" s="2">
         <v>298.60159299999998</v>
       </c>
-      <c r="H37" s="13">
+      <c r="H37" s="2">
         <v>10.610913999999999</v>
       </c>
-      <c r="I37" s="13">
+      <c r="I37" s="2">
         <v>4.8117099999999997</v>
       </c>
-      <c r="J37" s="13">
+      <c r="J37" s="2">
         <v>8.8404570000000007</v>
       </c>
-      <c r="K37" s="13">
+      <c r="K37" s="2">
         <v>737.62927200000001</v>
       </c>
-      <c r="L37" s="13">
+      <c r="L37" s="2">
         <v>93.234084999999993</v>
       </c>
-      <c r="M37" s="13">
+      <c r="M37" s="2">
         <v>1400.039673</v>
       </c>
-      <c r="N37" s="13">
+      <c r="N37" s="2">
         <v>1351.4182129999999</v>
       </c>
-      <c r="O37" s="14">
+      <c r="O37" s="3">
         <v>8159.9951170000004</v>
       </c>
-      <c r="P37" s="14">
+      <c r="P37" s="3">
         <v>29450.638672000001</v>
       </c>
-      <c r="Q37" s="13">
+      <c r="Q37" s="2">
         <v>1.205238</v>
       </c>
-      <c r="R37" s="15">
+      <c r="R37" s="4">
         <v>3.3599999999999998E-4</v>
       </c>
-      <c r="S37" s="8">
+      <c r="S37">
         <v>2010</v>
       </c>
     </row>
-    <row r="38" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38">
         <v>2010</v>
       </c>
       <c r="D38" s="2">
@@ -3773,12 +3772,12 @@
       <c r="R38" s="4">
         <v>-2.7099999999999997E-4</v>
       </c>
-      <c r="S38" s="8">
+      <c r="S38">
         <v>2010</v>
       </c>
     </row>
-    <row r="39" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="17">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B39" s="12">
         <v>44202</v>
       </c>
       <c r="D39" s="2">
@@ -3827,23 +3826,23 @@
         <v>3.4099999999999999E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="16"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="13"/>
-      <c r="R40" s="15"/>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="4"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
@@ -4415,18 +4414,18 @@
       <c r="R50" s="4">
         <v>-2.8933333333333328E-4</v>
       </c>
-      <c r="S50" s="8" t="s">
+      <c r="S50" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A51" s="8" t="s">
+      <c r="A51" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" t="s">
         <v>23</v>
       </c>
       <c r="D51" s="2">
@@ -4474,18 +4473,18 @@
       <c r="R51" s="4">
         <v>-2.8933333333333328E-4</v>
       </c>
-      <c r="S51" s="8" t="s">
+      <c r="S51" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A52" s="8" t="s">
+      <c r="A52" t="s">
         <v>16</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" t="s">
         <v>48</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" t="s">
         <v>23</v>
       </c>
       <c r="D52" s="2">
@@ -4533,18 +4532,18 @@
       <c r="R52" s="4">
         <v>-3.0444444444444448E-4</v>
       </c>
-      <c r="S52" s="8" t="s">
+      <c r="S52" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
+      <c r="A53" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" t="s">
         <v>23</v>
       </c>
       <c r="D53" s="2">
@@ -4593,18 +4592,18 @@
         <f t="shared" ref="E53:R55" si="0">AVERAGE(R44:R52)</f>
         <v>1.3632839506172842E-3</v>
       </c>
-      <c r="S53" s="8" t="s">
+      <c r="S53" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A54" s="8" t="s">
+      <c r="A54" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" t="s">
         <v>23</v>
       </c>
       <c r="D54" s="2">
@@ -4667,18 +4666,18 @@
         <f t="shared" si="0"/>
         <v>1.363093278463649E-3</v>
       </c>
-      <c r="S54" s="8" t="s">
+      <c r="S54" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
+      <c r="A55" t="s">
         <v>16</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" t="s">
         <v>23</v>
       </c>
       <c r="D55" s="2">
@@ -4740,18 +4739,18 @@
       <c r="R55" s="4">
         <v>-2.0755555555555555E-4</v>
       </c>
-      <c r="S55" s="8" t="s">
+      <c r="S55" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
+      <c r="A56" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" t="s">
         <v>23</v>
       </c>
       <c r="D56" s="2">
@@ -4799,18 +4798,18 @@
       <c r="R56" s="4">
         <v>-2.0744444444444445E-4</v>
       </c>
-      <c r="S56" s="8" t="s">
+      <c r="S56" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A57" s="8" t="s">
+      <c r="A57" t="s">
         <v>16</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" t="s">
         <v>23</v>
       </c>
       <c r="D57" s="2">
@@ -4858,18 +4857,18 @@
       <c r="R57" s="4">
         <v>-2.0744444444444445E-4</v>
       </c>
-      <c r="S57" s="8" t="s">
+      <c r="S57" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A58" s="8" t="s">
+      <c r="A58" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" t="s">
         <v>63</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" t="s">
         <v>23</v>
       </c>
       <c r="D58" s="2">
@@ -4917,18 +4916,18 @@
       <c r="R58" s="4">
         <v>-1.7433333333333333E-4</v>
       </c>
-      <c r="S58" s="8" t="s">
+      <c r="S58" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A59" s="8" t="s">
+      <c r="A59" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" t="s">
         <v>64</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" t="s">
         <v>23</v>
       </c>
       <c r="D59" s="2">
@@ -4976,7 +4975,7 @@
       <c r="R59" s="4">
         <v>-1.5888888888888889E-4</v>
       </c>
-      <c r="S59" s="8" t="s">
+      <c r="S59" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4987,7 +4986,7 @@
       <c r="B60" t="s">
         <v>65</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" t="s">
         <v>23</v>
       </c>
       <c r="D60" s="2">
@@ -5035,7 +5034,7 @@
       <c r="R60" s="4">
         <v>-1.5933333333333332E-4</v>
       </c>
-      <c r="S60" s="8" t="s">
+      <c r="S60" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5046,7 +5045,7 @@
       <c r="B61" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" t="s">
         <v>23</v>
       </c>
       <c r="D61" s="5">
@@ -5102,7 +5101,7 @@
       <c r="B62" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C62" t="s">
         <v>23</v>
       </c>
       <c r="D62" s="2">
@@ -5158,7 +5157,7 @@
       <c r="B63" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" t="s">
         <v>23</v>
       </c>
       <c r="D63" s="2">
@@ -5439,7 +5438,7 @@
       <c r="Q67" s="2">
         <v>0.28907633333333327</v>
       </c>
-      <c r="R67" s="15">
+      <c r="R67" s="4">
         <v>6.222222222222222E-5</v>
       </c>
       <c r="S67" t="s">
@@ -5456,46 +5455,46 @@
       <c r="C68" t="s">
         <v>23</v>
       </c>
-      <c r="D68" s="13">
+      <c r="D68" s="2">
         <v>1000.3124864444443</v>
       </c>
-      <c r="E68" s="13">
+      <c r="E68" s="2">
         <v>1763.5263265555557</v>
       </c>
-      <c r="F68" s="13">
+      <c r="F68" s="2">
         <v>0.999942</v>
       </c>
-      <c r="G68" s="13">
+      <c r="G68" s="2">
         <v>305.6782124444444</v>
       </c>
-      <c r="H68" s="13">
+      <c r="H68" s="2">
         <v>9.775355222222224</v>
       </c>
-      <c r="I68" s="13">
+      <c r="I68" s="2">
         <v>6.8948233333333331</v>
       </c>
-      <c r="J68" s="13">
+      <c r="J68" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K68" s="13">
+      <c r="K68" s="2">
         <v>673.17452677777771</v>
       </c>
-      <c r="L68" s="13">
+      <c r="L68" s="2">
         <v>60.018756111111117</v>
       </c>
-      <c r="M68" s="13">
+      <c r="M68" s="2">
         <v>1321.9402533333332</v>
       </c>
-      <c r="N68" s="13">
+      <c r="N68" s="2">
         <v>1024.1975572222223</v>
       </c>
-      <c r="O68" s="14">
+      <c r="O68" s="3">
         <v>4583.9874403333333</v>
       </c>
-      <c r="P68" s="14">
+      <c r="P68" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q68" s="13">
+      <c r="Q68" s="2">
         <v>0.28907633333333327</v>
       </c>
       <c r="R68" s="4">
@@ -5895,7 +5894,7 @@
       <c r="J75" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K75" s="13">
+      <c r="K75" s="2">
         <v>676.83127177777783</v>
       </c>
       <c r="L75" s="2">
@@ -5913,10 +5912,10 @@
       <c r="P75" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q75" s="13">
+      <c r="Q75" s="2">
         <v>0.14695311111111112</v>
       </c>
-      <c r="R75" s="18">
+      <c r="R75" s="13">
         <v>2.0111111111111117E-5</v>
       </c>
     </row>
@@ -5969,7 +5968,7 @@
       <c r="P76" s="3">
         <v>27227.338324888889</v>
       </c>
-      <c r="Q76" s="13">
+      <c r="Q76" s="2">
         <v>0.23182455555555562</v>
       </c>
       <c r="R76" s="4">
@@ -6107,7 +6106,7 @@
       <c r="F79" s="2">
         <v>1.0618724444444443</v>
       </c>
-      <c r="G79" s="13">
+      <c r="G79" s="2">
         <v>270.41205844444437</v>
       </c>
       <c r="H79" s="2">
@@ -6119,13 +6118,13 @@
       <c r="J79" s="2">
         <v>8.145128999999999</v>
       </c>
-      <c r="K79" s="13">
+      <c r="K79" s="2">
         <v>693.57013622222212</v>
       </c>
       <c r="L79" s="2">
         <v>82.308506444444433</v>
       </c>
-      <c r="M79" s="13">
+      <c r="M79" s="2">
         <v>1421.1105007777778</v>
       </c>
       <c r="N79" s="2">
@@ -6378,7 +6377,7 @@
       <c r="C84" t="s">
         <v>23</v>
       </c>
-      <c r="D84" s="19">
+      <c r="D84" s="14">
         <v>1047.3404814444443</v>
       </c>
       <c r="E84" s="2">
@@ -6437,7 +6436,7 @@
       <c r="D85" s="5">
         <v>930.3491414444444</v>
       </c>
-      <c r="E85" s="13">
+      <c r="E85" s="2">
         <v>1890.2624783333331</v>
       </c>
       <c r="F85" s="2">
@@ -6461,7 +6460,7 @@
       <c r="L85" s="5">
         <v>80.17382866666668</v>
       </c>
-      <c r="M85" s="13">
+      <c r="M85" s="2">
         <v>1419.6366374444444</v>
       </c>
       <c r="N85" s="5">
@@ -6480,7 +6479,7 @@
         <v>-1.5666666666666669E-4</v>
       </c>
     </row>
-    <row r="86" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -6490,53 +6489,53 @@
       <c r="C86" t="s">
         <v>23</v>
       </c>
-      <c r="D86" s="13">
+      <c r="D86" s="2">
         <v>930.3491414444444</v>
       </c>
-      <c r="E86" s="13">
+      <c r="E86" s="2">
         <v>1890.2624783333331</v>
       </c>
-      <c r="F86" s="13">
+      <c r="F86" s="2">
         <v>1.0534737777777776</v>
       </c>
-      <c r="G86" s="13">
+      <c r="G86" s="2">
         <v>270.41205844444437</v>
       </c>
-      <c r="H86" s="13">
+      <c r="H86" s="2">
         <v>9.8445367777777779</v>
       </c>
-      <c r="I86" s="13">
+      <c r="I86" s="2">
         <v>7.3367124444444443</v>
       </c>
-      <c r="J86" s="13">
+      <c r="J86" s="2">
         <v>8.2027718888888881</v>
       </c>
-      <c r="K86" s="13">
+      <c r="K86" s="2">
         <v>668.41088177777783</v>
       </c>
-      <c r="L86" s="13">
+      <c r="L86" s="2">
         <v>80.17382866666668</v>
       </c>
-      <c r="M86" s="13">
+      <c r="M86" s="2">
         <v>1419.6366374444444</v>
       </c>
-      <c r="N86" s="13">
+      <c r="N86" s="2">
         <v>932.39704044444443</v>
       </c>
-      <c r="O86" s="14">
+      <c r="O86" s="3">
         <v>5977.3932020000002</v>
       </c>
-      <c r="P86" s="14">
+      <c r="P86" s="3">
         <v>27412.728515555555</v>
       </c>
-      <c r="Q86" s="13">
+      <c r="Q86" s="2">
         <v>-0.43724066666666661</v>
       </c>
-      <c r="R86" s="15">
+      <c r="R86" s="4">
         <v>-1.5666666666666669E-4</v>
       </c>
     </row>
-    <row r="87" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -6546,49 +6545,49 @@
       <c r="C87" t="s">
         <v>23</v>
       </c>
-      <c r="D87" s="13">
+      <c r="D87" s="2">
         <v>930.32731133333334</v>
       </c>
-      <c r="E87" s="13">
+      <c r="E87" s="2">
         <v>1890.2624783333331</v>
       </c>
-      <c r="F87" s="13">
+      <c r="F87" s="2">
         <v>1.0534737777777776</v>
       </c>
-      <c r="G87" s="13">
+      <c r="G87" s="2">
         <v>270.41205844444437</v>
       </c>
-      <c r="H87" s="13">
+      <c r="H87" s="2">
         <v>9.8445367777777779</v>
       </c>
-      <c r="I87" s="13">
+      <c r="I87" s="2">
         <v>7.3405937777777792</v>
       </c>
-      <c r="J87" s="13">
+      <c r="J87" s="2">
         <v>8.2027718888888881</v>
       </c>
-      <c r="K87" s="13">
+      <c r="K87" s="2">
         <v>669.0623984444444</v>
       </c>
-      <c r="L87" s="13">
+      <c r="L87" s="2">
         <v>80.17382866666668</v>
       </c>
-      <c r="M87" s="13">
+      <c r="M87" s="2">
         <v>1418.9927843333332</v>
       </c>
-      <c r="N87" s="13">
+      <c r="N87" s="2">
         <v>932.37144644444436</v>
       </c>
-      <c r="O87" s="14">
+      <c r="O87" s="3">
         <v>5977.3680556666659</v>
       </c>
-      <c r="P87" s="14">
+      <c r="P87" s="3">
         <v>27412.728515555555</v>
       </c>
-      <c r="Q87" s="13">
+      <c r="Q87" s="2">
         <v>-0.43722288888888888</v>
       </c>
-      <c r="R87" s="15">
+      <c r="R87" s="4">
         <v>-1.5677777777777779E-4</v>
       </c>
     </row>
@@ -6641,10 +6640,10 @@
       <c r="P88" s="3">
         <v>27412.728515555555</v>
       </c>
-      <c r="Q88" s="23">
+      <c r="Q88" s="18">
         <v>-25.703044444444444</v>
       </c>
-      <c r="R88" s="24">
+      <c r="R88" s="19">
         <v>-7.9450000000000007E-3</v>
       </c>
     </row>
@@ -6685,7 +6684,7 @@
       <c r="L89" s="2">
         <v>80.5032391111111</v>
       </c>
-      <c r="M89" s="13">
+      <c r="M89" s="2">
         <v>1418.8638372222224</v>
       </c>
       <c r="N89" s="2">
@@ -6697,10 +6696,10 @@
       <c r="P89" s="3">
         <v>27412.728515555555</v>
       </c>
-      <c r="Q89" s="13">
+      <c r="Q89" s="2">
         <v>0.23640099999999997</v>
       </c>
-      <c r="R89" s="15">
+      <c r="R89" s="4">
         <v>4.7777777777777777E-5</v>
       </c>
     </row>
@@ -6741,7 +6740,7 @@
       <c r="L90" s="2">
         <v>80.503111000000018</v>
       </c>
-      <c r="M90" s="13">
+      <c r="M90" s="2">
         <v>1418.4739583333333</v>
       </c>
       <c r="N90" s="2">
@@ -6753,10 +6752,10 @@
       <c r="P90" s="3">
         <v>27412.728515555555</v>
       </c>
-      <c r="Q90" s="13">
+      <c r="Q90" s="2">
         <v>0.15054966666666666</v>
       </c>
-      <c r="R90" s="15">
+      <c r="R90" s="4">
         <v>2.0333333333333334E-5</v>
       </c>
     </row>
@@ -6797,7 +6796,7 @@
       <c r="L91" s="2">
         <v>80.503111000000018</v>
       </c>
-      <c r="M91" s="13">
+      <c r="M91" s="2">
         <v>1418.4597983333331</v>
       </c>
       <c r="N91" s="2">
@@ -6809,10 +6808,10 @@
       <c r="P91" s="3">
         <v>27412.728515555555</v>
       </c>
-      <c r="Q91" s="13">
+      <c r="Q91" s="2">
         <v>0.15504811111111116</v>
       </c>
-      <c r="R91" s="15">
+      <c r="R91" s="4">
         <v>2.1555555555555562E-5</v>
       </c>
     </row>
@@ -6856,7 +6855,7 @@
       <c r="M92" s="2">
         <v>1418.5096842222219</v>
       </c>
-      <c r="N92" s="13">
+      <c r="N92" s="2">
         <v>931.91537133333338</v>
       </c>
       <c r="O92" s="3">
@@ -6868,192 +6867,175 @@
       <c r="Q92" s="2">
         <v>0.15751733333333329</v>
       </c>
-      <c r="R92" s="15">
+      <c r="R92" s="4">
         <v>2.8666666666666658E-5</v>
       </c>
-      <c r="S92" s="15"/>
-    </row>
-    <row r="93" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93"/>
-      <c r="B93"/>
+      <c r="S92" s="4"/>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C93" s="2">
         <v>929.10792377777784</v>
       </c>
-      <c r="D93" s="13"/>
-      <c r="E93" s="20">
+      <c r="D93" s="2"/>
+      <c r="E93" s="15">
         <f>E87/$E95</f>
         <v>0.86752539266866613</v>
       </c>
-      <c r="F93" s="21">
+      <c r="F93" s="16">
         <f>(F87)/$E95</f>
         <v>4.8348589849734502E-4</v>
       </c>
-      <c r="G93" s="20">
+      <c r="G93" s="15">
         <f>G87/$E95</f>
         <v>0.12410410187647543</v>
       </c>
-      <c r="H93" s="21">
+      <c r="H93" s="16">
         <f>H87/$E95</f>
         <v>4.5180950961439771E-3</v>
       </c>
-      <c r="I93" s="20">
+      <c r="I93" s="15">
         <f>I87/$E95</f>
         <v>3.3689244602171388E-3</v>
       </c>
-      <c r="J93" s="20">
+      <c r="J93" s="15">
         <f>J87/$E87</f>
         <v>4.3394882895423969E-3</v>
       </c>
-      <c r="K93" s="20">
+      <c r="K93" s="15">
         <f t="shared" ref="K93:M93" si="1">K87/$E87</f>
         <v>0.35395211306017388</v>
       </c>
-      <c r="L93" s="20">
+      <c r="L93" s="15">
         <f t="shared" si="1"/>
         <v>4.241412480311036E-2</v>
       </c>
-      <c r="M93" s="20">
+      <c r="M93" s="15">
         <f t="shared" si="1"/>
         <v>0.75068557970027316</v>
       </c>
-      <c r="N93" s="13"/>
-      <c r="O93" s="14"/>
-      <c r="P93" s="14"/>
-      <c r="Q93" s="13"/>
-      <c r="R93" s="15"/>
-    </row>
-    <row r="94" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94"/>
-      <c r="B94"/>
-      <c r="C94"/>
-      <c r="D94" s="13"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="21"/>
-      <c r="G94" s="20"/>
-      <c r="H94" s="21"/>
-      <c r="I94" s="20"/>
-      <c r="J94" s="20">
+      <c r="N93" s="2"/>
+      <c r="O93" s="3"/>
+      <c r="P93" s="3"/>
+      <c r="Q93" s="2"/>
+      <c r="R93" s="4"/>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D94" s="2"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="15"/>
+      <c r="H94" s="16"/>
+      <c r="I94" s="15"/>
+      <c r="J94" s="15">
         <f>J87/$M87</f>
         <v>5.7807002117651277E-3</v>
       </c>
-      <c r="K94" s="20">
+      <c r="K94" s="15">
         <f t="shared" ref="K94:M94" si="2">K87/$M87</f>
         <v>0.4715051449389725</v>
       </c>
-      <c r="L94" s="20">
+      <c r="L94" s="15">
         <f t="shared" si="2"/>
         <v>5.6500518925706657E-2</v>
       </c>
-      <c r="M94" s="20">
+      <c r="M94" s="15">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N94" s="13"/>
-      <c r="O94" s="14"/>
-      <c r="P94" s="14"/>
-      <c r="Q94" s="13"/>
-      <c r="R94" s="15"/>
-    </row>
-    <row r="95" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95"/>
-      <c r="B95"/>
-      <c r="C95"/>
-      <c r="D95" s="13"/>
-      <c r="E95" s="13">
+      <c r="N94" s="2"/>
+      <c r="O94" s="3"/>
+      <c r="P94" s="3"/>
+      <c r="Q94" s="2"/>
+      <c r="R94" s="4"/>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D95" s="2"/>
+      <c r="E95" s="2">
         <f>SUM(E87:I87)</f>
         <v>2178.9131411111107</v>
       </c>
-      <c r="F95" s="20">
+      <c r="F95" s="15">
         <f>F93+H93</f>
         <v>5.0015809946413218E-3</v>
       </c>
-      <c r="G95" s="13"/>
-      <c r="H95" s="13"/>
-      <c r="I95" s="13"/>
-      <c r="J95" s="13">
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2">
         <f>SUM(J87:M87)</f>
         <v>2176.4317833333334</v>
       </c>
-      <c r="K95" s="13"/>
-      <c r="L95" s="13"/>
-      <c r="M95" s="13">
+      <c r="K95" s="2"/>
+      <c r="L95" s="2"/>
+      <c r="M95" s="2">
         <f>(M87/1000)*3307080000/(365.25*24*60*60)</f>
         <v>148.70340764865134</v>
       </c>
-      <c r="N95" s="13"/>
-      <c r="O95" s="14"/>
-      <c r="P95" s="14"/>
-      <c r="Q95" s="13"/>
-      <c r="R95" s="15"/>
-    </row>
-    <row r="96" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96"/>
-      <c r="B96"/>
-      <c r="C96"/>
-      <c r="D96" s="13"/>
-      <c r="E96" s="13"/>
-      <c r="F96" s="20"/>
-      <c r="G96" s="13"/>
-      <c r="H96" s="13"/>
-      <c r="I96" s="13"/>
-      <c r="J96" s="20">
+      <c r="N95" s="2"/>
+      <c r="O95" s="3"/>
+      <c r="P95" s="3"/>
+      <c r="Q95" s="2"/>
+      <c r="R95" s="4"/>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="15">
         <f>J95/E87</f>
         <v>1.1513913058531</v>
       </c>
-      <c r="K96" s="13"/>
-      <c r="L96" s="13"/>
-      <c r="M96" s="13"/>
-      <c r="N96" s="13"/>
-      <c r="O96" s="14"/>
-      <c r="P96" s="14"/>
-      <c r="Q96" s="13"/>
-      <c r="R96" s="15"/>
-    </row>
-    <row r="97" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97"/>
-      <c r="B97"/>
-      <c r="C97"/>
-      <c r="D97" s="13"/>
-      <c r="E97" s="13"/>
-      <c r="F97" s="20"/>
-      <c r="G97" s="13"/>
-      <c r="H97" s="13"/>
-      <c r="I97" s="13"/>
-      <c r="J97" s="22">
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
+      <c r="M96" s="2"/>
+      <c r="N96" s="2"/>
+      <c r="O96" s="3"/>
+      <c r="P96" s="3"/>
+      <c r="Q96" s="2"/>
+      <c r="R96" s="4"/>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="17">
         <f>J95-E95</f>
         <v>-2.481357777777248</v>
       </c>
-      <c r="K97" s="13"/>
-      <c r="L97" s="13"/>
-      <c r="M97" s="13"/>
-      <c r="N97" s="13"/>
-      <c r="O97" s="14"/>
-      <c r="P97" s="14"/>
-      <c r="Q97" s="13"/>
-      <c r="R97" s="15"/>
-    </row>
-    <row r="98" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98"/>
-      <c r="B98"/>
-      <c r="C98"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="20"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-      <c r="J98" s="21">
+      <c r="K97" s="2"/>
+      <c r="L97" s="2"/>
+      <c r="M97" s="2"/>
+      <c r="N97" s="2"/>
+      <c r="O97" s="3"/>
+      <c r="P97" s="3"/>
+      <c r="Q97" s="2"/>
+      <c r="R97" s="4"/>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="J98" s="16">
         <f>J97/E95</f>
         <v>-1.1388052745011715E-3</v>
       </c>
-      <c r="K98" s="13"/>
-      <c r="L98" s="13"/>
-      <c r="M98" s="13"/>
-      <c r="N98" s="13"/>
-      <c r="O98" s="14"/>
-      <c r="P98" s="14"/>
-      <c r="Q98" s="13"/>
-      <c r="R98" s="15"/>
+      <c r="K98" s="2"/>
+      <c r="L98" s="2"/>
+      <c r="M98" s="2"/>
+      <c r="N98" s="2"/>
+      <c r="O98" s="3"/>
+      <c r="P98" s="3"/>
+      <c r="Q98" s="2"/>
+      <c r="R98" s="4"/>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D99" s="2">
@@ -7075,46 +7057,46 @@
       <c r="D101" s="5">
         <v>928.42462833333332</v>
       </c>
-      <c r="E101" s="13">
+      <c r="E101" s="2">
         <v>1890.2624918888889</v>
       </c>
-      <c r="F101" s="13">
+      <c r="F101" s="2">
         <v>0.97914977777777779</v>
       </c>
-      <c r="G101" s="13">
+      <c r="G101" s="2">
         <v>270.41205844444437</v>
       </c>
-      <c r="H101" s="13">
+      <c r="H101" s="2">
         <v>9.8445367777777779</v>
       </c>
-      <c r="I101" s="13">
+      <c r="I101" s="2">
         <v>7.3341234444444439</v>
       </c>
-      <c r="J101" s="13">
+      <c r="J101" s="2">
         <v>8.2027718888888881</v>
       </c>
-      <c r="K101" s="13">
+      <c r="K101" s="2">
         <v>669.07213688888896</v>
       </c>
-      <c r="L101" s="13">
+      <c r="L101" s="2">
         <v>80.17382866666668</v>
       </c>
       <c r="M101" s="5">
         <v>1393.0887585555556</v>
       </c>
-      <c r="N101" s="13">
+      <c r="N101" s="2">
         <v>930.93472622222225</v>
       </c>
-      <c r="O101" s="14">
+      <c r="O101" s="3">
         <v>5483.3967555555555</v>
       </c>
-      <c r="P101" s="14">
+      <c r="P101" s="3">
         <v>27412.728515555555</v>
       </c>
-      <c r="Q101" s="23">
+      <c r="Q101" s="18">
         <v>-25.78476622222222</v>
       </c>
-      <c r="R101" s="24">
+      <c r="R101" s="19">
         <v>-7.9697777777777788E-3</v>
       </c>
     </row>
@@ -7167,10 +7149,10 @@
       <c r="P102" s="3">
         <v>27412.728515555555</v>
       </c>
-      <c r="Q102" s="23">
+      <c r="Q102" s="18">
         <v>-25.791903222222221</v>
       </c>
-      <c r="R102" s="24">
+      <c r="R102" s="19">
         <v>-7.9711111111111128E-3</v>
       </c>
     </row>
@@ -7223,10 +7205,10 @@
       <c r="P103" s="3">
         <v>27412.728515555555</v>
       </c>
-      <c r="Q103" s="13">
+      <c r="Q103" s="2">
         <v>0.15698588888888887</v>
       </c>
-      <c r="R103" s="15">
+      <c r="R103" s="4">
         <v>2.8555555555555569E-5</v>
       </c>
     </row>
@@ -7579,50 +7561,50 @@
       <c r="D110" s="5">
         <v>936.27124700000002</v>
       </c>
-      <c r="E110" s="13">
+      <c r="E110" s="2">
         <v>1890.2624918888889</v>
       </c>
-      <c r="F110" s="13">
+      <c r="F110" s="2">
         <v>1.1353011111111111</v>
       </c>
-      <c r="G110" s="13">
+      <c r="G110" s="2">
         <v>270.41205844444437</v>
       </c>
-      <c r="H110" s="13">
+      <c r="H110" s="2">
         <v>9.8446185555555559</v>
       </c>
-      <c r="I110" s="13">
+      <c r="I110" s="2">
         <v>7.3262145555555556</v>
       </c>
-      <c r="J110" s="13">
+      <c r="J110" s="2">
         <v>8.202840444444444</v>
       </c>
-      <c r="K110" s="13">
+      <c r="K110" s="2">
         <v>664.88439922222221</v>
       </c>
-      <c r="L110" s="13">
+      <c r="L110" s="2">
         <v>80.365177222222229</v>
       </c>
-      <c r="M110" s="13">
+      <c r="M110" s="2">
         <v>1422.648356222222</v>
       </c>
       <c r="N110" s="5">
         <v>939.30824099999984</v>
       </c>
-      <c r="O110" s="14">
+      <c r="O110" s="3">
         <v>6416.2319064444446</v>
       </c>
-      <c r="P110" s="14">
+      <c r="P110" s="3">
         <v>27412.947482666666</v>
       </c>
-      <c r="Q110" s="13">
+      <c r="Q110" s="2">
         <v>0.15708244444444447</v>
       </c>
-      <c r="R110" s="15">
+      <c r="R110" s="4">
         <v>-6.8888888888889176E-6</v>
       </c>
     </row>
-    <row r="111" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>148</v>
       </c>
@@ -7632,49 +7614,49 @@
       <c r="C111" t="s">
         <v>23</v>
       </c>
-      <c r="D111" s="13">
+      <c r="D111" s="2">
         <v>936.4586451111112</v>
       </c>
-      <c r="E111" s="13">
+      <c r="E111" s="2">
         <v>1890.2624918888889</v>
       </c>
-      <c r="F111" s="13">
+      <c r="F111" s="2">
         <v>1.1353011111111111</v>
       </c>
-      <c r="G111" s="13">
+      <c r="G111" s="2">
         <v>270.41205844444437</v>
       </c>
-      <c r="H111" s="13">
+      <c r="H111" s="2">
         <v>9.8446185555555559</v>
       </c>
-      <c r="I111" s="13">
+      <c r="I111" s="2">
         <v>7.3262146666666679</v>
       </c>
-      <c r="J111" s="13">
+      <c r="J111" s="2">
         <v>8.202840444444444</v>
       </c>
-      <c r="K111" s="13">
+      <c r="K111" s="2">
         <v>664.89181855555546</v>
       </c>
-      <c r="L111" s="13">
+      <c r="L111" s="2">
         <v>80.365177222222229</v>
       </c>
-      <c r="M111" s="13">
+      <c r="M111" s="2">
         <v>1422.6016167777777</v>
       </c>
-      <c r="N111" s="13">
+      <c r="N111" s="2">
         <v>939.5350204444444</v>
       </c>
-      <c r="O111" s="14">
+      <c r="O111" s="3">
         <v>6416.2319064444446</v>
       </c>
-      <c r="P111" s="14">
+      <c r="P111" s="3">
         <v>27412.947482666666</v>
       </c>
-      <c r="Q111" s="13">
+      <c r="Q111" s="2">
         <v>0.15714333333333327</v>
       </c>
-      <c r="R111" s="15">
+      <c r="R111" s="4">
         <v>4.0333333333333261E-5</v>
       </c>
     </row>
@@ -7780,7 +7762,7 @@
       <c r="O113" s="6">
         <v>4565.8835446666662</v>
       </c>
-      <c r="P113" s="25">
+      <c r="P113" s="20">
         <v>1017.8816121111109</v>
       </c>
       <c r="Q113" s="2">
@@ -7793,73 +7775,73 @@
         <v>153</v>
       </c>
     </row>
-    <row r="114" spans="1:36" s="26" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A114" s="26" t="s">
+    <row r="114" spans="1:36" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A114" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="B114" s="27" t="s">
+      <c r="B114" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="C114" s="26" t="s">
+      <c r="C114" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D114" s="28">
+      <c r="D114" s="23">
         <f>AVERAGE(D105:D113)</f>
         <v>932.52751403703689</v>
       </c>
-      <c r="E114" s="28">
+      <c r="E114" s="23">
         <f t="shared" ref="E114:R114" si="3">AVERAGE(E105:E113)</f>
         <v>1890.2624918888889</v>
       </c>
-      <c r="F114" s="28">
+      <c r="F114" s="23">
         <f t="shared" si="3"/>
         <v>1.0491967654320991</v>
       </c>
-      <c r="G114" s="28">
+      <c r="G114" s="23">
         <f t="shared" si="3"/>
         <v>270.41205844444443</v>
       </c>
-      <c r="H114" s="28">
+      <c r="H114" s="23">
         <f t="shared" si="3"/>
         <v>8.7525930740740741</v>
       </c>
-      <c r="I114" s="28">
+      <c r="I114" s="23">
         <f t="shared" si="3"/>
         <v>7.3194422222222233</v>
       </c>
-      <c r="J114" s="28">
+      <c r="J114" s="23">
         <f t="shared" si="3"/>
         <v>7.2929307283950617</v>
       </c>
-      <c r="K114" s="28">
+      <c r="K114" s="23">
         <f t="shared" si="3"/>
         <v>666.25400646913602</v>
       </c>
-      <c r="L114" s="28">
+      <c r="L114" s="23">
         <f t="shared" si="3"/>
         <v>80.414587382716064</v>
       </c>
-      <c r="M114" s="28">
+      <c r="M114" s="23">
         <f t="shared" si="3"/>
         <v>1420.9680507407409</v>
       </c>
-      <c r="N114" s="28">
+      <c r="N114" s="23">
         <f t="shared" si="3"/>
         <v>935.55100653086402</v>
       </c>
-      <c r="O114" s="29">
+      <c r="O114" s="24">
         <f t="shared" si="3"/>
         <v>5988.6604757530858</v>
       </c>
-      <c r="P114" s="29">
+      <c r="P114" s="24">
         <f t="shared" si="3"/>
         <v>24485.1996158642</v>
       </c>
-      <c r="Q114" s="28">
+      <c r="Q114" s="23">
         <f t="shared" si="3"/>
         <v>0.15728533333333333</v>
       </c>
-      <c r="R114" s="30">
+      <c r="R114" s="25">
         <f t="shared" si="3"/>
         <v>2.6925925925925932E-5</v>
       </c>
@@ -7907,10 +7889,10 @@
       <c r="N115" s="2">
         <v>939.32236066666655</v>
       </c>
-      <c r="O115" s="14">
+      <c r="O115" s="3">
         <v>4509.0119630000008</v>
       </c>
-      <c r="P115" s="14">
+      <c r="P115" s="3">
         <v>1017.8816121111109</v>
       </c>
       <c r="Q115" s="2">
@@ -7963,7 +7945,7 @@
       <c r="N116" s="2">
         <v>939.31270344444442</v>
       </c>
-      <c r="O116" s="14">
+      <c r="O116" s="3">
         <v>4509.0119630000008</v>
       </c>
       <c r="P116" s="6">
@@ -8019,10 +8001,10 @@
       <c r="N117" s="2">
         <v>937.72368688888901</v>
       </c>
-      <c r="O117" s="14">
+      <c r="O117" s="3">
         <v>4509.0119630000008</v>
       </c>
-      <c r="P117" s="14">
+      <c r="P117" s="3">
         <v>27393.764540111111</v>
       </c>
       <c r="Q117" s="2">
@@ -8075,10 +8057,10 @@
       <c r="N118" s="2">
         <v>937.57624644444456</v>
       </c>
-      <c r="O118" s="14">
+      <c r="O118" s="3">
         <v>4509.0119630000008</v>
       </c>
-      <c r="P118" s="14">
+      <c r="P118" s="3">
         <v>27393.764540111111</v>
       </c>
       <c r="Q118" s="2">
@@ -8314,7 +8296,7 @@
         <f t="shared" si="4"/>
         <v>4584.1563789602187</v>
       </c>
-      <c r="P122" s="25">
+      <c r="P122" s="20">
         <f t="shared" si="4"/>
         <v>21209.283342305902</v>
       </c>
@@ -8327,7 +8309,7 @@
         <v>-1.5008230452674883E-5</v>
       </c>
     </row>
-    <row r="123" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>169</v>
       </c>
@@ -8340,31 +8322,31 @@
       <c r="D123" s="5">
         <v>948.81717255555566</v>
       </c>
-      <c r="E123" s="13">
+      <c r="E123" s="2">
         <v>1890.2624918888889</v>
       </c>
-      <c r="F123" s="13">
+      <c r="F123" s="2">
         <v>0.58185044444444445</v>
       </c>
-      <c r="G123" s="13">
+      <c r="G123" s="2">
         <v>270.41205844444437</v>
       </c>
-      <c r="H123" s="13">
+      <c r="H123" s="2">
         <v>0</v>
       </c>
       <c r="I123" s="5">
         <v>0.4085577777777778</v>
       </c>
-      <c r="J123" s="13">
+      <c r="J123" s="2">
         <v>8.1970344444444443</v>
       </c>
-      <c r="K123" s="13">
+      <c r="K123" s="2">
         <v>663.99837922222218</v>
       </c>
-      <c r="L123" s="13">
+      <c r="L123" s="2">
         <v>80.101195444444443</v>
       </c>
-      <c r="M123" s="13">
+      <c r="M123" s="2">
         <v>1409.1117893333333</v>
       </c>
       <c r="N123" s="5">
@@ -8373,7 +8355,7 @@
       <c r="O123" s="6">
         <v>4003.1481661111111</v>
       </c>
-      <c r="P123" s="14">
+      <c r="P123" s="3">
         <v>27393.541449666667</v>
       </c>
       <c r="Q123" s="5">
@@ -8383,7 +8365,7 @@
         <v>6.0733333333333342E-4</v>
       </c>
     </row>
-    <row r="124" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>170</v>
       </c>
@@ -8393,43 +8375,43 @@
       <c r="C124" t="s">
         <v>23</v>
       </c>
-      <c r="D124" s="13">
+      <c r="D124" s="2">
         <v>948.8487955555554</v>
       </c>
-      <c r="E124" s="13">
+      <c r="E124" s="2">
         <v>1890.2624918888889</v>
       </c>
-      <c r="F124" s="13">
+      <c r="F124" s="2">
         <v>0.58118922222222236</v>
       </c>
-      <c r="G124" s="13">
+      <c r="G124" s="2">
         <v>270.41205844444437</v>
       </c>
-      <c r="H124" s="13">
+      <c r="H124" s="2">
         <v>0</v>
       </c>
-      <c r="I124" s="13">
+      <c r="I124" s="2">
         <v>0.21021766666666669</v>
       </c>
-      <c r="J124" s="13">
+      <c r="J124" s="2">
         <v>8.1970344444444443</v>
       </c>
-      <c r="K124" s="13">
+      <c r="K124" s="2">
         <v>663.99315055555553</v>
       </c>
-      <c r="L124" s="13">
+      <c r="L124" s="2">
         <v>80.101195444444443</v>
       </c>
-      <c r="M124" s="13">
+      <c r="M124" s="2">
         <v>1409.0905896666666</v>
       </c>
-      <c r="N124" s="13">
+      <c r="N124" s="2">
         <v>951.36199944444445</v>
       </c>
-      <c r="O124" s="14">
+      <c r="O124" s="3">
         <v>4003.2288682222224</v>
       </c>
-      <c r="P124" s="14">
+      <c r="P124" s="3">
         <v>27393.541449666667</v>
       </c>
       <c r="Q124" s="5">
@@ -8541,21 +8523,60 @@
       </c>
     </row>
     <row r="126" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="D126" s="2"/>
-      <c r="E126" s="2"/>
-      <c r="F126" s="2"/>
-      <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
-      <c r="I126" s="2"/>
-      <c r="J126" s="2"/>
-      <c r="K126" s="2"/>
-      <c r="L126" s="2"/>
-      <c r="M126" s="2"/>
-      <c r="N126" s="2"/>
-      <c r="O126" s="3"/>
-      <c r="P126" s="3"/>
-      <c r="Q126" s="2"/>
-      <c r="R126" s="4"/>
+      <c r="A126" t="s">
+        <v>185</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C126" t="s">
+        <v>23</v>
+      </c>
+      <c r="D126" s="2">
+        <v>946.20556644444434</v>
+      </c>
+      <c r="E126" s="2">
+        <v>1890.2624918888889</v>
+      </c>
+      <c r="F126" s="2">
+        <v>0.6274696666666667</v>
+      </c>
+      <c r="G126" s="2">
+        <v>270.41205844444437</v>
+      </c>
+      <c r="H126" s="2">
+        <v>0</v>
+      </c>
+      <c r="I126" s="2">
+        <v>0.20011922222222223</v>
+      </c>
+      <c r="J126" s="2">
+        <v>8.1970344444444443</v>
+      </c>
+      <c r="K126" s="2">
+        <v>664.92974855555565</v>
+      </c>
+      <c r="L126" s="2">
+        <v>80.288159777777793</v>
+      </c>
+      <c r="M126" s="2">
+        <v>1407.7394747777778</v>
+      </c>
+      <c r="N126" s="2">
+        <v>948.86118577777779</v>
+      </c>
+      <c r="O126" s="6">
+        <v>3445.6750623333337</v>
+      </c>
+      <c r="P126" s="3">
+        <v>27393.541449666667</v>
+      </c>
+      <c r="Q126" s="2">
+        <v>2.3078975555555554</v>
+      </c>
+      <c r="R126" s="4">
+        <v>6.2833333333333328E-4</v>
+      </c>
     </row>
     <row r="127" spans="1:36" x14ac:dyDescent="0.3">
       <c r="D127" s="2"/>
@@ -8707,8 +8728,59 @@
       </c>
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>185</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="C131" t="s">
         <v>92</v>
+      </c>
+      <c r="D131" s="2">
+        <v>939.54613649999988</v>
+      </c>
+      <c r="E131" s="2">
+        <v>1848.1457030999998</v>
+      </c>
+      <c r="F131" s="2">
+        <v>0.62118279999999992</v>
+      </c>
+      <c r="G131" s="2">
+        <v>270.39560539999991</v>
+      </c>
+      <c r="H131" s="2">
+        <v>0</v>
+      </c>
+      <c r="I131" s="2">
+        <v>0.19461389999999998</v>
+      </c>
+      <c r="J131" s="2">
+        <v>8.1640606999999985</v>
+      </c>
+      <c r="K131" s="2">
+        <v>665.77648320000003</v>
+      </c>
+      <c r="L131" s="2">
+        <v>79.338552200000009</v>
+      </c>
+      <c r="M131" s="2">
+        <v>1380.8797241</v>
+      </c>
+      <c r="N131" s="2">
+        <v>926.97863170000005</v>
+      </c>
+      <c r="O131" s="3">
+        <v>3369.6831420000003</v>
+      </c>
+      <c r="P131" s="3">
+        <v>27290.518554700004</v>
+      </c>
+      <c r="Q131" s="2">
+        <v>2.2342098999999997</v>
+      </c>
+      <c r="R131" s="4">
+        <v>6.2549999999999997E-4</v>
       </c>
     </row>
   </sheetData>
@@ -8739,49 +8811,49 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="11" t="s">
         <v>14</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -8963,7 +9035,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -8976,28 +9048,28 @@
       <c r="D5" s="5">
         <v>1172.1919312</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="2">
         <v>1790.8486085</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="2">
         <v>1.0922978000000001</v>
       </c>
       <c r="G5" s="5">
         <v>270.46964409999998</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="2">
         <v>9.3183378000000001</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="2">
         <v>6.7556768000000007</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="2">
         <v>7.7646284999999988</v>
       </c>
       <c r="K5" s="5">
         <v>688.43201299999998</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="2">
         <v>85.286533800000001</v>
       </c>
       <c r="M5" s="5">
@@ -9009,17 +9081,17 @@
       <c r="O5" s="6">
         <v>6275.9019530999994</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="3">
         <v>25979.647461100001</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="2">
         <v>-0.40740790000000005</v>
       </c>
-      <c r="R5" s="15">
+      <c r="R5" s="4">
         <v>-1.683E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -9032,50 +9104,50 @@
       <c r="D6" s="5">
         <v>710.48948979999989</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="2">
         <v>1790.8486085</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="2">
         <v>1.0913157999999998</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="2">
         <v>270.46964409999998</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="2">
         <v>9.3450500000000005</v>
       </c>
       <c r="I6" s="5">
         <v>9.9604478000000007</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="2">
         <v>7.7868856999999991</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="2">
         <v>681.48979490000011</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="2">
         <v>84.457442000000015</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="2">
         <v>1242.3430969999999</v>
       </c>
       <c r="N6" s="5">
         <v>775.89280400000007</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="3">
         <v>6120.3169676999996</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="3">
         <v>26051.2640627</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="2">
         <v>-0.23453229999999983</v>
       </c>
-      <c r="R6" s="15">
+      <c r="R6" s="4">
         <v>-1.3900000000000007E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -9131,7 +9203,7 @@
         <v>-2.0030000000000004E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -9141,43 +9213,43 @@
       <c r="C8" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="2">
         <v>712.12102060000007</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="2">
         <v>1790.8486085</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="2">
         <v>1.0089707999999999</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="2">
         <v>270.46964409999998</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="2">
         <v>9.3802727000000008</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="2">
         <v>9.5556570000000001</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="2">
         <v>7.8162368999999998</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="2">
         <v>669.23419800000011</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="2">
         <v>83.385008899999988</v>
       </c>
       <c r="M8" s="5">
         <v>1232.4494689999997</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="2">
         <v>781.45020760000011</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="3">
         <v>5728.1892335000002</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8" s="3">
         <v>26145.6904297</v>
       </c>
       <c r="Q8" s="5">

</xml_diff>